<commit_message>
check in weekly contest
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huanminw\Documents\GitHub\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59760CB-E84B-493E-80D9-FB85F98E9B0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162F1B0F-4E4E-45BD-9613-AF41D7957F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6204" uniqueCount="2332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6224" uniqueCount="2340">
   <si>
     <t>Difficulty</t>
   </si>
@@ -7030,6 +7030,30 @@
   </si>
   <si>
     <t>remember longest inreasing path by priority queue</t>
+  </si>
+  <si>
+    <t>Decrypt String from Alphabet to Integer Mapping</t>
+  </si>
+  <si>
+    <t>when see '#' pop up two digits.</t>
+  </si>
+  <si>
+    <t>XOR Queries of a Subarray</t>
+  </si>
+  <si>
+    <t>Accumulate XOR result</t>
+  </si>
+  <si>
+    <t>Get Watched Videos by Your Friends</t>
+  </si>
+  <si>
+    <t>BFS multiple levels.</t>
+  </si>
+  <si>
+    <t>Minimum Insertion Steps to Make a String Palindrome</t>
+  </si>
+  <si>
+    <t>From center and spread.</t>
   </si>
 </sst>
 </file>
@@ -7495,8 +7519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A313" sqref="A313"/>
+    <sheetView tabSelected="1" topLeftCell="C1200" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1207" sqref="G1207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -34861,16 +34885,96 @@
       </c>
     </row>
     <row r="1203" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1203" s="1"/>
+      <c r="A1203" s="25">
+        <v>1309</v>
+      </c>
+      <c r="B1203" s="1" t="s">
+        <v>2332</v>
+      </c>
+      <c r="C1203" s="25">
+        <v>2</v>
+      </c>
+      <c r="D1203" s="25" t="s">
+        <v>1745</v>
+      </c>
+      <c r="E1203" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1203" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1203" s="25" t="s">
+        <v>2333</v>
+      </c>
     </row>
     <row r="1204" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1204" s="1"/>
+      <c r="A1204" s="25">
+        <v>1310</v>
+      </c>
+      <c r="B1204" s="1" t="s">
+        <v>2334</v>
+      </c>
+      <c r="C1204" s="25">
+        <v>2</v>
+      </c>
+      <c r="D1204" s="25" t="s">
+        <v>1729</v>
+      </c>
+      <c r="E1204" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1204" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1204" s="25" t="s">
+        <v>2335</v>
+      </c>
     </row>
     <row r="1205" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1205" s="1"/>
+      <c r="A1205" s="25">
+        <v>1311</v>
+      </c>
+      <c r="B1205" s="1" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C1205" s="25">
+        <v>3</v>
+      </c>
+      <c r="D1205" s="25" t="s">
+        <v>1729</v>
+      </c>
+      <c r="E1205" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1205" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1205" s="25" t="s">
+        <v>2337</v>
+      </c>
     </row>
     <row r="1206" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1206" s="1"/>
+      <c r="A1206" s="25">
+        <v>1312</v>
+      </c>
+      <c r="B1206" s="1" t="s">
+        <v>2338</v>
+      </c>
+      <c r="C1206" s="25">
+        <v>4</v>
+      </c>
+      <c r="D1206" s="25" t="s">
+        <v>1729</v>
+      </c>
+      <c r="E1206" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1206" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1206" s="25" t="s">
+        <v>2339</v>
+      </c>
     </row>
     <row r="1207" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1207" s="1"/>
@@ -36169,10 +36273,14 @@
     <hyperlink ref="B1200" r:id="rId1179" display="https://leetcode.com/problems/all-elements-in-two-binary-search-trees" xr:uid="{839770B3-19A7-4975-B887-10D83B9A1D4B}"/>
     <hyperlink ref="B1201" r:id="rId1180" display="https://leetcode.com/problems/jump-game-iii" xr:uid="{F3C143FE-C17D-4131-9591-73C55ED450EB}"/>
     <hyperlink ref="B1202" r:id="rId1181" display="https://leetcode.com/problems/verbal-arithmetic-puzzle" xr:uid="{D531DE7D-75A1-4D4D-AC23-47920A8862FB}"/>
+    <hyperlink ref="B1203" r:id="rId1182" display="https://leetcode.com/problems/decrypt-string-from-alphabet-to-integer-mapping" xr:uid="{A837B942-BA22-4040-AFCB-3F648582CC69}"/>
+    <hyperlink ref="B1204" r:id="rId1183" display="https://leetcode.com/problems/xor-queries-of-a-subarray" xr:uid="{77587CC1-552C-477A-935B-6DC30EA5C97E}"/>
+    <hyperlink ref="B1205" r:id="rId1184" display="https://leetcode.com/problems/get-watched-videos-by-your-friends" xr:uid="{84DE9E01-6267-4BA0-8D20-715102257B01}"/>
+    <hyperlink ref="B1206" r:id="rId1185" display="https://leetcode.com/problems/minimum-insertion-steps-to-make-a-string-palindrome" xr:uid="{80F52E65-1E86-42B3-9A72-4BE50D111D0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1182"/>
-  <drawing r:id="rId1183"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1186"/>
+  <drawing r:id="rId1187"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Code refactoring for String
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huanminw\Documents\GitHub\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365210F4-8B80-4EC3-9F49-E0F8FF778837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B66222-03E6-483A-8788-EDB1C0208798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6264" uniqueCount="2356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6265" uniqueCount="2356">
   <si>
     <t>Difficulty</t>
   </si>
@@ -7567,8 +7567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A736" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A746" sqref="A746"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D415" sqref="D415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16862,6 +16862,9 @@
       </c>
       <c r="C415">
         <v>4</v>
+      </c>
+      <c r="D415" t="s">
+        <v>1777</v>
       </c>
       <c r="E415" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
check in weekly contest part I
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huanminw\Documents\GitHub\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C624D146-A1B2-4B5D-949D-B4C9852B2477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4E10FB-265A-43BD-A3D5-1700B1B32CE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6290" uniqueCount="2365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6310" uniqueCount="2373">
   <si>
     <t>Difficulty</t>
   </si>
@@ -7129,6 +7129,30 @@
   </si>
   <si>
     <t>Check every number pair based on the sequence, count the length of arithmetic slices</t>
+  </si>
+  <si>
+    <t>Break a Palindrome </t>
+  </si>
+  <si>
+    <t>Sort the Matrix Diagonally</t>
+  </si>
+  <si>
+    <t>Reverse Subarray To Maximize Array Value</t>
+  </si>
+  <si>
+    <t>Rank Transform of an Array </t>
+  </si>
+  <si>
+    <t>Change the left most non a to a, or change the last a to b</t>
+  </si>
+  <si>
+    <t>Start from first row or col, loop until out of boundary</t>
+  </si>
+  <si>
+    <t>Calculate max of minium of neighbor pair and min of max of neighbor pair</t>
+  </si>
+  <si>
+    <t>Use map with value as key, index array as value.</t>
   </si>
 </sst>
 </file>
@@ -7594,8 +7618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A420" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C429" sqref="C429"/>
+    <sheetView tabSelected="1" topLeftCell="A1210" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1229" sqref="G1229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -35346,16 +35370,96 @@
       </c>
     </row>
     <row r="1219" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1219" s="1"/>
+      <c r="A1219" s="25">
+        <v>1328</v>
+      </c>
+      <c r="B1219" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C1219" s="25">
+        <v>2</v>
+      </c>
+      <c r="D1219" s="25" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E1219" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1219" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1219" s="25" t="s">
+        <v>2369</v>
+      </c>
     </row>
     <row r="1220" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1220" s="1"/>
+      <c r="A1220" s="25">
+        <v>1329</v>
+      </c>
+      <c r="B1220" s="1" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C1220" s="25">
+        <v>3</v>
+      </c>
+      <c r="D1220" s="25" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E1220" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1220" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1220" s="25" t="s">
+        <v>2370</v>
+      </c>
     </row>
     <row r="1221" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1221" s="1"/>
+      <c r="A1221" s="25">
+        <v>1330</v>
+      </c>
+      <c r="B1221" s="1" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C1221" s="25">
+        <v>4</v>
+      </c>
+      <c r="D1221" s="25" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E1221" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1221" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1221" s="25" t="s">
+        <v>2371</v>
+      </c>
     </row>
     <row r="1222" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1222" s="1"/>
+      <c r="A1222" s="25">
+        <v>1331</v>
+      </c>
+      <c r="B1222" s="1" t="s">
+        <v>2368</v>
+      </c>
+      <c r="C1222" s="25">
+        <v>3</v>
+      </c>
+      <c r="D1222" s="25" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E1222" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1222" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1222" s="25" t="s">
+        <v>2372</v>
+      </c>
     </row>
     <row r="1223" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1223" s="1"/>
@@ -36622,10 +36726,14 @@
     <hyperlink ref="B1217" r:id="rId1195" display="https://leetcode.com/problems/delete-leaves-with-a-given-value" xr:uid="{6266164E-75B9-49E8-9BC6-CCF34DE15F20}"/>
     <hyperlink ref="B1216" r:id="rId1196" display="https://leetcode.com/problems/print-words-vertically" xr:uid="{52B02227-E77D-498F-AD51-43E28DB61F3E}"/>
     <hyperlink ref="B1215" r:id="rId1197" display="https://leetcode.com/problems/maximum-69-number" xr:uid="{786AA970-24AA-4679-9C27-1D56607C0E23}"/>
+    <hyperlink ref="B1219" r:id="rId1198" display="https://leetcode.com/problems/break-a-palindrome" xr:uid="{C9265E26-BA1A-4EBA-B4BC-33420E72F627}"/>
+    <hyperlink ref="B1220" r:id="rId1199" display="https://leetcode.com/problems/sort-the-matrix-diagonally" xr:uid="{BFB45A24-58F9-4146-87C0-2A622576A6C5}"/>
+    <hyperlink ref="B1221" r:id="rId1200" display="https://leetcode.com/problems/reverse-subarray-to-maximize-array-value" xr:uid="{7DB02FD3-34F1-438F-AE16-E237D59275AB}"/>
+    <hyperlink ref="B1222" r:id="rId1201" display="https://leetcode.com/problems/rank-transform-of-an-array" xr:uid="{F79E4984-0EF1-47E3-9679-675F3F8052E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1198"/>
-  <drawing r:id="rId1199"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1202"/>
+  <drawing r:id="rId1203"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in weekly contest part II
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huanminw\Documents\GitHub\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4E10FB-265A-43BD-A3D5-1700B1B32CE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD3BE7B-D968-4DFB-8893-FDFA28E01091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6310" uniqueCount="2373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6330" uniqueCount="2381">
   <si>
     <t>Difficulty</t>
   </si>
@@ -7153,6 +7153,30 @@
   </si>
   <si>
     <t>Use map with value as key, index array as value.</t>
+  </si>
+  <si>
+    <t>Remove Palindromic Subsequences </t>
+  </si>
+  <si>
+    <t>if not palindromic, remove a then remove b twice.</t>
+  </si>
+  <si>
+    <t>Filter Restaurants by Vegan-Friendly, Price and Distance </t>
+  </si>
+  <si>
+    <t>Filter each restaurant, sort by rateing and id in priority_queue</t>
+  </si>
+  <si>
+    <t>Find the City With the Smallest Number of Neighbors at a Threshold Distance</t>
+  </si>
+  <si>
+    <t>Minimum Difficulty of a Job Schedule</t>
+  </si>
+  <si>
+    <t>BFS from every node</t>
+  </si>
+  <si>
+    <t>Time O(nnd), from every job, check back until start, dp[i][k] = dp[j][k-1] + max_num, j &lt; i</t>
   </si>
 </sst>
 </file>
@@ -7618,8 +7642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1210" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1229" sqref="G1229"/>
+    <sheetView tabSelected="1" topLeftCell="C1219" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1226" sqref="G1226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -35462,16 +35486,96 @@
       </c>
     </row>
     <row r="1223" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1223" s="1"/>
+      <c r="A1223" s="25">
+        <v>1332</v>
+      </c>
+      <c r="B1223" s="1" t="s">
+        <v>2373</v>
+      </c>
+      <c r="C1223" s="25">
+        <v>2</v>
+      </c>
+      <c r="D1223" s="25" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E1223" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1223" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1223" s="25" t="s">
+        <v>2374</v>
+      </c>
     </row>
     <row r="1224" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1224" s="1"/>
+      <c r="A1224" s="25">
+        <v>1333</v>
+      </c>
+      <c r="B1224" s="1" t="s">
+        <v>2375</v>
+      </c>
+      <c r="C1224" s="25">
+        <v>2</v>
+      </c>
+      <c r="D1224" s="25" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E1224" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1224" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1224" s="25" t="s">
+        <v>2376</v>
+      </c>
     </row>
     <row r="1225" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1225" s="1"/>
+      <c r="A1225" s="25">
+        <v>1334</v>
+      </c>
+      <c r="B1225" s="1" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C1225" s="25">
+        <v>3</v>
+      </c>
+      <c r="D1225" s="25" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E1225" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1225" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1225" s="25" t="s">
+        <v>2379</v>
+      </c>
     </row>
     <row r="1226" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1226" s="1"/>
+      <c r="A1226" s="25">
+        <v>1335</v>
+      </c>
+      <c r="B1226" s="1" t="s">
+        <v>2378</v>
+      </c>
+      <c r="C1226" s="25">
+        <v>4</v>
+      </c>
+      <c r="D1226" s="25" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E1226" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1226" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1226" s="25" t="s">
+        <v>2380</v>
+      </c>
     </row>
     <row r="1227" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1227" s="1"/>
@@ -36730,10 +36834,14 @@
     <hyperlink ref="B1220" r:id="rId1199" display="https://leetcode.com/problems/sort-the-matrix-diagonally" xr:uid="{BFB45A24-58F9-4146-87C0-2A622576A6C5}"/>
     <hyperlink ref="B1221" r:id="rId1200" display="https://leetcode.com/problems/reverse-subarray-to-maximize-array-value" xr:uid="{7DB02FD3-34F1-438F-AE16-E237D59275AB}"/>
     <hyperlink ref="B1222" r:id="rId1201" display="https://leetcode.com/problems/rank-transform-of-an-array" xr:uid="{F79E4984-0EF1-47E3-9679-675F3F8052E6}"/>
+    <hyperlink ref="B1223" r:id="rId1202" display="https://leetcode.com/problems/remove-palindromic-subsequences" xr:uid="{EA6C9E35-A292-4BFA-ADCF-781D60B025E5}"/>
+    <hyperlink ref="B1224" r:id="rId1203" display="https://leetcode.com/problems/filter-restaurants-by-vegan-friendly-price-and-distance" xr:uid="{2CFDB941-C33F-45AA-B18B-BD79DDEC7380}"/>
+    <hyperlink ref="B1225" r:id="rId1204" display="https://leetcode.com/problems/find-the-city-with-the-smallest-number-of-neighbors-at-a-threshold-distance" xr:uid="{784459F4-D56B-4D09-AF7C-561FA398DE2E}"/>
+    <hyperlink ref="B1226" r:id="rId1205" display="https://leetcode.com/problems/minimum-difficulty-of-a-job-schedule" xr:uid="{63E1F640-139B-4D8B-83C6-44FB1595CEE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1202"/>
-  <drawing r:id="rId1203"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1206"/>
+  <drawing r:id="rId1207"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
code refactoring on Array
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huanminw\Documents\GitHub\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E2CB25-A61B-48EB-924B-C9B32EC8E206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666B22F0-8B9D-4089-A266-58D0E47C95A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7715,7 +7715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1230" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G1248" sqref="G1248"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Weekly Contest Check in
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huanminw\Documents\GitHub\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABE072B-31D6-48D7-A79F-D08753176902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17176BB3-75E0-445D-A313-E1111B3CC27D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$I$1245</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$I$1254</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6410" uniqueCount="2413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6450" uniqueCount="2429">
   <si>
     <t>Difficulty</t>
   </si>
@@ -7273,6 +7273,54 @@
   </si>
   <si>
     <t>BFS, using value mapping to index.</t>
+  </si>
+  <si>
+    <t>Sort Integers by The Number of 1 Bits</t>
+  </si>
+  <si>
+    <t>Apply Discount Every n Orders</t>
+  </si>
+  <si>
+    <t>Number of Substrings Containing All Three Characters </t>
+  </si>
+  <si>
+    <t>Count All Valid Pickup and Delivery Options </t>
+  </si>
+  <si>
+    <t>Number of Days Between Two Dates</t>
+  </si>
+  <si>
+    <t>Validate Binary Tree Nodes </t>
+  </si>
+  <si>
+    <t>Closest Divisors</t>
+  </si>
+  <si>
+    <t>Largest Multiple of Three</t>
+  </si>
+  <si>
+    <t>store smallest 2 digits with remainder as 1 and 2 when divide 3</t>
+  </si>
+  <si>
+    <t>Iterate from the sqrt of num+2 down to 1, return first divisible result.</t>
+  </si>
+  <si>
+    <t>Use two flag, one is someone claim it as child another is that its children are visited.</t>
+  </si>
+  <si>
+    <t>Calculate leap year and day of the year.</t>
+  </si>
+  <si>
+    <t>Add one package based on previous result, starting with 2*I + 1 positions</t>
+  </si>
+  <si>
+    <t>String coverage, two pointers</t>
+  </si>
+  <si>
+    <t>count bits and sort</t>
+  </si>
+  <si>
+    <t>Simulate the behavior</t>
   </si>
 </sst>
 </file>
@@ -7317,7 +7365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7344,6 +7392,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -7738,10 +7787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1245"/>
+  <dimension ref="A1:I1254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1225" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1234" sqref="G1234"/>
+    <sheetView tabSelected="1" topLeftCell="C1228" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1244" sqref="G1244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -36043,36 +36092,223 @@
         <v>2411</v>
       </c>
     </row>
-    <row r="1243" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1243" s="1"/>
-    </row>
-    <row r="1244" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1244" s="30" t="s">
+    <row r="1243" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1243" s="30">
+        <v>1356</v>
+      </c>
+      <c r="B1243" s="1" t="s">
+        <v>2413</v>
+      </c>
+      <c r="C1243" s="30">
+        <v>2</v>
+      </c>
+      <c r="D1243" s="30" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E1243" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1243" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1243" s="30" t="s">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1244" s="30">
+        <v>1357</v>
+      </c>
+      <c r="B1244" s="1" t="s">
+        <v>2414</v>
+      </c>
+      <c r="C1244" s="30">
+        <v>3</v>
+      </c>
+      <c r="D1244" s="30" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E1244" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1244" s="30" t="s">
+        <v>459</v>
+      </c>
+      <c r="G1244" s="30" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1245" s="30">
+        <v>1358</v>
+      </c>
+      <c r="B1245" s="1" t="s">
+        <v>2415</v>
+      </c>
+      <c r="C1245" s="30">
+        <v>3</v>
+      </c>
+      <c r="D1245" s="30" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E1245" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1245" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1245" s="30" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1246" s="30">
+        <v>1359</v>
+      </c>
+      <c r="B1246" s="1" t="s">
+        <v>2416</v>
+      </c>
+      <c r="C1246" s="30">
+        <v>4</v>
+      </c>
+      <c r="D1246" s="30" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E1246" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1246" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1246" s="30" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1247" s="30">
+        <v>1360</v>
+      </c>
+      <c r="B1247" s="1" t="s">
+        <v>2417</v>
+      </c>
+      <c r="C1247" s="30">
+        <v>3</v>
+      </c>
+      <c r="D1247" s="30" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E1247" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1247" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1247" s="30" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1248" s="30">
+        <v>1361</v>
+      </c>
+      <c r="B1248" s="1" t="s">
+        <v>2418</v>
+      </c>
+      <c r="C1248" s="30">
+        <v>4</v>
+      </c>
+      <c r="D1248" s="30" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E1248" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1248" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1248" s="30" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1249" s="30">
+        <v>1362</v>
+      </c>
+      <c r="B1249" s="1" t="s">
+        <v>2419</v>
+      </c>
+      <c r="C1249" s="30">
+        <v>2</v>
+      </c>
+      <c r="D1249" s="30" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E1249" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1249" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1249" s="30" t="s">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1250" s="30">
+        <v>1363</v>
+      </c>
+      <c r="B1250" s="1" t="s">
+        <v>2420</v>
+      </c>
+      <c r="C1250" s="30">
+        <v>4</v>
+      </c>
+      <c r="D1250" s="30" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E1250" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1250" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1250" s="30" t="s">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1251" s="1"/>
+    </row>
+    <row r="1252" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1252" s="1"/>
+    </row>
+    <row r="1253" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1253" s="31" t="s">
         <v>1726</v>
       </c>
-      <c r="B1244" s="30"/>
-      <c r="C1244" s="30"/>
-      <c r="D1244" s="30"/>
-      <c r="E1244" s="30"/>
-      <c r="F1244" s="30"/>
-      <c r="G1244" s="30"/>
-    </row>
-    <row r="1245" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1245" s="31" t="s">
+      <c r="B1253" s="31"/>
+      <c r="C1253" s="31"/>
+      <c r="D1253" s="31"/>
+      <c r="E1253" s="31"/>
+      <c r="F1253" s="31"/>
+      <c r="G1253" s="31"/>
+    </row>
+    <row r="1254" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1254" s="32" t="s">
         <v>1774</v>
       </c>
-      <c r="B1245" s="31"/>
-      <c r="C1245" s="31"/>
-      <c r="D1245" s="31"/>
-      <c r="E1245" s="31"/>
-      <c r="F1245" s="31"/>
-      <c r="G1245" s="31"/>
+      <c r="B1254" s="32"/>
+      <c r="C1254" s="32"/>
+      <c r="D1254" s="32"/>
+      <c r="E1254" s="32"/>
+      <c r="F1254" s="32"/>
+      <c r="G1254" s="32"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1245" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:I1254" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1244:G1244"/>
-    <mergeCell ref="A1245:G1245"/>
+    <mergeCell ref="A1253:G1253"/>
+    <mergeCell ref="A1254:G1254"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -37296,10 +37532,18 @@
     <hyperlink ref="B1240" r:id="rId1219" display="https://leetcode.com/problems/product-of-the-last-k-numbers" xr:uid="{9CDE6EA2-7CA2-46C5-8877-374FB14DD3EA}"/>
     <hyperlink ref="B1241" r:id="rId1220" display="https://leetcode.com/problems/maximum-number-of-events-that-can-be-attended" xr:uid="{258FB3FD-2123-4FD9-9D91-7C88F6D6C2C2}"/>
     <hyperlink ref="B1242" r:id="rId1221" display="https://leetcode.com/problems/construct-target-array-with-multiple-sums" xr:uid="{F04F17B1-B2C5-4A98-ACC4-2EA8B6693A6F}"/>
+    <hyperlink ref="B1243" r:id="rId1222" display="https://leetcode.com/problems/sort-integers-by-the-number-of-1-bits" xr:uid="{4C8874CD-7738-4EC9-9DC9-7AF4F8340254}"/>
+    <hyperlink ref="B1244" r:id="rId1223" display="https://leetcode.com/problems/apply-discount-every-n-orders" xr:uid="{A7DFC8EF-B667-434A-B39E-E236667CBA44}"/>
+    <hyperlink ref="B1245" r:id="rId1224" display="https://leetcode.com/problems/number-of-substrings-containing-all-three-characters" xr:uid="{E1FCF586-E975-4444-80BA-06B38F896582}"/>
+    <hyperlink ref="B1246" r:id="rId1225" display="https://leetcode.com/problems/count-all-valid-pickup-and-delivery-options" xr:uid="{14D09337-9159-4E43-AAB7-4001BDC65890}"/>
+    <hyperlink ref="B1247" r:id="rId1226" display="https://leetcode.com/problems/number-of-days-between-two-dates" xr:uid="{CD1FDAFC-D166-459B-B290-3291EF5FC912}"/>
+    <hyperlink ref="B1248" r:id="rId1227" display="https://leetcode.com/problems/validate-binary-tree-nodes" xr:uid="{813CF731-F43C-4B3B-8593-132B454F8C8D}"/>
+    <hyperlink ref="B1249" r:id="rId1228" display="https://leetcode.com/problems/closest-divisors" xr:uid="{E6EA0C9A-D70E-4D6E-93EA-8F04128E1BC8}"/>
+    <hyperlink ref="B1250" r:id="rId1229" display="https://leetcode.com/problems/largest-multiple-of-three" xr:uid="{0E32F9E6-86AE-401D-A290-F4EC8E0B1F90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1222"/>
-  <drawing r:id="rId1223"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1230"/>
+  <drawing r:id="rId1231"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in weekly contest and SQL
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4942CC02-FCDC-49FD-BF76-C636C56590C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC73B094-1E4D-4D0F-A5F2-FDB587F0028D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$I$1306</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$I$1319</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6715" uniqueCount="2533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6780" uniqueCount="2560">
   <si>
     <t>Difficulty</t>
   </si>
@@ -7636,6 +7636,87 @@
   </si>
   <si>
     <t>Track decreasing sum within K distance in stack</t>
+  </si>
+  <si>
+    <t>Counting Elements</t>
+  </si>
+  <si>
+    <t>Track numbers in hashtable</t>
+  </si>
+  <si>
+    <t>Perform String Shifts</t>
+  </si>
+  <si>
+    <t>Calculate shift position first then do shift once.</t>
+  </si>
+  <si>
+    <t>Leftmost Column with at Least a One</t>
+  </si>
+  <si>
+    <t>Search from right top of the array, move down if 0, move left if 1.</t>
+  </si>
+  <si>
+    <t>First Unique Number</t>
+  </si>
+  <si>
+    <t>Track single and duplicates, single with position in list.</t>
+  </si>
+  <si>
+    <t>Check If a String Is a Valid Sequence from Root to Leaves Path in a Binary Tree</t>
+  </si>
+  <si>
+    <t>Preorder traverse,  should check leafs</t>
+  </si>
+  <si>
+    <t>Kids With the Greatest Number of Candies</t>
+  </si>
+  <si>
+    <t>Add any element by extra and compare with maximum.</t>
+  </si>
+  <si>
+    <t>Max Difference You Can Get From Changing an Integer</t>
+  </si>
+  <si>
+    <t>Replace number to '9' for maximum, and number to 1 or 1 for minimum.</t>
+  </si>
+  <si>
+    <t>Check If a String Can Break Another String</t>
+  </si>
+  <si>
+    <t>Sort these two string first and compare order.</t>
+  </si>
+  <si>
+    <t>Number of Ways to Wear Different Hats to Each Other</t>
+  </si>
+  <si>
+    <t>P, F</t>
+  </si>
+  <si>
+    <t>Assign each hat to person, we only have 10 people, use bit map.</t>
+  </si>
+  <si>
+    <t>Destination City</t>
+  </si>
+  <si>
+    <t>Track source city and destination city, count source</t>
+  </si>
+  <si>
+    <t>Check If All 1's Are at Least Length K Places Away</t>
+  </si>
+  <si>
+    <t>Track last 1 and calculate distance</t>
+  </si>
+  <si>
+    <t>Longest Continuous Subarray With Absolute Diff Less Than or Equal to Limit</t>
+  </si>
+  <si>
+    <t>Track maximum and minimum by mono stack</t>
+  </si>
+  <si>
+    <t>Find the Kth Smallest Sum of a Matrix With Sorted Rows</t>
+  </si>
+  <si>
+    <t>Track sum in every row and keep only size of K</t>
   </si>
 </sst>
 </file>
@@ -7680,7 +7761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7707,6 +7788,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -8109,10 +8191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1306"/>
+  <dimension ref="A1:I1319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1290" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1303" sqref="G1303"/>
+    <sheetView tabSelected="1" topLeftCell="A1301" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1317" sqref="A1317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -37817,36 +37899,335 @@
         <v>2532</v>
       </c>
     </row>
-    <row r="1304" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B1304" s="1"/>
-    </row>
-    <row r="1305" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1305" s="38" t="s">
+    <row r="1304" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1304" s="38">
+        <v>1426</v>
+      </c>
+      <c r="B1304" s="1" t="s">
+        <v>2533</v>
+      </c>
+      <c r="C1304" s="38">
+        <v>1</v>
+      </c>
+      <c r="D1304" s="38" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E1304" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1304" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1304" s="38" t="s">
+        <v>2534</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1305" s="38">
+        <v>1427</v>
+      </c>
+      <c r="B1305" s="1" t="s">
+        <v>2535</v>
+      </c>
+      <c r="C1305" s="38">
+        <v>2</v>
+      </c>
+      <c r="D1305" s="38" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E1305" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1305" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1305" s="38" t="s">
+        <v>2536</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1306" s="38">
+        <v>1428</v>
+      </c>
+      <c r="B1306" s="1" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C1306" s="38">
+        <v>2</v>
+      </c>
+      <c r="D1306" s="38" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E1306" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1306" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1306" s="38" t="s">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1307" s="38">
+        <v>1429</v>
+      </c>
+      <c r="B1307" s="1" t="s">
+        <v>2539</v>
+      </c>
+      <c r="C1307" s="38">
+        <v>2</v>
+      </c>
+      <c r="D1307" s="38" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E1307" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1307" s="38" t="s">
+        <v>459</v>
+      </c>
+      <c r="G1307" s="38" t="s">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1308" s="38">
+        <v>1430</v>
+      </c>
+      <c r="B1308" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C1308" s="38">
+        <v>2</v>
+      </c>
+      <c r="D1308" s="38" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E1308" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1308" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1308" s="38" t="s">
+        <v>2542</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1309" s="38">
+        <v>1431</v>
+      </c>
+      <c r="B1309" s="1" t="s">
+        <v>2543</v>
+      </c>
+      <c r="C1309" s="38">
+        <v>1</v>
+      </c>
+      <c r="D1309" s="38" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E1309" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1309" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1309" s="38" t="s">
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1310" s="38">
+        <v>1432</v>
+      </c>
+      <c r="B1310" s="1" t="s">
+        <v>2545</v>
+      </c>
+      <c r="C1310" s="38">
+        <v>2</v>
+      </c>
+      <c r="D1310" s="38" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E1310" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1310" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1310" s="38" t="s">
+        <v>2546</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1311" s="38">
+        <v>1433</v>
+      </c>
+      <c r="B1311" s="1" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C1311" s="38">
+        <v>2</v>
+      </c>
+      <c r="D1311" s="38" t="s">
+        <v>2550</v>
+      </c>
+      <c r="E1311" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1311" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1311" s="38" t="s">
+        <v>2548</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1312" s="38">
+        <v>1434</v>
+      </c>
+      <c r="B1312" s="1" t="s">
+        <v>2549</v>
+      </c>
+      <c r="C1312" s="38">
+        <v>4</v>
+      </c>
+      <c r="D1312" s="38" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E1312" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1312" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1312" s="38" t="s">
+        <v>2551</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1313" s="38">
+        <v>1436</v>
+      </c>
+      <c r="B1313" s="1" t="s">
+        <v>2552</v>
+      </c>
+      <c r="C1313" s="38">
+        <v>2</v>
+      </c>
+      <c r="D1313" s="38" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E1313" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1313" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1313" s="38" t="s">
+        <v>2553</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1314" s="38">
+        <v>1437</v>
+      </c>
+      <c r="B1314" s="1" t="s">
+        <v>2554</v>
+      </c>
+      <c r="C1314" s="38">
+        <v>2</v>
+      </c>
+      <c r="D1314" s="38" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E1314" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1314" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1314" s="38" t="s">
+        <v>2555</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1315" s="38">
+        <v>1438</v>
+      </c>
+      <c r="B1315" s="1" t="s">
+        <v>2556</v>
+      </c>
+      <c r="C1315" s="38">
+        <v>4</v>
+      </c>
+      <c r="D1315" s="38" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E1315" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1315" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1315" s="38" t="s">
+        <v>2557</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1316" s="38">
+        <v>1439</v>
+      </c>
+      <c r="B1316" s="1" t="s">
+        <v>2558</v>
+      </c>
+      <c r="C1316" s="38">
+        <v>4</v>
+      </c>
+      <c r="D1316" s="38" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E1316" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1316" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1316" s="38" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1317" s="1"/>
+    </row>
+    <row r="1318" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1318" s="39" t="s">
         <v>1726</v>
       </c>
-      <c r="B1305" s="38"/>
-      <c r="C1305" s="38"/>
-      <c r="D1305" s="38"/>
-      <c r="E1305" s="38"/>
-      <c r="F1305" s="38"/>
-      <c r="G1305" s="38"/>
-    </row>
-    <row r="1306" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1306" s="39" t="s">
+      <c r="B1318" s="39"/>
+      <c r="C1318" s="39"/>
+      <c r="D1318" s="39"/>
+      <c r="E1318" s="39"/>
+      <c r="F1318" s="39"/>
+      <c r="G1318" s="39"/>
+    </row>
+    <row r="1319" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1319" s="40" t="s">
         <v>1774</v>
       </c>
-      <c r="B1306" s="39"/>
-      <c r="C1306" s="39"/>
-      <c r="D1306" s="39"/>
-      <c r="E1306" s="39"/>
-      <c r="F1306" s="39"/>
-      <c r="G1306" s="39"/>
+      <c r="B1319" s="40"/>
+      <c r="C1319" s="40"/>
+      <c r="D1319" s="40"/>
+      <c r="E1319" s="40"/>
+      <c r="F1319" s="40"/>
+      <c r="G1319" s="40"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1306" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:I1319" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1305:G1305"/>
-    <mergeCell ref="A1306:G1306"/>
+    <mergeCell ref="A1318:G1318"/>
+    <mergeCell ref="A1319:G1319"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
code refactor for tree
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB8C891-E6ED-443E-BDE2-38F709CB2C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D460B8D7-0C56-4B6E-A0E8-1CD392054099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6833" uniqueCount="2581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6837" uniqueCount="2581">
   <si>
     <t>Difficulty</t>
   </si>
@@ -8258,8 +8258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1305" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1325" sqref="G1325"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D635" sqref="D635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26584,6 +26584,9 @@
       <c r="C814">
         <v>3</v>
       </c>
+      <c r="D814" t="s">
+        <v>1724</v>
+      </c>
       <c r="E814" t="s">
         <v>9</v>
       </c>
@@ -27122,7 +27125,10 @@
         <v>1282</v>
       </c>
       <c r="C838">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D838" t="s">
+        <v>1724</v>
       </c>
       <c r="E838" t="s">
         <v>9</v>
@@ -27779,6 +27785,9 @@
       <c r="C867">
         <v>2</v>
       </c>
+      <c r="D867" t="s">
+        <v>1717</v>
+      </c>
       <c r="E867" t="s">
         <v>9</v>
       </c>
@@ -28216,6 +28225,9 @@
       <c r="C886">
         <v>3</v>
       </c>
+      <c r="D886" t="s">
+        <v>1717</v>
+      </c>
       <c r="E886" t="s">
         <v>9</v>
       </c>
@@ -30287,7 +30299,7 @@
         <v>4</v>
       </c>
       <c r="D976" t="s">
-        <v>1777</v>
+        <v>1788</v>
       </c>
       <c r="E976" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
code refactor for union find
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CF365E-03E0-499E-9FAE-65459ACCE849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2B5CC6-80E6-49E9-9587-6836956A83C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8307,8 +8307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1313" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1333" sqref="A1333"/>
+    <sheetView tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D308" sqref="D308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15320,7 +15320,7 @@
         <v>411</v>
       </c>
       <c r="C308">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D308" t="s">
         <v>1739</v>

</xml_diff>

<commit_message>
Check in weely contest
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3535ED-5971-4D52-9237-205E15A1E956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77133201-17C2-410E-8D03-A4F69DBA7967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$I$1356</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$I$1366</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6983" uniqueCount="2633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7008" uniqueCount="2642">
   <si>
     <t>Difficulty</t>
   </si>
@@ -7936,6 +7936,33 @@
   </si>
   <si>
     <t>Prefix sum</t>
+  </si>
+  <si>
+    <t>Clone Binary Tree With Random Pointer</t>
+  </si>
+  <si>
+    <t>XOR Operation in an Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Critical and Pseudo-Critical Edges in Minimum Spanning Tree </t>
+  </si>
+  <si>
+    <t>Avoid Flood in The City</t>
+  </si>
+  <si>
+    <t>Making File Names Unique</t>
+  </si>
+  <si>
+    <t>Hashtable mapping from old node to new node.</t>
+  </si>
+  <si>
+    <t>Track maximum alias for each name</t>
+  </si>
+  <si>
+    <t>Link potential flood to next dry day.</t>
+  </si>
+  <si>
+    <t>Calculate MST, take every edge and MUST and IGNORE, to recalculate total weight.</t>
   </si>
 </sst>
 </file>
@@ -7980,7 +8007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8007,6 +8034,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -8415,10 +8443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1356"/>
+  <dimension ref="A1:I1366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1334" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1345" sqref="G1345"/>
+    <sheetView tabSelected="1" topLeftCell="C1339" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1358" sqref="G1358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -39327,36 +39355,166 @@
         <v>2629</v>
       </c>
     </row>
-    <row r="1354" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1354" s="1"/>
-    </row>
-    <row r="1355" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1355" s="44" t="s">
+    <row r="1354" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1354" s="44">
+        <v>1485</v>
+      </c>
+      <c r="B1354" s="1" t="s">
+        <v>2633</v>
+      </c>
+      <c r="C1354" s="44">
+        <v>3</v>
+      </c>
+      <c r="D1354" s="44" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E1354" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1354" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1354" s="44" t="s">
+        <v>2638</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1355" s="44">
+        <v>1486</v>
+      </c>
+      <c r="B1355" s="1" t="s">
+        <v>2634</v>
+      </c>
+      <c r="C1355" s="44">
+        <v>1</v>
+      </c>
+      <c r="D1355" s="44" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1355" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1355" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1355" s="44" t="s">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1356" s="44">
+        <v>1487</v>
+      </c>
+      <c r="B1356" s="1" t="s">
+        <v>2637</v>
+      </c>
+      <c r="C1356" s="44">
+        <v>3</v>
+      </c>
+      <c r="D1356" s="44" t="s">
+        <v>1776</v>
+      </c>
+      <c r="E1356" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1356" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1356" s="44" t="s">
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1357" s="44">
+        <v>1488</v>
+      </c>
+      <c r="B1357" s="1" t="s">
+        <v>2636</v>
+      </c>
+      <c r="C1357" s="44">
+        <v>3</v>
+      </c>
+      <c r="D1357" s="44" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E1357" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1357" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1357" s="44" t="s">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1358" s="44">
+        <v>1489</v>
+      </c>
+      <c r="B1358" s="1" t="s">
+        <v>2635</v>
+      </c>
+      <c r="C1358" s="44">
+        <v>5</v>
+      </c>
+      <c r="D1358" s="44" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E1358" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1358" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1358" s="44" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1359" s="1"/>
+    </row>
+    <row r="1360" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1360" s="1"/>
+    </row>
+    <row r="1361" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1361" s="1"/>
+    </row>
+    <row r="1362" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1362" s="1"/>
+    </row>
+    <row r="1363" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1363" s="1"/>
+    </row>
+    <row r="1364" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1364" s="1"/>
+    </row>
+    <row r="1365" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1365" s="45" t="s">
         <v>1724</v>
       </c>
-      <c r="B1355" s="44"/>
-      <c r="C1355" s="44"/>
-      <c r="D1355" s="44"/>
-      <c r="E1355" s="44"/>
-      <c r="F1355" s="44"/>
-      <c r="G1355" s="44"/>
-    </row>
-    <row r="1356" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1356" s="45" t="s">
+      <c r="B1365" s="45"/>
+      <c r="C1365" s="45"/>
+      <c r="D1365" s="45"/>
+      <c r="E1365" s="45"/>
+      <c r="F1365" s="45"/>
+      <c r="G1365" s="45"/>
+    </row>
+    <row r="1366" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1366" s="46" t="s">
         <v>1770</v>
       </c>
-      <c r="B1356" s="45"/>
-      <c r="C1356" s="45"/>
-      <c r="D1356" s="45"/>
-      <c r="E1356" s="45"/>
-      <c r="F1356" s="45"/>
-      <c r="G1356" s="45"/>
+      <c r="B1366" s="46"/>
+      <c r="C1366" s="46"/>
+      <c r="D1366" s="46"/>
+      <c r="E1366" s="46"/>
+      <c r="F1366" s="46"/>
+      <c r="G1366" s="46"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1356" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:I1366" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1355:G1355"/>
-    <mergeCell ref="A1356:G1356"/>
+    <mergeCell ref="A1365:G1365"/>
+    <mergeCell ref="A1366:G1366"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
check weekly hard problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E894042-A36A-4E2F-8BC8-205E465DBE19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04405D45-3E62-4938-9966-34E855CCDB79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="19170" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19058" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Algorithm" sheetId="1" r:id="rId1"/>
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$I$1494</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$I$1507</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7690" uniqueCount="2897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7722" uniqueCount="2917">
   <si>
     <t>Difficulty</t>
   </si>
@@ -8728,6 +8728,66 @@
   </si>
   <si>
     <t>Sort all value, then for same value use union find to adjust rank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort Array by Increasing Frequency </t>
+  </si>
+  <si>
+    <t>Widest Vertical Area Between Two Points Containing No Points</t>
+  </si>
+  <si>
+    <t>Count Substrings That Differ by One Character</t>
+  </si>
+  <si>
+    <t>Number of Ways to Form a Target String Given a Dictionary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Array Formation Through Concatenation </t>
+  </si>
+  <si>
+    <t>Count Sorted Vowel Strings</t>
+  </si>
+  <si>
+    <t>Furthest Building You Can Reach</t>
+  </si>
+  <si>
+    <t>Kth Smallest Instructions</t>
+  </si>
+  <si>
+    <t>Get Maximum in Generated Array</t>
+  </si>
+  <si>
+    <t>Minimum Deletions to Make Character Frequencies Unique</t>
+  </si>
+  <si>
+    <t>Sell Diminishing-Valued Colored Balls</t>
+  </si>
+  <si>
+    <t>Create Sorted Array through Instructions</t>
+  </si>
+  <si>
+    <t>Defuse the Bomb</t>
+  </si>
+  <si>
+    <t>Minimum Deletions to Make String Balanced</t>
+  </si>
+  <si>
+    <t>Minimum Jumps to Reach Home</t>
+  </si>
+  <si>
+    <t>Distribute Repeating Integers</t>
+  </si>
+  <si>
+    <t>Select at most m max repeated piles of numbers, the search against quantity</t>
+  </si>
+  <si>
+    <t>Binary Index Tree or Segment Tree</t>
+  </si>
+  <si>
+    <t>Calculate Pascal triangle to get C(m,n), the try see try V from left to right.</t>
+  </si>
+  <si>
+    <t>Build ith character from i-th characters in target</t>
   </si>
 </sst>
 </file>
@@ -8772,7 +8832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8799,6 +8859,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -9221,10 +9282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1494"/>
+  <dimension ref="A1:I1507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1469" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1485" sqref="A1485"/>
+    <sheetView tabSelected="1" topLeftCell="C1482" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1488" sqref="G1488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -43303,56 +43364,235 @@
       </c>
     </row>
     <row r="1485" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1485" s="1"/>
-    </row>
-    <row r="1486" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1486" s="1"/>
-    </row>
-    <row r="1487" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1487" s="1"/>
-    </row>
-    <row r="1488" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1488" s="1"/>
-    </row>
-    <row r="1489" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1489" s="1"/>
-    </row>
-    <row r="1490" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1490" s="1"/>
-    </row>
-    <row r="1491" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1491" s="1"/>
-    </row>
-    <row r="1492" spans="1:7" s="52" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1492" s="1"/>
-    </row>
-    <row r="1493" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1493" s="58" t="s">
+      <c r="A1485" s="57">
+        <v>1636</v>
+      </c>
+      <c r="B1485" s="1" t="s">
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1486" s="58">
+        <v>1637</v>
+      </c>
+      <c r="B1486" s="1" t="s">
+        <v>2898</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1487" s="58">
+        <v>1638</v>
+      </c>
+      <c r="B1487" s="1" t="s">
+        <v>2899</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1488" s="58">
+        <v>1639</v>
+      </c>
+      <c r="B1488" s="1" t="s">
+        <v>2900</v>
+      </c>
+      <c r="C1488" s="58">
+        <v>4</v>
+      </c>
+      <c r="D1488" s="58" t="s">
+        <v>1780</v>
+      </c>
+      <c r="E1488" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1488" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1488" s="58" t="s">
+        <v>2916</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1489" s="58">
+        <v>1640</v>
+      </c>
+      <c r="B1489" s="1" t="s">
+        <v>2901</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1490" s="58">
+        <v>1641</v>
+      </c>
+      <c r="B1490" s="1" t="s">
+        <v>2902</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1491" s="58">
+        <v>1642</v>
+      </c>
+      <c r="B1491" s="1" t="s">
+        <v>2903</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1492" s="58">
+        <v>1643</v>
+      </c>
+      <c r="B1492" s="1" t="s">
+        <v>2904</v>
+      </c>
+      <c r="C1492" s="58">
+        <v>4</v>
+      </c>
+      <c r="D1492" s="58" t="s">
+        <v>1722</v>
+      </c>
+      <c r="E1492" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1492" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1492" s="58" t="s">
+        <v>2915</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1493" s="58">
+        <v>1646</v>
+      </c>
+      <c r="B1493" s="1" t="s">
+        <v>2905</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1494" s="58">
+        <v>1647</v>
+      </c>
+      <c r="B1494" s="1" t="s">
+        <v>2906</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1495" s="58">
+        <v>1648</v>
+      </c>
+      <c r="B1495" s="1" t="s">
+        <v>2907</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1496" s="58">
+        <v>1649</v>
+      </c>
+      <c r="B1496" s="1" t="s">
+        <v>2908</v>
+      </c>
+      <c r="C1496" s="58">
+        <v>5</v>
+      </c>
+      <c r="D1496" s="58" t="s">
+        <v>1722</v>
+      </c>
+      <c r="E1496" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1496" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1496" s="58" t="s">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1497" s="58">
+        <v>1652</v>
+      </c>
+      <c r="B1497" s="1" t="s">
+        <v>2909</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1498" s="58">
+        <v>1653</v>
+      </c>
+      <c r="B1498" s="1" t="s">
+        <v>2910</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1499" s="57">
+        <v>1654</v>
+      </c>
+      <c r="B1499" s="1" t="s">
+        <v>2911</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1500" s="57">
+        <v>1655</v>
+      </c>
+      <c r="B1500" s="1" t="s">
+        <v>2912</v>
+      </c>
+      <c r="C1500" s="57">
+        <v>4</v>
+      </c>
+      <c r="D1500" s="57" t="s">
+        <v>1780</v>
+      </c>
+      <c r="E1500" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1500" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1500" s="57" t="s">
+        <v>2913</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1501" s="1"/>
+    </row>
+    <row r="1502" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1502" s="1"/>
+    </row>
+    <row r="1503" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1503" s="1"/>
+    </row>
+    <row r="1504" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1504" s="1"/>
+    </row>
+    <row r="1505" spans="1:7" s="52" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1505" s="1"/>
+    </row>
+    <row r="1506" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1506" s="59" t="s">
         <v>1723</v>
       </c>
-      <c r="B1493" s="58"/>
-      <c r="C1493" s="58"/>
-      <c r="D1493" s="58"/>
-      <c r="E1493" s="58"/>
-      <c r="F1493" s="58"/>
-      <c r="G1493" s="58"/>
-    </row>
-    <row r="1494" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1494" s="59" t="s">
+      <c r="B1506" s="59"/>
+      <c r="C1506" s="59"/>
+      <c r="D1506" s="59"/>
+      <c r="E1506" s="59"/>
+      <c r="F1506" s="59"/>
+      <c r="G1506" s="59"/>
+    </row>
+    <row r="1507" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1507" s="60" t="s">
         <v>2769</v>
       </c>
-      <c r="B1494" s="59"/>
-      <c r="C1494" s="59"/>
-      <c r="D1494" s="59"/>
-      <c r="E1494" s="59"/>
-      <c r="F1494" s="59"/>
-      <c r="G1494" s="59"/>
+      <c r="B1507" s="60"/>
+      <c r="C1507" s="60"/>
+      <c r="D1507" s="60"/>
+      <c r="E1507" s="60"/>
+      <c r="F1507" s="60"/>
+      <c r="G1507" s="60"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1494" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:I1507" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1493:G1493"/>
-    <mergeCell ref="A1494:G1494"/>
+    <mergeCell ref="A1506:G1506"/>
+    <mergeCell ref="A1507:G1507"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
check in locked problem and SQL problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C98C23D-3FA8-429C-888E-AA3D0688D7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E611328-1526-473F-89BF-47D6BE7972A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="165" yWindow="0" windowWidth="19035" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9782,8 +9782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1539" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1563" sqref="H1563"/>
+    <sheetView tabSelected="1" topLeftCell="C1102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1115" sqref="C1115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -35607,7 +35607,7 @@
         <v>1914</v>
       </c>
       <c r="C1115" s="13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1115" s="13" t="s">
         <v>1720</v>

</xml_diff>

<commit_message>
check in locked problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E611328-1526-473F-89BF-47D6BE7972A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B194A4-46FB-4C48-AF12-AFDBC990CB4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="0" windowWidth="19035" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="0" windowWidth="18900" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Algorithm" sheetId="1" r:id="rId1"/>
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1566</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1637</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8276" uniqueCount="3079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8360" uniqueCount="3107">
   <si>
     <t>Difficulty</t>
   </si>
@@ -9274,6 +9274,90 @@
   </si>
   <si>
     <t>Accumulate cells in column on rows, then sort and calculate</t>
+  </si>
+  <si>
+    <t>Cat and Mouse II</t>
+  </si>
+  <si>
+    <t>limit the steps within 70</t>
+  </si>
+  <si>
+    <t>E ^ N</t>
+  </si>
+  <si>
+    <t>Shortest Path to Get Food </t>
+  </si>
+  <si>
+    <t>BFS to look for all paths</t>
+  </si>
+  <si>
+    <t>Find the Highest Altitude</t>
+  </si>
+  <si>
+    <t>Latest Time by Replacing Hidden Digits </t>
+  </si>
+  <si>
+    <t>Calculate highest altitude on the way</t>
+  </si>
+  <si>
+    <t>Branch Logic</t>
+  </si>
+  <si>
+    <t>Maximum Number of Balls in a Box</t>
+  </si>
+  <si>
+    <t>Sum of Unique Elements</t>
+  </si>
+  <si>
+    <t>Count unique number in array</t>
+  </si>
+  <si>
+    <t>Check if Array Is Sorted and Rotated</t>
+  </si>
+  <si>
+    <t>Count dip and if dip is 1 compare first and last element</t>
+  </si>
+  <si>
+    <t>Design Most Recently Used Queue</t>
+  </si>
+  <si>
+    <t>Simply move elements in array, a more advanced version will be using BIT</t>
+  </si>
+  <si>
+    <t>N * N -&gt; N Log(N)</t>
+  </si>
+  <si>
+    <t>Maximum Subarray Sum After One Operation</t>
+  </si>
+  <si>
+    <t>Calculate presum and presum with one operation</t>
+  </si>
+  <si>
+    <t>Find Distance in a Binary Tree</t>
+  </si>
+  <si>
+    <t>Calculate depth for nodes and calculate result by post-order</t>
+  </si>
+  <si>
+    <t>Checking Existence of Edge Length Limited Paths II </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Union Find with weights memorizied </t>
+  </si>
+  <si>
+    <t>Sum Of Special Evenly-Spaced Elements In Array </t>
+  </si>
+  <si>
+    <t>Memorize the query steps</t>
+  </si>
+  <si>
+    <t>N * Sqrt(N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Largest Subarray Length K </t>
+  </si>
+  <si>
+    <t>Reset head of sub array</t>
   </si>
 </sst>
 </file>
@@ -9318,7 +9402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -9345,6 +9429,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -9780,10 +9865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1566"/>
+  <dimension ref="A1:J1637"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1115" sqref="C1115"/>
+    <sheetView tabSelected="1" topLeftCell="A1555" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1555" sqref="A1555"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -46034,7 +46119,7 @@
         <v>2922</v>
       </c>
       <c r="F1540" s="64" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1540" s="64" t="s">
         <v>36</v>
@@ -46205,7 +46290,7 @@
         <v>3041</v>
       </c>
       <c r="I1546" s="69" t="s">
-        <v>3018</v>
+        <v>3029</v>
       </c>
     </row>
     <row r="1547" spans="1:9" s="69" customFormat="1" x14ac:dyDescent="0.45">
@@ -46260,88 +46345,85 @@
         <v>3046</v>
       </c>
       <c r="I1548" s="63" t="s">
-        <v>3018</v>
-      </c>
-    </row>
-    <row r="1549" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1549" s="70">
-        <v>1710</v>
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1549" s="71">
+        <v>1708</v>
       </c>
       <c r="B1549" s="1" t="s">
-        <v>3047</v>
-      </c>
-      <c r="C1549" s="70">
-        <v>1</v>
-      </c>
-      <c r="D1549" s="70" t="s">
+        <v>3105</v>
+      </c>
+      <c r="C1549" s="71">
+        <v>2</v>
+      </c>
+      <c r="D1549" s="71" t="s">
         <v>1720</v>
       </c>
-      <c r="F1549" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1549" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1549" s="70" t="s">
-        <v>3049</v>
-      </c>
-      <c r="I1549" s="70" t="s">
-        <v>3018</v>
+      <c r="F1549" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1549" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1549" s="71" t="s">
+        <v>3106</v>
+      </c>
+      <c r="I1549" s="71" t="s">
+        <v>3000</v>
       </c>
     </row>
     <row r="1550" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1550" s="70">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="B1550" s="1" t="s">
-        <v>3048</v>
+        <v>3047</v>
       </c>
       <c r="C1550" s="70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1550" s="70" t="s">
         <v>1720</v>
       </c>
-      <c r="E1550" s="70" t="s">
-        <v>2924</v>
-      </c>
       <c r="F1550" s="70" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1550" s="70" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="H1550" s="70" t="s">
-        <v>3050</v>
+        <v>3049</v>
       </c>
       <c r="I1550" s="70" t="s">
-        <v>3000</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="1551" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1551" s="70">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="B1551" s="1" t="s">
-        <v>3051</v>
+        <v>3048</v>
       </c>
       <c r="C1551" s="70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1551" s="70" t="s">
         <v>1720</v>
       </c>
       <c r="E1551" s="70" t="s">
-        <v>2922</v>
+        <v>2924</v>
       </c>
       <c r="F1551" s="70" t="s">
         <v>9</v>
       </c>
       <c r="G1551" s="70" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H1551" s="70" t="s">
-        <v>3053</v>
+        <v>3050</v>
       </c>
       <c r="I1551" s="70" t="s">
         <v>3000</v>
@@ -46349,236 +46431,233 @@
     </row>
     <row r="1552" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1552" s="70">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B1552" s="1" t="s">
-        <v>3052</v>
+        <v>3051</v>
       </c>
       <c r="C1552" s="70">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1552" s="70" t="s">
         <v>1720</v>
       </c>
       <c r="E1552" s="70" t="s">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="F1552" s="70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1552" s="70" t="s">
         <v>21</v>
       </c>
       <c r="H1552" s="70" t="s">
-        <v>3054</v>
+        <v>3053</v>
       </c>
       <c r="I1552" s="70" t="s">
-        <v>3018</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1553" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1553" s="70">
-        <v>1716</v>
+        <v>1713</v>
       </c>
       <c r="B1553" s="1" t="s">
-        <v>3055</v>
+        <v>3052</v>
       </c>
       <c r="C1553" s="70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1553" s="70" t="s">
         <v>1720</v>
       </c>
+      <c r="E1553" s="70" t="s">
+        <v>2923</v>
+      </c>
       <c r="F1553" s="70" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1553" s="70" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H1553" s="70" t="s">
-        <v>3056</v>
+        <v>3054</v>
       </c>
       <c r="I1553" s="70" t="s">
-        <v>3057</v>
-      </c>
-    </row>
-    <row r="1554" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1554" s="70">
-        <v>1717</v>
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1554" s="71">
+        <v>1714</v>
       </c>
       <c r="B1554" s="1" t="s">
-        <v>3058</v>
-      </c>
-      <c r="C1554" s="70">
-        <v>3</v>
-      </c>
-      <c r="D1554" s="70" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1554" s="70" t="s">
-        <v>2922</v>
-      </c>
-      <c r="F1554" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1554" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1554" s="70" t="s">
-        <v>3059</v>
-      </c>
-      <c r="I1554" s="70" t="s">
-        <v>3000</v>
+        <v>3102</v>
+      </c>
+      <c r="C1554" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1554" s="71" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1554" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1554" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1554" s="71" t="s">
+        <v>3103</v>
+      </c>
+      <c r="I1554" s="71" t="s">
+        <v>3104</v>
       </c>
     </row>
     <row r="1555" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1555" s="70">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="B1555" s="1" t="s">
-        <v>3060</v>
+        <v>3055</v>
       </c>
       <c r="C1555" s="70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1555" s="70" t="s">
         <v>1720</v>
       </c>
       <c r="F1555" s="70" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1555" s="70" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="H1555" s="70" t="s">
-        <v>3061</v>
+        <v>3056</v>
       </c>
       <c r="I1555" s="70" t="s">
-        <v>3062</v>
+        <v>3057</v>
       </c>
     </row>
     <row r="1556" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1556" s="70">
-        <v>1719</v>
+        <v>1717</v>
       </c>
       <c r="B1556" s="1" t="s">
-        <v>3063</v>
+        <v>3058</v>
       </c>
       <c r="C1556" s="70">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1556" s="70" t="s">
-        <v>2810</v>
+        <v>1720</v>
       </c>
       <c r="E1556" s="70" t="s">
-        <v>2924</v>
+        <v>2922</v>
       </c>
       <c r="F1556" s="70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1556" s="70" t="s">
-        <v>187</v>
+        <v>36</v>
       </c>
       <c r="H1556" s="70" t="s">
-        <v>3064</v>
+        <v>3059</v>
       </c>
       <c r="I1556" s="70" t="s">
-        <v>3026</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1557" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1557" s="70">
+        <v>1718</v>
+      </c>
+      <c r="B1557" s="1" t="s">
+        <v>3060</v>
+      </c>
+      <c r="C1557" s="70">
+        <v>3</v>
+      </c>
+      <c r="D1557" s="70" t="s">
         <v>1720</v>
       </c>
-      <c r="B1557" s="1" t="s">
-        <v>3065</v>
-      </c>
-      <c r="C1557" s="70">
-        <v>1</v>
-      </c>
-      <c r="D1557" s="70" t="s">
-        <v>1717</v>
-      </c>
       <c r="F1557" s="70" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1557" s="70" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H1557" s="70" t="s">
-        <v>3066</v>
+        <v>3061</v>
       </c>
       <c r="I1557" s="70" t="s">
-        <v>3000</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="1558" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1558" s="70">
-        <v>1721</v>
+        <v>1719</v>
       </c>
       <c r="B1558" s="1" t="s">
-        <v>3067</v>
+        <v>3063</v>
       </c>
       <c r="C1558" s="70">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1558" s="70" t="s">
-        <v>1720</v>
+        <v>2810</v>
       </c>
       <c r="E1558" s="70" t="s">
-        <v>2935</v>
+        <v>2924</v>
       </c>
       <c r="F1558" s="70" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G1558" s="70" t="s">
-        <v>10</v>
+        <v>187</v>
       </c>
       <c r="H1558" s="70" t="s">
-        <v>3068</v>
+        <v>3064</v>
       </c>
       <c r="I1558" s="70" t="s">
-        <v>3000</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="1559" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1559" s="70">
-        <v>1722</v>
+        <v>1720</v>
       </c>
       <c r="B1559" s="1" t="s">
-        <v>3069</v>
+        <v>3065</v>
       </c>
       <c r="C1559" s="70">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1559" s="70" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1559" s="70" t="s">
-        <v>2923</v>
+        <v>1717</v>
       </c>
       <c r="F1559" s="70" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1559" s="70" t="s">
-        <v>187</v>
+        <v>21</v>
       </c>
       <c r="H1559" s="70" t="s">
-        <v>3071</v>
+        <v>3066</v>
       </c>
       <c r="I1559" s="70" t="s">
-        <v>3018</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1560" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1560" s="70">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="B1560" s="1" t="s">
-        <v>3070</v>
+        <v>3067</v>
       </c>
       <c r="C1560" s="70">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1560" s="70" t="s">
         <v>1720</v>
@@ -46587,53 +46666,56 @@
         <v>2935</v>
       </c>
       <c r="F1560" s="70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1560" s="70" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="H1560" s="70" t="s">
-        <v>3072</v>
+        <v>3068</v>
       </c>
       <c r="I1560" s="70" t="s">
-        <v>3062</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1561" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1561" s="70">
-        <v>1725</v>
+        <v>1722</v>
       </c>
       <c r="B1561" s="1" t="s">
-        <v>3073</v>
+        <v>3069</v>
       </c>
       <c r="C1561" s="70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1561" s="70" t="s">
-        <v>1717</v>
+        <v>1720</v>
+      </c>
+      <c r="E1561" s="70" t="s">
+        <v>2923</v>
       </c>
       <c r="F1561" s="70" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1561" s="70" t="s">
-        <v>21</v>
+        <v>187</v>
       </c>
       <c r="H1561" s="70" t="s">
-        <v>3074</v>
+        <v>3071</v>
       </c>
       <c r="I1561" s="70" t="s">
-        <v>3000</v>
+        <v>3029</v>
       </c>
     </row>
     <row r="1562" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1562" s="70">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="B1562" s="1" t="s">
-        <v>3075</v>
+        <v>3070</v>
       </c>
       <c r="C1562" s="70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1562" s="70" t="s">
         <v>1720</v>
@@ -46642,76 +46724,609 @@
         <v>2935</v>
       </c>
       <c r="F1562" s="70" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G1562" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1562" s="70" t="s">
+        <v>3072</v>
+      </c>
+      <c r="I1562" s="70" t="s">
+        <v>3062</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1563" s="71">
+        <v>1724</v>
+      </c>
+      <c r="B1563" s="1" t="s">
+        <v>3100</v>
+      </c>
+      <c r="C1563" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1563" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1563" s="71" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1563" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1563" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1563" s="71" t="s">
+        <v>3101</v>
+      </c>
+      <c r="I1563" s="71" t="s">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1564" s="70">
+        <v>1725</v>
+      </c>
+      <c r="B1564" s="1" t="s">
+        <v>3073</v>
+      </c>
+      <c r="C1564" s="70">
+        <v>1</v>
+      </c>
+      <c r="D1564" s="70" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1564" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1564" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="H1562" s="70" t="s">
+      <c r="H1564" s="70" t="s">
+        <v>3074</v>
+      </c>
+      <c r="I1564" s="70" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1565" s="70">
+        <v>1726</v>
+      </c>
+      <c r="B1565" s="1" t="s">
+        <v>3075</v>
+      </c>
+      <c r="C1565" s="70">
+        <v>2</v>
+      </c>
+      <c r="D1565" s="70" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1565" s="70" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1565" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1565" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1565" s="70" t="s">
         <v>3077</v>
       </c>
-      <c r="I1562" s="70" t="s">
+      <c r="I1565" s="70" t="s">
         <v>3026</v>
       </c>
     </row>
-    <row r="1563" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1563" s="70">
+    <row r="1566" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1566" s="70">
         <v>1727</v>
       </c>
-      <c r="B1563" s="1" t="s">
+      <c r="B1566" s="1" t="s">
         <v>3076</v>
       </c>
-      <c r="C1563" s="70">
+      <c r="C1566" s="70">
         <v>4</v>
       </c>
-      <c r="D1563" s="70" t="s">
+      <c r="D1566" s="70" t="s">
         <v>1720</v>
       </c>
-      <c r="E1563" s="70" t="s">
+      <c r="E1566" s="70" t="s">
         <v>2922</v>
       </c>
-      <c r="F1563" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1563" s="70" t="s">
+      <c r="F1566" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1566" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="H1563" s="70" t="s">
+      <c r="H1566" s="70" t="s">
         <v>3078</v>
       </c>
-    </row>
-    <row r="1564" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1564" s="1"/>
-    </row>
-    <row r="1565" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1565" s="71" t="s">
+      <c r="I1566" s="70" t="s">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1567" s="71">
+        <v>1728</v>
+      </c>
+      <c r="B1567" s="1" t="s">
+        <v>3079</v>
+      </c>
+      <c r="C1567" s="71">
+        <v>6</v>
+      </c>
+      <c r="D1567" s="71" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1567" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1567" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1567" s="71" t="s">
+        <v>3080</v>
+      </c>
+      <c r="I1567" s="71" t="s">
+        <v>3081</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1568" s="71">
+        <v>1730</v>
+      </c>
+      <c r="B1568" s="1" t="s">
+        <v>3082</v>
+      </c>
+      <c r="C1568" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1568" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1568" s="71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1568" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1568" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1568" s="71" t="s">
+        <v>3083</v>
+      </c>
+      <c r="I1568" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1569" s="71">
+        <v>1732</v>
+      </c>
+      <c r="B1569" s="1" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C1569" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1569" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1569" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1569" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1569" s="71" t="s">
+        <v>3086</v>
+      </c>
+      <c r="I1569" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1570" s="71">
+        <v>1736</v>
+      </c>
+      <c r="B1570" s="1" t="s">
+        <v>3085</v>
+      </c>
+      <c r="C1570" s="71">
+        <v>2</v>
+      </c>
+      <c r="D1570" s="71" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1570" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1570" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1570" s="71" t="s">
+        <v>3087</v>
+      </c>
+      <c r="I1570" s="71" t="s">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1571" s="71">
+        <v>1740</v>
+      </c>
+      <c r="B1571" s="1" t="s">
+        <v>3098</v>
+      </c>
+      <c r="C1571" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1571" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1571" s="71" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1571" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1571" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1571" s="71" t="s">
+        <v>3099</v>
+      </c>
+      <c r="I1571" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1572" s="71">
+        <v>1742</v>
+      </c>
+      <c r="B1572" s="1" t="s">
+        <v>3088</v>
+      </c>
+      <c r="C1572" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1572" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1572" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1572" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1572" s="71" t="s">
+        <v>2082</v>
+      </c>
+      <c r="I1572" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1573" s="71">
+        <v>1746</v>
+      </c>
+      <c r="B1573" s="1" t="s">
+        <v>3096</v>
+      </c>
+      <c r="C1573" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1573" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1573" s="71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1573" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1573" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1573" s="71" t="s">
+        <v>3097</v>
+      </c>
+      <c r="I1573" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1574" s="71">
+        <v>1748</v>
+      </c>
+      <c r="B1574" s="1" t="s">
+        <v>3089</v>
+      </c>
+      <c r="C1574" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1574" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1574" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1574" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1574" s="71" t="s">
+        <v>3090</v>
+      </c>
+      <c r="I1574" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1575" s="71">
+        <v>1752</v>
+      </c>
+      <c r="B1575" s="1" t="s">
+        <v>3091</v>
+      </c>
+      <c r="C1575" s="71">
+        <v>2</v>
+      </c>
+      <c r="D1575" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1575" s="71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1575" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1575" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1575" s="71" t="s">
+        <v>3092</v>
+      </c>
+      <c r="I1575" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1576" s="71">
+        <v>1756</v>
+      </c>
+      <c r="B1576" s="1" t="s">
+        <v>3093</v>
+      </c>
+      <c r="C1576" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1576" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1576" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1576" s="71" t="s">
+        <v>457</v>
+      </c>
+      <c r="H1576" s="71" t="s">
+        <v>3094</v>
+      </c>
+      <c r="I1576" s="71" t="s">
+        <v>3095</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1577" s="1"/>
+    </row>
+    <row r="1578" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1578" s="1"/>
+    </row>
+    <row r="1579" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1579" s="1"/>
+    </row>
+    <row r="1580" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1580" s="1"/>
+    </row>
+    <row r="1581" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1581" s="1"/>
+    </row>
+    <row r="1582" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1582" s="1"/>
+    </row>
+    <row r="1583" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1583" s="1"/>
+    </row>
+    <row r="1584" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1584" s="1"/>
+    </row>
+    <row r="1585" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1585" s="1"/>
+    </row>
+    <row r="1586" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1586" s="1"/>
+    </row>
+    <row r="1587" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1587" s="1"/>
+    </row>
+    <row r="1588" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1588" s="1"/>
+    </row>
+    <row r="1589" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1589" s="1"/>
+    </row>
+    <row r="1590" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1590" s="1"/>
+    </row>
+    <row r="1591" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1591" s="1"/>
+    </row>
+    <row r="1592" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1592" s="1"/>
+    </row>
+    <row r="1593" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1593" s="1"/>
+    </row>
+    <row r="1594" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1594" s="1"/>
+    </row>
+    <row r="1595" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1595" s="1"/>
+    </row>
+    <row r="1596" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1596" s="1"/>
+    </row>
+    <row r="1597" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1597" s="1"/>
+    </row>
+    <row r="1598" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1598" s="1"/>
+    </row>
+    <row r="1599" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1599" s="1"/>
+    </row>
+    <row r="1600" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1600" s="1"/>
+    </row>
+    <row r="1601" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1601" s="1"/>
+    </row>
+    <row r="1602" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1602" s="1"/>
+    </row>
+    <row r="1603" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1603" s="1"/>
+    </row>
+    <row r="1604" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1604" s="1"/>
+    </row>
+    <row r="1605" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1605" s="1"/>
+    </row>
+    <row r="1606" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1606" s="1"/>
+    </row>
+    <row r="1607" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1607" s="1"/>
+    </row>
+    <row r="1608" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1608" s="1"/>
+    </row>
+    <row r="1609" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1609" s="1"/>
+    </row>
+    <row r="1610" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1610" s="1"/>
+    </row>
+    <row r="1611" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1611" s="1"/>
+    </row>
+    <row r="1612" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1612" s="1"/>
+    </row>
+    <row r="1613" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1613" s="1"/>
+    </row>
+    <row r="1614" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1614" s="1"/>
+    </row>
+    <row r="1615" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1615" s="1"/>
+    </row>
+    <row r="1616" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1616" s="1"/>
+    </row>
+    <row r="1617" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1617" s="1"/>
+    </row>
+    <row r="1618" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1618" s="1"/>
+    </row>
+    <row r="1619" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1619" s="1"/>
+    </row>
+    <row r="1620" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1620" s="1"/>
+    </row>
+    <row r="1621" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1621" s="1"/>
+    </row>
+    <row r="1622" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1622" s="1"/>
+    </row>
+    <row r="1623" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1623" s="1"/>
+    </row>
+    <row r="1624" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1624" s="1"/>
+    </row>
+    <row r="1625" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1625" s="1"/>
+    </row>
+    <row r="1626" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1626" s="1"/>
+    </row>
+    <row r="1627" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1627" s="1"/>
+    </row>
+    <row r="1628" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1628" s="1"/>
+    </row>
+    <row r="1629" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1629" s="1"/>
+    </row>
+    <row r="1630" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1630" s="1"/>
+    </row>
+    <row r="1631" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1631" s="1"/>
+    </row>
+    <row r="1632" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1632" s="1"/>
+    </row>
+    <row r="1633" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1633" s="1"/>
+    </row>
+    <row r="1634" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1634" s="1"/>
+    </row>
+    <row r="1635" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1635" s="1"/>
+    </row>
+    <row r="1636" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1636" s="72" t="s">
         <v>1721</v>
       </c>
-      <c r="B1565" s="71"/>
-      <c r="C1565" s="71"/>
-      <c r="D1565" s="71"/>
-      <c r="E1565" s="71"/>
-      <c r="F1565" s="71"/>
-      <c r="G1565" s="71"/>
-      <c r="H1565" s="71"/>
-    </row>
-    <row r="1566" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1566" s="72" t="s">
+      <c r="B1636" s="72"/>
+      <c r="C1636" s="72"/>
+      <c r="D1636" s="72"/>
+      <c r="E1636" s="72"/>
+      <c r="F1636" s="72"/>
+      <c r="G1636" s="72"/>
+      <c r="H1636" s="72"/>
+    </row>
+    <row r="1637" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1637" s="73" t="s">
         <v>2760</v>
       </c>
-      <c r="B1566" s="72"/>
-      <c r="C1566" s="72"/>
-      <c r="D1566" s="72"/>
-      <c r="E1566" s="72"/>
-      <c r="F1566" s="72"/>
-      <c r="G1566" s="72"/>
-      <c r="H1566" s="72"/>
+      <c r="B1637" s="73"/>
+      <c r="C1637" s="73"/>
+      <c r="D1637" s="73"/>
+      <c r="E1637" s="73"/>
+      <c r="F1637" s="73"/>
+      <c r="G1637" s="73"/>
+      <c r="H1637" s="73"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1566" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1637" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1565:H1565"/>
-    <mergeCell ref="A1566:H1566"/>
+    <mergeCell ref="A1636:H1636"/>
+    <mergeCell ref="A1637:H1637"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -48052,25 +48667,37 @@
     <hyperlink ref="B1546" r:id="rId1336" display="https://leetcode.com/problems/maximum-number-of-eaten-apples" xr:uid="{51810A39-CD35-42C8-99A0-89485FD327DD}"/>
     <hyperlink ref="B1547" r:id="rId1337" display="https://leetcode.com/problems/where-will-the-ball-fall" xr:uid="{5F6F112E-0A35-49CE-BFFA-46F8C5C79F91}"/>
     <hyperlink ref="B1548" r:id="rId1338" display="https://leetcode.com/problems/maximum-xor-with-an-element-from-array" xr:uid="{9BF62A49-6718-4423-8433-DB86DC82824F}"/>
-    <hyperlink ref="B1549" r:id="rId1339" display="https://leetcode.com/problems/maximum-units-on-a-truck" xr:uid="{FA401603-3720-4E2D-B41B-750A14701D79}"/>
-    <hyperlink ref="B1550" r:id="rId1340" display="https://leetcode.com/problems/count-good-meals" xr:uid="{7D054C68-287C-4CDA-84E9-ABB8672601B9}"/>
-    <hyperlink ref="B1551" r:id="rId1341" display="https://leetcode.com/problems/ways-to-split-array-into-three-subarrays" xr:uid="{EB39B226-B1EA-4385-908B-CA58EAF15E2A}"/>
-    <hyperlink ref="B1552" r:id="rId1342" display="https://leetcode.com/problems/minimum-operations-to-make-a-subsequence" xr:uid="{3BF58768-569A-48ED-916E-9B5B92E9A489}"/>
-    <hyperlink ref="B1553" r:id="rId1343" display="https://leetcode.com/problems/calculate-money-in-leetcode-bank" xr:uid="{9A5AA38F-37C0-4252-B28C-B1571495B9D8}"/>
-    <hyperlink ref="B1554" r:id="rId1344" display="https://leetcode.com/problems/maximum-score-from-removing-substrings" xr:uid="{20802F12-8929-4B53-9288-3D2053019349}"/>
-    <hyperlink ref="B1555" r:id="rId1345" display="https://leetcode.com/problems/construct-the-lexicographically-largest-valid-sequence" xr:uid="{B73EB4B2-83E4-4F74-9B5B-B569CA68580B}"/>
-    <hyperlink ref="B1556" r:id="rId1346" display="https://leetcode.com/problems/number-of-ways-to-reconstruct-a-tree" xr:uid="{E6998458-D32E-4365-BC4B-FEBEE05D52B6}"/>
-    <hyperlink ref="B1557" r:id="rId1347" display="https://leetcode.com/problems/decode-xored-array" xr:uid="{0BA9C45F-4B21-497A-93AA-C47D2F0FB2B8}"/>
-    <hyperlink ref="B1558" r:id="rId1348" display="https://leetcode.com/problems/swapping-nodes-in-a-linked-list" xr:uid="{5D9D3F5C-5DD2-4F18-B382-B562212DAFB8}"/>
-    <hyperlink ref="B1559" r:id="rId1349" display="https://leetcode.com/problems/minimize-hamming-distance-after-swap-operations" xr:uid="{0D233304-DCA8-4ACD-BA33-ABA007389765}"/>
-    <hyperlink ref="B1560" r:id="rId1350" display="https://leetcode.com/problems/find-minimum-time-to-finish-all-jobs" xr:uid="{34306947-008A-4748-89D4-C6894490198D}"/>
-    <hyperlink ref="B1561" r:id="rId1351" display="https://leetcode.com/problems/number-of-rectangles-that-can-form-the-largest-square" xr:uid="{F2DC20DE-9474-4173-A170-F0ED4BD77F31}"/>
-    <hyperlink ref="B1562" r:id="rId1352" display="https://leetcode.com/problems/tuple-with-same-product" xr:uid="{8ACCF7DE-E5E5-4246-9298-0C5F53184D31}"/>
-    <hyperlink ref="B1563" r:id="rId1353" display="https://leetcode.com/problems/largest-submatrix-with-rearrangements" xr:uid="{1B4C7B82-E77E-4ACA-BC37-45E56FB369EA}"/>
+    <hyperlink ref="B1550" r:id="rId1339" display="https://leetcode.com/problems/maximum-units-on-a-truck" xr:uid="{FA401603-3720-4E2D-B41B-750A14701D79}"/>
+    <hyperlink ref="B1551" r:id="rId1340" display="https://leetcode.com/problems/count-good-meals" xr:uid="{7D054C68-287C-4CDA-84E9-ABB8672601B9}"/>
+    <hyperlink ref="B1552" r:id="rId1341" display="https://leetcode.com/problems/ways-to-split-array-into-three-subarrays" xr:uid="{EB39B226-B1EA-4385-908B-CA58EAF15E2A}"/>
+    <hyperlink ref="B1553" r:id="rId1342" display="https://leetcode.com/problems/minimum-operations-to-make-a-subsequence" xr:uid="{3BF58768-569A-48ED-916E-9B5B92E9A489}"/>
+    <hyperlink ref="B1555" r:id="rId1343" display="https://leetcode.com/problems/calculate-money-in-leetcode-bank" xr:uid="{9A5AA38F-37C0-4252-B28C-B1571495B9D8}"/>
+    <hyperlink ref="B1556" r:id="rId1344" display="https://leetcode.com/problems/maximum-score-from-removing-substrings" xr:uid="{20802F12-8929-4B53-9288-3D2053019349}"/>
+    <hyperlink ref="B1557" r:id="rId1345" display="https://leetcode.com/problems/construct-the-lexicographically-largest-valid-sequence" xr:uid="{B73EB4B2-83E4-4F74-9B5B-B569CA68580B}"/>
+    <hyperlink ref="B1558" r:id="rId1346" display="https://leetcode.com/problems/number-of-ways-to-reconstruct-a-tree" xr:uid="{E6998458-D32E-4365-BC4B-FEBEE05D52B6}"/>
+    <hyperlink ref="B1559" r:id="rId1347" display="https://leetcode.com/problems/decode-xored-array" xr:uid="{0BA9C45F-4B21-497A-93AA-C47D2F0FB2B8}"/>
+    <hyperlink ref="B1560" r:id="rId1348" display="https://leetcode.com/problems/swapping-nodes-in-a-linked-list" xr:uid="{5D9D3F5C-5DD2-4F18-B382-B562212DAFB8}"/>
+    <hyperlink ref="B1561" r:id="rId1349" display="https://leetcode.com/problems/minimize-hamming-distance-after-swap-operations" xr:uid="{0D233304-DCA8-4ACD-BA33-ABA007389765}"/>
+    <hyperlink ref="B1562" r:id="rId1350" display="https://leetcode.com/problems/find-minimum-time-to-finish-all-jobs" xr:uid="{34306947-008A-4748-89D4-C6894490198D}"/>
+    <hyperlink ref="B1564" r:id="rId1351" display="https://leetcode.com/problems/number-of-rectangles-that-can-form-the-largest-square" xr:uid="{F2DC20DE-9474-4173-A170-F0ED4BD77F31}"/>
+    <hyperlink ref="B1565" r:id="rId1352" display="https://leetcode.com/problems/tuple-with-same-product" xr:uid="{8ACCF7DE-E5E5-4246-9298-0C5F53184D31}"/>
+    <hyperlink ref="B1566" r:id="rId1353" display="https://leetcode.com/problems/largest-submatrix-with-rearrangements" xr:uid="{1B4C7B82-E77E-4ACA-BC37-45E56FB369EA}"/>
+    <hyperlink ref="B1567" r:id="rId1354" display="https://leetcode.com/problems/cat-and-mouse-ii" xr:uid="{1BE50E36-6C70-4366-8C0C-ABAB86AC2FA1}"/>
+    <hyperlink ref="B1568" r:id="rId1355" display="https://leetcode.com/problems/shortest-path-to-get-food" xr:uid="{94E61D7A-2B84-43BA-95AD-6D92AB56598C}"/>
+    <hyperlink ref="B1569" r:id="rId1356" display="https://leetcode.com/problems/find-the-highest-altitude" xr:uid="{B2085815-293D-42BF-A84D-6F7F0CC198BE}"/>
+    <hyperlink ref="B1570" r:id="rId1357" display="https://leetcode.com/problems/latest-time-by-replacing-hidden-digits" xr:uid="{FFB49099-001C-44BA-B278-B00A3A11671D}"/>
+    <hyperlink ref="B1572" r:id="rId1358" display="https://leetcode.com/problems/maximum-number-of-balls-in-a-box" xr:uid="{18366F0A-A3CF-4126-BA67-AE626616A691}"/>
+    <hyperlink ref="B1574" r:id="rId1359" display="https://leetcode.com/problems/sum-of-unique-elements" xr:uid="{B93FC0DC-83AD-4019-B434-79BA3ECF3C27}"/>
+    <hyperlink ref="B1575" r:id="rId1360" display="https://leetcode.com/problems/check-if-array-is-sorted-and-rotated" xr:uid="{EFE2F4D1-0950-49F4-B136-E72B4AF0D449}"/>
+    <hyperlink ref="B1576" r:id="rId1361" display="https://leetcode.com/problems/design-most-recently-used-queue" xr:uid="{74130DE4-2D04-4D3B-BEF6-58D20F61C5E0}"/>
+    <hyperlink ref="B1573" r:id="rId1362" display="https://leetcode.com/problems/maximum-subarray-sum-after-one-operation" xr:uid="{9ABF6461-8E02-44BB-9725-D17CBB89070F}"/>
+    <hyperlink ref="B1571" r:id="rId1363" display="https://leetcode.com/problems/find-distance-in-a-binary-tree" xr:uid="{92429178-67ED-4AD2-859E-9E026EEAF7BD}"/>
+    <hyperlink ref="B1563" r:id="rId1364" display="https://leetcode.com/problems/checking-existence-of-edge-length-limited-paths-ii" xr:uid="{A09CC7F8-57B2-4D18-8FCA-F1B91534ED7F}"/>
+    <hyperlink ref="B1554" r:id="rId1365" display="https://leetcode.com/problems/sum-of-special-evenly-spaced-elements-in-array" xr:uid="{6CC25C62-1D5D-4F0D-96CA-DD0F34BB1CA9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1354"/>
-  <drawing r:id="rId1355"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1366"/>
+  <drawing r:id="rId1367"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in two weeks problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B194A4-46FB-4C48-AF12-AFDBC990CB4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD9F236-55C2-4BF0-809B-5F9908AEED0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="0" windowWidth="18900" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18900" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Algorithm" sheetId="1" r:id="rId1"/>
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1637</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1648</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8360" uniqueCount="3107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8430" uniqueCount="3132">
   <si>
     <t>Difficulty</t>
   </si>
@@ -9358,6 +9358,81 @@
   </si>
   <si>
     <t>Reset head of sub array</t>
+  </si>
+  <si>
+    <t>Minimum Number of People to Teach</t>
+  </si>
+  <si>
+    <t>Count friends can not talk, then count common language</t>
+  </si>
+  <si>
+    <t>Decode XORed Permutation</t>
+  </si>
+  <si>
+    <t>Calculate 1 to N XOR, then XOR with A[1]^A[3]^... ^A[N-1]</t>
+  </si>
+  <si>
+    <t>Count Ways to Make Array With Product</t>
+  </si>
+  <si>
+    <t>Star and Bar theory</t>
+  </si>
+  <si>
+    <t>Change Minimum Characters to Satisfy One of Three Conditions</t>
+  </si>
+  <si>
+    <t>Count from A to Z</t>
+  </si>
+  <si>
+    <t>Find Kth Largest XOR Coordinate Value</t>
+  </si>
+  <si>
+    <t>Iterate row by row with accumulated XOR</t>
+  </si>
+  <si>
+    <t>N*M</t>
+  </si>
+  <si>
+    <t>Building Boxes</t>
+  </si>
+  <si>
+    <t>Build the series of numbers 1 + (1+2) + (1+…+N)</t>
+  </si>
+  <si>
+    <t>N^ (1/3)</t>
+  </si>
+  <si>
+    <t>Restore the Array From Adjacent Pairs</t>
+  </si>
+  <si>
+    <t>Simplified topology sort</t>
+  </si>
+  <si>
+    <t>Can You Eat Your Favorite Candy on Your Favorite Day?</t>
+  </si>
+  <si>
+    <t>Calculate presum</t>
+  </si>
+  <si>
+    <t>Maximum Score From Removing Stones</t>
+  </si>
+  <si>
+    <t>Compare the maximum with remaing 2</t>
+  </si>
+  <si>
+    <t>Largest Merge Of Two Strings</t>
+  </si>
+  <si>
+    <t>pick the first character from larger string</t>
+  </si>
+  <si>
+    <t>Closest Subsequence Sum</t>
+  </si>
+  <si>
+    <t>Divide the array into two groups</t>
+  </si>
+  <si>
+    <t>E ^ (N/2)</t>
   </si>
 </sst>
 </file>
@@ -9402,7 +9477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -9429,6 +9504,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -9865,10 +9942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1637"/>
+  <dimension ref="A1:J1648"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1555" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1555" sqref="A1555"/>
+    <sheetView tabSelected="1" topLeftCell="A1562" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1587" sqref="A1587"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12977,7 +13054,7 @@
         <v>4</v>
       </c>
       <c r="D133" t="s">
-        <v>2810</v>
+        <v>1720</v>
       </c>
       <c r="F133" t="s">
         <v>12</v>
@@ -46930,267 +47007,532 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="1570" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1570" s="71">
-        <v>1736</v>
+    <row r="1570" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1570" s="72">
+        <v>1733</v>
       </c>
       <c r="B1570" s="1" t="s">
-        <v>3085</v>
-      </c>
-      <c r="C1570" s="71">
-        <v>2</v>
-      </c>
-      <c r="D1570" s="71" t="s">
+        <v>3107</v>
+      </c>
+      <c r="C1570" s="72">
+        <v>3</v>
+      </c>
+      <c r="D1570" s="72" t="s">
         <v>1713</v>
       </c>
-      <c r="F1570" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1570" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1570" s="71" t="s">
-        <v>3087</v>
-      </c>
-      <c r="I1570" s="71" t="s">
-        <v>3057</v>
-      </c>
-    </row>
-    <row r="1571" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1571" s="71">
-        <v>1740</v>
+      <c r="F1570" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1570" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1570" s="72" t="s">
+        <v>3108</v>
+      </c>
+      <c r="I1570" s="72" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1571" s="72">
+        <v>1734</v>
       </c>
       <c r="B1571" s="1" t="s">
-        <v>3098</v>
-      </c>
-      <c r="C1571" s="71">
-        <v>3</v>
-      </c>
-      <c r="D1571" s="71" t="s">
+        <v>3109</v>
+      </c>
+      <c r="C1571" s="72">
+        <v>3</v>
+      </c>
+      <c r="D1571" s="72" t="s">
         <v>1720</v>
       </c>
-      <c r="E1571" s="71" t="s">
-        <v>2924</v>
-      </c>
-      <c r="F1571" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1571" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1571" s="71" t="s">
-        <v>3099</v>
-      </c>
-      <c r="I1571" s="71" t="s">
+      <c r="E1571" s="72" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1571" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1571" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1571" s="72" t="s">
+        <v>3110</v>
+      </c>
+      <c r="I1571" s="72" t="s">
         <v>3000</v>
       </c>
     </row>
-    <row r="1572" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1572" s="71">
-        <v>1742</v>
+    <row r="1572" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1572" s="73">
+        <v>1735</v>
       </c>
       <c r="B1572" s="1" t="s">
-        <v>3088</v>
-      </c>
-      <c r="C1572" s="71">
-        <v>1</v>
-      </c>
-      <c r="D1572" s="71" t="s">
-        <v>1717</v>
-      </c>
-      <c r="F1572" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1572" s="71" t="s">
+        <v>3111</v>
+      </c>
+      <c r="C1572" s="73">
+        <v>4</v>
+      </c>
+      <c r="D1572" s="73" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1572" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1572" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="H1572" s="71" t="s">
-        <v>2082</v>
-      </c>
-      <c r="I1572" s="71" t="s">
+      <c r="H1572" s="73" t="s">
+        <v>3112</v>
+      </c>
+      <c r="I1572" s="73" t="s">
         <v>3000</v>
       </c>
     </row>
     <row r="1573" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1573" s="71">
+        <v>1736</v>
+      </c>
+      <c r="B1573" s="1" t="s">
+        <v>3085</v>
+      </c>
+      <c r="C1573" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1573" s="71" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1573" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1573" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1573" s="71" t="s">
+        <v>3087</v>
+      </c>
+      <c r="I1573" s="71" t="s">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1574" s="73">
+        <v>1737</v>
+      </c>
+      <c r="B1574" s="1" t="s">
+        <v>3113</v>
+      </c>
+      <c r="C1574" s="73">
+        <v>4</v>
+      </c>
+      <c r="D1574" s="73" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1574" s="73" t="s">
+        <v>2922</v>
+      </c>
+      <c r="F1574" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1574" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1574" s="73" t="s">
+        <v>3114</v>
+      </c>
+      <c r="I1574" s="73" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1575" s="73">
+        <v>1738</v>
+      </c>
+      <c r="B1575" s="1" t="s">
+        <v>3115</v>
+      </c>
+      <c r="C1575" s="73">
+        <v>3</v>
+      </c>
+      <c r="D1575" s="73" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1575" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1575" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1575" s="73" t="s">
+        <v>3116</v>
+      </c>
+      <c r="I1575" s="73" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1576" s="73">
+        <v>1739</v>
+      </c>
+      <c r="B1576" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="C1576" s="73">
+        <v>4</v>
+      </c>
+      <c r="D1576" s="73" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1576" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1576" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1576" s="73" t="s">
+        <v>3119</v>
+      </c>
+      <c r="I1576" s="73" t="s">
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1577" s="71">
+        <v>1740</v>
+      </c>
+      <c r="B1577" s="1" t="s">
+        <v>3098</v>
+      </c>
+      <c r="C1577" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1577" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1577" s="71" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1577" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1577" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1577" s="71" t="s">
+        <v>3099</v>
+      </c>
+      <c r="I1577" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1578" s="71">
+        <v>1742</v>
+      </c>
+      <c r="B1578" s="1" t="s">
+        <v>3088</v>
+      </c>
+      <c r="C1578" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1578" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1578" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1578" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1578" s="71" t="s">
+        <v>2082</v>
+      </c>
+      <c r="I1578" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1579" s="73">
+        <v>1743</v>
+      </c>
+      <c r="B1579" s="1" t="s">
+        <v>3121</v>
+      </c>
+      <c r="C1579" s="73">
+        <v>3</v>
+      </c>
+      <c r="D1579" s="73" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1579" s="73" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1579" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1579" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1579" s="73" t="s">
+        <v>3122</v>
+      </c>
+      <c r="I1579" s="73" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1580" s="73">
+        <v>1744</v>
+      </c>
+      <c r="B1580" s="1" t="s">
+        <v>3123</v>
+      </c>
+      <c r="C1580" s="73">
+        <v>3</v>
+      </c>
+      <c r="D1580" s="73" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1580" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1580" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1580" s="73" t="s">
+        <v>3124</v>
+      </c>
+      <c r="I1580" s="73" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1581" s="71">
         <v>1746</v>
       </c>
-      <c r="B1573" s="1" t="s">
+      <c r="B1581" s="1" t="s">
         <v>3096</v>
       </c>
-      <c r="C1573" s="71">
-        <v>3</v>
-      </c>
-      <c r="D1573" s="71" t="s">
+      <c r="C1581" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1581" s="71" t="s">
         <v>1720</v>
       </c>
-      <c r="E1573" s="71" t="s">
+      <c r="E1581" s="71" t="s">
         <v>2935</v>
       </c>
-      <c r="F1573" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1573" s="71" t="s">
+      <c r="F1581" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1581" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="H1573" s="71" t="s">
+      <c r="H1581" s="71" t="s">
         <v>3097</v>
       </c>
-      <c r="I1573" s="71" t="s">
+      <c r="I1581" s="71" t="s">
         <v>3000</v>
       </c>
     </row>
-    <row r="1574" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1574" s="71">
+    <row r="1582" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1582" s="71">
         <v>1748</v>
       </c>
-      <c r="B1574" s="1" t="s">
+      <c r="B1582" s="1" t="s">
         <v>3089</v>
       </c>
-      <c r="C1574" s="71">
+      <c r="C1582" s="71">
         <v>1</v>
       </c>
-      <c r="D1574" s="71" t="s">
+      <c r="D1582" s="71" t="s">
         <v>1717</v>
       </c>
-      <c r="F1574" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1574" s="71" t="s">
+      <c r="F1582" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1582" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="H1574" s="71" t="s">
+      <c r="H1582" s="71" t="s">
         <v>3090</v>
       </c>
-      <c r="I1574" s="71" t="s">
+      <c r="I1582" s="71" t="s">
         <v>3000</v>
       </c>
     </row>
-    <row r="1575" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1575" s="71">
+    <row r="1583" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1583" s="71">
         <v>1752</v>
       </c>
-      <c r="B1575" s="1" t="s">
+      <c r="B1583" s="1" t="s">
         <v>3091</v>
       </c>
-      <c r="C1575" s="71">
+      <c r="C1583" s="71">
         <v>2</v>
       </c>
-      <c r="D1575" s="71" t="s">
+      <c r="D1583" s="71" t="s">
         <v>1720</v>
       </c>
-      <c r="E1575" s="71" t="s">
+      <c r="E1583" s="71" t="s">
         <v>2935</v>
       </c>
-      <c r="F1575" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1575" s="71" t="s">
+      <c r="F1583" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1583" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="H1575" s="71" t="s">
+      <c r="H1583" s="71" t="s">
         <v>3092</v>
       </c>
-      <c r="I1575" s="71" t="s">
+      <c r="I1583" s="71" t="s">
         <v>3000</v>
       </c>
     </row>
-    <row r="1576" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1576" s="71">
+    <row r="1584" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1584" s="73">
+        <v>1753</v>
+      </c>
+      <c r="B1584" s="1" t="s">
+        <v>3125</v>
+      </c>
+      <c r="C1584" s="73">
+        <v>3</v>
+      </c>
+      <c r="D1584" s="73" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1584" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1584" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1584" s="73" t="s">
+        <v>3126</v>
+      </c>
+      <c r="I1584" s="73" t="s">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1585" s="73">
+        <v>1754</v>
+      </c>
+      <c r="B1585" s="1" t="s">
+        <v>3127</v>
+      </c>
+      <c r="C1585" s="73">
+        <v>4</v>
+      </c>
+      <c r="D1585" s="73" t="s">
+        <v>2810</v>
+      </c>
+      <c r="E1585" s="73" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1585" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1585" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1585" s="73" t="s">
+        <v>3128</v>
+      </c>
+      <c r="I1585" s="73" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1586" s="73">
+        <v>1755</v>
+      </c>
+      <c r="B1586" s="1" t="s">
+        <v>3129</v>
+      </c>
+      <c r="C1586" s="73">
+        <v>4</v>
+      </c>
+      <c r="D1586" s="73" t="s">
+        <v>2810</v>
+      </c>
+      <c r="F1586" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1586" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1586" s="73" t="s">
+        <v>3130</v>
+      </c>
+      <c r="I1586" s="73" t="s">
+        <v>3131</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1587" s="71">
         <v>1756</v>
       </c>
-      <c r="B1576" s="1" t="s">
+      <c r="B1587" s="1" t="s">
         <v>3093</v>
       </c>
-      <c r="C1576" s="71">
-        <v>3</v>
-      </c>
-      <c r="D1576" s="71" t="s">
+      <c r="C1587" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1587" s="71" t="s">
         <v>1720</v>
       </c>
-      <c r="F1576" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1576" s="71" t="s">
+      <c r="F1587" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1587" s="71" t="s">
         <v>457</v>
       </c>
-      <c r="H1576" s="71" t="s">
+      <c r="H1587" s="71" t="s">
         <v>3094</v>
       </c>
-      <c r="I1576" s="71" t="s">
+      <c r="I1587" s="71" t="s">
         <v>3095</v>
       </c>
     </row>
-    <row r="1577" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1577" s="1"/>
-    </row>
-    <row r="1578" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1578" s="1"/>
-    </row>
-    <row r="1579" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1579" s="1"/>
-    </row>
-    <row r="1580" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1580" s="1"/>
-    </row>
-    <row r="1581" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1581" s="1"/>
-    </row>
-    <row r="1582" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1582" s="1"/>
-    </row>
-    <row r="1583" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1583" s="1"/>
-    </row>
-    <row r="1584" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1584" s="1"/>
-    </row>
-    <row r="1585" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1585" s="1"/>
-    </row>
-    <row r="1586" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1586" s="1"/>
-    </row>
-    <row r="1587" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1587" s="1"/>
-    </row>
-    <row r="1588" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1588" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1588" s="1"/>
     </row>
-    <row r="1589" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1589" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1589" s="1"/>
     </row>
-    <row r="1590" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1590" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1590" s="1"/>
     </row>
-    <row r="1591" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1591" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1591" s="1"/>
     </row>
-    <row r="1592" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1592" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1592" s="1"/>
     </row>
-    <row r="1593" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1593" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1593" s="1"/>
     </row>
-    <row r="1594" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1594" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1594" s="1"/>
     </row>
-    <row r="1595" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1595" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1595" s="1"/>
     </row>
-    <row r="1596" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1596" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1596" s="1"/>
     </row>
-    <row r="1597" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1597" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1597" s="1"/>
     </row>
-    <row r="1598" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1598" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1598" s="1"/>
     </row>
-    <row r="1599" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1599" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1599" s="1"/>
     </row>
-    <row r="1600" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1600" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1600" s="1"/>
     </row>
     <row r="1601" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
@@ -47295,38 +47637,71 @@
     <row r="1634" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1634" s="1"/>
     </row>
-    <row r="1635" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1635" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1635" s="1"/>
     </row>
-    <row r="1636" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1636" s="72" t="s">
+    <row r="1636" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1636" s="1"/>
+    </row>
+    <row r="1637" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1637" s="1"/>
+    </row>
+    <row r="1638" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1638" s="1"/>
+    </row>
+    <row r="1639" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1639" s="1"/>
+    </row>
+    <row r="1640" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1640" s="1"/>
+    </row>
+    <row r="1641" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1641" s="1"/>
+    </row>
+    <row r="1642" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1642" s="1"/>
+    </row>
+    <row r="1643" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1643" s="1"/>
+    </row>
+    <row r="1644" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1644" s="1"/>
+    </row>
+    <row r="1645" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1645" s="1"/>
+    </row>
+    <row r="1646" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1646" s="1"/>
+    </row>
+    <row r="1647" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1647" s="74" t="s">
         <v>1721</v>
       </c>
-      <c r="B1636" s="72"/>
-      <c r="C1636" s="72"/>
-      <c r="D1636" s="72"/>
-      <c r="E1636" s="72"/>
-      <c r="F1636" s="72"/>
-      <c r="G1636" s="72"/>
-      <c r="H1636" s="72"/>
-    </row>
-    <row r="1637" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1637" s="73" t="s">
+      <c r="B1647" s="74"/>
+      <c r="C1647" s="74"/>
+      <c r="D1647" s="74"/>
+      <c r="E1647" s="74"/>
+      <c r="F1647" s="74"/>
+      <c r="G1647" s="74"/>
+      <c r="H1647" s="74"/>
+    </row>
+    <row r="1648" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1648" s="75" t="s">
         <v>2760</v>
       </c>
-      <c r="B1637" s="73"/>
-      <c r="C1637" s="73"/>
-      <c r="D1637" s="73"/>
-      <c r="E1637" s="73"/>
-      <c r="F1637" s="73"/>
-      <c r="G1637" s="73"/>
-      <c r="H1637" s="73"/>
+      <c r="B1648" s="75"/>
+      <c r="C1648" s="75"/>
+      <c r="D1648" s="75"/>
+      <c r="E1648" s="75"/>
+      <c r="F1648" s="75"/>
+      <c r="G1648" s="75"/>
+      <c r="H1648" s="75"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1637" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1648" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1636:H1636"/>
-    <mergeCell ref="A1637:H1637"/>
+    <mergeCell ref="A1647:H1647"/>
+    <mergeCell ref="A1648:H1648"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -48685,19 +49060,29 @@
     <hyperlink ref="B1567" r:id="rId1354" display="https://leetcode.com/problems/cat-and-mouse-ii" xr:uid="{1BE50E36-6C70-4366-8C0C-ABAB86AC2FA1}"/>
     <hyperlink ref="B1568" r:id="rId1355" display="https://leetcode.com/problems/shortest-path-to-get-food" xr:uid="{94E61D7A-2B84-43BA-95AD-6D92AB56598C}"/>
     <hyperlink ref="B1569" r:id="rId1356" display="https://leetcode.com/problems/find-the-highest-altitude" xr:uid="{B2085815-293D-42BF-A84D-6F7F0CC198BE}"/>
-    <hyperlink ref="B1570" r:id="rId1357" display="https://leetcode.com/problems/latest-time-by-replacing-hidden-digits" xr:uid="{FFB49099-001C-44BA-B278-B00A3A11671D}"/>
-    <hyperlink ref="B1572" r:id="rId1358" display="https://leetcode.com/problems/maximum-number-of-balls-in-a-box" xr:uid="{18366F0A-A3CF-4126-BA67-AE626616A691}"/>
-    <hyperlink ref="B1574" r:id="rId1359" display="https://leetcode.com/problems/sum-of-unique-elements" xr:uid="{B93FC0DC-83AD-4019-B434-79BA3ECF3C27}"/>
-    <hyperlink ref="B1575" r:id="rId1360" display="https://leetcode.com/problems/check-if-array-is-sorted-and-rotated" xr:uid="{EFE2F4D1-0950-49F4-B136-E72B4AF0D449}"/>
-    <hyperlink ref="B1576" r:id="rId1361" display="https://leetcode.com/problems/design-most-recently-used-queue" xr:uid="{74130DE4-2D04-4D3B-BEF6-58D20F61C5E0}"/>
-    <hyperlink ref="B1573" r:id="rId1362" display="https://leetcode.com/problems/maximum-subarray-sum-after-one-operation" xr:uid="{9ABF6461-8E02-44BB-9725-D17CBB89070F}"/>
-    <hyperlink ref="B1571" r:id="rId1363" display="https://leetcode.com/problems/find-distance-in-a-binary-tree" xr:uid="{92429178-67ED-4AD2-859E-9E026EEAF7BD}"/>
+    <hyperlink ref="B1573" r:id="rId1357" display="https://leetcode.com/problems/latest-time-by-replacing-hidden-digits" xr:uid="{FFB49099-001C-44BA-B278-B00A3A11671D}"/>
+    <hyperlink ref="B1578" r:id="rId1358" display="https://leetcode.com/problems/maximum-number-of-balls-in-a-box" xr:uid="{18366F0A-A3CF-4126-BA67-AE626616A691}"/>
+    <hyperlink ref="B1582" r:id="rId1359" display="https://leetcode.com/problems/sum-of-unique-elements" xr:uid="{B93FC0DC-83AD-4019-B434-79BA3ECF3C27}"/>
+    <hyperlink ref="B1583" r:id="rId1360" display="https://leetcode.com/problems/check-if-array-is-sorted-and-rotated" xr:uid="{EFE2F4D1-0950-49F4-B136-E72B4AF0D449}"/>
+    <hyperlink ref="B1587" r:id="rId1361" display="https://leetcode.com/problems/design-most-recently-used-queue" xr:uid="{74130DE4-2D04-4D3B-BEF6-58D20F61C5E0}"/>
+    <hyperlink ref="B1581" r:id="rId1362" display="https://leetcode.com/problems/maximum-subarray-sum-after-one-operation" xr:uid="{9ABF6461-8E02-44BB-9725-D17CBB89070F}"/>
+    <hyperlink ref="B1577" r:id="rId1363" display="https://leetcode.com/problems/find-distance-in-a-binary-tree" xr:uid="{92429178-67ED-4AD2-859E-9E026EEAF7BD}"/>
     <hyperlink ref="B1563" r:id="rId1364" display="https://leetcode.com/problems/checking-existence-of-edge-length-limited-paths-ii" xr:uid="{A09CC7F8-57B2-4D18-8FCA-F1B91534ED7F}"/>
     <hyperlink ref="B1554" r:id="rId1365" display="https://leetcode.com/problems/sum-of-special-evenly-spaced-elements-in-array" xr:uid="{6CC25C62-1D5D-4F0D-96CA-DD0F34BB1CA9}"/>
+    <hyperlink ref="B1570" r:id="rId1366" display="https://leetcode.com/problems/minimum-number-of-people-to-teach" xr:uid="{01884F04-6E6D-4298-B749-235016439D32}"/>
+    <hyperlink ref="B1571" r:id="rId1367" display="https://leetcode.com/problems/decode-xored-permutation" xr:uid="{61FB12DA-4C34-4EB8-A96A-D1D8DD6C496F}"/>
+    <hyperlink ref="B1572" r:id="rId1368" display="https://leetcode.com/problems/count-ways-to-make-array-with-product" xr:uid="{A9E0D378-1AAB-4EAD-B1B4-5702110BF8E0}"/>
+    <hyperlink ref="B1574" r:id="rId1369" display="https://leetcode.com/problems/change-minimum-characters-to-satisfy-one-of-three-conditions" xr:uid="{6C2C8CC0-F97B-40D9-B23A-AC99489A1B9B}"/>
+    <hyperlink ref="B1575" r:id="rId1370" display="https://leetcode.com/problems/find-kth-largest-xor-coordinate-value" xr:uid="{4E6C3629-D879-47B1-A840-9CC82C824C47}"/>
+    <hyperlink ref="B1576" r:id="rId1371" display="https://leetcode.com/problems/building-boxes" xr:uid="{BAA2B99F-FF9E-4F72-B24E-7E96F1A3F674}"/>
+    <hyperlink ref="B1579" r:id="rId1372" display="https://leetcode.com/problems/restore-the-array-from-adjacent-pairs" xr:uid="{700623B8-2FF0-4710-A00D-C7B2A0A7ABA6}"/>
+    <hyperlink ref="B1580" r:id="rId1373" display="https://leetcode.com/problems/can-you-eat-your-favorite-candy-on-your-favorite-day" xr:uid="{BEE070B5-F64C-4698-BCE5-1E36A8583440}"/>
+    <hyperlink ref="B1584" r:id="rId1374" display="https://leetcode.com/problems/maximum-score-from-removing-stones" xr:uid="{B7AA18C7-E58A-447A-915A-42D4F13D6310}"/>
+    <hyperlink ref="B1586" r:id="rId1375" display="https://leetcode.com/problems/closest-subsequence-sum" xr:uid="{F32459B0-DF4C-462A-9356-83F25EC7DAA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1366"/>
-  <drawing r:id="rId1367"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1376"/>
+  <drawing r:id="rId1377"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in easy and medium problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD9F236-55C2-4BF0-809B-5F9908AEED0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CCD789-E5BD-43A0-BB1B-9D96E4B1BD63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18900" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Algorithm" sheetId="1" r:id="rId1"/>
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1648</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1659</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8430" uniqueCount="3132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8548" uniqueCount="3170">
   <si>
     <t>Difficulty</t>
   </si>
@@ -9433,6 +9433,120 @@
   </si>
   <si>
     <t>E ^ (N/2)</t>
+  </si>
+  <si>
+    <t>Number of Restricted Paths From First to Last Node</t>
+  </si>
+  <si>
+    <t>Minimum Elements to Add to Form a Given Sum </t>
+  </si>
+  <si>
+    <t>Check if Binary String Has at Most One Segment of Ones </t>
+  </si>
+  <si>
+    <t>Sum of Beauty of All Substrings</t>
+  </si>
+  <si>
+    <t>Check if Number is a Sum of Powers of Three</t>
+  </si>
+  <si>
+    <t>Find Nearest Point That Has the Same X or Y Coordinate </t>
+  </si>
+  <si>
+    <t>Equal Sum Arrays With Minimum Number of Operations</t>
+  </si>
+  <si>
+    <t>Closest Dessert Cost</t>
+  </si>
+  <si>
+    <t>Count Items Matching a Rule</t>
+  </si>
+  <si>
+    <t>Minimum Changes To Make Alternating Binary String </t>
+  </si>
+  <si>
+    <t>Count Number of Homogenous Substrings</t>
+  </si>
+  <si>
+    <t>Minimum Limit of Balls in a Bag</t>
+  </si>
+  <si>
+    <t>Longest Nice Substring </t>
+  </si>
+  <si>
+    <t>Form Array by Concatenating Subarrays of Another Array</t>
+  </si>
+  <si>
+    <t>Map of Highest Peak </t>
+  </si>
+  <si>
+    <t>Merge Strings Alternately  </t>
+  </si>
+  <si>
+    <t>Minimum Number of Operations to Move All Balls to Each Box</t>
+  </si>
+  <si>
+    <t>Maximum Score from Performing Multiplication Operations</t>
+  </si>
+  <si>
+    <t>Make even=0 odd=1 or make even = 1 odd = 0, choose the minimum operations</t>
+  </si>
+  <si>
+    <t>Accumulated sum with homogenous substring.</t>
+  </si>
+  <si>
+    <t>Guess the maximum number</t>
+  </si>
+  <si>
+    <t>Count characters</t>
+  </si>
+  <si>
+    <t>Count in group, reset index</t>
+  </si>
+  <si>
+    <t>BFS, from water to hill</t>
+  </si>
+  <si>
+    <t>Rotate and insert</t>
+  </si>
+  <si>
+    <t>Acculate from left to right and from right to left.</t>
+  </si>
+  <si>
+    <t>DFS with memorization or DP</t>
+  </si>
+  <si>
+    <t>Map the key</t>
+  </si>
+  <si>
+    <t>Bag up all the possible values.</t>
+  </si>
+  <si>
+    <t>2 ^N</t>
+  </si>
+  <si>
+    <t>Move low to 6 or high to 1</t>
+  </si>
+  <si>
+    <t>Get minimum distance.</t>
+  </si>
+  <si>
+    <t>Mod 3 the check if 1</t>
+  </si>
+  <si>
+    <t>Get substring and remember frequency</t>
+  </si>
+  <si>
+    <t>N ^ N</t>
+  </si>
+  <si>
+    <t>Check if we see zero</t>
+  </si>
+  <si>
+    <t>Shortest path from last node, two passes, first get distance, second count paths.</t>
+  </si>
+  <si>
+    <t>Calculate gap and divided by limit, watch overflow</t>
   </si>
 </sst>
 </file>
@@ -9477,7 +9591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -9504,6 +9618,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -9942,10 +10057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1648"/>
+  <dimension ref="A1:J1659"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1562" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1587" sqref="A1587"/>
+    <sheetView tabSelected="1" topLeftCell="G1581" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1605" sqref="H1605"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -47496,91 +47611,535 @@
         <v>3095</v>
       </c>
     </row>
-    <row r="1588" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1588" s="1"/>
-    </row>
-    <row r="1589" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1589" s="1"/>
-    </row>
-    <row r="1590" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1590" s="1"/>
-    </row>
-    <row r="1591" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1591" s="1"/>
-    </row>
-    <row r="1592" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1592" s="1"/>
-    </row>
-    <row r="1593" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1593" s="1"/>
-    </row>
-    <row r="1594" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1594" s="1"/>
-    </row>
-    <row r="1595" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1595" s="1"/>
-    </row>
-    <row r="1596" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1596" s="1"/>
-    </row>
-    <row r="1597" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1597" s="1"/>
-    </row>
-    <row r="1598" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1598" s="1"/>
+    <row r="1588" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1588" s="74">
+        <v>1758</v>
+      </c>
+      <c r="B1588" s="1" t="s">
+        <v>3141</v>
+      </c>
+      <c r="C1588" s="74">
+        <v>2</v>
+      </c>
+      <c r="D1588" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1588" s="74" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1588" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1588" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1588" s="74" t="s">
+        <v>3150</v>
+      </c>
+      <c r="I1588" s="74" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1589" s="74">
+        <v>1759</v>
+      </c>
+      <c r="B1589" s="1" t="s">
+        <v>3142</v>
+      </c>
+      <c r="C1589" s="74">
+        <v>3</v>
+      </c>
+      <c r="D1589" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1589" s="74" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1589" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1589" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1589" s="74" t="s">
+        <v>3151</v>
+      </c>
+      <c r="I1589" s="74" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1590" s="74">
+        <v>1760</v>
+      </c>
+      <c r="B1590" s="1" t="s">
+        <v>3143</v>
+      </c>
+      <c r="C1590" s="74">
+        <v>4</v>
+      </c>
+      <c r="D1590" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1590" s="74" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1590" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1590" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1590" s="74" t="s">
+        <v>3152</v>
+      </c>
+      <c r="I1590" s="74" t="s">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1591" s="74">
+        <v>1763</v>
+      </c>
+      <c r="B1591" s="1" t="s">
+        <v>3144</v>
+      </c>
+      <c r="C1591" s="74">
+        <v>2</v>
+      </c>
+      <c r="D1591" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1591" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1591" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1591" s="74" t="s">
+        <v>3153</v>
+      </c>
+      <c r="I1591" s="74" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1592" s="74">
+        <v>1764</v>
+      </c>
+      <c r="B1592" s="1" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C1592" s="74">
+        <v>3</v>
+      </c>
+      <c r="D1592" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1592" s="74" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1592" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1592" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1592" s="74" t="s">
+        <v>3154</v>
+      </c>
+      <c r="I1592" s="74" t="s">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1593" s="74">
+        <v>1765</v>
+      </c>
+      <c r="B1593" s="1" t="s">
+        <v>3146</v>
+      </c>
+      <c r="C1593" s="74">
+        <v>3</v>
+      </c>
+      <c r="D1593" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1593" s="74" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1593" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1593" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1593" s="74" t="s">
+        <v>3155</v>
+      </c>
+      <c r="I1593" s="74" t="s">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1594" s="74">
+        <v>1768</v>
+      </c>
+      <c r="B1594" s="1" t="s">
+        <v>3147</v>
+      </c>
+      <c r="C1594" s="74">
+        <v>1</v>
+      </c>
+      <c r="D1594" s="74" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1594" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1594" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1594" s="74" t="s">
+        <v>3156</v>
+      </c>
+      <c r="I1594" s="74" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1595" s="74">
+        <v>1769</v>
+      </c>
+      <c r="B1595" s="1" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C1595" s="74">
+        <v>3</v>
+      </c>
+      <c r="D1595" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1595" s="74" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1595" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1595" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1595" s="74" t="s">
+        <v>3157</v>
+      </c>
+      <c r="I1595" s="74" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1596" s="74">
+        <v>1770</v>
+      </c>
+      <c r="B1596" s="1" t="s">
+        <v>3149</v>
+      </c>
+      <c r="C1596" s="74">
+        <v>4</v>
+      </c>
+      <c r="D1596" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1596" s="74" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1596" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1596" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1596" s="74" t="s">
+        <v>3158</v>
+      </c>
+      <c r="I1596" s="74" t="s">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1597" s="74">
+        <v>1773</v>
+      </c>
+      <c r="B1597" s="1" t="s">
+        <v>3140</v>
+      </c>
+      <c r="C1597" s="74">
+        <v>1</v>
+      </c>
+      <c r="D1597" s="74" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1597" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1597" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1597" s="74" t="s">
+        <v>3159</v>
+      </c>
+      <c r="I1597" s="74" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1598" s="74">
+        <v>1774</v>
+      </c>
+      <c r="B1598" s="1" t="s">
+        <v>3139</v>
+      </c>
+      <c r="C1598" s="74">
+        <v>3</v>
+      </c>
+      <c r="D1598" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1598" s="74" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1598" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1598" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1598" s="74" t="s">
+        <v>3160</v>
+      </c>
+      <c r="I1598" s="74" t="s">
+        <v>3161</v>
+      </c>
     </row>
     <row r="1599" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1599" s="1"/>
+      <c r="A1599" s="71">
+        <v>1775</v>
+      </c>
+      <c r="B1599" s="1" t="s">
+        <v>3138</v>
+      </c>
+      <c r="C1599" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1599" s="71" t="s">
+        <v>2810</v>
+      </c>
+      <c r="F1599" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1599" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1599" s="71" t="s">
+        <v>3162</v>
+      </c>
+      <c r="I1599" s="71" t="s">
+        <v>3000</v>
+      </c>
     </row>
     <row r="1600" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1600" s="1"/>
-    </row>
-    <row r="1601" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1601" s="1"/>
-    </row>
-    <row r="1602" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1602" s="1"/>
-    </row>
-    <row r="1603" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1603" s="1"/>
-    </row>
-    <row r="1604" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1604" s="1"/>
-    </row>
-    <row r="1605" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1605" s="1"/>
-    </row>
-    <row r="1606" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1600" s="71">
+        <v>1779</v>
+      </c>
+      <c r="B1600" s="1" t="s">
+        <v>3137</v>
+      </c>
+      <c r="C1600" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1600" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1600" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1600" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1600" s="71" t="s">
+        <v>3163</v>
+      </c>
+      <c r="I1600" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1601" s="71">
+        <v>1780</v>
+      </c>
+      <c r="B1601" s="1" t="s">
+        <v>3136</v>
+      </c>
+      <c r="C1601" s="71">
+        <v>2</v>
+      </c>
+      <c r="D1601" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1601" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1601" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1601" s="71" t="s">
+        <v>3164</v>
+      </c>
+      <c r="I1601" s="71" t="s">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1602" s="71">
+        <v>1781</v>
+      </c>
+      <c r="B1602" s="1" t="s">
+        <v>3135</v>
+      </c>
+      <c r="C1602" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1602" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1602" s="71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1602" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1602" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1602" s="71" t="s">
+        <v>3165</v>
+      </c>
+      <c r="I1602" s="71" t="s">
+        <v>3166</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1603" s="71">
+        <v>1784</v>
+      </c>
+      <c r="B1603" s="1" t="s">
+        <v>3134</v>
+      </c>
+      <c r="C1603" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1603" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1603" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1603" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1603" s="71" t="s">
+        <v>3167</v>
+      </c>
+      <c r="I1603" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1604" s="71">
+        <v>1785</v>
+      </c>
+      <c r="B1604" s="1" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C1604" s="71">
+        <v>2</v>
+      </c>
+      <c r="D1604" s="71" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1604" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1604" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1604" s="71" t="s">
+        <v>3169</v>
+      </c>
+      <c r="I1604" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1605" s="71">
+        <v>1786</v>
+      </c>
+      <c r="B1605" s="1" t="s">
+        <v>3132</v>
+      </c>
+      <c r="C1605" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1605" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1605" s="71" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1605" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1605" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1605" s="71" t="s">
+        <v>3168</v>
+      </c>
+      <c r="I1605" s="71" t="s">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1606" s="1"/>
     </row>
-    <row r="1607" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1607" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1607" s="1"/>
     </row>
-    <row r="1608" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1608" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1608" s="1"/>
     </row>
-    <row r="1609" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1609" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1609" s="1"/>
     </row>
-    <row r="1610" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1610" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1610" s="1"/>
     </row>
-    <row r="1611" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1611" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1611" s="1"/>
     </row>
-    <row r="1612" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1612" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1612" s="1"/>
     </row>
-    <row r="1613" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1613" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1613" s="1"/>
     </row>
-    <row r="1614" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1614" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1614" s="1"/>
     </row>
-    <row r="1615" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1615" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1615" s="1"/>
     </row>
-    <row r="1616" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1616" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1616" s="1"/>
     </row>
     <row r="1617" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
@@ -47631,77 +48190,110 @@
     <row r="1632" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1632" s="1"/>
     </row>
-    <row r="1633" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1633" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1633" s="1"/>
     </row>
-    <row r="1634" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1634" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1634" s="1"/>
     </row>
-    <row r="1635" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1635" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1635" s="1"/>
     </row>
-    <row r="1636" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1636" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1636" s="1"/>
     </row>
-    <row r="1637" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1637" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1637" s="1"/>
     </row>
-    <row r="1638" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1638" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1638" s="1"/>
     </row>
-    <row r="1639" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1639" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1639" s="1"/>
     </row>
-    <row r="1640" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1640" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1640" s="1"/>
     </row>
-    <row r="1641" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1641" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1641" s="1"/>
     </row>
-    <row r="1642" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1642" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1642" s="1"/>
     </row>
-    <row r="1643" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1643" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1643" s="1"/>
     </row>
-    <row r="1644" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1644" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1644" s="1"/>
     </row>
-    <row r="1645" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1645" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1645" s="1"/>
     </row>
-    <row r="1646" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1646" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1646" s="1"/>
     </row>
-    <row r="1647" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1647" s="74" t="s">
+    <row r="1647" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1647" s="1"/>
+    </row>
+    <row r="1648" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1648" s="1"/>
+    </row>
+    <row r="1649" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1649" s="1"/>
+    </row>
+    <row r="1650" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1650" s="1"/>
+    </row>
+    <row r="1651" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1651" s="1"/>
+    </row>
+    <row r="1652" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1652" s="1"/>
+    </row>
+    <row r="1653" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1653" s="1"/>
+    </row>
+    <row r="1654" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1654" s="1"/>
+    </row>
+    <row r="1655" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1655" s="1"/>
+    </row>
+    <row r="1656" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1656" s="1"/>
+    </row>
+    <row r="1657" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1657" s="1"/>
+    </row>
+    <row r="1658" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1658" s="75" t="s">
         <v>1721</v>
       </c>
-      <c r="B1647" s="74"/>
-      <c r="C1647" s="74"/>
-      <c r="D1647" s="74"/>
-      <c r="E1647" s="74"/>
-      <c r="F1647" s="74"/>
-      <c r="G1647" s="74"/>
-      <c r="H1647" s="74"/>
-    </row>
-    <row r="1648" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1648" s="75" t="s">
+      <c r="B1658" s="75"/>
+      <c r="C1658" s="75"/>
+      <c r="D1658" s="75"/>
+      <c r="E1658" s="75"/>
+      <c r="F1658" s="75"/>
+      <c r="G1658" s="75"/>
+      <c r="H1658" s="75"/>
+    </row>
+    <row r="1659" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1659" s="76" t="s">
         <v>2760</v>
       </c>
-      <c r="B1648" s="75"/>
-      <c r="C1648" s="75"/>
-      <c r="D1648" s="75"/>
-      <c r="E1648" s="75"/>
-      <c r="F1648" s="75"/>
-      <c r="G1648" s="75"/>
-      <c r="H1648" s="75"/>
+      <c r="B1659" s="76"/>
+      <c r="C1659" s="76"/>
+      <c r="D1659" s="76"/>
+      <c r="E1659" s="76"/>
+      <c r="F1659" s="76"/>
+      <c r="G1659" s="76"/>
+      <c r="H1659" s="76"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1648" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1659" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1647:H1647"/>
-    <mergeCell ref="A1648:H1648"/>
+    <mergeCell ref="A1658:H1658"/>
+    <mergeCell ref="A1659:H1659"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -49079,10 +49671,28 @@
     <hyperlink ref="B1580" r:id="rId1373" display="https://leetcode.com/problems/can-you-eat-your-favorite-candy-on-your-favorite-day" xr:uid="{BEE070B5-F64C-4698-BCE5-1E36A8583440}"/>
     <hyperlink ref="B1584" r:id="rId1374" display="https://leetcode.com/problems/maximum-score-from-removing-stones" xr:uid="{B7AA18C7-E58A-447A-915A-42D4F13D6310}"/>
     <hyperlink ref="B1586" r:id="rId1375" display="https://leetcode.com/problems/closest-subsequence-sum" xr:uid="{F32459B0-DF4C-462A-9356-83F25EC7DAA2}"/>
+    <hyperlink ref="B1605" r:id="rId1376" display="https://leetcode.com/problems/number-of-restricted-paths-from-first-to-last-node" xr:uid="{7E8F4145-52CC-410A-8E6D-496A93BC9F35}"/>
+    <hyperlink ref="B1604" r:id="rId1377" display="https://leetcode.com/problems/minimum-elements-to-add-to-form-a-given-sum" xr:uid="{4588D88F-C977-4AC1-9131-6787B276C83B}"/>
+    <hyperlink ref="B1603" r:id="rId1378" display="https://leetcode.com/problems/check-if-binary-string-has-at-most-one-segment-of-ones" xr:uid="{CE9F4064-AD9A-45F5-8FA5-3D837B5BD888}"/>
+    <hyperlink ref="B1602" r:id="rId1379" display="https://leetcode.com/problems/sum-of-beauty-of-all-substrings" xr:uid="{F5D12DA0-6DB0-4E8E-A268-602716EC1E07}"/>
+    <hyperlink ref="B1601" r:id="rId1380" display="https://leetcode.com/problems/check-if-number-is-a-sum-of-powers-of-three" xr:uid="{4602803B-7988-4D38-ABF2-61BC86BCDAC5}"/>
+    <hyperlink ref="B1600" r:id="rId1381" display="https://leetcode.com/problems/find-nearest-point-that-has-the-same-x-or-y-coordinate" xr:uid="{5F651CEF-E9E7-4A94-8963-9659B92CF321}"/>
+    <hyperlink ref="B1599" r:id="rId1382" display="https://leetcode.com/problems/equal-sum-arrays-with-minimum-number-of-operations" xr:uid="{C7244173-A5DF-4CFD-8B2A-1EE21E557BC1}"/>
+    <hyperlink ref="B1598" r:id="rId1383" display="https://leetcode.com/problems/closest-dessert-cost" xr:uid="{F7BEECC4-44E4-47B9-8596-B7703815C60F}"/>
+    <hyperlink ref="B1597" r:id="rId1384" display="https://leetcode.com/problems/count-items-matching-a-rule" xr:uid="{C7425EBD-8CAE-4C06-8E35-71176FE3E292}"/>
+    <hyperlink ref="B1588" r:id="rId1385" display="https://leetcode.com/problems/minimum-changes-to-make-alternating-binary-string" xr:uid="{5E47CEE9-BA48-462F-B4F8-1AF99888DEB3}"/>
+    <hyperlink ref="B1589" r:id="rId1386" display="https://leetcode.com/problems/count-number-of-homogenous-substrings" xr:uid="{9343BDD1-5100-4986-BADF-74E77C30CD7C}"/>
+    <hyperlink ref="B1590" r:id="rId1387" display="https://leetcode.com/problems/minimum-limit-of-balls-in-a-bag" xr:uid="{F6C3BBF6-E091-49FF-8239-45C98E39DC8C}"/>
+    <hyperlink ref="B1591" r:id="rId1388" display="https://leetcode.com/problems/longest-nice-substring" xr:uid="{8E4DAA57-D075-4129-AAC9-2F7D747D4861}"/>
+    <hyperlink ref="B1592" r:id="rId1389" display="https://leetcode.com/problems/form-array-by-concatenating-subarrays-of-another-array" xr:uid="{BBB12904-D1D8-45C5-A73B-4D227A33C7A0}"/>
+    <hyperlink ref="B1593" r:id="rId1390" display="https://leetcode.com/problems/map-of-highest-peak" xr:uid="{D94EC984-B85A-480E-8580-8F6D0807308B}"/>
+    <hyperlink ref="B1594" r:id="rId1391" display="https://leetcode.com/problems/merge-strings-alternately" xr:uid="{10A36CE3-B9BF-4B0B-A7DF-E0BA62BBC363}"/>
+    <hyperlink ref="B1595" r:id="rId1392" display="https://leetcode.com/problems/minimum-number-of-operations-to-move-all-balls-to-each-box" xr:uid="{D44C79CA-AF26-42E8-BA0E-F083D426240B}"/>
+    <hyperlink ref="B1596" r:id="rId1393" display="https://leetcode.com/problems/maximum-score-from-performing-multiplication-operations" xr:uid="{CBFA2C81-65C2-4B16-BD7D-228C47EBD55C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1376"/>
-  <drawing r:id="rId1377"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1394"/>
+  <drawing r:id="rId1395"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in 3 weeks contest
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CCD789-E5BD-43A0-BB1B-9D96E4B1BD63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F381ED-9050-476F-B282-40B2833F91C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1659</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1662</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8548" uniqueCount="3170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8642" uniqueCount="3203">
   <si>
     <t>Difficulty</t>
   </si>
@@ -9547,6 +9547,105 @@
   </si>
   <si>
     <t>Calculate gap and divided by limit, watch overflow</t>
+  </si>
+  <si>
+    <t>Make the XOR of All Segments Equal to Zero</t>
+  </si>
+  <si>
+    <t>For every position from 0 to k-1, if we make it 0 - 1023, how many elements we need to change</t>
+  </si>
+  <si>
+    <t>Check if One String Swap Can Make Strings Equal</t>
+  </si>
+  <si>
+    <t>Find Center of Star Graph</t>
+  </si>
+  <si>
+    <t>Compare string and check difference</t>
+  </si>
+  <si>
+    <t>Check degree</t>
+  </si>
+  <si>
+    <t>Maximum Average Pass Ratio</t>
+  </si>
+  <si>
+    <t>Maximum Score of a Good Subarray</t>
+  </si>
+  <si>
+    <t>From position K to expand two directions with higher number first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N </t>
+  </si>
+  <si>
+    <t>Put all margin profit in the heap and process one on the top.</t>
+  </si>
+  <si>
+    <t>Count Pairs Of Nodes </t>
+  </si>
+  <si>
+    <t>Sorting by edges, two pointers scan deduct by common path.</t>
+  </si>
+  <si>
+    <t>Palindrome Partitioning IV</t>
+  </si>
+  <si>
+    <t>Double loop from front to end.</t>
+  </si>
+  <si>
+    <t>N * N</t>
+  </si>
+  <si>
+    <t>Minimum Degree of a Connected Trio in a Graph</t>
+  </si>
+  <si>
+    <t>Sort by neibours then by degree.</t>
+  </si>
+  <si>
+    <t>Second Largest Digit in a String</t>
+  </si>
+  <si>
+    <t>Design Authentication Manager</t>
+  </si>
+  <si>
+    <t>Maximum Number of Consecutive Values You Can Make</t>
+  </si>
+  <si>
+    <t>Maximize Score After N Operations </t>
+  </si>
+  <si>
+    <t>Maximum Ascending Subarray Sum </t>
+  </si>
+  <si>
+    <t>Number of Orders in the Backlog</t>
+  </si>
+  <si>
+    <t>Maximum Value at a Given Index in a Bounded Array </t>
+  </si>
+  <si>
+    <t>Count 0-9</t>
+  </si>
+  <si>
+    <t>Put expired time in TreeMap</t>
+  </si>
+  <si>
+    <t>Accumulate from smallest number which not exceed sum + 1</t>
+  </si>
+  <si>
+    <t>DFS with bitmap memorization</t>
+  </si>
+  <si>
+    <t>2 ^ N * N^2</t>
+  </si>
+  <si>
+    <t>Scan array, remember last number</t>
+  </si>
+  <si>
+    <t>Keep buy and sell orders in priority queue</t>
+  </si>
+  <si>
+    <t>Guess number for peak, calculate sum in array</t>
   </si>
 </sst>
 </file>
@@ -9591,7 +9690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -9618,6 +9717,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -10057,10 +10157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1659"/>
+  <dimension ref="A1:J1662"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1581" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1605" sqref="H1605"/>
+    <sheetView tabSelected="1" topLeftCell="E1606" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1620" sqref="I1620"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -47420,56 +47520,59 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="1581" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1581" s="71">
-        <v>1746</v>
+    <row r="1581" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1581" s="75">
+        <v>1745</v>
       </c>
       <c r="B1581" s="1" t="s">
-        <v>3096</v>
-      </c>
-      <c r="C1581" s="71">
-        <v>3</v>
-      </c>
-      <c r="D1581" s="71" t="s">
+        <v>3183</v>
+      </c>
+      <c r="C1581" s="75">
+        <v>4</v>
+      </c>
+      <c r="D1581" s="75" t="s">
         <v>1720</v>
       </c>
-      <c r="E1581" s="71" t="s">
-        <v>2935</v>
-      </c>
-      <c r="F1581" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1581" s="71" t="s">
+      <c r="E1581" s="75" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1581" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1581" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="H1581" s="71" t="s">
-        <v>3097</v>
-      </c>
-      <c r="I1581" s="71" t="s">
-        <v>3000</v>
+      <c r="H1581" s="75" t="s">
+        <v>3184</v>
+      </c>
+      <c r="I1581" s="75" t="s">
+        <v>3185</v>
       </c>
     </row>
     <row r="1582" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1582" s="71">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="B1582" s="1" t="s">
-        <v>3089</v>
+        <v>3096</v>
       </c>
       <c r="C1582" s="71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1582" s="71" t="s">
-        <v>1717</v>
+        <v>1720</v>
+      </c>
+      <c r="E1582" s="71" t="s">
+        <v>2935</v>
       </c>
       <c r="F1582" s="71" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1582" s="71" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="H1582" s="71" t="s">
-        <v>3090</v>
+        <v>3097</v>
       </c>
       <c r="I1582" s="71" t="s">
         <v>3000</v>
@@ -47477,94 +47580,91 @@
     </row>
     <row r="1583" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1583" s="71">
-        <v>1752</v>
+        <v>1748</v>
       </c>
       <c r="B1583" s="1" t="s">
-        <v>3091</v>
+        <v>3089</v>
       </c>
       <c r="C1583" s="71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1583" s="71" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1583" s="71" t="s">
-        <v>2935</v>
+        <v>1717</v>
       </c>
       <c r="F1583" s="71" t="s">
         <v>5</v>
       </c>
       <c r="G1583" s="71" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="H1583" s="71" t="s">
-        <v>3092</v>
+        <v>3090</v>
       </c>
       <c r="I1583" s="71" t="s">
         <v>3000</v>
       </c>
     </row>
-    <row r="1584" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1584" s="73">
-        <v>1753</v>
+    <row r="1584" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1584" s="71">
+        <v>1752</v>
       </c>
       <c r="B1584" s="1" t="s">
-        <v>3125</v>
-      </c>
-      <c r="C1584" s="73">
-        <v>3</v>
-      </c>
-      <c r="D1584" s="73" t="s">
+        <v>3091</v>
+      </c>
+      <c r="C1584" s="71">
+        <v>2</v>
+      </c>
+      <c r="D1584" s="71" t="s">
         <v>1720</v>
       </c>
-      <c r="F1584" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1584" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1584" s="73" t="s">
-        <v>3126</v>
-      </c>
-      <c r="I1584" s="73" t="s">
-        <v>3057</v>
+      <c r="E1584" s="71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1584" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1584" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1584" s="71" t="s">
+        <v>3092</v>
+      </c>
+      <c r="I1584" s="71" t="s">
+        <v>3000</v>
       </c>
     </row>
     <row r="1585" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1585" s="73">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="B1585" s="1" t="s">
-        <v>3127</v>
+        <v>3125</v>
       </c>
       <c r="C1585" s="73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1585" s="73" t="s">
-        <v>2810</v>
-      </c>
-      <c r="E1585" s="73" t="s">
-        <v>2935</v>
+        <v>1720</v>
       </c>
       <c r="F1585" s="73" t="s">
         <v>9</v>
       </c>
       <c r="G1585" s="73" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H1585" s="73" t="s">
-        <v>3128</v>
+        <v>3126</v>
       </c>
       <c r="I1585" s="73" t="s">
-        <v>3000</v>
+        <v>3057</v>
       </c>
     </row>
     <row r="1586" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1586" s="73">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="B1586" s="1" t="s">
-        <v>3129</v>
+        <v>3127</v>
       </c>
       <c r="C1586" s="73">
         <v>4</v>
@@ -47572,98 +47672,98 @@
       <c r="D1586" s="73" t="s">
         <v>2810</v>
       </c>
+      <c r="E1586" s="73" t="s">
+        <v>2935</v>
+      </c>
       <c r="F1586" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1586" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1586" s="73" t="s">
+        <v>3128</v>
+      </c>
+      <c r="I1586" s="73" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1587" s="73">
+        <v>1755</v>
+      </c>
+      <c r="B1587" s="1" t="s">
+        <v>3129</v>
+      </c>
+      <c r="C1587" s="73">
+        <v>4</v>
+      </c>
+      <c r="D1587" s="73" t="s">
+        <v>2810</v>
+      </c>
+      <c r="F1587" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="G1586" s="73" t="s">
+      <c r="G1587" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="H1586" s="73" t="s">
+      <c r="H1587" s="73" t="s">
         <v>3130</v>
       </c>
-      <c r="I1586" s="73" t="s">
+      <c r="I1587" s="73" t="s">
         <v>3131</v>
       </c>
     </row>
-    <row r="1587" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1587" s="71">
+    <row r="1588" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1588" s="71">
         <v>1756</v>
       </c>
-      <c r="B1587" s="1" t="s">
+      <c r="B1588" s="1" t="s">
         <v>3093</v>
       </c>
-      <c r="C1587" s="71">
-        <v>3</v>
-      </c>
-      <c r="D1587" s="71" t="s">
+      <c r="C1588" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1588" s="71" t="s">
         <v>1720</v>
       </c>
-      <c r="F1587" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1587" s="71" t="s">
+      <c r="F1588" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1588" s="71" t="s">
         <v>457</v>
       </c>
-      <c r="H1587" s="71" t="s">
+      <c r="H1588" s="71" t="s">
         <v>3094</v>
       </c>
-      <c r="I1587" s="71" t="s">
+      <c r="I1588" s="71" t="s">
         <v>3095</v>
-      </c>
-    </row>
-    <row r="1588" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1588" s="74">
-        <v>1758</v>
-      </c>
-      <c r="B1588" s="1" t="s">
-        <v>3141</v>
-      </c>
-      <c r="C1588" s="74">
-        <v>2</v>
-      </c>
-      <c r="D1588" s="74" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1588" s="74" t="s">
-        <v>2935</v>
-      </c>
-      <c r="F1588" s="74" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1588" s="74" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1588" s="74" t="s">
-        <v>3150</v>
-      </c>
-      <c r="I1588" s="74" t="s">
-        <v>3000</v>
       </c>
     </row>
     <row r="1589" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1589" s="74">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="B1589" s="1" t="s">
-        <v>3142</v>
+        <v>3141</v>
       </c>
       <c r="C1589" s="74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1589" s="74" t="s">
         <v>1720</v>
       </c>
       <c r="E1589" s="74" t="s">
-        <v>2923</v>
+        <v>2935</v>
       </c>
       <c r="F1589" s="74" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1589" s="74" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H1589" s="74" t="s">
-        <v>3151</v>
+        <v>3150</v>
       </c>
       <c r="I1589" s="74" t="s">
         <v>3000</v>
@@ -47671,13 +47771,13 @@
     </row>
     <row r="1590" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1590" s="74">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="B1590" s="1" t="s">
-        <v>3143</v>
+        <v>3142</v>
       </c>
       <c r="C1590" s="74">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1590" s="74" t="s">
         <v>1720</v>
@@ -47689,131 +47789,128 @@
         <v>9</v>
       </c>
       <c r="G1590" s="74" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H1590" s="74" t="s">
-        <v>3152</v>
+        <v>3151</v>
       </c>
       <c r="I1590" s="74" t="s">
-        <v>3029</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1591" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1591" s="74">
-        <v>1763</v>
+        <v>1760</v>
       </c>
       <c r="B1591" s="1" t="s">
-        <v>3144</v>
+        <v>3143</v>
       </c>
       <c r="C1591" s="74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1591" s="74" t="s">
         <v>1720</v>
       </c>
+      <c r="E1591" s="74" t="s">
+        <v>2923</v>
+      </c>
       <c r="F1591" s="74" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1591" s="74" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="H1591" s="74" t="s">
-        <v>3153</v>
+        <v>3152</v>
       </c>
       <c r="I1591" s="74" t="s">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="1592" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1592" s="74">
-        <v>1764</v>
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1592" s="75">
+        <v>1761</v>
       </c>
       <c r="B1592" s="1" t="s">
-        <v>3145</v>
-      </c>
-      <c r="C1592" s="74">
-        <v>3</v>
-      </c>
-      <c r="D1592" s="74" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1592" s="74" t="s">
-        <v>2924</v>
-      </c>
-      <c r="F1592" s="74" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1592" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1592" s="74" t="s">
-        <v>3154</v>
-      </c>
-      <c r="I1592" s="74" t="s">
-        <v>3026</v>
+        <v>3186</v>
+      </c>
+      <c r="C1592" s="75">
+        <v>4</v>
+      </c>
+      <c r="D1592" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1592" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1592" s="75" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1592" s="75" t="s">
+        <v>3187</v>
       </c>
     </row>
     <row r="1593" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1593" s="74">
-        <v>1765</v>
+        <v>1763</v>
       </c>
       <c r="B1593" s="1" t="s">
-        <v>3146</v>
+        <v>3144</v>
       </c>
       <c r="C1593" s="74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1593" s="74" t="s">
         <v>1720</v>
       </c>
-      <c r="E1593" s="74" t="s">
-        <v>2935</v>
-      </c>
       <c r="F1593" s="74" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1593" s="74" t="s">
-        <v>187</v>
+        <v>36</v>
       </c>
       <c r="H1593" s="74" t="s">
-        <v>3155</v>
+        <v>3153</v>
       </c>
       <c r="I1593" s="74" t="s">
-        <v>3045</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1594" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1594" s="74">
-        <v>1768</v>
+        <v>1764</v>
       </c>
       <c r="B1594" s="1" t="s">
-        <v>3147</v>
+        <v>3145</v>
       </c>
       <c r="C1594" s="74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1594" s="74" t="s">
-        <v>1717</v>
+        <v>1720</v>
+      </c>
+      <c r="E1594" s="74" t="s">
+        <v>2924</v>
       </c>
       <c r="F1594" s="74" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1594" s="74" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="H1594" s="74" t="s">
-        <v>3156</v>
+        <v>3154</v>
       </c>
       <c r="I1594" s="74" t="s">
-        <v>3000</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="1595" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1595" s="74">
-        <v>1769</v>
+        <v>1765</v>
       </c>
       <c r="B1595" s="1" t="s">
-        <v>3148</v>
+        <v>3146</v>
       </c>
       <c r="C1595" s="74">
         <v>3</v>
@@ -47822,71 +47919,71 @@
         <v>1720</v>
       </c>
       <c r="E1595" s="74" t="s">
-        <v>2924</v>
+        <v>2935</v>
       </c>
       <c r="F1595" s="74" t="s">
         <v>9</v>
       </c>
       <c r="G1595" s="74" t="s">
-        <v>21</v>
+        <v>187</v>
       </c>
       <c r="H1595" s="74" t="s">
-        <v>3157</v>
+        <v>3155</v>
       </c>
       <c r="I1595" s="74" t="s">
-        <v>3000</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="1596" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1596" s="74">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="B1596" s="1" t="s">
-        <v>3149</v>
+        <v>3147</v>
       </c>
       <c r="C1596" s="74">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1596" s="74" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1596" s="74" t="s">
-        <v>2935</v>
+        <v>1717</v>
       </c>
       <c r="F1596" s="74" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1596" s="74" t="s">
-        <v>121</v>
+        <v>36</v>
       </c>
       <c r="H1596" s="74" t="s">
-        <v>3158</v>
+        <v>3156</v>
       </c>
       <c r="I1596" s="74" t="s">
-        <v>3026</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1597" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1597" s="74">
-        <v>1773</v>
+        <v>1769</v>
       </c>
       <c r="B1597" s="1" t="s">
-        <v>3140</v>
+        <v>3148</v>
       </c>
       <c r="C1597" s="74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1597" s="74" t="s">
-        <v>1717</v>
+        <v>1720</v>
+      </c>
+      <c r="E1597" s="74" t="s">
+        <v>2924</v>
       </c>
       <c r="F1597" s="74" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1597" s="74" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="H1597" s="74" t="s">
-        <v>3159</v>
+        <v>3157</v>
       </c>
       <c r="I1597" s="74" t="s">
         <v>3000</v>
@@ -47894,13 +47991,13 @@
     </row>
     <row r="1598" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1598" s="74">
-        <v>1774</v>
+        <v>1770</v>
       </c>
       <c r="B1598" s="1" t="s">
-        <v>3139</v>
+        <v>3149</v>
       </c>
       <c r="C1598" s="74">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1598" s="74" t="s">
         <v>1720</v>
@@ -47912,282 +48009,642 @@
         <v>9</v>
       </c>
       <c r="G1598" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1598" s="74" t="s">
+        <v>3158</v>
+      </c>
+      <c r="I1598" s="74" t="s">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1599" s="74">
+        <v>1773</v>
+      </c>
+      <c r="B1599" s="1" t="s">
+        <v>3140</v>
+      </c>
+      <c r="C1599" s="74">
+        <v>1</v>
+      </c>
+      <c r="D1599" s="74" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1599" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1599" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1599" s="74" t="s">
+        <v>3159</v>
+      </c>
+      <c r="I1599" s="74" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:9" s="74" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1600" s="74">
+        <v>1774</v>
+      </c>
+      <c r="B1600" s="1" t="s">
+        <v>3139</v>
+      </c>
+      <c r="C1600" s="74">
+        <v>3</v>
+      </c>
+      <c r="D1600" s="74" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1600" s="74" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1600" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1600" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="H1598" s="74" t="s">
+      <c r="H1600" s="74" t="s">
         <v>3160</v>
       </c>
-      <c r="I1598" s="74" t="s">
+      <c r="I1600" s="74" t="s">
         <v>3161</v>
-      </c>
-    </row>
-    <row r="1599" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1599" s="71">
-        <v>1775</v>
-      </c>
-      <c r="B1599" s="1" t="s">
-        <v>3138</v>
-      </c>
-      <c r="C1599" s="71">
-        <v>3</v>
-      </c>
-      <c r="D1599" s="71" t="s">
-        <v>2810</v>
-      </c>
-      <c r="F1599" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1599" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1599" s="71" t="s">
-        <v>3162</v>
-      </c>
-      <c r="I1599" s="71" t="s">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="1600" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1600" s="71">
-        <v>1779</v>
-      </c>
-      <c r="B1600" s="1" t="s">
-        <v>3137</v>
-      </c>
-      <c r="C1600" s="71">
-        <v>1</v>
-      </c>
-      <c r="D1600" s="71" t="s">
-        <v>1717</v>
-      </c>
-      <c r="F1600" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1600" s="71" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1600" s="71" t="s">
-        <v>3163</v>
-      </c>
-      <c r="I1600" s="71" t="s">
-        <v>3000</v>
       </c>
     </row>
     <row r="1601" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1601" s="71">
-        <v>1780</v>
+        <v>1775</v>
       </c>
       <c r="B1601" s="1" t="s">
-        <v>3136</v>
+        <v>3138</v>
       </c>
       <c r="C1601" s="71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1601" s="71" t="s">
-        <v>1720</v>
+        <v>2810</v>
       </c>
       <c r="F1601" s="71" t="s">
         <v>9</v>
       </c>
       <c r="G1601" s="71" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H1601" s="71" t="s">
-        <v>3164</v>
+        <v>3162</v>
       </c>
       <c r="I1601" s="71" t="s">
-        <v>3002</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1602" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1602" s="71">
-        <v>1781</v>
+        <v>1779</v>
       </c>
       <c r="B1602" s="1" t="s">
-        <v>3135</v>
+        <v>3137</v>
       </c>
       <c r="C1602" s="71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1602" s="71" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1602" s="71" t="s">
-        <v>2935</v>
+        <v>1717</v>
       </c>
       <c r="F1602" s="71" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1602" s="71" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="H1602" s="71" t="s">
-        <v>3165</v>
+        <v>3163</v>
       </c>
       <c r="I1602" s="71" t="s">
-        <v>3166</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="1603" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1603" s="71">
-        <v>1784</v>
+        <v>1780</v>
       </c>
       <c r="B1603" s="1" t="s">
-        <v>3134</v>
+        <v>3136</v>
       </c>
       <c r="C1603" s="71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1603" s="71" t="s">
-        <v>1717</v>
+        <v>1720</v>
       </c>
       <c r="F1603" s="71" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1603" s="71" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H1603" s="71" t="s">
-        <v>3167</v>
+        <v>3164</v>
       </c>
       <c r="I1603" s="71" t="s">
-        <v>3000</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="1604" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1604" s="71">
+        <v>1781</v>
+      </c>
+      <c r="B1604" s="1" t="s">
+        <v>3135</v>
+      </c>
+      <c r="C1604" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1604" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1604" s="71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1604" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1604" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1604" s="71" t="s">
+        <v>3165</v>
+      </c>
+      <c r="I1604" s="71" t="s">
+        <v>3166</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1605" s="75">
+        <v>1782</v>
+      </c>
+      <c r="B1605" s="1" t="s">
+        <v>3181</v>
+      </c>
+      <c r="C1605" s="75">
+        <v>4</v>
+      </c>
+      <c r="D1605" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1605" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1605" s="75" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1605" s="75" t="s">
+        <v>3182</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1606" s="71">
+        <v>1784</v>
+      </c>
+      <c r="B1606" s="1" t="s">
+        <v>3134</v>
+      </c>
+      <c r="C1606" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1606" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1606" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1606" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1606" s="71" t="s">
+        <v>3167</v>
+      </c>
+      <c r="I1606" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1607" s="71">
         <v>1785</v>
       </c>
-      <c r="B1604" s="1" t="s">
+      <c r="B1607" s="1" t="s">
         <v>3133</v>
       </c>
-      <c r="C1604" s="71">
+      <c r="C1607" s="71">
         <v>2</v>
       </c>
-      <c r="D1604" s="71" t="s">
+      <c r="D1607" s="71" t="s">
         <v>1718</v>
       </c>
-      <c r="F1604" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1604" s="71" t="s">
+      <c r="F1607" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1607" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="H1604" s="71" t="s">
+      <c r="H1607" s="71" t="s">
         <v>3169</v>
       </c>
-      <c r="I1604" s="71" t="s">
+      <c r="I1607" s="71" t="s">
         <v>3000</v>
       </c>
     </row>
-    <row r="1605" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1605" s="71">
+    <row r="1608" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1608" s="71">
         <v>1786</v>
       </c>
-      <c r="B1605" s="1" t="s">
+      <c r="B1608" s="1" t="s">
         <v>3132</v>
       </c>
-      <c r="C1605" s="71">
+      <c r="C1608" s="71">
         <v>4</v>
       </c>
-      <c r="D1605" s="71" t="s">
+      <c r="D1608" s="71" t="s">
         <v>1720</v>
       </c>
-      <c r="E1605" s="71" t="s">
+      <c r="E1608" s="71" t="s">
         <v>2923</v>
       </c>
-      <c r="F1605" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1605" s="71" t="s">
+      <c r="F1608" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1608" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="H1605" s="71" t="s">
+      <c r="H1608" s="71" t="s">
         <v>3168</v>
       </c>
-      <c r="I1605" s="71" t="s">
+      <c r="I1608" s="71" t="s">
         <v>3029</v>
       </c>
     </row>
-    <row r="1606" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1606" s="1"/>
-    </row>
-    <row r="1607" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1607" s="1"/>
-    </row>
-    <row r="1608" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1608" s="1"/>
-    </row>
     <row r="1609" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1609" s="1"/>
+      <c r="A1609" s="71">
+        <v>1787</v>
+      </c>
+      <c r="B1609" s="1" t="s">
+        <v>3170</v>
+      </c>
+      <c r="C1609" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1609" s="71" t="s">
+        <v>2810</v>
+      </c>
+      <c r="F1609" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1609" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1609" s="71" t="s">
+        <v>3171</v>
+      </c>
+      <c r="I1609" s="71" t="s">
+        <v>3023</v>
+      </c>
     </row>
     <row r="1610" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1610" s="1"/>
+      <c r="A1610" s="71">
+        <v>1790</v>
+      </c>
+      <c r="B1610" s="1" t="s">
+        <v>3172</v>
+      </c>
+      <c r="C1610" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1610" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1610" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1610" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1610" s="71" t="s">
+        <v>3174</v>
+      </c>
+      <c r="I1610" s="71" t="s">
+        <v>3000</v>
+      </c>
     </row>
     <row r="1611" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1611" s="1"/>
+      <c r="A1611" s="71">
+        <v>1791</v>
+      </c>
+      <c r="B1611" s="1" t="s">
+        <v>3173</v>
+      </c>
+      <c r="C1611" s="71">
+        <v>2</v>
+      </c>
+      <c r="D1611" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1611" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1611" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1611" s="71" t="s">
+        <v>3175</v>
+      </c>
+      <c r="I1611" s="71" t="s">
+        <v>3000</v>
+      </c>
     </row>
     <row r="1612" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1612" s="1"/>
+      <c r="A1612" s="71">
+        <v>1792</v>
+      </c>
+      <c r="B1612" s="1" t="s">
+        <v>3176</v>
+      </c>
+      <c r="C1612" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1612" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1612" s="71" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1612" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1612" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1612" s="71" t="s">
+        <v>3180</v>
+      </c>
+      <c r="I1612" s="71" t="s">
+        <v>3029</v>
+      </c>
     </row>
     <row r="1613" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1613" s="1"/>
+      <c r="A1613" s="71">
+        <v>1793</v>
+      </c>
+      <c r="B1613" s="1" t="s">
+        <v>3177</v>
+      </c>
+      <c r="C1613" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1613" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1613" s="71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1613" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1613" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1613" s="71" t="s">
+        <v>3178</v>
+      </c>
+      <c r="I1613" s="71" t="s">
+        <v>3179</v>
+      </c>
     </row>
     <row r="1614" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1614" s="1"/>
+      <c r="A1614" s="71">
+        <v>1796</v>
+      </c>
+      <c r="B1614" s="1" t="s">
+        <v>3188</v>
+      </c>
+      <c r="C1614" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1614" s="71" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1614" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1614" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1614" s="71" t="s">
+        <v>3195</v>
+      </c>
+      <c r="I1614" s="71" t="s">
+        <v>3000</v>
+      </c>
     </row>
     <row r="1615" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1615" s="1"/>
+      <c r="A1615" s="71">
+        <v>1797</v>
+      </c>
+      <c r="B1615" s="1" t="s">
+        <v>3189</v>
+      </c>
+      <c r="C1615" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1615" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1615" s="71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1615" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1615" s="71" t="s">
+        <v>457</v>
+      </c>
+      <c r="H1615" s="71" t="s">
+        <v>3196</v>
+      </c>
+      <c r="I1615" s="71" t="s">
+        <v>3029</v>
+      </c>
     </row>
     <row r="1616" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1616" s="1"/>
-    </row>
-    <row r="1617" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1617" s="1"/>
-    </row>
-    <row r="1618" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1618" s="1"/>
-    </row>
-    <row r="1619" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1619" s="1"/>
-    </row>
-    <row r="1620" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1620" s="1"/>
-    </row>
-    <row r="1621" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1616" s="71">
+        <v>1798</v>
+      </c>
+      <c r="B1616" s="1" t="s">
+        <v>3190</v>
+      </c>
+      <c r="C1616" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1616" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1616" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1616" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1616" s="71" t="s">
+        <v>3197</v>
+      </c>
+      <c r="I1616" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1617" s="71">
+        <v>1799</v>
+      </c>
+      <c r="B1617" s="1" t="s">
+        <v>3191</v>
+      </c>
+      <c r="C1617" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1617" s="71" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1617" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1617" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1617" s="71" t="s">
+        <v>3198</v>
+      </c>
+      <c r="I1617" s="71" t="s">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1618" s="71">
+        <v>1800</v>
+      </c>
+      <c r="B1618" s="1" t="s">
+        <v>3192</v>
+      </c>
+      <c r="C1618" s="71">
+        <v>1</v>
+      </c>
+      <c r="D1618" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1618" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1618" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1618" s="71" t="s">
+        <v>3200</v>
+      </c>
+      <c r="I1618" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1619" s="71">
+        <v>1801</v>
+      </c>
+      <c r="B1619" s="1" t="s">
+        <v>3193</v>
+      </c>
+      <c r="C1619" s="71">
+        <v>3</v>
+      </c>
+      <c r="D1619" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1619" s="71" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1619" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1619" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1619" s="71" t="s">
+        <v>3201</v>
+      </c>
+      <c r="I1619" s="71" t="s">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1620" s="71">
+        <v>1802</v>
+      </c>
+      <c r="B1620" s="1" t="s">
+        <v>3194</v>
+      </c>
+      <c r="C1620" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1620" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1620" s="71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1620" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1620" s="71" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1620" s="71" t="s">
+        <v>3202</v>
+      </c>
+      <c r="I1620" s="71" t="s">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1621" s="1"/>
     </row>
-    <row r="1622" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1622" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1622" s="1"/>
     </row>
-    <row r="1623" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1623" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1623" s="1"/>
     </row>
-    <row r="1624" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1624" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1624" s="1"/>
     </row>
-    <row r="1625" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1625" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1625" s="1"/>
     </row>
-    <row r="1626" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1626" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1626" s="1"/>
     </row>
-    <row r="1627" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1627" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1627" s="1"/>
     </row>
-    <row r="1628" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1628" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1628" s="1"/>
     </row>
-    <row r="1629" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1629" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1629" s="1"/>
     </row>
-    <row r="1630" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1630" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1630" s="1"/>
     </row>
-    <row r="1631" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1631" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1631" s="1"/>
     </row>
-    <row r="1632" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1632" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1632" s="1"/>
     </row>
     <row r="1633" spans="2:2" s="71" customFormat="1" x14ac:dyDescent="0.45">
@@ -48262,38 +48719,47 @@
     <row r="1656" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1656" s="1"/>
     </row>
-    <row r="1657" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1657" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1657" s="1"/>
     </row>
-    <row r="1658" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1658" s="75" t="s">
+    <row r="1658" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1658" s="1"/>
+    </row>
+    <row r="1659" spans="1:8" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1659" s="1"/>
+    </row>
+    <row r="1660" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1660" s="1"/>
+    </row>
+    <row r="1661" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1661" s="76" t="s">
         <v>1721</v>
       </c>
-      <c r="B1658" s="75"/>
-      <c r="C1658" s="75"/>
-      <c r="D1658" s="75"/>
-      <c r="E1658" s="75"/>
-      <c r="F1658" s="75"/>
-      <c r="G1658" s="75"/>
-      <c r="H1658" s="75"/>
-    </row>
-    <row r="1659" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1659" s="76" t="s">
+      <c r="B1661" s="76"/>
+      <c r="C1661" s="76"/>
+      <c r="D1661" s="76"/>
+      <c r="E1661" s="76"/>
+      <c r="F1661" s="76"/>
+      <c r="G1661" s="76"/>
+      <c r="H1661" s="76"/>
+    </row>
+    <row r="1662" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1662" s="77" t="s">
         <v>2760</v>
       </c>
-      <c r="B1659" s="76"/>
-      <c r="C1659" s="76"/>
-      <c r="D1659" s="76"/>
-      <c r="E1659" s="76"/>
-      <c r="F1659" s="76"/>
-      <c r="G1659" s="76"/>
-      <c r="H1659" s="76"/>
+      <c r="B1662" s="77"/>
+      <c r="C1662" s="77"/>
+      <c r="D1662" s="77"/>
+      <c r="E1662" s="77"/>
+      <c r="F1662" s="77"/>
+      <c r="G1662" s="77"/>
+      <c r="H1662" s="77"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1659" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1662" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1658:H1658"/>
-    <mergeCell ref="A1659:H1659"/>
+    <mergeCell ref="A1661:H1661"/>
+    <mergeCell ref="A1662:H1662"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -49654,10 +50120,10 @@
     <hyperlink ref="B1569" r:id="rId1356" display="https://leetcode.com/problems/find-the-highest-altitude" xr:uid="{B2085815-293D-42BF-A84D-6F7F0CC198BE}"/>
     <hyperlink ref="B1573" r:id="rId1357" display="https://leetcode.com/problems/latest-time-by-replacing-hidden-digits" xr:uid="{FFB49099-001C-44BA-B278-B00A3A11671D}"/>
     <hyperlink ref="B1578" r:id="rId1358" display="https://leetcode.com/problems/maximum-number-of-balls-in-a-box" xr:uid="{18366F0A-A3CF-4126-BA67-AE626616A691}"/>
-    <hyperlink ref="B1582" r:id="rId1359" display="https://leetcode.com/problems/sum-of-unique-elements" xr:uid="{B93FC0DC-83AD-4019-B434-79BA3ECF3C27}"/>
-    <hyperlink ref="B1583" r:id="rId1360" display="https://leetcode.com/problems/check-if-array-is-sorted-and-rotated" xr:uid="{EFE2F4D1-0950-49F4-B136-E72B4AF0D449}"/>
-    <hyperlink ref="B1587" r:id="rId1361" display="https://leetcode.com/problems/design-most-recently-used-queue" xr:uid="{74130DE4-2D04-4D3B-BEF6-58D20F61C5E0}"/>
-    <hyperlink ref="B1581" r:id="rId1362" display="https://leetcode.com/problems/maximum-subarray-sum-after-one-operation" xr:uid="{9ABF6461-8E02-44BB-9725-D17CBB89070F}"/>
+    <hyperlink ref="B1583" r:id="rId1359" display="https://leetcode.com/problems/sum-of-unique-elements" xr:uid="{B93FC0DC-83AD-4019-B434-79BA3ECF3C27}"/>
+    <hyperlink ref="B1584" r:id="rId1360" display="https://leetcode.com/problems/check-if-array-is-sorted-and-rotated" xr:uid="{EFE2F4D1-0950-49F4-B136-E72B4AF0D449}"/>
+    <hyperlink ref="B1588" r:id="rId1361" display="https://leetcode.com/problems/design-most-recently-used-queue" xr:uid="{74130DE4-2D04-4D3B-BEF6-58D20F61C5E0}"/>
+    <hyperlink ref="B1582" r:id="rId1362" display="https://leetcode.com/problems/maximum-subarray-sum-after-one-operation" xr:uid="{9ABF6461-8E02-44BB-9725-D17CBB89070F}"/>
     <hyperlink ref="B1577" r:id="rId1363" display="https://leetcode.com/problems/find-distance-in-a-binary-tree" xr:uid="{92429178-67ED-4AD2-859E-9E026EEAF7BD}"/>
     <hyperlink ref="B1563" r:id="rId1364" display="https://leetcode.com/problems/checking-existence-of-edge-length-limited-paths-ii" xr:uid="{A09CC7F8-57B2-4D18-8FCA-F1B91534ED7F}"/>
     <hyperlink ref="B1554" r:id="rId1365" display="https://leetcode.com/problems/sum-of-special-evenly-spaced-elements-in-array" xr:uid="{6CC25C62-1D5D-4F0D-96CA-DD0F34BB1CA9}"/>
@@ -49669,30 +50135,44 @@
     <hyperlink ref="B1576" r:id="rId1371" display="https://leetcode.com/problems/building-boxes" xr:uid="{BAA2B99F-FF9E-4F72-B24E-7E96F1A3F674}"/>
     <hyperlink ref="B1579" r:id="rId1372" display="https://leetcode.com/problems/restore-the-array-from-adjacent-pairs" xr:uid="{700623B8-2FF0-4710-A00D-C7B2A0A7ABA6}"/>
     <hyperlink ref="B1580" r:id="rId1373" display="https://leetcode.com/problems/can-you-eat-your-favorite-candy-on-your-favorite-day" xr:uid="{BEE070B5-F64C-4698-BCE5-1E36A8583440}"/>
-    <hyperlink ref="B1584" r:id="rId1374" display="https://leetcode.com/problems/maximum-score-from-removing-stones" xr:uid="{B7AA18C7-E58A-447A-915A-42D4F13D6310}"/>
-    <hyperlink ref="B1586" r:id="rId1375" display="https://leetcode.com/problems/closest-subsequence-sum" xr:uid="{F32459B0-DF4C-462A-9356-83F25EC7DAA2}"/>
-    <hyperlink ref="B1605" r:id="rId1376" display="https://leetcode.com/problems/number-of-restricted-paths-from-first-to-last-node" xr:uid="{7E8F4145-52CC-410A-8E6D-496A93BC9F35}"/>
-    <hyperlink ref="B1604" r:id="rId1377" display="https://leetcode.com/problems/minimum-elements-to-add-to-form-a-given-sum" xr:uid="{4588D88F-C977-4AC1-9131-6787B276C83B}"/>
-    <hyperlink ref="B1603" r:id="rId1378" display="https://leetcode.com/problems/check-if-binary-string-has-at-most-one-segment-of-ones" xr:uid="{CE9F4064-AD9A-45F5-8FA5-3D837B5BD888}"/>
-    <hyperlink ref="B1602" r:id="rId1379" display="https://leetcode.com/problems/sum-of-beauty-of-all-substrings" xr:uid="{F5D12DA0-6DB0-4E8E-A268-602716EC1E07}"/>
-    <hyperlink ref="B1601" r:id="rId1380" display="https://leetcode.com/problems/check-if-number-is-a-sum-of-powers-of-three" xr:uid="{4602803B-7988-4D38-ABF2-61BC86BCDAC5}"/>
-    <hyperlink ref="B1600" r:id="rId1381" display="https://leetcode.com/problems/find-nearest-point-that-has-the-same-x-or-y-coordinate" xr:uid="{5F651CEF-E9E7-4A94-8963-9659B92CF321}"/>
-    <hyperlink ref="B1599" r:id="rId1382" display="https://leetcode.com/problems/equal-sum-arrays-with-minimum-number-of-operations" xr:uid="{C7244173-A5DF-4CFD-8B2A-1EE21E557BC1}"/>
-    <hyperlink ref="B1598" r:id="rId1383" display="https://leetcode.com/problems/closest-dessert-cost" xr:uid="{F7BEECC4-44E4-47B9-8596-B7703815C60F}"/>
-    <hyperlink ref="B1597" r:id="rId1384" display="https://leetcode.com/problems/count-items-matching-a-rule" xr:uid="{C7425EBD-8CAE-4C06-8E35-71176FE3E292}"/>
-    <hyperlink ref="B1588" r:id="rId1385" display="https://leetcode.com/problems/minimum-changes-to-make-alternating-binary-string" xr:uid="{5E47CEE9-BA48-462F-B4F8-1AF99888DEB3}"/>
-    <hyperlink ref="B1589" r:id="rId1386" display="https://leetcode.com/problems/count-number-of-homogenous-substrings" xr:uid="{9343BDD1-5100-4986-BADF-74E77C30CD7C}"/>
-    <hyperlink ref="B1590" r:id="rId1387" display="https://leetcode.com/problems/minimum-limit-of-balls-in-a-bag" xr:uid="{F6C3BBF6-E091-49FF-8239-45C98E39DC8C}"/>
-    <hyperlink ref="B1591" r:id="rId1388" display="https://leetcode.com/problems/longest-nice-substring" xr:uid="{8E4DAA57-D075-4129-AAC9-2F7D747D4861}"/>
-    <hyperlink ref="B1592" r:id="rId1389" display="https://leetcode.com/problems/form-array-by-concatenating-subarrays-of-another-array" xr:uid="{BBB12904-D1D8-45C5-A73B-4D227A33C7A0}"/>
-    <hyperlink ref="B1593" r:id="rId1390" display="https://leetcode.com/problems/map-of-highest-peak" xr:uid="{D94EC984-B85A-480E-8580-8F6D0807308B}"/>
-    <hyperlink ref="B1594" r:id="rId1391" display="https://leetcode.com/problems/merge-strings-alternately" xr:uid="{10A36CE3-B9BF-4B0B-A7DF-E0BA62BBC363}"/>
-    <hyperlink ref="B1595" r:id="rId1392" display="https://leetcode.com/problems/minimum-number-of-operations-to-move-all-balls-to-each-box" xr:uid="{D44C79CA-AF26-42E8-BA0E-F083D426240B}"/>
-    <hyperlink ref="B1596" r:id="rId1393" display="https://leetcode.com/problems/maximum-score-from-performing-multiplication-operations" xr:uid="{CBFA2C81-65C2-4B16-BD7D-228C47EBD55C}"/>
+    <hyperlink ref="B1585" r:id="rId1374" display="https://leetcode.com/problems/maximum-score-from-removing-stones" xr:uid="{B7AA18C7-E58A-447A-915A-42D4F13D6310}"/>
+    <hyperlink ref="B1587" r:id="rId1375" display="https://leetcode.com/problems/closest-subsequence-sum" xr:uid="{F32459B0-DF4C-462A-9356-83F25EC7DAA2}"/>
+    <hyperlink ref="B1608" r:id="rId1376" display="https://leetcode.com/problems/number-of-restricted-paths-from-first-to-last-node" xr:uid="{7E8F4145-52CC-410A-8E6D-496A93BC9F35}"/>
+    <hyperlink ref="B1607" r:id="rId1377" display="https://leetcode.com/problems/minimum-elements-to-add-to-form-a-given-sum" xr:uid="{4588D88F-C977-4AC1-9131-6787B276C83B}"/>
+    <hyperlink ref="B1604" r:id="rId1378" display="https://leetcode.com/problems/sum-of-beauty-of-all-substrings" xr:uid="{F5D12DA0-6DB0-4E8E-A268-602716EC1E07}"/>
+    <hyperlink ref="B1603" r:id="rId1379" display="https://leetcode.com/problems/check-if-number-is-a-sum-of-powers-of-three" xr:uid="{4602803B-7988-4D38-ABF2-61BC86BCDAC5}"/>
+    <hyperlink ref="B1602" r:id="rId1380" display="https://leetcode.com/problems/find-nearest-point-that-has-the-same-x-or-y-coordinate" xr:uid="{5F651CEF-E9E7-4A94-8963-9659B92CF321}"/>
+    <hyperlink ref="B1601" r:id="rId1381" display="https://leetcode.com/problems/equal-sum-arrays-with-minimum-number-of-operations" xr:uid="{C7244173-A5DF-4CFD-8B2A-1EE21E557BC1}"/>
+    <hyperlink ref="B1600" r:id="rId1382" display="https://leetcode.com/problems/closest-dessert-cost" xr:uid="{F7BEECC4-44E4-47B9-8596-B7703815C60F}"/>
+    <hyperlink ref="B1599" r:id="rId1383" display="https://leetcode.com/problems/count-items-matching-a-rule" xr:uid="{C7425EBD-8CAE-4C06-8E35-71176FE3E292}"/>
+    <hyperlink ref="B1589" r:id="rId1384" display="https://leetcode.com/problems/minimum-changes-to-make-alternating-binary-string" xr:uid="{5E47CEE9-BA48-462F-B4F8-1AF99888DEB3}"/>
+    <hyperlink ref="B1590" r:id="rId1385" display="https://leetcode.com/problems/count-number-of-homogenous-substrings" xr:uid="{9343BDD1-5100-4986-BADF-74E77C30CD7C}"/>
+    <hyperlink ref="B1591" r:id="rId1386" display="https://leetcode.com/problems/minimum-limit-of-balls-in-a-bag" xr:uid="{F6C3BBF6-E091-49FF-8239-45C98E39DC8C}"/>
+    <hyperlink ref="B1593" r:id="rId1387" display="https://leetcode.com/problems/longest-nice-substring" xr:uid="{8E4DAA57-D075-4129-AAC9-2F7D747D4861}"/>
+    <hyperlink ref="B1594" r:id="rId1388" display="https://leetcode.com/problems/form-array-by-concatenating-subarrays-of-another-array" xr:uid="{BBB12904-D1D8-45C5-A73B-4D227A33C7A0}"/>
+    <hyperlink ref="B1595" r:id="rId1389" display="https://leetcode.com/problems/map-of-highest-peak" xr:uid="{D94EC984-B85A-480E-8580-8F6D0807308B}"/>
+    <hyperlink ref="B1596" r:id="rId1390" display="https://leetcode.com/problems/merge-strings-alternately" xr:uid="{10A36CE3-B9BF-4B0B-A7DF-E0BA62BBC363}"/>
+    <hyperlink ref="B1597" r:id="rId1391" display="https://leetcode.com/problems/minimum-number-of-operations-to-move-all-balls-to-each-box" xr:uid="{D44C79CA-AF26-42E8-BA0E-F083D426240B}"/>
+    <hyperlink ref="B1598" r:id="rId1392" display="https://leetcode.com/problems/maximum-score-from-performing-multiplication-operations" xr:uid="{CBFA2C81-65C2-4B16-BD7D-228C47EBD55C}"/>
+    <hyperlink ref="B1609" r:id="rId1393" display="https://leetcode.com/problems/make-the-xor-of-all-segments-equal-to-zero" xr:uid="{F9F7F3F8-AE15-4C3F-90C0-C87C5787CF85}"/>
+    <hyperlink ref="B1610" r:id="rId1394" display="https://leetcode.com/problems/check-if-one-string-swap-can-make-strings-equal" xr:uid="{94C3AB55-2DA1-4F06-A31A-03B510CB7FE6}"/>
+    <hyperlink ref="B1611" r:id="rId1395" display="https://leetcode.com/problems/find-center-of-star-graph" xr:uid="{92C112DA-1E26-4B3F-A26D-5485D079770C}"/>
+    <hyperlink ref="B1613" r:id="rId1396" display="https://leetcode.com/problems/maximum-score-of-a-good-subarray" xr:uid="{04CA3301-F2BD-44FE-8D80-D37D23948A03}"/>
+    <hyperlink ref="B1606" r:id="rId1397" display="https://leetcode.com/problems/check-if-binary-string-has-at-most-one-segment-of-ones" xr:uid="{CE9F4064-AD9A-45F5-8FA5-3D837B5BD888}"/>
+    <hyperlink ref="B1605" r:id="rId1398" display="https://leetcode.com/problems/count-pairs-of-nodes" xr:uid="{4BE12A90-1128-42D6-8B67-87E8493D607F}"/>
+    <hyperlink ref="B1581" r:id="rId1399" display="https://leetcode.com/problems/palindrome-partitioning-iv" xr:uid="{E9727F4E-397D-4808-93D3-81A8EA2BA6FA}"/>
+    <hyperlink ref="B1592" r:id="rId1400" display="https://leetcode.com/problems/minimum-degree-of-a-connected-trio-in-a-graph" xr:uid="{2139E7CC-36A0-4372-9D37-5FD513CDD9B0}"/>
+    <hyperlink ref="B1614" r:id="rId1401" display="https://leetcode.com/problems/second-largest-digit-in-a-string" xr:uid="{4A66E7D8-75C8-4F8E-B9DB-8E399F951B16}"/>
+    <hyperlink ref="B1615" r:id="rId1402" display="https://leetcode.com/problems/design-authentication-manager" xr:uid="{480710DA-1C7D-455D-8D12-167C92DBF633}"/>
+    <hyperlink ref="B1616" r:id="rId1403" display="https://leetcode.com/problems/maximum-number-of-consecutive-values-you-can-make" xr:uid="{194727C9-C65E-44E7-A8A3-E7D9E7AD678B}"/>
+    <hyperlink ref="B1617" r:id="rId1404" display="https://leetcode.com/problems/maximize-score-after-n-operations" xr:uid="{98125BD7-0B8C-4106-A5E4-C55938B917E0}"/>
+    <hyperlink ref="B1618" r:id="rId1405" display="https://leetcode.com/problems/maximum-ascending-subarray-sum" xr:uid="{4206F736-48C2-4C51-BC45-0F7AA538AA31}"/>
+    <hyperlink ref="B1619" r:id="rId1406" display="https://leetcode.com/problems/number-of-orders-in-the-backlog" xr:uid="{A4B7F67E-4F72-4FF8-9023-A90CE712BA15}"/>
+    <hyperlink ref="B1620" r:id="rId1407" display="https://leetcode.com/problems/maximum-value-at-a-given-index-in-a-bounded-array" xr:uid="{E6D3D4E3-7FB4-464D-9389-88A8FB9AB699}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1394"/>
-  <drawing r:id="rId1395"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1408"/>
+  <drawing r:id="rId1409"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in only hard problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A1404A-C7F3-48E3-952D-2DF01EB81037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B61B09-C01D-43C9-BC94-9E854E6F9E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1670</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1686</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8926" uniqueCount="3300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8964" uniqueCount="3313">
   <si>
     <t>Difficulty</t>
   </si>
@@ -9937,6 +9937,45 @@
   </si>
   <si>
     <t>Keep increasing number in stack</t>
+  </si>
+  <si>
+    <t>Count multiples for every number, the scan and sum</t>
+  </si>
+  <si>
+    <t>Number of Ways to Rearrange Sticks With K Sticks Visible</t>
+  </si>
+  <si>
+    <t>Sum of Floored Pairs </t>
+  </si>
+  <si>
+    <t>At every n sticks, consider longest as last or not</t>
+  </si>
+  <si>
+    <t>Stone Game VIII</t>
+  </si>
+  <si>
+    <t>From right to left, calculate every position optimal number</t>
+  </si>
+  <si>
+    <t>Minimum XOR Sum of Two Arrays</t>
+  </si>
+  <si>
+    <t>Use bit mask to calculate every combination</t>
+  </si>
+  <si>
+    <t>2 ^ N</t>
+  </si>
+  <si>
+    <t>Minimum Skips to Arrive at Meeting On Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate at every position at (i) and skip 0 to (i) based on previous position. </t>
+  </si>
+  <si>
+    <t>Minimum Space Wasted From Packaging</t>
+  </si>
+  <si>
+    <t>Sort packages and boxes, find any size of box will cover how many packages</t>
   </si>
 </sst>
 </file>
@@ -9981,7 +10020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10008,6 +10047,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -10452,10 +10493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1670"/>
+  <dimension ref="A1:J1686"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1645" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1665" sqref="A1665"/>
+    <sheetView tabSelected="1" topLeftCell="A1654" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1677" sqref="B1677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -43443,7 +43484,7 @@
     </row>
     <row r="1410" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1410" s="48">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="B1410" s="1" t="s">
         <v>2711</v>
@@ -50118,44 +50159,236 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="1666" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1666" s="1"/>
+    <row r="1666" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1666" s="80">
+        <v>1862</v>
+      </c>
+      <c r="B1666" s="1" t="s">
+        <v>3302</v>
+      </c>
+      <c r="C1666" s="80">
+        <v>4</v>
+      </c>
+      <c r="D1666" s="80" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1666" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1666" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1666" s="80" t="s">
+        <v>3300</v>
+      </c>
+      <c r="I1666" s="80" t="s">
+        <v>3224</v>
+      </c>
     </row>
     <row r="1667" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1667" s="1"/>
-    </row>
-    <row r="1668" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1668" s="1"/>
-    </row>
-    <row r="1669" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1669" s="80" t="s">
+      <c r="A1667" s="71">
+        <v>1866</v>
+      </c>
+      <c r="B1667" s="1" t="s">
+        <v>3301</v>
+      </c>
+      <c r="C1667" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1667" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1667" s="71" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1667" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1667" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1667" s="71" t="s">
+        <v>3303</v>
+      </c>
+      <c r="I1667" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1668" s="80">
+        <v>1872</v>
+      </c>
+      <c r="B1668" s="1" t="s">
+        <v>3304</v>
+      </c>
+      <c r="C1668" s="80">
+        <v>5</v>
+      </c>
+      <c r="D1668" s="80" t="s">
+        <v>2810</v>
+      </c>
+      <c r="F1668" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1668" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1668" s="80" t="s">
+        <v>3305</v>
+      </c>
+      <c r="I1668" s="80" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1669" s="80">
+        <v>1879</v>
+      </c>
+      <c r="B1669" s="1" t="s">
+        <v>3306</v>
+      </c>
+      <c r="C1669" s="80">
+        <v>4</v>
+      </c>
+      <c r="D1669" s="80" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1669" s="80" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1669" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1669" s="80" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1669" s="80" t="s">
+        <v>3307</v>
+      </c>
+      <c r="I1669" s="80" t="s">
+        <v>3308</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1670" s="71">
+        <v>1883</v>
+      </c>
+      <c r="B1670" s="1" t="s">
+        <v>3309</v>
+      </c>
+      <c r="C1670" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1670" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1670" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1670" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1670" s="71" t="s">
+        <v>3310</v>
+      </c>
+      <c r="I1670" s="71" t="s">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1671" s="62">
+        <v>1889</v>
+      </c>
+      <c r="B1671" s="1" t="s">
+        <v>3311</v>
+      </c>
+      <c r="C1671" s="62">
+        <v>4</v>
+      </c>
+      <c r="D1671" s="62" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1671" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1671" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1671" s="62" t="s">
+        <v>3312</v>
+      </c>
+      <c r="I1671" s="62" t="s">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1672" s="1"/>
+    </row>
+    <row r="1673" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1673" s="1"/>
+    </row>
+    <row r="1674" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1674" s="1"/>
+    </row>
+    <row r="1675" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1675" s="1"/>
+    </row>
+    <row r="1676" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1676" s="1"/>
+    </row>
+    <row r="1677" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1677" s="1"/>
+    </row>
+    <row r="1678" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1678" s="1"/>
+    </row>
+    <row r="1679" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1679" s="1"/>
+    </row>
+    <row r="1680" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1680" s="1"/>
+    </row>
+    <row r="1681" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1681" s="1"/>
+    </row>
+    <row r="1682" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1682" s="1"/>
+    </row>
+    <row r="1683" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1683" s="1"/>
+    </row>
+    <row r="1684" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1684" s="1"/>
+    </row>
+    <row r="1685" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1685" s="82" t="s">
         <v>1721</v>
       </c>
-      <c r="B1669" s="80"/>
-      <c r="C1669" s="80"/>
-      <c r="D1669" s="80"/>
-      <c r="E1669" s="80"/>
-      <c r="F1669" s="80"/>
-      <c r="G1669" s="80"/>
-      <c r="H1669" s="80"/>
-    </row>
-    <row r="1670" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1670" s="81" t="s">
+      <c r="B1685" s="82"/>
+      <c r="C1685" s="82"/>
+      <c r="D1685" s="82"/>
+      <c r="E1685" s="82"/>
+      <c r="F1685" s="82"/>
+      <c r="G1685" s="82"/>
+      <c r="H1685" s="82"/>
+    </row>
+    <row r="1686" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1686" s="83" t="s">
         <v>2760</v>
       </c>
-      <c r="B1670" s="81"/>
-      <c r="C1670" s="81"/>
-      <c r="D1670" s="81"/>
-      <c r="E1670" s="81"/>
-      <c r="F1670" s="81"/>
-      <c r="G1670" s="81"/>
-      <c r="H1670" s="81"/>
+      <c r="B1686" s="83"/>
+      <c r="C1686" s="83"/>
+      <c r="D1686" s="83"/>
+      <c r="E1686" s="83"/>
+      <c r="F1686" s="83"/>
+      <c r="G1686" s="83"/>
+      <c r="H1686" s="83"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1670" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1686" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1669:H1669"/>
-    <mergeCell ref="A1670:H1670"/>
+    <mergeCell ref="A1685:H1685"/>
+    <mergeCell ref="A1686:H1686"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -51604,10 +51837,17 @@
     <hyperlink ref="B1662" r:id="rId1444" display="https://leetcode.com/problems/maximum-population-year" xr:uid="{8B601B30-68A1-40B2-8CC4-5ADE4F1AADB0}"/>
     <hyperlink ref="B1663" r:id="rId1445" display="https://leetcode.com/problems/maximum-distance-between-a-pair-of-values" xr:uid="{6526D9AA-7EF1-4DDB-8A45-0E58240D35C1}"/>
     <hyperlink ref="B1664" r:id="rId1446" display="https://leetcode.com/problems/maximum-subarray-min-product" xr:uid="{652F1242-245F-4CDD-80E1-CD2643BBF1DD}"/>
+    <hyperlink ref="B1410" r:id="rId1447" display="https://leetcode.com/problems/minimum-cost-to-cut-a-stick" xr:uid="{43E29B64-294E-4116-AA83-2FC7A623AF15}"/>
+    <hyperlink ref="B1667" r:id="rId1448" display="https://leetcode.com/problems/number-of-ways-to-rearrange-sticks-with-k-sticks-visible" xr:uid="{E35D13B0-22B7-490D-B5AB-4A7212373890}"/>
+    <hyperlink ref="B1666" r:id="rId1449" display="https://leetcode.com/problems/sum-of-floored-pairs" xr:uid="{093A209E-68BA-452C-AA91-6C7000A5F2E3}"/>
+    <hyperlink ref="B1668" r:id="rId1450" display="https://leetcode.com/problems/stone-game-viii" xr:uid="{61F21AD1-64FA-4012-9BE3-4243D664B6E2}"/>
+    <hyperlink ref="B1669" r:id="rId1451" display="https://leetcode.com/problems/minimum-xor-sum-of-two-arrays" xr:uid="{FD7F5FAD-8697-4398-A6A7-4EF44D3CEA63}"/>
+    <hyperlink ref="B1670" r:id="rId1452" display="https://leetcode.com/problems/minimum-skips-to-arrive-at-meeting-on-time" xr:uid="{9E93822D-BDD4-48D6-A1B5-4CB1349E95EC}"/>
+    <hyperlink ref="B1671" r:id="rId1453" display="https://leetcode.com/problems/minimum-space-wasted-from-packaging" xr:uid="{FD882ECA-EAB3-432E-B354-871F2953F4AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1447"/>
-  <drawing r:id="rId1448"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1454"/>
+  <drawing r:id="rId1455"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in latest week hard problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B61B09-C01D-43C9-BC94-9E854E6F9E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789EA149-F92F-49E5-8284-82A8A4CEB905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8964" uniqueCount="3313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8976" uniqueCount="3318">
   <si>
     <t>Difficulty</t>
   </si>
@@ -9976,6 +9976,21 @@
   </si>
   <si>
     <t>Sort packages and boxes, find any size of box will cover how many packages</t>
+  </si>
+  <si>
+    <t>Minimum Cost to Change the Final Value of Expression</t>
+  </si>
+  <si>
+    <t>The Earliest and Latest Rounds Where Players Compete</t>
+  </si>
+  <si>
+    <t>Parse the string to build expression tree then calculate</t>
+  </si>
+  <si>
+    <t>2^N</t>
+  </si>
+  <si>
+    <t>Iterate loser with bit mask from two ends and take new round when two pointers meet</t>
   </si>
 </sst>
 </file>
@@ -10496,7 +10511,7 @@
   <dimension ref="A1:J1686"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1654" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1677" sqref="B1677"/>
+      <selection activeCell="A1673" sqref="A1673"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -50322,10 +50337,56 @@
       </c>
     </row>
     <row r="1672" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1672" s="1"/>
+      <c r="A1672" s="81">
+        <v>1896</v>
+      </c>
+      <c r="B1672" s="1" t="s">
+        <v>3313</v>
+      </c>
+      <c r="C1672" s="81">
+        <v>6</v>
+      </c>
+      <c r="D1672" s="81" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1672" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1672" s="81" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1672" s="81" t="s">
+        <v>3315</v>
+      </c>
+      <c r="I1672" s="81" t="s">
+        <v>3000</v>
+      </c>
     </row>
     <row r="1673" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1673" s="1"/>
+      <c r="A1673" s="81">
+        <v>1900</v>
+      </c>
+      <c r="B1673" s="1" t="s">
+        <v>3314</v>
+      </c>
+      <c r="C1673" s="81">
+        <v>5</v>
+      </c>
+      <c r="D1673" s="81" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1673" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1673" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1673" s="81" t="s">
+        <v>3317</v>
+      </c>
+      <c r="I1673" s="81" t="s">
+        <v>3316</v>
+      </c>
     </row>
     <row r="1674" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1674" s="1"/>
@@ -51844,10 +51905,12 @@
     <hyperlink ref="B1669" r:id="rId1451" display="https://leetcode.com/problems/minimum-xor-sum-of-two-arrays" xr:uid="{FD7F5FAD-8697-4398-A6A7-4EF44D3CEA63}"/>
     <hyperlink ref="B1670" r:id="rId1452" display="https://leetcode.com/problems/minimum-skips-to-arrive-at-meeting-on-time" xr:uid="{9E93822D-BDD4-48D6-A1B5-4CB1349E95EC}"/>
     <hyperlink ref="B1671" r:id="rId1453" display="https://leetcode.com/problems/minimum-space-wasted-from-packaging" xr:uid="{FD882ECA-EAB3-432E-B354-871F2953F4AE}"/>
+    <hyperlink ref="B1672" r:id="rId1454" display="https://leetcode.com/problems/minimum-cost-to-change-the-final-value-of-expression" xr:uid="{8AEEABF2-8972-41C9-9EAC-7A4DC947DB04}"/>
+    <hyperlink ref="B1673" r:id="rId1455" display="https://leetcode.com/problems/the-earliest-and-latest-rounds-where-players-compete" xr:uid="{1BA05603-7474-4610-A2E6-E0FE942FC497}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1454"/>
-  <drawing r:id="rId1455"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1456"/>
+  <drawing r:id="rId1457"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check easy problems in past weeks
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789EA149-F92F-49E5-8284-82A8A4CEB905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489F1A54-D542-4850-8201-974ABEA50119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1686</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1694</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8976" uniqueCount="3318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9026" uniqueCount="3335">
   <si>
     <t>Difficulty</t>
   </si>
@@ -9991,6 +9991,57 @@
   </si>
   <si>
     <t>Iterate loser with bit mask from two ends and take new round when two pointers meet</t>
+  </si>
+  <si>
+    <t>Sorting the Sentence</t>
+  </si>
+  <si>
+    <t>Parse string and write to array</t>
+  </si>
+  <si>
+    <t>Sum of All Subset XOR Totals </t>
+  </si>
+  <si>
+    <t>if a bit is set it will generate 2^(n-1) sum.</t>
+  </si>
+  <si>
+    <t>Longer Contiguous Segments of Ones than Zeros</t>
+  </si>
+  <si>
+    <t>Accumulate count for zero and one</t>
+  </si>
+  <si>
+    <t>Substrings of Size Three with Distinct Characters</t>
+  </si>
+  <si>
+    <t>Count new character and character removed</t>
+  </si>
+  <si>
+    <t>Check if Word Equals Summation of Two Words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convert to integer </t>
+  </si>
+  <si>
+    <t>Determine Whether Matrix Can Be Obtained By Rotation</t>
+  </si>
+  <si>
+    <t>Coordination transformation</t>
+  </si>
+  <si>
+    <t>Check if All the Integers in a Range Are Covered</t>
+  </si>
+  <si>
+    <t>Sweep line</t>
+  </si>
+  <si>
+    <t>Incremental Memory Leak</t>
+  </si>
+  <si>
+    <t>Simulate on operation</t>
+  </si>
+  <si>
+    <t>sqrt(N)</t>
   </si>
 </sst>
 </file>
@@ -10035,7 +10086,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10062,6 +10113,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -10508,10 +10562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1686"/>
+  <dimension ref="A1:J1694"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1654" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1673" sqref="A1673"/>
+    <sheetView tabSelected="1" topLeftCell="A1658" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1667" sqref="I1667"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10981,7 +11035,7 @@
         <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="H18" t="s">
         <v>1753</v>
@@ -11108,7 +11162,7 @@
         <v>9</v>
       </c>
       <c r="G23" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="H23" t="s">
         <v>2305</v>
@@ -11295,7 +11349,7 @@
         <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="H31" t="s">
         <v>61</v>
@@ -11462,7 +11516,7 @@
         <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="H38" t="s">
         <v>2719</v>
@@ -11511,7 +11565,7 @@
         <v>9</v>
       </c>
       <c r="G40" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="H40" t="s">
         <v>2720</v>
@@ -11537,7 +11591,7 @@
         <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="H41" t="s">
         <v>1803</v>
@@ -11678,7 +11732,7 @@
         <v>9</v>
       </c>
       <c r="G47" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="H47" t="s">
         <v>2720</v>
@@ -11704,7 +11758,7 @@
         <v>9</v>
       </c>
       <c r="G48" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="H48" s="51" t="s">
         <v>1803</v>
@@ -50174,122 +50228,119 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="1666" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1666" s="80">
-        <v>1862</v>
+    <row r="1666" spans="1:9" s="82" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1666" s="82">
+        <v>1859</v>
       </c>
       <c r="B1666" s="1" t="s">
-        <v>3302</v>
-      </c>
-      <c r="C1666" s="80">
-        <v>4</v>
-      </c>
-      <c r="D1666" s="80" t="s">
+        <v>3318</v>
+      </c>
+      <c r="C1666" s="82">
+        <v>1</v>
+      </c>
+      <c r="D1666" s="82" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1666" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1666" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1666" s="82" t="s">
+        <v>3319</v>
+      </c>
+      <c r="I1666" s="82" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:9" s="84" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1667" s="84">
+        <v>1860</v>
+      </c>
+      <c r="B1667" s="1" t="s">
+        <v>3332</v>
+      </c>
+      <c r="C1667" s="84">
+        <v>3</v>
+      </c>
+      <c r="D1667" s="84" t="s">
         <v>1718</v>
       </c>
-      <c r="F1666" s="80" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1666" s="80" t="s">
+      <c r="F1667" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1667" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="H1666" s="80" t="s">
-        <v>3300</v>
-      </c>
-      <c r="I1666" s="80" t="s">
-        <v>3224</v>
-      </c>
-    </row>
-    <row r="1667" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1667" s="71">
-        <v>1866</v>
-      </c>
-      <c r="B1667" s="1" t="s">
-        <v>3301</v>
-      </c>
-      <c r="C1667" s="71">
-        <v>4</v>
-      </c>
-      <c r="D1667" s="71" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1667" s="71" t="s">
-        <v>2924</v>
-      </c>
-      <c r="F1667" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1667" s="71" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1667" s="71" t="s">
-        <v>3303</v>
-      </c>
-      <c r="I1667" s="71" t="s">
-        <v>3000</v>
+      <c r="H1667" s="84" t="s">
+        <v>3333</v>
+      </c>
+      <c r="I1667" s="84" t="s">
+        <v>3334</v>
       </c>
     </row>
     <row r="1668" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1668" s="80">
-        <v>1872</v>
+        <v>1862</v>
       </c>
       <c r="B1668" s="1" t="s">
-        <v>3304</v>
+        <v>3302</v>
       </c>
       <c r="C1668" s="80">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1668" s="80" t="s">
-        <v>2810</v>
+        <v>1718</v>
       </c>
       <c r="F1668" s="80" t="s">
         <v>12</v>
       </c>
       <c r="G1668" s="80" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H1668" s="80" t="s">
-        <v>3305</v>
+        <v>3300</v>
       </c>
       <c r="I1668" s="80" t="s">
+        <v>3224</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:9" s="82" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1669" s="82">
+        <v>1863</v>
+      </c>
+      <c r="B1669" s="1" t="s">
+        <v>3320</v>
+      </c>
+      <c r="C1669" s="82">
+        <v>3</v>
+      </c>
+      <c r="D1669" s="82" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E1669" s="82" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1669" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1669" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1669" s="82" t="s">
+        <v>3321</v>
+      </c>
+      <c r="I1669" s="82" t="s">
         <v>3000</v>
-      </c>
-    </row>
-    <row r="1669" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1669" s="80">
-        <v>1879</v>
-      </c>
-      <c r="B1669" s="1" t="s">
-        <v>3306</v>
-      </c>
-      <c r="C1669" s="80">
-        <v>4</v>
-      </c>
-      <c r="D1669" s="80" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1669" s="80" t="s">
-        <v>2935</v>
-      </c>
-      <c r="F1669" s="80" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1669" s="80" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1669" s="80" t="s">
-        <v>3307</v>
-      </c>
-      <c r="I1669" s="80" t="s">
-        <v>3308</v>
       </c>
     </row>
     <row r="1670" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1670" s="71">
-        <v>1883</v>
+        <v>1866</v>
       </c>
       <c r="B1670" s="1" t="s">
-        <v>3309</v>
+        <v>3301</v>
       </c>
       <c r="C1670" s="71">
         <v>4</v>
@@ -50297,6 +50348,9 @@
       <c r="D1670" s="71" t="s">
         <v>1720</v>
       </c>
+      <c r="E1670" s="71" t="s">
+        <v>2924</v>
+      </c>
       <c r="F1670" s="71" t="s">
         <v>12</v>
       </c>
@@ -50304,152 +50358,366 @@
         <v>28</v>
       </c>
       <c r="H1670" s="71" t="s">
+        <v>3303</v>
+      </c>
+      <c r="I1670" s="71" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:9" s="82" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1671" s="82">
+        <v>1869</v>
+      </c>
+      <c r="B1671" s="1" t="s">
+        <v>3322</v>
+      </c>
+      <c r="C1671" s="82">
+        <v>2</v>
+      </c>
+      <c r="D1671" s="82" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1671" s="82" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1671" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1671" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1671" s="82" t="s">
+        <v>3323</v>
+      </c>
+      <c r="I1671" s="82" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1672" s="80">
+        <v>1872</v>
+      </c>
+      <c r="B1672" s="1" t="s">
+        <v>3304</v>
+      </c>
+      <c r="C1672" s="80">
+        <v>5</v>
+      </c>
+      <c r="D1672" s="80" t="s">
+        <v>2810</v>
+      </c>
+      <c r="F1672" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1672" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1672" s="80" t="s">
+        <v>3305</v>
+      </c>
+      <c r="I1672" s="80" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:9" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1673" s="83">
+        <v>1876</v>
+      </c>
+      <c r="B1673" s="1" t="s">
+        <v>3324</v>
+      </c>
+      <c r="C1673" s="83">
+        <v>2</v>
+      </c>
+      <c r="D1673" s="83" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1673" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1673" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1673" s="83" t="s">
+        <v>3325</v>
+      </c>
+      <c r="I1673" s="83" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1674" s="80">
+        <v>1879</v>
+      </c>
+      <c r="B1674" s="1" t="s">
+        <v>3306</v>
+      </c>
+      <c r="C1674" s="80">
+        <v>4</v>
+      </c>
+      <c r="D1674" s="80" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1674" s="80" t="s">
+        <v>2935</v>
+      </c>
+      <c r="F1674" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1674" s="80" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1674" s="80" t="s">
+        <v>3307</v>
+      </c>
+      <c r="I1674" s="80" t="s">
+        <v>3308</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:9" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1675" s="83">
+        <v>1880</v>
+      </c>
+      <c r="B1675" s="1" t="s">
+        <v>3326</v>
+      </c>
+      <c r="C1675" s="83">
+        <v>1</v>
+      </c>
+      <c r="D1675" s="83" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1675" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1675" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1675" s="83" t="s">
+        <v>3327</v>
+      </c>
+      <c r="I1675" s="83" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1676" s="71">
+        <v>1883</v>
+      </c>
+      <c r="B1676" s="1" t="s">
+        <v>3309</v>
+      </c>
+      <c r="C1676" s="71">
+        <v>4</v>
+      </c>
+      <c r="D1676" s="71" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1676" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1676" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1676" s="71" t="s">
         <v>3310</v>
       </c>
-      <c r="I1670" s="71" t="s">
+      <c r="I1676" s="71" t="s">
         <v>3026</v>
       </c>
     </row>
-    <row r="1671" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1671" s="62">
+    <row r="1677" spans="1:9" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1677" s="83">
+        <v>1886</v>
+      </c>
+      <c r="B1677" s="1" t="s">
+        <v>3328</v>
+      </c>
+      <c r="C1677" s="83">
+        <v>3</v>
+      </c>
+      <c r="D1677" s="83" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1677" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1677" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1677" s="83" t="s">
+        <v>3329</v>
+      </c>
+      <c r="I1677" s="83" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1678" s="62">
         <v>1889</v>
       </c>
-      <c r="B1671" s="1" t="s">
+      <c r="B1678" s="1" t="s">
         <v>3311</v>
       </c>
-      <c r="C1671" s="62">
+      <c r="C1678" s="62">
         <v>4</v>
       </c>
-      <c r="D1671" s="62" t="s">
+      <c r="D1678" s="62" t="s">
         <v>1720</v>
       </c>
-      <c r="F1671" s="62" t="s">
+      <c r="F1678" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="G1671" s="62" t="s">
+      <c r="G1678" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="H1671" s="62" t="s">
+      <c r="H1678" s="62" t="s">
         <v>3312</v>
       </c>
-      <c r="I1671" s="62" t="s">
+      <c r="I1678" s="62" t="s">
         <v>3029</v>
       </c>
     </row>
-    <row r="1672" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1672" s="81">
+    <row r="1679" spans="1:9" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1679" s="83">
+        <v>1893</v>
+      </c>
+      <c r="B1679" s="1" t="s">
+        <v>3330</v>
+      </c>
+      <c r="C1679" s="83">
+        <v>3</v>
+      </c>
+      <c r="D1679" s="83" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1679" s="83" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1679" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1679" s="83" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1679" s="83" t="s">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1680" s="81">
         <v>1896</v>
       </c>
-      <c r="B1672" s="1" t="s">
+      <c r="B1680" s="1" t="s">
         <v>3313</v>
       </c>
-      <c r="C1672" s="81">
+      <c r="C1680" s="81">
         <v>6</v>
       </c>
-      <c r="D1672" s="81" t="s">
+      <c r="D1680" s="81" t="s">
         <v>1720</v>
       </c>
-      <c r="F1672" s="81" t="s">
+      <c r="F1680" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="G1672" s="81" t="s">
+      <c r="G1680" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="H1672" s="81" t="s">
+      <c r="H1680" s="81" t="s">
         <v>3315</v>
       </c>
-      <c r="I1672" s="81" t="s">
+      <c r="I1680" s="81" t="s">
         <v>3000</v>
       </c>
     </row>
-    <row r="1673" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1673" s="81">
+    <row r="1681" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1681" s="81">
         <v>1900</v>
       </c>
-      <c r="B1673" s="1" t="s">
+      <c r="B1681" s="1" t="s">
         <v>3314</v>
       </c>
-      <c r="C1673" s="81">
-        <v>5</v>
-      </c>
-      <c r="D1673" s="81" t="s">
+      <c r="C1681" s="81">
+        <v>5</v>
+      </c>
+      <c r="D1681" s="81" t="s">
         <v>1713</v>
       </c>
-      <c r="F1673" s="81" t="s">
+      <c r="F1681" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="G1673" s="81" t="s">
+      <c r="G1681" s="81" t="s">
         <v>121</v>
       </c>
-      <c r="H1673" s="81" t="s">
+      <c r="H1681" s="81" t="s">
         <v>3317</v>
       </c>
-      <c r="I1673" s="81" t="s">
+      <c r="I1681" s="81" t="s">
         <v>3316</v>
       </c>
     </row>
-    <row r="1674" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1674" s="1"/>
-    </row>
-    <row r="1675" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1675" s="1"/>
-    </row>
-    <row r="1676" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1676" s="1"/>
-    </row>
-    <row r="1677" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1677" s="1"/>
-    </row>
-    <row r="1678" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1678" s="1"/>
-    </row>
-    <row r="1679" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1679" s="1"/>
-    </row>
-    <row r="1680" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1680" s="1"/>
-    </row>
-    <row r="1681" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1681" s="1"/>
-    </row>
-    <row r="1682" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1682" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1682" s="1"/>
     </row>
-    <row r="1683" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1683" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1683" s="1"/>
     </row>
-    <row r="1684" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1684" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1684" s="1"/>
     </row>
-    <row r="1685" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1685" s="82" t="s">
+    <row r="1685" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1685" s="1"/>
+    </row>
+    <row r="1686" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1686" s="1"/>
+    </row>
+    <row r="1687" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1687" s="1"/>
+    </row>
+    <row r="1688" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1688" s="1"/>
+    </row>
+    <row r="1689" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1689" s="1"/>
+    </row>
+    <row r="1690" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1690" s="1"/>
+    </row>
+    <row r="1691" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1691" s="1"/>
+    </row>
+    <row r="1692" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1692" s="1"/>
+    </row>
+    <row r="1693" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1693" s="85" t="s">
         <v>1721</v>
       </c>
-      <c r="B1685" s="82"/>
-      <c r="C1685" s="82"/>
-      <c r="D1685" s="82"/>
-      <c r="E1685" s="82"/>
-      <c r="F1685" s="82"/>
-      <c r="G1685" s="82"/>
-      <c r="H1685" s="82"/>
-    </row>
-    <row r="1686" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1686" s="83" t="s">
+      <c r="B1693" s="85"/>
+      <c r="C1693" s="85"/>
+      <c r="D1693" s="85"/>
+      <c r="E1693" s="85"/>
+      <c r="F1693" s="85"/>
+      <c r="G1693" s="85"/>
+      <c r="H1693" s="85"/>
+    </row>
+    <row r="1694" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1694" s="86" t="s">
         <v>2760</v>
       </c>
-      <c r="B1686" s="83"/>
-      <c r="C1686" s="83"/>
-      <c r="D1686" s="83"/>
-      <c r="E1686" s="83"/>
-      <c r="F1686" s="83"/>
-      <c r="G1686" s="83"/>
-      <c r="H1686" s="83"/>
+      <c r="B1694" s="86"/>
+      <c r="C1694" s="86"/>
+      <c r="D1694" s="86"/>
+      <c r="E1694" s="86"/>
+      <c r="F1694" s="86"/>
+      <c r="G1694" s="86"/>
+      <c r="H1694" s="86"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1686" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1694" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1685:H1685"/>
-    <mergeCell ref="A1686:H1686"/>
+    <mergeCell ref="A1693:H1693"/>
+    <mergeCell ref="A1694:H1694"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -51899,18 +52167,25 @@
     <hyperlink ref="B1663" r:id="rId1445" display="https://leetcode.com/problems/maximum-distance-between-a-pair-of-values" xr:uid="{6526D9AA-7EF1-4DDB-8A45-0E58240D35C1}"/>
     <hyperlink ref="B1664" r:id="rId1446" display="https://leetcode.com/problems/maximum-subarray-min-product" xr:uid="{652F1242-245F-4CDD-80E1-CD2643BBF1DD}"/>
     <hyperlink ref="B1410" r:id="rId1447" display="https://leetcode.com/problems/minimum-cost-to-cut-a-stick" xr:uid="{43E29B64-294E-4116-AA83-2FC7A623AF15}"/>
-    <hyperlink ref="B1667" r:id="rId1448" display="https://leetcode.com/problems/number-of-ways-to-rearrange-sticks-with-k-sticks-visible" xr:uid="{E35D13B0-22B7-490D-B5AB-4A7212373890}"/>
-    <hyperlink ref="B1666" r:id="rId1449" display="https://leetcode.com/problems/sum-of-floored-pairs" xr:uid="{093A209E-68BA-452C-AA91-6C7000A5F2E3}"/>
-    <hyperlink ref="B1668" r:id="rId1450" display="https://leetcode.com/problems/stone-game-viii" xr:uid="{61F21AD1-64FA-4012-9BE3-4243D664B6E2}"/>
-    <hyperlink ref="B1669" r:id="rId1451" display="https://leetcode.com/problems/minimum-xor-sum-of-two-arrays" xr:uid="{FD7F5FAD-8697-4398-A6A7-4EF44D3CEA63}"/>
-    <hyperlink ref="B1670" r:id="rId1452" display="https://leetcode.com/problems/minimum-skips-to-arrive-at-meeting-on-time" xr:uid="{9E93822D-BDD4-48D6-A1B5-4CB1349E95EC}"/>
-    <hyperlink ref="B1671" r:id="rId1453" display="https://leetcode.com/problems/minimum-space-wasted-from-packaging" xr:uid="{FD882ECA-EAB3-432E-B354-871F2953F4AE}"/>
-    <hyperlink ref="B1672" r:id="rId1454" display="https://leetcode.com/problems/minimum-cost-to-change-the-final-value-of-expression" xr:uid="{8AEEABF2-8972-41C9-9EAC-7A4DC947DB04}"/>
-    <hyperlink ref="B1673" r:id="rId1455" display="https://leetcode.com/problems/the-earliest-and-latest-rounds-where-players-compete" xr:uid="{1BA05603-7474-4610-A2E6-E0FE942FC497}"/>
+    <hyperlink ref="B1670" r:id="rId1448" display="https://leetcode.com/problems/number-of-ways-to-rearrange-sticks-with-k-sticks-visible" xr:uid="{E35D13B0-22B7-490D-B5AB-4A7212373890}"/>
+    <hyperlink ref="B1668" r:id="rId1449" display="https://leetcode.com/problems/sum-of-floored-pairs" xr:uid="{093A209E-68BA-452C-AA91-6C7000A5F2E3}"/>
+    <hyperlink ref="B1672" r:id="rId1450" display="https://leetcode.com/problems/stone-game-viii" xr:uid="{61F21AD1-64FA-4012-9BE3-4243D664B6E2}"/>
+    <hyperlink ref="B1674" r:id="rId1451" display="https://leetcode.com/problems/minimum-xor-sum-of-two-arrays" xr:uid="{FD7F5FAD-8697-4398-A6A7-4EF44D3CEA63}"/>
+    <hyperlink ref="B1676" r:id="rId1452" display="https://leetcode.com/problems/minimum-skips-to-arrive-at-meeting-on-time" xr:uid="{9E93822D-BDD4-48D6-A1B5-4CB1349E95EC}"/>
+    <hyperlink ref="B1678" r:id="rId1453" display="https://leetcode.com/problems/minimum-space-wasted-from-packaging" xr:uid="{FD882ECA-EAB3-432E-B354-871F2953F4AE}"/>
+    <hyperlink ref="B1680" r:id="rId1454" display="https://leetcode.com/problems/minimum-cost-to-change-the-final-value-of-expression" xr:uid="{8AEEABF2-8972-41C9-9EAC-7A4DC947DB04}"/>
+    <hyperlink ref="B1681" r:id="rId1455" display="https://leetcode.com/problems/the-earliest-and-latest-rounds-where-players-compete" xr:uid="{1BA05603-7474-4610-A2E6-E0FE942FC497}"/>
+    <hyperlink ref="B1669" r:id="rId1456" display="https://leetcode.com/problems/sum-of-all-subset-xor-totals" xr:uid="{916CBCE4-8E4F-4C1A-ADC8-D712E20E7078}"/>
+    <hyperlink ref="B1671" r:id="rId1457" display="https://leetcode.com/problems/longer-contiguous-segments-of-ones-than-zeros" xr:uid="{F0373E6C-9FDE-4708-BDE4-1BAF6BC3DAF9}"/>
+    <hyperlink ref="B1673" r:id="rId1458" display="https://leetcode.com/problems/substrings-of-size-three-with-distinct-characters" xr:uid="{1D3C16AD-27DB-4D26-B4C5-CB3468282314}"/>
+    <hyperlink ref="B1675" r:id="rId1459" display="https://leetcode.com/problems/check-if-word-equals-summation-of-two-words" xr:uid="{26751097-8588-426A-9778-1F2134E99BA0}"/>
+    <hyperlink ref="B1677" r:id="rId1460" display="https://leetcode.com/problems/determine-whether-matrix-can-be-obtained-by-rotation" xr:uid="{DAAF2CCC-883E-4313-871A-8A735A3F5ADA}"/>
+    <hyperlink ref="B1679" r:id="rId1461" display="https://leetcode.com/problems/check-if-all-the-integers-in-a-range-are-covered" xr:uid="{1E1CE91C-D79D-487A-A76A-6DE39C6CDD96}"/>
+    <hyperlink ref="B1667" r:id="rId1462" display="https://leetcode.com/problems/incremental-memory-leak" xr:uid="{CA1A11F1-F4F6-4D65-9D69-A6197119EA1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1456"/>
-  <drawing r:id="rId1457"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1463"/>
+  <drawing r:id="rId1464"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add some easy problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2409EF06-B89C-4981-83E6-08A4675FEF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9D914E-6BE6-48D0-AB29-CFB0549E2C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1707</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1715</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9228" uniqueCount="3384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9266" uniqueCount="3397">
   <si>
     <t>Difficulty</t>
   </si>
@@ -10189,6 +10189,45 @@
   </si>
   <si>
     <t>Bit Trie and combine traverse and query</t>
+  </si>
+  <si>
+    <t>Find the Student that Will Replace the Chalk</t>
+  </si>
+  <si>
+    <t>Add sum of the array</t>
+  </si>
+  <si>
+    <t>N *M</t>
+  </si>
+  <si>
+    <t>Sum of Digits of String After Convert</t>
+  </si>
+  <si>
+    <t>Convert string to digit repeatedly</t>
+  </si>
+  <si>
+    <t>Check if All Characters Have Equal Number of Occurrences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check character count </t>
+  </si>
+  <si>
+    <t>Maximum Number of Words You Can</t>
+  </si>
+  <si>
+    <t>String split and check broken letter in map</t>
+  </si>
+  <si>
+    <t>Maximum Number of Removable Characters</t>
+  </si>
+  <si>
+    <t>Guess the number and skip deleted characters</t>
+  </si>
+  <si>
+    <t>Merge Triplets to Form Target Triplet</t>
+  </si>
+  <si>
+    <t>Skip triplets with maximum overflow and then merge remaining</t>
   </si>
 </sst>
 </file>
@@ -10233,7 +10272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10260,6 +10299,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -10713,10 +10753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1707"/>
+  <dimension ref="A1:J1715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1683" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1705" sqref="G1705"/>
+    <sheetView tabSelected="1" topLeftCell="A1698" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1699" sqref="A1699:XFD1699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -51229,212 +51269,215 @@
         <v>3028</v>
       </c>
     </row>
-    <row r="1692" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1692" s="87">
+    <row r="1692" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1692" s="89">
+        <v>1894</v>
+      </c>
+      <c r="B1692" s="1" t="s">
+        <v>3384</v>
+      </c>
+      <c r="C1692" s="89">
+        <v>2</v>
+      </c>
+      <c r="D1692" s="89" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1692" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1692" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1692" s="89" t="s">
+        <v>3385</v>
+      </c>
+      <c r="I1692" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:9" s="87" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1693" s="87">
         <v>1895</v>
       </c>
-      <c r="B1692" s="1" t="s">
+      <c r="B1693" s="1" t="s">
         <v>3361</v>
       </c>
-      <c r="C1692" s="87">
-        <v>3</v>
-      </c>
-      <c r="D1692" s="87" t="s">
+      <c r="C1693" s="87">
+        <v>3</v>
+      </c>
+      <c r="D1693" s="87" t="s">
         <v>1713</v>
       </c>
-      <c r="F1692" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1692" s="87" t="s">
+      <c r="F1693" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1693" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="H1692" s="87" t="s">
+      <c r="H1693" s="87" t="s">
         <v>3362</v>
       </c>
-    </row>
-    <row r="1693" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1693" s="81">
+      <c r="I1693" s="87" t="s">
+        <v>3386</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1694" s="81">
         <v>1896</v>
       </c>
-      <c r="B1693" s="1" t="s">
+      <c r="B1694" s="1" t="s">
         <v>3312</v>
       </c>
-      <c r="C1693" s="81">
+      <c r="C1694" s="81">
         <v>6</v>
       </c>
-      <c r="D1693" s="81" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1693" s="81" t="s">
+      <c r="D1694" s="81" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1694" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="G1693" s="81" t="s">
+      <c r="G1694" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="H1693" s="81" t="s">
+      <c r="H1694" s="81" t="s">
         <v>3314</v>
       </c>
-      <c r="I1693" s="81" t="s">
+      <c r="I1694" s="81" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1694" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1694" s="88">
+    <row r="1695" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1695" s="88">
         <v>1897</v>
       </c>
-      <c r="B1694" s="1" t="s">
+      <c r="B1695" s="1" t="s">
         <v>3373</v>
       </c>
-      <c r="C1694" s="88">
+      <c r="C1695" s="88">
         <v>1</v>
       </c>
-      <c r="D1694" s="88" t="s">
+      <c r="D1695" s="88" t="s">
         <v>1767</v>
       </c>
-      <c r="E1694" s="88" t="s">
+      <c r="E1695" s="88" t="s">
         <v>2934</v>
       </c>
-      <c r="F1694" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1694" s="88" t="s">
+      <c r="F1695" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1695" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="H1694" s="88" t="s">
+      <c r="H1695" s="88" t="s">
         <v>3374</v>
       </c>
-      <c r="I1694" s="88" t="s">
+      <c r="I1695" s="88" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1695" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1695" s="81">
-        <v>1900</v>
-      </c>
-      <c r="B1695" s="1" t="s">
-        <v>3313</v>
-      </c>
-      <c r="C1695" s="81">
-        <v>5</v>
-      </c>
-      <c r="D1695" s="81" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1695" s="81" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1695" s="81" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1695" s="81" t="s">
-        <v>3316</v>
-      </c>
-      <c r="I1695" s="81" t="s">
-        <v>3315</v>
-      </c>
-    </row>
-    <row r="1696" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1696" s="81">
-        <v>1903</v>
+    <row r="1696" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1696" s="89">
+        <v>1898</v>
       </c>
       <c r="B1696" s="1" t="s">
-        <v>3336</v>
-      </c>
-      <c r="C1696" s="81">
-        <v>1</v>
-      </c>
-      <c r="D1696" s="81" t="s">
-        <v>1717</v>
-      </c>
-      <c r="F1696" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1696" s="81" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1696" s="81" t="s">
-        <v>3337</v>
-      </c>
-      <c r="I1696" s="81" t="s">
+        <v>3393</v>
+      </c>
+      <c r="C1696" s="89">
+        <v>3</v>
+      </c>
+      <c r="D1696" s="89" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1696" s="89" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1696" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1696" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1696" s="89" t="s">
+        <v>3394</v>
+      </c>
+      <c r="I1696" s="89" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1697" s="89">
+        <v>1899</v>
+      </c>
+      <c r="B1697" s="1" t="s">
+        <v>3395</v>
+      </c>
+      <c r="C1697" s="89">
+        <v>2</v>
+      </c>
+      <c r="D1697" s="89" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1697" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1697" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1697" s="89" t="s">
+        <v>3396</v>
+      </c>
+      <c r="I1697" s="89" t="s">
         <v>2999</v>
-      </c>
-    </row>
-    <row r="1697" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1697" s="81">
-        <v>1906</v>
-      </c>
-      <c r="B1697" s="1" t="s">
-        <v>3338</v>
-      </c>
-      <c r="C1697" s="81">
-        <v>4</v>
-      </c>
-      <c r="D1697" s="81" t="s">
-        <v>2809</v>
-      </c>
-      <c r="F1697" s="81" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1697" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1697" s="81" t="s">
-        <v>3339</v>
-      </c>
-      <c r="I1697" s="81" t="s">
-        <v>3344</v>
       </c>
     </row>
     <row r="1698" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1698" s="81">
-        <v>1909</v>
+        <v>1900</v>
       </c>
       <c r="B1698" s="1" t="s">
-        <v>3340</v>
+        <v>3313</v>
       </c>
       <c r="C1698" s="81">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1698" s="81" t="s">
-        <v>1767</v>
-      </c>
-      <c r="E1698" s="81" t="s">
-        <v>2934</v>
+        <v>1713</v>
       </c>
       <c r="F1698" s="81" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1698" s="81" t="s">
-        <v>41</v>
+        <v>121</v>
       </c>
       <c r="H1698" s="81" t="s">
-        <v>3341</v>
+        <v>3316</v>
       </c>
       <c r="I1698" s="81" t="s">
-        <v>2999</v>
+        <v>3315</v>
       </c>
     </row>
     <row r="1699" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1699" s="81">
-        <v>1913</v>
+        <v>1903</v>
       </c>
       <c r="B1699" s="1" t="s">
-        <v>3342</v>
+        <v>3336</v>
       </c>
       <c r="C1699" s="81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1699" s="81" t="s">
-        <v>1767</v>
+        <v>1717</v>
       </c>
       <c r="F1699" s="81" t="s">
         <v>5</v>
       </c>
       <c r="G1699" s="81" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H1699" s="81" t="s">
-        <v>3343</v>
+        <v>3337</v>
       </c>
       <c r="I1699" s="81" t="s">
         <v>2999</v>
@@ -51442,189 +51485,354 @@
     </row>
     <row r="1700" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1700" s="81">
-        <v>1914</v>
+        <v>1906</v>
       </c>
       <c r="B1700" s="1" t="s">
-        <v>3345</v>
+        <v>3338</v>
       </c>
       <c r="C1700" s="81">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1700" s="81" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1700" s="81" t="s">
-        <v>2934</v>
+        <v>2809</v>
       </c>
       <c r="F1700" s="81" t="s">
         <v>9</v>
       </c>
       <c r="G1700" s="81" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H1700" s="81" t="s">
-        <v>3347</v>
+        <v>3339</v>
       </c>
       <c r="I1700" s="81" t="s">
-        <v>2999</v>
+        <v>3344</v>
       </c>
     </row>
     <row r="1701" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1701" s="81">
-        <v>1916</v>
+        <v>1909</v>
       </c>
       <c r="B1701" s="1" t="s">
-        <v>3346</v>
+        <v>3340</v>
       </c>
       <c r="C1701" s="81">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1701" s="81" t="s">
-        <v>1718</v>
+        <v>1767</v>
+      </c>
+      <c r="E1701" s="81" t="s">
+        <v>2934</v>
       </c>
       <c r="F1701" s="81" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G1701" s="81" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H1701" s="81" t="s">
-        <v>3348</v>
+        <v>3341</v>
       </c>
       <c r="I1701" s="81" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1702" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1702" s="88">
-        <v>1920</v>
+    <row r="1702" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1702" s="81">
+        <v>1913</v>
       </c>
       <c r="B1702" s="1" t="s">
-        <v>3375</v>
-      </c>
-      <c r="C1702" s="88">
-        <v>1</v>
-      </c>
-      <c r="D1702" s="88" t="s">
+        <v>3342</v>
+      </c>
+      <c r="C1702" s="81">
+        <v>2</v>
+      </c>
+      <c r="D1702" s="81" t="s">
         <v>1767</v>
       </c>
-      <c r="F1702" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1702" s="88" t="s">
+      <c r="F1702" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1702" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1702" s="81" t="s">
+        <v>3343</v>
+      </c>
+      <c r="I1702" s="81" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1703" s="81">
+        <v>1914</v>
+      </c>
+      <c r="B1703" s="1" t="s">
+        <v>3345</v>
+      </c>
+      <c r="C1703" s="81">
+        <v>3</v>
+      </c>
+      <c r="D1703" s="81" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1703" s="81" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1703" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1703" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="H1702" s="88" t="s">
-        <v>3376</v>
-      </c>
-      <c r="I1702" s="88" t="s">
+      <c r="H1703" s="81" t="s">
+        <v>3347</v>
+      </c>
+      <c r="I1703" s="81" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1703" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1703" s="88">
-        <v>1923</v>
-      </c>
-      <c r="B1703" s="1" t="s">
-        <v>3377</v>
-      </c>
-      <c r="C1703" s="88">
-        <v>6</v>
-      </c>
-      <c r="D1703" s="88" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1703" s="88" t="s">
+    <row r="1704" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1704" s="81">
+        <v>1916</v>
+      </c>
+      <c r="B1704" s="1" t="s">
+        <v>3346</v>
+      </c>
+      <c r="C1704" s="81">
+        <v>4</v>
+      </c>
+      <c r="D1704" s="81" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1704" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="G1703" s="88" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1703" s="88" t="s">
-        <v>3378</v>
-      </c>
-      <c r="I1703" s="88" t="s">
-        <v>3381</v>
-      </c>
-    </row>
-    <row r="1704" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1704" s="88">
-        <v>1932</v>
-      </c>
-      <c r="B1704" s="1" t="s">
-        <v>3379</v>
-      </c>
-      <c r="C1704" s="88">
-        <v>4</v>
-      </c>
-      <c r="D1704" s="88" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1704" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1704" s="88" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1704" s="88" t="s">
-        <v>3380</v>
-      </c>
-      <c r="I1704" s="88" t="s">
+      <c r="G1704" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1704" s="81" t="s">
+        <v>3348</v>
+      </c>
+      <c r="I1704" s="81" t="s">
         <v>2999</v>
       </c>
     </row>
     <row r="1705" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1705" s="88">
+        <v>1920</v>
+      </c>
+      <c r="B1705" s="1" t="s">
+        <v>3375</v>
+      </c>
+      <c r="C1705" s="88">
+        <v>1</v>
+      </c>
+      <c r="D1705" s="88" t="s">
+        <v>1767</v>
+      </c>
+      <c r="F1705" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1705" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1705" s="88" t="s">
+        <v>3376</v>
+      </c>
+      <c r="I1705" s="88" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1706" s="88">
+        <v>1923</v>
+      </c>
+      <c r="B1706" s="1" t="s">
+        <v>3377</v>
+      </c>
+      <c r="C1706" s="88">
+        <v>6</v>
+      </c>
+      <c r="D1706" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1706" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1706" s="88" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1706" s="88" t="s">
+        <v>3378</v>
+      </c>
+      <c r="I1706" s="88" t="s">
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1707" s="88">
+        <v>1932</v>
+      </c>
+      <c r="B1707" s="1" t="s">
+        <v>3379</v>
+      </c>
+      <c r="C1707" s="88">
+        <v>4</v>
+      </c>
+      <c r="D1707" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1707" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1707" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1707" s="88" t="s">
+        <v>3380</v>
+      </c>
+      <c r="I1707" s="88" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1708" s="89">
+        <v>1935</v>
+      </c>
+      <c r="B1708" s="1" t="s">
+        <v>3391</v>
+      </c>
+      <c r="C1708" s="89">
+        <v>2</v>
+      </c>
+      <c r="D1708" s="89" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1708" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1708" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1708" s="89" t="s">
+        <v>3392</v>
+      </c>
+      <c r="I1708" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1709" s="88">
         <v>1938</v>
       </c>
-      <c r="B1705" s="1" t="s">
+      <c r="B1709" s="1" t="s">
         <v>3382</v>
       </c>
-      <c r="C1705" s="88">
-        <v>5</v>
-      </c>
-      <c r="D1705" s="88" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1705" s="88" t="s">
+      <c r="C1709" s="88">
+        <v>5</v>
+      </c>
+      <c r="D1709" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1709" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="G1705" s="88" t="s">
+      <c r="G1709" s="88" t="s">
         <v>134</v>
       </c>
-      <c r="H1705" s="88" t="s">
+      <c r="H1709" s="88" t="s">
         <v>3383</v>
       </c>
     </row>
-    <row r="1706" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1706" s="89" t="s">
+    <row r="1710" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1710" s="1"/>
+    </row>
+    <row r="1711" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1711" s="1"/>
+    </row>
+    <row r="1712" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1712" s="89">
+        <v>1941</v>
+      </c>
+      <c r="B1712" s="1" t="s">
+        <v>3389</v>
+      </c>
+      <c r="C1712" s="89">
+        <v>1</v>
+      </c>
+      <c r="D1712" s="89" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1712" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1712" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1712" s="89" t="s">
+        <v>3390</v>
+      </c>
+      <c r="I1712" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1713" s="89">
+        <v>1945</v>
+      </c>
+      <c r="B1713" s="1" t="s">
+        <v>3387</v>
+      </c>
+      <c r="C1713" s="89">
+        <v>1</v>
+      </c>
+      <c r="D1713" s="89" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1713" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1713" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1713" s="89" t="s">
+        <v>3388</v>
+      </c>
+      <c r="I1713" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1714" s="90" t="s">
         <v>1721</v>
       </c>
-      <c r="B1706" s="89"/>
-      <c r="C1706" s="89"/>
-      <c r="D1706" s="89"/>
-      <c r="E1706" s="89"/>
-      <c r="F1706" s="89"/>
-      <c r="G1706" s="89"/>
-      <c r="H1706" s="89"/>
-    </row>
-    <row r="1707" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1707" s="90" t="s">
+      <c r="B1714" s="90"/>
+      <c r="C1714" s="90"/>
+      <c r="D1714" s="90"/>
+      <c r="E1714" s="90"/>
+      <c r="F1714" s="90"/>
+      <c r="G1714" s="90"/>
+      <c r="H1714" s="90"/>
+    </row>
+    <row r="1715" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1715" s="91" t="s">
         <v>2759</v>
       </c>
-      <c r="B1707" s="90"/>
-      <c r="C1707" s="90"/>
-      <c r="D1707" s="90"/>
-      <c r="E1707" s="90"/>
-      <c r="F1707" s="90"/>
-      <c r="G1707" s="90"/>
-      <c r="H1707" s="90"/>
+      <c r="B1715" s="91"/>
+      <c r="C1715" s="91"/>
+      <c r="D1715" s="91"/>
+      <c r="E1715" s="91"/>
+      <c r="F1715" s="91"/>
+      <c r="G1715" s="91"/>
+      <c r="H1715" s="91"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1707" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1715" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1706:H1706"/>
-    <mergeCell ref="A1707:H1707"/>
+    <mergeCell ref="A1714:H1714"/>
+    <mergeCell ref="A1715:H1715"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -53080,8 +53288,8 @@
     <hyperlink ref="B1681" r:id="rId1451" display="https://leetcode.com/problems/minimum-xor-sum-of-two-arrays" xr:uid="{FD7F5FAD-8697-4398-A6A7-4EF44D3CEA63}"/>
     <hyperlink ref="B1685" r:id="rId1452" display="https://leetcode.com/problems/minimum-skips-to-arrive-at-meeting-on-time" xr:uid="{9E93822D-BDD4-48D6-A1B5-4CB1349E95EC}"/>
     <hyperlink ref="B1690" r:id="rId1453" display="https://leetcode.com/problems/minimum-space-wasted-from-packaging" xr:uid="{FD882ECA-EAB3-432E-B354-871F2953F4AE}"/>
-    <hyperlink ref="B1693" r:id="rId1454" display="https://leetcode.com/problems/minimum-cost-to-change-the-final-value-of-expression" xr:uid="{8AEEABF2-8972-41C9-9EAC-7A4DC947DB04}"/>
-    <hyperlink ref="B1695" r:id="rId1455" display="https://leetcode.com/problems/the-earliest-and-latest-rounds-where-players-compete" xr:uid="{1BA05603-7474-4610-A2E6-E0FE942FC497}"/>
+    <hyperlink ref="B1694" r:id="rId1454" display="https://leetcode.com/problems/minimum-cost-to-change-the-final-value-of-expression" xr:uid="{8AEEABF2-8972-41C9-9EAC-7A4DC947DB04}"/>
+    <hyperlink ref="B1698" r:id="rId1455" display="https://leetcode.com/problems/the-earliest-and-latest-rounds-where-players-compete" xr:uid="{1BA05603-7474-4610-A2E6-E0FE942FC497}"/>
     <hyperlink ref="B1670" r:id="rId1456" display="https://leetcode.com/problems/sum-of-all-subset-xor-totals" xr:uid="{916CBCE4-8E4F-4C1A-ADC8-D712E20E7078}"/>
     <hyperlink ref="B1674" r:id="rId1457" display="https://leetcode.com/problems/longer-contiguous-segments-of-ones-than-zeros" xr:uid="{F0373E6C-9FDE-4708-BDE4-1BAF6BC3DAF9}"/>
     <hyperlink ref="B1678" r:id="rId1458" display="https://leetcode.com/problems/substrings-of-size-three-with-distinct-characters" xr:uid="{1D3C16AD-27DB-4D26-B4C5-CB3468282314}"/>
@@ -53090,32 +53298,38 @@
     <hyperlink ref="B1691" r:id="rId1461" display="https://leetcode.com/problems/check-if-all-the-integers-in-a-range-are-covered" xr:uid="{1E1CE91C-D79D-487A-A76A-6DE39C6CDD96}"/>
     <hyperlink ref="B1667" r:id="rId1462" display="https://leetcode.com/problems/incremental-memory-leak" xr:uid="{CA1A11F1-F4F6-4D65-9D69-A6197119EA1E}"/>
     <hyperlink ref="B1668" r:id="rId1463" display="https://leetcode.com/problems/rotating-the-box" xr:uid="{1DBA9A18-E1D2-4148-8C3A-048CE82287C0}"/>
-    <hyperlink ref="B1696" r:id="rId1464" display="https://leetcode.com/problems/largest-odd-number-in-string" xr:uid="{C1F070FE-5338-44D3-AC2F-454F2F234B37}"/>
-    <hyperlink ref="B1697" r:id="rId1465" display="https://leetcode.com/problems/minimum-absolute-difference-queries" xr:uid="{BC2F4066-1A7C-40E6-807A-59A6290C5130}"/>
-    <hyperlink ref="B1698" r:id="rId1466" xr:uid="{701B89CB-0972-4CC9-B496-BFC2EA4D6053}"/>
-    <hyperlink ref="B1699" r:id="rId1467" xr:uid="{8495B600-B833-4B44-9931-395989DBBB7D}"/>
-    <hyperlink ref="B1700" r:id="rId1468" display="https://leetcode.com/problems/cyclically-rotating-a-grid" xr:uid="{3AFFE1F3-E05C-4E5B-AB9D-548519408295}"/>
-    <hyperlink ref="B1701" r:id="rId1469" display=" Count Ways to Build Rooms in an Ant Colony" xr:uid="{E356F1D9-1378-42C3-B1EC-4016F02C08FE}"/>
+    <hyperlink ref="B1699" r:id="rId1464" display="https://leetcode.com/problems/largest-odd-number-in-string" xr:uid="{C1F070FE-5338-44D3-AC2F-454F2F234B37}"/>
+    <hyperlink ref="B1700" r:id="rId1465" display="https://leetcode.com/problems/minimum-absolute-difference-queries" xr:uid="{BC2F4066-1A7C-40E6-807A-59A6290C5130}"/>
+    <hyperlink ref="B1701" r:id="rId1466" xr:uid="{701B89CB-0972-4CC9-B496-BFC2EA4D6053}"/>
+    <hyperlink ref="B1702" r:id="rId1467" xr:uid="{8495B600-B833-4B44-9931-395989DBBB7D}"/>
+    <hyperlink ref="B1703" r:id="rId1468" display="https://leetcode.com/problems/cyclically-rotating-a-grid" xr:uid="{3AFFE1F3-E05C-4E5B-AB9D-548519408295}"/>
+    <hyperlink ref="B1704" r:id="rId1469" display=" Count Ways to Build Rooms in an Ant Colony" xr:uid="{E356F1D9-1378-42C3-B1EC-4016F02C08FE}"/>
     <hyperlink ref="B1671" r:id="rId1470" xr:uid="{68B63B60-AA23-4767-8102-9AA46D58D32F}"/>
     <hyperlink ref="B1672" r:id="rId1471" display="https://leetcode.com/problems/finding-pairs-with-a-certain-sum" xr:uid="{37561B08-BC65-437E-B174-B127301F6D30}"/>
     <hyperlink ref="B1675" r:id="rId1472" display="https://leetcode.com/problems/minimum-speed-to-arrive-on-time" xr:uid="{544CF080-940E-4B3B-8C0D-B8C5A249310B}"/>
     <hyperlink ref="B1680" r:id="rId1473" display=" Get Biggest Three Rhombus Sums in a Grid" xr:uid="{C9ED9B55-F0EC-476B-8A98-0E74857AAAFC}"/>
     <hyperlink ref="B1676" r:id="rId1474" display="https://leetcode.com/problems/jump-game-vii" xr:uid="{D4DE1BAE-1CC3-4DD3-9C0A-914FC5B5661F}"/>
     <hyperlink ref="B1683" r:id="rId1475" display="https://leetcode.com/problems/maximum-value-after-insertion" xr:uid="{1CE67B2F-87CD-4FD5-B4F7-25783440228A}"/>
-    <hyperlink ref="B1692" r:id="rId1476" display="https://leetcode.com/problems/largest-magic-square" xr:uid="{1DB8991F-9DCC-4BF1-AF94-E99D460D113B}"/>
+    <hyperlink ref="B1693" r:id="rId1476" display="https://leetcode.com/problems/largest-magic-square" xr:uid="{1DB8991F-9DCC-4BF1-AF94-E99D460D113B}"/>
     <hyperlink ref="B1679" r:id="rId1477" display="https://leetcode.com/problems/minimize-maximum-pair-sum-in-array" xr:uid="{D3735233-4AEB-4C89-B82C-4CA4DF8B68B4}"/>
     <hyperlink ref="B1684" r:id="rId1478" display="https://leetcode.com/problems/process-tasks-using-servers" xr:uid="{E6E0ED0E-18FD-4748-90EB-5D666411330C}"/>
     <hyperlink ref="B1686" r:id="rId1479" display="https://leetcode.com/problems/egg-drop-with-2-eggs-and-n-floors" xr:uid="{8F3F40B0-8D67-46A7-B467-4EEA5B9A8063}"/>
     <hyperlink ref="B1688" r:id="rId1480" display="https://leetcode.com/problems/reduction-operations-to-make-the-array-elements-equal" xr:uid="{93CBEB02-546F-4B36-807B-CAA599C9C2E1}"/>
-    <hyperlink ref="B1694" r:id="rId1481" display="https://leetcode.com/problems/redistribute-characters-to-make-all-strings-equal" xr:uid="{514AD256-6C6F-423E-93EA-68F73246AB3C}"/>
-    <hyperlink ref="B1702" r:id="rId1482" display="https://leetcode.com/problems/build-array-from-permutation" xr:uid="{A7BA82A2-3CCD-45FF-8CCB-DCE423A9403F}"/>
-    <hyperlink ref="B1703" r:id="rId1483" display="https://leetcode.com/problems/longest-common-subpath" xr:uid="{62FFD7C8-6B95-49CF-877E-D2923644D1FD}"/>
-    <hyperlink ref="B1704" r:id="rId1484" display="https://leetcode.com/problems/merge-bsts-to-create-single-bst" xr:uid="{3C90ED05-B4E6-4A5B-8B92-92274CD6E3CB}"/>
-    <hyperlink ref="B1705" r:id="rId1485" display="https://leetcode.com/problems/maximum-genetic-difference-query" xr:uid="{1A25DDAD-A0E9-4DEA-9978-DBF0F9D4D3DF}"/>
+    <hyperlink ref="B1695" r:id="rId1481" display="https://leetcode.com/problems/redistribute-characters-to-make-all-strings-equal" xr:uid="{514AD256-6C6F-423E-93EA-68F73246AB3C}"/>
+    <hyperlink ref="B1705" r:id="rId1482" display="https://leetcode.com/problems/build-array-from-permutation" xr:uid="{A7BA82A2-3CCD-45FF-8CCB-DCE423A9403F}"/>
+    <hyperlink ref="B1706" r:id="rId1483" display="https://leetcode.com/problems/longest-common-subpath" xr:uid="{62FFD7C8-6B95-49CF-877E-D2923644D1FD}"/>
+    <hyperlink ref="B1707" r:id="rId1484" display="https://leetcode.com/problems/merge-bsts-to-create-single-bst" xr:uid="{3C90ED05-B4E6-4A5B-8B92-92274CD6E3CB}"/>
+    <hyperlink ref="B1709" r:id="rId1485" display="https://leetcode.com/problems/maximum-genetic-difference-query" xr:uid="{1A25DDAD-A0E9-4DEA-9978-DBF0F9D4D3DF}"/>
+    <hyperlink ref="B1692" r:id="rId1486" display="https://leetcode.com/problems/find-the-student-that-will-replace-the-chalk" xr:uid="{9D146C0C-5A16-4375-BDF0-B60367842FF7}"/>
+    <hyperlink ref="B1713" r:id="rId1487" display="https://leetcode.com/problems/sum-of-digits-of-string-after-convert" xr:uid="{6F22ECDB-6A6B-41D3-8CA9-6D76CAF5B4E8}"/>
+    <hyperlink ref="B1712" r:id="rId1488" xr:uid="{67E882AF-68DB-41AF-8071-513205274BD9}"/>
+    <hyperlink ref="B1708" r:id="rId1489" display="https://leetcode.com/problems/maximum-number-of-words-you-can-type" xr:uid="{8E21FA9C-EBEA-4E91-AD8C-B9177EF763E8}"/>
+    <hyperlink ref="B1696" r:id="rId1490" xr:uid="{A3071BE6-0034-43AE-BDF8-5799BAD6EB13}"/>
+    <hyperlink ref="B1697" r:id="rId1491" display="https://leetcode.com/problems/merge-triplets-to-form-target-triplet" xr:uid="{EFBBCE90-7311-45FC-B707-92A6E1252460}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1486"/>
-  <drawing r:id="rId1487"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1492"/>
+  <drawing r:id="rId1493"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add hard problems in recent weeks
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9D914E-6BE6-48D0-AB29-CFB0549E2C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A859DEA-C82F-4E40-9B32-77DEC2B310E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1715</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1720</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9266" uniqueCount="3397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9313" uniqueCount="3412">
   <si>
     <t>Difficulty</t>
   </si>
@@ -10228,6 +10228,51 @@
   </si>
   <si>
     <t>Skip triplets with maximum overflow and then merge remaining</t>
+  </si>
+  <si>
+    <t>Maximum Product of the Length of Two Palindromic Substrings</t>
+  </si>
+  <si>
+    <t>Manacher's algorithm</t>
+  </si>
+  <si>
+    <t>Count Number of Special Subsequences</t>
+  </si>
+  <si>
+    <t>Delete Duplicate Folders in System</t>
+  </si>
+  <si>
+    <t>0: dp[0] += dp[0] +1, 1: dp[1] += dp[0]+dp[1], 2: dp[2] += dp[1]+dp[2]</t>
+  </si>
+  <si>
+    <t>construct a tree, seralize subtree to string and map the duplicate</t>
+  </si>
+  <si>
+    <t>Number of Visible People in a Queue</t>
+  </si>
+  <si>
+    <t>Monotone stack track increasing heights</t>
+  </si>
+  <si>
+    <t>Painting a Grid With Three Different </t>
+  </si>
+  <si>
+    <t>memorize last column and search column by column</t>
+  </si>
+  <si>
+    <t>Minimum Cost to Reach Destination in Time</t>
+  </si>
+  <si>
+    <t>Shortested Path with cost update by time and cost</t>
+  </si>
+  <si>
+    <t>C* 3^ R</t>
+  </si>
+  <si>
+    <t>Design Movie Rental System</t>
+  </si>
+  <si>
+    <t>Store movie in Sorted Tree Map by price, shop under hastable of moives</t>
   </si>
 </sst>
 </file>
@@ -10272,7 +10317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10299,6 +10344,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -10753,10 +10799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1715"/>
+  <dimension ref="A1:J1720"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1698" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1699" sqref="A1699:XFD1699"/>
+    <sheetView tabSelected="1" topLeftCell="B1698" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1712" sqref="C1712"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -51538,56 +51584,56 @@
         <v>2999</v>
       </c>
     </row>
-    <row r="1702" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1702" s="81">
-        <v>1913</v>
+    <row r="1702" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1702" s="90">
+        <v>1912</v>
       </c>
       <c r="B1702" s="1" t="s">
-        <v>3342</v>
-      </c>
-      <c r="C1702" s="81">
-        <v>2</v>
-      </c>
-      <c r="D1702" s="81" t="s">
-        <v>1767</v>
-      </c>
-      <c r="F1702" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1702" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1702" s="81" t="s">
-        <v>3343</v>
-      </c>
-      <c r="I1702" s="81" t="s">
-        <v>2999</v>
+        <v>3410</v>
+      </c>
+      <c r="C1702" s="90">
+        <v>4</v>
+      </c>
+      <c r="D1702" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1702" s="90" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1702" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1702" s="90" t="s">
+        <v>457</v>
+      </c>
+      <c r="H1702" s="90" t="s">
+        <v>3411</v>
+      </c>
+      <c r="I1702" s="90" t="s">
+        <v>3028</v>
       </c>
     </row>
     <row r="1703" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1703" s="81">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B1703" s="1" t="s">
-        <v>3345</v>
+        <v>3342</v>
       </c>
       <c r="C1703" s="81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1703" s="81" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1703" s="81" t="s">
-        <v>2934</v>
+        <v>1767</v>
       </c>
       <c r="F1703" s="81" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1703" s="81" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H1703" s="81" t="s">
-        <v>3347</v>
+        <v>3343</v>
       </c>
       <c r="I1703" s="81" t="s">
         <v>2999</v>
@@ -51595,91 +51641,94 @@
     </row>
     <row r="1704" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1704" s="81">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="B1704" s="1" t="s">
-        <v>3346</v>
+        <v>3345</v>
       </c>
       <c r="C1704" s="81">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1704" s="81" t="s">
-        <v>1718</v>
+        <v>1720</v>
+      </c>
+      <c r="E1704" s="81" t="s">
+        <v>2934</v>
       </c>
       <c r="F1704" s="81" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1704" s="81" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H1704" s="81" t="s">
-        <v>3348</v>
+        <v>3347</v>
       </c>
       <c r="I1704" s="81" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1705" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1705" s="88">
-        <v>1920</v>
+    <row r="1705" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1705" s="81">
+        <v>1916</v>
       </c>
       <c r="B1705" s="1" t="s">
-        <v>3375</v>
-      </c>
-      <c r="C1705" s="88">
-        <v>1</v>
-      </c>
-      <c r="D1705" s="88" t="s">
-        <v>1767</v>
-      </c>
-      <c r="F1705" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1705" s="88" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1705" s="88" t="s">
-        <v>3376</v>
-      </c>
-      <c r="I1705" s="88" t="s">
+        <v>3346</v>
+      </c>
+      <c r="C1705" s="81">
+        <v>4</v>
+      </c>
+      <c r="D1705" s="81" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1705" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1705" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1705" s="81" t="s">
+        <v>3348</v>
+      </c>
+      <c r="I1705" s="81" t="s">
         <v>2999</v>
       </c>
     </row>
     <row r="1706" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1706" s="88">
-        <v>1923</v>
+        <v>1920</v>
       </c>
       <c r="B1706" s="1" t="s">
-        <v>3377</v>
+        <v>3375</v>
       </c>
       <c r="C1706" s="88">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1706" s="88" t="s">
-        <v>1720</v>
+        <v>1767</v>
       </c>
       <c r="F1706" s="88" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G1706" s="88" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H1706" s="88" t="s">
-        <v>3378</v>
+        <v>3376</v>
       </c>
       <c r="I1706" s="88" t="s">
-        <v>3381</v>
+        <v>2999</v>
       </c>
     </row>
     <row r="1707" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1707" s="88">
-        <v>1932</v>
+        <v>1923</v>
       </c>
       <c r="B1707" s="1" t="s">
-        <v>3379</v>
+        <v>3377</v>
       </c>
       <c r="C1707" s="88">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1707" s="88" t="s">
         <v>1720</v>
@@ -51688,102 +51737,154 @@
         <v>12</v>
       </c>
       <c r="G1707" s="88" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1707" s="88" t="s">
+        <v>3378</v>
+      </c>
+      <c r="I1707" s="88" t="s">
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1708" s="90">
+        <v>1928</v>
+      </c>
+      <c r="B1708" s="1" t="s">
+        <v>3407</v>
+      </c>
+      <c r="C1708" s="90">
+        <v>4</v>
+      </c>
+      <c r="D1708" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1708" s="90" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1708" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1708" s="90" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1708" s="90" t="s">
+        <v>3408</v>
+      </c>
+      <c r="I1708" s="90" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1709" s="90">
+        <v>1931</v>
+      </c>
+      <c r="B1709" s="1" t="s">
+        <v>3405</v>
+      </c>
+      <c r="C1709" s="90">
+        <v>4</v>
+      </c>
+      <c r="D1709" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1709" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1709" s="90" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1709" s="90" t="s">
+        <v>3406</v>
+      </c>
+      <c r="I1709" s="90" t="s">
+        <v>3409</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1710" s="88">
+        <v>1932</v>
+      </c>
+      <c r="B1710" s="1" t="s">
+        <v>3379</v>
+      </c>
+      <c r="C1710" s="88">
+        <v>4</v>
+      </c>
+      <c r="D1710" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1710" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1710" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="H1707" s="88" t="s">
+      <c r="H1710" s="88" t="s">
         <v>3380</v>
       </c>
-      <c r="I1707" s="88" t="s">
+      <c r="I1710" s="88" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1708" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1708" s="89">
+    <row r="1711" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1711" s="89">
         <v>1935</v>
       </c>
-      <c r="B1708" s="1" t="s">
+      <c r="B1711" s="1" t="s">
         <v>3391</v>
       </c>
-      <c r="C1708" s="89">
+      <c r="C1711" s="89">
         <v>2</v>
       </c>
-      <c r="D1708" s="89" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1708" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1708" s="89" t="s">
+      <c r="D1711" s="89" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1711" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1711" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="H1708" s="89" t="s">
+      <c r="H1711" s="89" t="s">
         <v>3392</v>
       </c>
-      <c r="I1708" s="89" t="s">
+      <c r="I1711" s="89" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1709" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1709" s="88">
+    <row r="1712" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1712" s="88">
         <v>1938</v>
       </c>
-      <c r="B1709" s="1" t="s">
+      <c r="B1712" s="1" t="s">
         <v>3382</v>
       </c>
-      <c r="C1709" s="88">
-        <v>5</v>
-      </c>
-      <c r="D1709" s="88" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1709" s="88" t="s">
+      <c r="C1712" s="88">
+        <v>6</v>
+      </c>
+      <c r="D1712" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1712" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="G1709" s="88" t="s">
+      <c r="G1712" s="88" t="s">
         <v>134</v>
       </c>
-      <c r="H1709" s="88" t="s">
+      <c r="H1712" s="88" t="s">
         <v>3383</v>
       </c>
-    </row>
-    <row r="1710" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1710" s="1"/>
-    </row>
-    <row r="1711" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1711" s="1"/>
-    </row>
-    <row r="1712" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1712" s="89">
-        <v>1941</v>
-      </c>
-      <c r="B1712" s="1" t="s">
-        <v>3389</v>
-      </c>
-      <c r="C1712" s="89">
-        <v>1</v>
-      </c>
-      <c r="D1712" s="89" t="s">
-        <v>1717</v>
-      </c>
-      <c r="F1712" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1712" s="89" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1712" s="89" t="s">
-        <v>3390</v>
-      </c>
-      <c r="I1712" s="89" t="s">
-        <v>2999</v>
+      <c r="I1712" s="88" t="s">
+        <v>3178</v>
       </c>
     </row>
     <row r="1713" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1713" s="89">
-        <v>1945</v>
+        <v>1941</v>
       </c>
       <c r="B1713" s="1" t="s">
-        <v>3387</v>
+        <v>3389</v>
       </c>
       <c r="C1713" s="89">
         <v>1</v>
@@ -51795,44 +51896,180 @@
         <v>5</v>
       </c>
       <c r="G1713" s="89" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="H1713" s="89" t="s">
-        <v>3388</v>
+        <v>3390</v>
       </c>
       <c r="I1713" s="89" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1714" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1714" s="90" t="s">
+    <row r="1714" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1714" s="90">
+        <v>1944</v>
+      </c>
+      <c r="B1714" s="1" t="s">
+        <v>3403</v>
+      </c>
+      <c r="C1714" s="90">
+        <v>4</v>
+      </c>
+      <c r="D1714" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1714" s="90" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1714" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1714" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1714" s="90" t="s">
+        <v>3404</v>
+      </c>
+      <c r="I1714" s="90" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1715" s="89">
+        <v>1945</v>
+      </c>
+      <c r="B1715" s="1" t="s">
+        <v>3387</v>
+      </c>
+      <c r="C1715" s="89">
+        <v>1</v>
+      </c>
+      <c r="D1715" s="89" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1715" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1715" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1715" s="89" t="s">
+        <v>3388</v>
+      </c>
+      <c r="I1715" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1716" s="90">
+        <v>1948</v>
+      </c>
+      <c r="B1716" s="1" t="s">
+        <v>3400</v>
+      </c>
+      <c r="C1716" s="90">
+        <v>5</v>
+      </c>
+      <c r="D1716" s="90" t="s">
+        <v>2809</v>
+      </c>
+      <c r="F1716" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1716" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1716" s="90" t="s">
+        <v>3402</v>
+      </c>
+      <c r="I1716" s="90" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1717" s="90">
+        <v>1955</v>
+      </c>
+      <c r="B1717" s="1" t="s">
+        <v>3399</v>
+      </c>
+      <c r="C1717" s="90">
+        <v>4</v>
+      </c>
+      <c r="D1717" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1717" s="90" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1717" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1717" s="90" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1717" s="90" t="s">
+        <v>3401</v>
+      </c>
+      <c r="I1717" s="90" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1718" s="90">
+        <v>1960</v>
+      </c>
+      <c r="B1718" s="1" t="s">
+        <v>3397</v>
+      </c>
+      <c r="C1718" s="90">
+        <v>6</v>
+      </c>
+      <c r="D1718" s="90" t="s">
+        <v>2809</v>
+      </c>
+      <c r="F1718" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1718" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1718" s="90" t="s">
+        <v>3398</v>
+      </c>
+      <c r="I1718" s="90" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1719" s="91" t="s">
         <v>1721</v>
       </c>
-      <c r="B1714" s="90"/>
-      <c r="C1714" s="90"/>
-      <c r="D1714" s="90"/>
-      <c r="E1714" s="90"/>
-      <c r="F1714" s="90"/>
-      <c r="G1714" s="90"/>
-      <c r="H1714" s="90"/>
-    </row>
-    <row r="1715" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1715" s="91" t="s">
+      <c r="B1719" s="91"/>
+      <c r="C1719" s="91"/>
+      <c r="D1719" s="91"/>
+      <c r="E1719" s="91"/>
+      <c r="F1719" s="91"/>
+      <c r="G1719" s="91"/>
+      <c r="H1719" s="91"/>
+    </row>
+    <row r="1720" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1720" s="92" t="s">
         <v>2759</v>
       </c>
-      <c r="B1715" s="91"/>
-      <c r="C1715" s="91"/>
-      <c r="D1715" s="91"/>
-      <c r="E1715" s="91"/>
-      <c r="F1715" s="91"/>
-      <c r="G1715" s="91"/>
-      <c r="H1715" s="91"/>
+      <c r="B1720" s="92"/>
+      <c r="C1720" s="92"/>
+      <c r="D1720" s="92"/>
+      <c r="E1720" s="92"/>
+      <c r="F1720" s="92"/>
+      <c r="G1720" s="92"/>
+      <c r="H1720" s="92"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1715" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1720" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1714:H1714"/>
-    <mergeCell ref="A1715:H1715"/>
+    <mergeCell ref="A1719:H1719"/>
+    <mergeCell ref="A1720:H1720"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -53301,9 +53538,9 @@
     <hyperlink ref="B1699" r:id="rId1464" display="https://leetcode.com/problems/largest-odd-number-in-string" xr:uid="{C1F070FE-5338-44D3-AC2F-454F2F234B37}"/>
     <hyperlink ref="B1700" r:id="rId1465" display="https://leetcode.com/problems/minimum-absolute-difference-queries" xr:uid="{BC2F4066-1A7C-40E6-807A-59A6290C5130}"/>
     <hyperlink ref="B1701" r:id="rId1466" xr:uid="{701B89CB-0972-4CC9-B496-BFC2EA4D6053}"/>
-    <hyperlink ref="B1702" r:id="rId1467" xr:uid="{8495B600-B833-4B44-9931-395989DBBB7D}"/>
-    <hyperlink ref="B1703" r:id="rId1468" display="https://leetcode.com/problems/cyclically-rotating-a-grid" xr:uid="{3AFFE1F3-E05C-4E5B-AB9D-548519408295}"/>
-    <hyperlink ref="B1704" r:id="rId1469" display=" Count Ways to Build Rooms in an Ant Colony" xr:uid="{E356F1D9-1378-42C3-B1EC-4016F02C08FE}"/>
+    <hyperlink ref="B1703" r:id="rId1467" xr:uid="{8495B600-B833-4B44-9931-395989DBBB7D}"/>
+    <hyperlink ref="B1704" r:id="rId1468" display="https://leetcode.com/problems/cyclically-rotating-a-grid" xr:uid="{3AFFE1F3-E05C-4E5B-AB9D-548519408295}"/>
+    <hyperlink ref="B1705" r:id="rId1469" display=" Count Ways to Build Rooms in an Ant Colony" xr:uid="{E356F1D9-1378-42C3-B1EC-4016F02C08FE}"/>
     <hyperlink ref="B1671" r:id="rId1470" xr:uid="{68B63B60-AA23-4767-8102-9AA46D58D32F}"/>
     <hyperlink ref="B1672" r:id="rId1471" display="https://leetcode.com/problems/finding-pairs-with-a-certain-sum" xr:uid="{37561B08-BC65-437E-B174-B127301F6D30}"/>
     <hyperlink ref="B1675" r:id="rId1472" display="https://leetcode.com/problems/minimum-speed-to-arrive-on-time" xr:uid="{544CF080-940E-4B3B-8C0D-B8C5A249310B}"/>
@@ -53316,20 +53553,27 @@
     <hyperlink ref="B1686" r:id="rId1479" display="https://leetcode.com/problems/egg-drop-with-2-eggs-and-n-floors" xr:uid="{8F3F40B0-8D67-46A7-B467-4EEA5B9A8063}"/>
     <hyperlink ref="B1688" r:id="rId1480" display="https://leetcode.com/problems/reduction-operations-to-make-the-array-elements-equal" xr:uid="{93CBEB02-546F-4B36-807B-CAA599C9C2E1}"/>
     <hyperlink ref="B1695" r:id="rId1481" display="https://leetcode.com/problems/redistribute-characters-to-make-all-strings-equal" xr:uid="{514AD256-6C6F-423E-93EA-68F73246AB3C}"/>
-    <hyperlink ref="B1705" r:id="rId1482" display="https://leetcode.com/problems/build-array-from-permutation" xr:uid="{A7BA82A2-3CCD-45FF-8CCB-DCE423A9403F}"/>
-    <hyperlink ref="B1706" r:id="rId1483" display="https://leetcode.com/problems/longest-common-subpath" xr:uid="{62FFD7C8-6B95-49CF-877E-D2923644D1FD}"/>
-    <hyperlink ref="B1707" r:id="rId1484" display="https://leetcode.com/problems/merge-bsts-to-create-single-bst" xr:uid="{3C90ED05-B4E6-4A5B-8B92-92274CD6E3CB}"/>
-    <hyperlink ref="B1709" r:id="rId1485" display="https://leetcode.com/problems/maximum-genetic-difference-query" xr:uid="{1A25DDAD-A0E9-4DEA-9978-DBF0F9D4D3DF}"/>
+    <hyperlink ref="B1706" r:id="rId1482" display="https://leetcode.com/problems/build-array-from-permutation" xr:uid="{A7BA82A2-3CCD-45FF-8CCB-DCE423A9403F}"/>
+    <hyperlink ref="B1707" r:id="rId1483" display="https://leetcode.com/problems/longest-common-subpath" xr:uid="{62FFD7C8-6B95-49CF-877E-D2923644D1FD}"/>
+    <hyperlink ref="B1710" r:id="rId1484" display="https://leetcode.com/problems/merge-bsts-to-create-single-bst" xr:uid="{3C90ED05-B4E6-4A5B-8B92-92274CD6E3CB}"/>
+    <hyperlink ref="B1712" r:id="rId1485" display="https://leetcode.com/problems/maximum-genetic-difference-query" xr:uid="{1A25DDAD-A0E9-4DEA-9978-DBF0F9D4D3DF}"/>
     <hyperlink ref="B1692" r:id="rId1486" display="https://leetcode.com/problems/find-the-student-that-will-replace-the-chalk" xr:uid="{9D146C0C-5A16-4375-BDF0-B60367842FF7}"/>
-    <hyperlink ref="B1713" r:id="rId1487" display="https://leetcode.com/problems/sum-of-digits-of-string-after-convert" xr:uid="{6F22ECDB-6A6B-41D3-8CA9-6D76CAF5B4E8}"/>
-    <hyperlink ref="B1712" r:id="rId1488" xr:uid="{67E882AF-68DB-41AF-8071-513205274BD9}"/>
-    <hyperlink ref="B1708" r:id="rId1489" display="https://leetcode.com/problems/maximum-number-of-words-you-can-type" xr:uid="{8E21FA9C-EBEA-4E91-AD8C-B9177EF763E8}"/>
+    <hyperlink ref="B1715" r:id="rId1487" display="https://leetcode.com/problems/sum-of-digits-of-string-after-convert" xr:uid="{6F22ECDB-6A6B-41D3-8CA9-6D76CAF5B4E8}"/>
+    <hyperlink ref="B1713" r:id="rId1488" xr:uid="{67E882AF-68DB-41AF-8071-513205274BD9}"/>
+    <hyperlink ref="B1711" r:id="rId1489" display="https://leetcode.com/problems/maximum-number-of-words-you-can-type" xr:uid="{8E21FA9C-EBEA-4E91-AD8C-B9177EF763E8}"/>
     <hyperlink ref="B1696" r:id="rId1490" xr:uid="{A3071BE6-0034-43AE-BDF8-5799BAD6EB13}"/>
     <hyperlink ref="B1697" r:id="rId1491" display="https://leetcode.com/problems/merge-triplets-to-form-target-triplet" xr:uid="{EFBBCE90-7311-45FC-B707-92A6E1252460}"/>
+    <hyperlink ref="B1718" r:id="rId1492" xr:uid="{B409B537-7A7A-463A-A75E-53528F8E2853}"/>
+    <hyperlink ref="B1717" r:id="rId1493" xr:uid="{02C2B215-E3E3-4548-A2F1-DDB689E2C454}"/>
+    <hyperlink ref="B1716" r:id="rId1494" display="https://leetcode.com/problems/delete-duplicate-folders-in-system" xr:uid="{16B4D03D-ED3A-423A-8036-4E96E3C16067}"/>
+    <hyperlink ref="B1714" r:id="rId1495" xr:uid="{7C979346-7740-4A52-9F7D-050A4F57896C}"/>
+    <hyperlink ref="B1709" r:id="rId1496" display="https://leetcode.com/problems/painting-a-grid-with-three-different-colors" xr:uid="{B5ED7AD1-6A0E-45F7-B1AC-3F3817E32416}"/>
+    <hyperlink ref="B1708" r:id="rId1497" display="Minimum Cost to Reach Destination i" xr:uid="{3D85BE5F-F0CC-42FF-A640-8A8AE91D07EA}"/>
+    <hyperlink ref="B1702" r:id="rId1498" display="https://leetcode.com/problems/design-movie-rental-system" xr:uid="{19AF9215-7A21-4D3F-A616-43F376496623}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1492"/>
-  <drawing r:id="rId1493"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1499"/>
+  <drawing r:id="rId1500"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in some easy problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A859DEA-C82F-4E40-9B32-77DEC2B310E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E3DDAD-0DED-4A0F-8DB4-21380D1AAE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1720</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1727</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9313" uniqueCount="3412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9358" uniqueCount="3426">
   <si>
     <t>Difficulty</t>
   </si>
@@ -10273,6 +10273,48 @@
   </si>
   <si>
     <t>Store movie in Sorted Tree Map by price, shop under hastable of moives</t>
+  </si>
+  <si>
+    <t>Concatenation of Array</t>
+  </si>
+  <si>
+    <t>Roundup indexes</t>
+  </si>
+  <si>
+    <t>Find a Peak Element II</t>
+  </si>
+  <si>
+    <t>Search neighbors higher than current</t>
+  </si>
+  <si>
+    <t>Count Sub Islands</t>
+  </si>
+  <si>
+    <t>BFS search for island</t>
+  </si>
+  <si>
+    <t>The Number of Full Rounds You Have Played</t>
+  </si>
+  <si>
+    <t>Round by quarter</t>
+  </si>
+  <si>
+    <t>Count Square Sum Triples</t>
+  </si>
+  <si>
+    <t>Loop first numbers with incremental order</t>
+  </si>
+  <si>
+    <t>Three Divisors</t>
+  </si>
+  <si>
+    <t>Find all divisors</t>
+  </si>
+  <si>
+    <t>Delete Characters to Make Fancy String</t>
+  </si>
+  <si>
+    <t>Count repeated characters</t>
   </si>
 </sst>
 </file>
@@ -10317,7 +10359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10344,6 +10386,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -10799,10 +10842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1720"/>
+  <dimension ref="A1:J1727"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1698" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1712" sqref="C1712"/>
+    <sheetView tabSelected="1" topLeftCell="A1700" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1725" sqref="A1725"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -51503,313 +51546,316 @@
         <v>3315</v>
       </c>
     </row>
-    <row r="1699" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1699" s="81">
-        <v>1903</v>
+    <row r="1699" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1699" s="91">
+        <v>1901</v>
       </c>
       <c r="B1699" s="1" t="s">
-        <v>3336</v>
-      </c>
-      <c r="C1699" s="81">
-        <v>1</v>
-      </c>
-      <c r="D1699" s="81" t="s">
-        <v>1717</v>
-      </c>
-      <c r="F1699" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1699" s="81" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1699" s="81" t="s">
-        <v>3337</v>
-      </c>
-      <c r="I1699" s="81" t="s">
+        <v>3414</v>
+      </c>
+      <c r="C1699" s="91">
+        <v>2</v>
+      </c>
+      <c r="D1699" s="91" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1699" s="91" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1699" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1699" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1699" s="91" t="s">
+        <v>3415</v>
+      </c>
+      <c r="I1699" s="91" t="s">
         <v>2999</v>
       </c>
     </row>
     <row r="1700" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1700" s="81">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="B1700" s="1" t="s">
-        <v>3338</v>
+        <v>3336</v>
       </c>
       <c r="C1700" s="81">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1700" s="81" t="s">
-        <v>2809</v>
+        <v>1717</v>
       </c>
       <c r="F1700" s="81" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1700" s="81" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1700" s="81" t="s">
+        <v>3337</v>
+      </c>
+      <c r="I1700" s="81" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1701" s="91">
+        <v>1904</v>
+      </c>
+      <c r="B1701" s="1" t="s">
+        <v>3418</v>
+      </c>
+      <c r="C1701" s="91">
+        <v>2</v>
+      </c>
+      <c r="D1701" s="91" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1701" s="91" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1701" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1701" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="H1700" s="81" t="s">
-        <v>3339</v>
-      </c>
-      <c r="I1700" s="81" t="s">
-        <v>3344</v>
-      </c>
-    </row>
-    <row r="1701" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1701" s="81">
-        <v>1909</v>
-      </c>
-      <c r="B1701" s="1" t="s">
-        <v>3340</v>
-      </c>
-      <c r="C1701" s="81">
+      <c r="H1701" s="91" t="s">
+        <v>3419</v>
+      </c>
+      <c r="I1701" s="91" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1702" s="91">
+        <v>1905</v>
+      </c>
+      <c r="B1702" s="1" t="s">
+        <v>3416</v>
+      </c>
+      <c r="C1702" s="91">
         <v>2</v>
       </c>
-      <c r="D1701" s="81" t="s">
-        <v>1767</v>
-      </c>
-      <c r="E1701" s="81" t="s">
-        <v>2934</v>
-      </c>
-      <c r="F1701" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1701" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1701" s="81" t="s">
-        <v>3341</v>
-      </c>
-      <c r="I1701" s="81" t="s">
+      <c r="D1702" s="91" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1702" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1702" s="91" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1702" s="91" t="s">
+        <v>3417</v>
+      </c>
+      <c r="I1702" s="91" t="s">
         <v>2999</v>
-      </c>
-    </row>
-    <row r="1702" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1702" s="90">
-        <v>1912</v>
-      </c>
-      <c r="B1702" s="1" t="s">
-        <v>3410</v>
-      </c>
-      <c r="C1702" s="90">
-        <v>4</v>
-      </c>
-      <c r="D1702" s="90" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1702" s="90" t="s">
-        <v>2923</v>
-      </c>
-      <c r="F1702" s="90" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1702" s="90" t="s">
-        <v>457</v>
-      </c>
-      <c r="H1702" s="90" t="s">
-        <v>3411</v>
-      </c>
-      <c r="I1702" s="90" t="s">
-        <v>3028</v>
       </c>
     </row>
     <row r="1703" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1703" s="81">
-        <v>1913</v>
+        <v>1906</v>
       </c>
       <c r="B1703" s="1" t="s">
-        <v>3342</v>
+        <v>3338</v>
       </c>
       <c r="C1703" s="81">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1703" s="81" t="s">
-        <v>1767</v>
+        <v>2809</v>
       </c>
       <c r="F1703" s="81" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1703" s="81" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="H1703" s="81" t="s">
-        <v>3343</v>
+        <v>3339</v>
       </c>
       <c r="I1703" s="81" t="s">
-        <v>2999</v>
+        <v>3344</v>
       </c>
     </row>
     <row r="1704" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1704" s="81">
-        <v>1914</v>
+        <v>1909</v>
       </c>
       <c r="B1704" s="1" t="s">
-        <v>3345</v>
+        <v>3340</v>
       </c>
       <c r="C1704" s="81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1704" s="81" t="s">
-        <v>1720</v>
+        <v>1767</v>
       </c>
       <c r="E1704" s="81" t="s">
         <v>2934</v>
       </c>
       <c r="F1704" s="81" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1704" s="81" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H1704" s="81" t="s">
-        <v>3347</v>
+        <v>3341</v>
       </c>
       <c r="I1704" s="81" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1705" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1705" s="81">
+    <row r="1705" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1705" s="90">
+        <v>1912</v>
+      </c>
+      <c r="B1705" s="1" t="s">
+        <v>3410</v>
+      </c>
+      <c r="C1705" s="90">
+        <v>4</v>
+      </c>
+      <c r="D1705" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1705" s="90" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1705" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1705" s="90" t="s">
+        <v>457</v>
+      </c>
+      <c r="H1705" s="90" t="s">
+        <v>3411</v>
+      </c>
+      <c r="I1705" s="90" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1706" s="81">
+        <v>1913</v>
+      </c>
+      <c r="B1706" s="1" t="s">
+        <v>3342</v>
+      </c>
+      <c r="C1706" s="81">
+        <v>2</v>
+      </c>
+      <c r="D1706" s="81" t="s">
+        <v>1767</v>
+      </c>
+      <c r="F1706" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1706" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1706" s="81" t="s">
+        <v>3343</v>
+      </c>
+      <c r="I1706" s="81" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1707" s="81">
+        <v>1914</v>
+      </c>
+      <c r="B1707" s="1" t="s">
+        <v>3345</v>
+      </c>
+      <c r="C1707" s="81">
+        <v>3</v>
+      </c>
+      <c r="D1707" s="81" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1707" s="81" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1707" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1707" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1707" s="81" t="s">
+        <v>3347</v>
+      </c>
+      <c r="I1707" s="81" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1708" s="81">
         <v>1916</v>
       </c>
-      <c r="B1705" s="1" t="s">
+      <c r="B1708" s="1" t="s">
         <v>3346</v>
       </c>
-      <c r="C1705" s="81">
+      <c r="C1708" s="81">
         <v>4</v>
       </c>
-      <c r="D1705" s="81" t="s">
+      <c r="D1708" s="81" t="s">
         <v>1718</v>
       </c>
-      <c r="F1705" s="81" t="s">
+      <c r="F1708" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="G1705" s="81" t="s">
+      <c r="G1708" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="H1705" s="81" t="s">
+      <c r="H1708" s="81" t="s">
         <v>3348</v>
       </c>
-      <c r="I1705" s="81" t="s">
+      <c r="I1708" s="81" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1706" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1706" s="88">
+    <row r="1709" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1709" s="88">
         <v>1920</v>
       </c>
-      <c r="B1706" s="1" t="s">
+      <c r="B1709" s="1" t="s">
         <v>3375</v>
       </c>
-      <c r="C1706" s="88">
+      <c r="C1709" s="88">
         <v>1</v>
       </c>
-      <c r="D1706" s="88" t="s">
+      <c r="D1709" s="88" t="s">
         <v>1767</v>
       </c>
-      <c r="F1706" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1706" s="88" t="s">
+      <c r="F1709" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1709" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="H1706" s="88" t="s">
+      <c r="H1709" s="88" t="s">
         <v>3376</v>
       </c>
-      <c r="I1706" s="88" t="s">
+      <c r="I1709" s="88" t="s">
         <v>2999</v>
-      </c>
-    </row>
-    <row r="1707" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1707" s="88">
-        <v>1923</v>
-      </c>
-      <c r="B1707" s="1" t="s">
-        <v>3377</v>
-      </c>
-      <c r="C1707" s="88">
-        <v>6</v>
-      </c>
-      <c r="D1707" s="88" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1707" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1707" s="88" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1707" s="88" t="s">
-        <v>3378</v>
-      </c>
-      <c r="I1707" s="88" t="s">
-        <v>3381</v>
-      </c>
-    </row>
-    <row r="1708" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1708" s="90">
-        <v>1928</v>
-      </c>
-      <c r="B1708" s="1" t="s">
-        <v>3407</v>
-      </c>
-      <c r="C1708" s="90">
-        <v>4</v>
-      </c>
-      <c r="D1708" s="90" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1708" s="90" t="s">
-        <v>2923</v>
-      </c>
-      <c r="F1708" s="90" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1708" s="90" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1708" s="90" t="s">
-        <v>3408</v>
-      </c>
-      <c r="I1708" s="90" t="s">
-        <v>3028</v>
-      </c>
-    </row>
-    <row r="1709" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1709" s="90">
-        <v>1931</v>
-      </c>
-      <c r="B1709" s="1" t="s">
-        <v>3405</v>
-      </c>
-      <c r="C1709" s="90">
-        <v>4</v>
-      </c>
-      <c r="D1709" s="90" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1709" s="90" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1709" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1709" s="90" t="s">
-        <v>3406</v>
-      </c>
-      <c r="I1709" s="90" t="s">
-        <v>3409</v>
       </c>
     </row>
     <row r="1710" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1710" s="88">
-        <v>1932</v>
+        <v>1923</v>
       </c>
       <c r="B1710" s="1" t="s">
-        <v>3379</v>
+        <v>3377</v>
       </c>
       <c r="C1710" s="88">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1710" s="88" t="s">
         <v>1720</v>
@@ -51818,99 +51864,102 @@
         <v>12</v>
       </c>
       <c r="G1710" s="88" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
       <c r="H1710" s="88" t="s">
-        <v>3380</v>
+        <v>3378</v>
       </c>
       <c r="I1710" s="88" t="s">
-        <v>2999</v>
-      </c>
-    </row>
-    <row r="1711" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1711" s="89">
-        <v>1935</v>
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1711" s="91">
+        <v>1925</v>
       </c>
       <c r="B1711" s="1" t="s">
-        <v>3391</v>
-      </c>
-      <c r="C1711" s="89">
-        <v>2</v>
-      </c>
-      <c r="D1711" s="89" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1711" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1711" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1711" s="89" t="s">
-        <v>3392</v>
-      </c>
-      <c r="I1711" s="89" t="s">
-        <v>2999</v>
-      </c>
-    </row>
-    <row r="1712" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1712" s="88">
-        <v>1938</v>
+        <v>3420</v>
+      </c>
+      <c r="C1711" s="91">
+        <v>1</v>
+      </c>
+      <c r="D1711" s="91" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1711" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1711" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1711" s="91" t="s">
+        <v>3421</v>
+      </c>
+      <c r="I1711" s="91" t="s">
+        <v>3184</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1712" s="90">
+        <v>1928</v>
       </c>
       <c r="B1712" s="1" t="s">
-        <v>3382</v>
-      </c>
-      <c r="C1712" s="88">
-        <v>6</v>
-      </c>
-      <c r="D1712" s="88" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1712" s="88" t="s">
+        <v>3407</v>
+      </c>
+      <c r="C1712" s="90">
+        <v>4</v>
+      </c>
+      <c r="D1712" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1712" s="90" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1712" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G1712" s="88" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1712" s="88" t="s">
-        <v>3383</v>
-      </c>
-      <c r="I1712" s="88" t="s">
-        <v>3178</v>
-      </c>
-    </row>
-    <row r="1713" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1713" s="89">
-        <v>1941</v>
+      <c r="G1712" s="90" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1712" s="90" t="s">
+        <v>3408</v>
+      </c>
+      <c r="I1712" s="90" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1713" s="91">
+        <v>1929</v>
       </c>
       <c r="B1713" s="1" t="s">
-        <v>3389</v>
-      </c>
-      <c r="C1713" s="89">
+        <v>3412</v>
+      </c>
+      <c r="C1713" s="91">
         <v>1</v>
       </c>
-      <c r="D1713" s="89" t="s">
+      <c r="D1713" s="91" t="s">
         <v>1717</v>
       </c>
-      <c r="F1713" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1713" s="89" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1713" s="89" t="s">
-        <v>3390</v>
-      </c>
-      <c r="I1713" s="89" t="s">
+      <c r="F1713" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1713" s="91" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1713" s="91" t="s">
+        <v>3413</v>
+      </c>
+      <c r="I1713" s="91" t="s">
         <v>2999</v>
       </c>
     </row>
     <row r="1714" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1714" s="90">
-        <v>1944</v>
+        <v>1931</v>
       </c>
       <c r="B1714" s="1" t="s">
-        <v>3403</v>
+        <v>3405</v>
       </c>
       <c r="C1714" s="90">
         <v>4</v>
@@ -51918,158 +51967,343 @@
       <c r="D1714" s="90" t="s">
         <v>1720</v>
       </c>
-      <c r="E1714" s="90" t="s">
-        <v>2923</v>
-      </c>
       <c r="F1714" s="90" t="s">
         <v>12</v>
       </c>
       <c r="G1714" s="90" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1714" s="90" t="s">
+        <v>3406</v>
+      </c>
+      <c r="I1714" s="90" t="s">
+        <v>3409</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1715" s="88">
+        <v>1932</v>
+      </c>
+      <c r="B1715" s="1" t="s">
+        <v>3379</v>
+      </c>
+      <c r="C1715" s="88">
+        <v>4</v>
+      </c>
+      <c r="D1715" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1715" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1715" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1715" s="88" t="s">
+        <v>3380</v>
+      </c>
+      <c r="I1715" s="88" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1716" s="89">
+        <v>1935</v>
+      </c>
+      <c r="B1716" s="1" t="s">
+        <v>3391</v>
+      </c>
+      <c r="C1716" s="89">
+        <v>2</v>
+      </c>
+      <c r="D1716" s="89" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1716" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1716" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="H1714" s="90" t="s">
+      <c r="H1716" s="89" t="s">
+        <v>3392</v>
+      </c>
+      <c r="I1716" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1717" s="88">
+        <v>1938</v>
+      </c>
+      <c r="B1717" s="1" t="s">
+        <v>3382</v>
+      </c>
+      <c r="C1717" s="88">
+        <v>6</v>
+      </c>
+      <c r="D1717" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1717" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1717" s="88" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1717" s="88" t="s">
+        <v>3383</v>
+      </c>
+      <c r="I1717" s="88" t="s">
+        <v>3178</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1718" s="89">
+        <v>1941</v>
+      </c>
+      <c r="B1718" s="1" t="s">
+        <v>3389</v>
+      </c>
+      <c r="C1718" s="89">
+        <v>1</v>
+      </c>
+      <c r="D1718" s="89" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1718" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1718" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1718" s="89" t="s">
+        <v>3390</v>
+      </c>
+      <c r="I1718" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1719" s="90">
+        <v>1944</v>
+      </c>
+      <c r="B1719" s="1" t="s">
+        <v>3403</v>
+      </c>
+      <c r="C1719" s="90">
+        <v>4</v>
+      </c>
+      <c r="D1719" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1719" s="90" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1719" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1719" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1719" s="90" t="s">
         <v>3404</v>
       </c>
-      <c r="I1714" s="90" t="s">
+      <c r="I1719" s="90" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1715" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1715" s="89">
+    <row r="1720" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1720" s="89">
         <v>1945</v>
       </c>
-      <c r="B1715" s="1" t="s">
+      <c r="B1720" s="1" t="s">
         <v>3387</v>
       </c>
-      <c r="C1715" s="89">
+      <c r="C1720" s="89">
         <v>1</v>
       </c>
-      <c r="D1715" s="89" t="s">
+      <c r="D1720" s="89" t="s">
         <v>1717</v>
       </c>
-      <c r="F1715" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1715" s="89" t="s">
+      <c r="F1720" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1720" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="H1715" s="89" t="s">
+      <c r="H1720" s="89" t="s">
         <v>3388</v>
       </c>
-      <c r="I1715" s="89" t="s">
+      <c r="I1720" s="89" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1716" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1716" s="90">
+    <row r="1721" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1721" s="90">
         <v>1948</v>
       </c>
-      <c r="B1716" s="1" t="s">
+      <c r="B1721" s="1" t="s">
         <v>3400</v>
       </c>
-      <c r="C1716" s="90">
-        <v>5</v>
-      </c>
-      <c r="D1716" s="90" t="s">
+      <c r="C1721" s="90">
+        <v>5</v>
+      </c>
+      <c r="D1721" s="90" t="s">
         <v>2809</v>
       </c>
-      <c r="F1716" s="90" t="s">
+      <c r="F1721" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G1716" s="90" t="s">
+      <c r="G1721" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="H1716" s="90" t="s">
+      <c r="H1721" s="90" t="s">
         <v>3402</v>
       </c>
-      <c r="I1716" s="90" t="s">
+      <c r="I1721" s="90" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1717" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1717" s="90">
+    <row r="1722" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1722" s="91">
+        <v>1952</v>
+      </c>
+      <c r="B1722" s="1" t="s">
+        <v>3422</v>
+      </c>
+      <c r="C1722" s="91">
+        <v>2</v>
+      </c>
+      <c r="D1722" s="91" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1722" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1722" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1722" s="91" t="s">
+        <v>3423</v>
+      </c>
+      <c r="I1722" s="91" t="s">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1723" s="90">
         <v>1955</v>
       </c>
-      <c r="B1717" s="1" t="s">
+      <c r="B1723" s="1" t="s">
         <v>3399</v>
       </c>
-      <c r="C1717" s="90">
+      <c r="C1723" s="90">
         <v>4</v>
       </c>
-      <c r="D1717" s="90" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1717" s="90" t="s">
+      <c r="D1723" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1723" s="90" t="s">
         <v>2934</v>
       </c>
-      <c r="F1717" s="90" t="s">
+      <c r="F1723" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G1717" s="90" t="s">
+      <c r="G1723" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="H1717" s="90" t="s">
+      <c r="H1723" s="90" t="s">
         <v>3401</v>
       </c>
-      <c r="I1717" s="90" t="s">
+      <c r="I1723" s="90" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1718" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1718" s="90">
+    <row r="1724" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1724" s="91">
+        <v>1957</v>
+      </c>
+      <c r="B1724" s="1" t="s">
+        <v>3424</v>
+      </c>
+      <c r="C1724" s="91">
+        <v>2</v>
+      </c>
+      <c r="D1724" s="91" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1724" s="91" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1724" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1724" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1724" s="91" t="s">
+        <v>3425</v>
+      </c>
+      <c r="I1724" s="91" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1725" s="90">
         <v>1960</v>
       </c>
-      <c r="B1718" s="1" t="s">
+      <c r="B1725" s="1" t="s">
         <v>3397</v>
       </c>
-      <c r="C1718" s="90">
+      <c r="C1725" s="90">
         <v>6</v>
       </c>
-      <c r="D1718" s="90" t="s">
+      <c r="D1725" s="90" t="s">
         <v>2809</v>
       </c>
-      <c r="F1718" s="90" t="s">
+      <c r="F1725" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G1718" s="90" t="s">
+      <c r="G1725" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="H1718" s="90" t="s">
+      <c r="H1725" s="90" t="s">
         <v>3398</v>
       </c>
-      <c r="I1718" s="90" t="s">
+      <c r="I1725" s="90" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1719" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1719" s="91" t="s">
+    <row r="1726" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1726" s="92" t="s">
         <v>1721</v>
       </c>
-      <c r="B1719" s="91"/>
-      <c r="C1719" s="91"/>
-      <c r="D1719" s="91"/>
-      <c r="E1719" s="91"/>
-      <c r="F1719" s="91"/>
-      <c r="G1719" s="91"/>
-      <c r="H1719" s="91"/>
-    </row>
-    <row r="1720" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1720" s="92" t="s">
+      <c r="B1726" s="92"/>
+      <c r="C1726" s="92"/>
+      <c r="D1726" s="92"/>
+      <c r="E1726" s="92"/>
+      <c r="F1726" s="92"/>
+      <c r="G1726" s="92"/>
+      <c r="H1726" s="92"/>
+    </row>
+    <row r="1727" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1727" s="93" t="s">
         <v>2759</v>
       </c>
-      <c r="B1720" s="92"/>
-      <c r="C1720" s="92"/>
-      <c r="D1720" s="92"/>
-      <c r="E1720" s="92"/>
-      <c r="F1720" s="92"/>
-      <c r="G1720" s="92"/>
-      <c r="H1720" s="92"/>
+      <c r="B1727" s="93"/>
+      <c r="C1727" s="93"/>
+      <c r="D1727" s="93"/>
+      <c r="E1727" s="93"/>
+      <c r="F1727" s="93"/>
+      <c r="G1727" s="93"/>
+      <c r="H1727" s="93"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1720" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1727" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1719:H1719"/>
-    <mergeCell ref="A1720:H1720"/>
+    <mergeCell ref="A1726:H1726"/>
+    <mergeCell ref="A1727:H1727"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -53535,12 +53769,12 @@
     <hyperlink ref="B1691" r:id="rId1461" display="https://leetcode.com/problems/check-if-all-the-integers-in-a-range-are-covered" xr:uid="{1E1CE91C-D79D-487A-A76A-6DE39C6CDD96}"/>
     <hyperlink ref="B1667" r:id="rId1462" display="https://leetcode.com/problems/incremental-memory-leak" xr:uid="{CA1A11F1-F4F6-4D65-9D69-A6197119EA1E}"/>
     <hyperlink ref="B1668" r:id="rId1463" display="https://leetcode.com/problems/rotating-the-box" xr:uid="{1DBA9A18-E1D2-4148-8C3A-048CE82287C0}"/>
-    <hyperlink ref="B1699" r:id="rId1464" display="https://leetcode.com/problems/largest-odd-number-in-string" xr:uid="{C1F070FE-5338-44D3-AC2F-454F2F234B37}"/>
-    <hyperlink ref="B1700" r:id="rId1465" display="https://leetcode.com/problems/minimum-absolute-difference-queries" xr:uid="{BC2F4066-1A7C-40E6-807A-59A6290C5130}"/>
-    <hyperlink ref="B1701" r:id="rId1466" xr:uid="{701B89CB-0972-4CC9-B496-BFC2EA4D6053}"/>
-    <hyperlink ref="B1703" r:id="rId1467" xr:uid="{8495B600-B833-4B44-9931-395989DBBB7D}"/>
-    <hyperlink ref="B1704" r:id="rId1468" display="https://leetcode.com/problems/cyclically-rotating-a-grid" xr:uid="{3AFFE1F3-E05C-4E5B-AB9D-548519408295}"/>
-    <hyperlink ref="B1705" r:id="rId1469" display=" Count Ways to Build Rooms in an Ant Colony" xr:uid="{E356F1D9-1378-42C3-B1EC-4016F02C08FE}"/>
+    <hyperlink ref="B1700" r:id="rId1464" display="https://leetcode.com/problems/largest-odd-number-in-string" xr:uid="{C1F070FE-5338-44D3-AC2F-454F2F234B37}"/>
+    <hyperlink ref="B1703" r:id="rId1465" display="https://leetcode.com/problems/minimum-absolute-difference-queries" xr:uid="{BC2F4066-1A7C-40E6-807A-59A6290C5130}"/>
+    <hyperlink ref="B1704" r:id="rId1466" xr:uid="{701B89CB-0972-4CC9-B496-BFC2EA4D6053}"/>
+    <hyperlink ref="B1706" r:id="rId1467" xr:uid="{8495B600-B833-4B44-9931-395989DBBB7D}"/>
+    <hyperlink ref="B1707" r:id="rId1468" display="https://leetcode.com/problems/cyclically-rotating-a-grid" xr:uid="{3AFFE1F3-E05C-4E5B-AB9D-548519408295}"/>
+    <hyperlink ref="B1708" r:id="rId1469" display=" Count Ways to Build Rooms in an Ant Colony" xr:uid="{E356F1D9-1378-42C3-B1EC-4016F02C08FE}"/>
     <hyperlink ref="B1671" r:id="rId1470" xr:uid="{68B63B60-AA23-4767-8102-9AA46D58D32F}"/>
     <hyperlink ref="B1672" r:id="rId1471" display="https://leetcode.com/problems/finding-pairs-with-a-certain-sum" xr:uid="{37561B08-BC65-437E-B174-B127301F6D30}"/>
     <hyperlink ref="B1675" r:id="rId1472" display="https://leetcode.com/problems/minimum-speed-to-arrive-on-time" xr:uid="{544CF080-940E-4B3B-8C0D-B8C5A249310B}"/>
@@ -53553,27 +53787,32 @@
     <hyperlink ref="B1686" r:id="rId1479" display="https://leetcode.com/problems/egg-drop-with-2-eggs-and-n-floors" xr:uid="{8F3F40B0-8D67-46A7-B467-4EEA5B9A8063}"/>
     <hyperlink ref="B1688" r:id="rId1480" display="https://leetcode.com/problems/reduction-operations-to-make-the-array-elements-equal" xr:uid="{93CBEB02-546F-4B36-807B-CAA599C9C2E1}"/>
     <hyperlink ref="B1695" r:id="rId1481" display="https://leetcode.com/problems/redistribute-characters-to-make-all-strings-equal" xr:uid="{514AD256-6C6F-423E-93EA-68F73246AB3C}"/>
-    <hyperlink ref="B1706" r:id="rId1482" display="https://leetcode.com/problems/build-array-from-permutation" xr:uid="{A7BA82A2-3CCD-45FF-8CCB-DCE423A9403F}"/>
-    <hyperlink ref="B1707" r:id="rId1483" display="https://leetcode.com/problems/longest-common-subpath" xr:uid="{62FFD7C8-6B95-49CF-877E-D2923644D1FD}"/>
-    <hyperlink ref="B1710" r:id="rId1484" display="https://leetcode.com/problems/merge-bsts-to-create-single-bst" xr:uid="{3C90ED05-B4E6-4A5B-8B92-92274CD6E3CB}"/>
-    <hyperlink ref="B1712" r:id="rId1485" display="https://leetcode.com/problems/maximum-genetic-difference-query" xr:uid="{1A25DDAD-A0E9-4DEA-9978-DBF0F9D4D3DF}"/>
+    <hyperlink ref="B1709" r:id="rId1482" display="https://leetcode.com/problems/build-array-from-permutation" xr:uid="{A7BA82A2-3CCD-45FF-8CCB-DCE423A9403F}"/>
+    <hyperlink ref="B1710" r:id="rId1483" display="https://leetcode.com/problems/longest-common-subpath" xr:uid="{62FFD7C8-6B95-49CF-877E-D2923644D1FD}"/>
+    <hyperlink ref="B1715" r:id="rId1484" display="https://leetcode.com/problems/merge-bsts-to-create-single-bst" xr:uid="{3C90ED05-B4E6-4A5B-8B92-92274CD6E3CB}"/>
+    <hyperlink ref="B1717" r:id="rId1485" display="https://leetcode.com/problems/maximum-genetic-difference-query" xr:uid="{1A25DDAD-A0E9-4DEA-9978-DBF0F9D4D3DF}"/>
     <hyperlink ref="B1692" r:id="rId1486" display="https://leetcode.com/problems/find-the-student-that-will-replace-the-chalk" xr:uid="{9D146C0C-5A16-4375-BDF0-B60367842FF7}"/>
-    <hyperlink ref="B1715" r:id="rId1487" display="https://leetcode.com/problems/sum-of-digits-of-string-after-convert" xr:uid="{6F22ECDB-6A6B-41D3-8CA9-6D76CAF5B4E8}"/>
-    <hyperlink ref="B1713" r:id="rId1488" xr:uid="{67E882AF-68DB-41AF-8071-513205274BD9}"/>
-    <hyperlink ref="B1711" r:id="rId1489" display="https://leetcode.com/problems/maximum-number-of-words-you-can-type" xr:uid="{8E21FA9C-EBEA-4E91-AD8C-B9177EF763E8}"/>
+    <hyperlink ref="B1720" r:id="rId1487" display="https://leetcode.com/problems/sum-of-digits-of-string-after-convert" xr:uid="{6F22ECDB-6A6B-41D3-8CA9-6D76CAF5B4E8}"/>
+    <hyperlink ref="B1718" r:id="rId1488" xr:uid="{67E882AF-68DB-41AF-8071-513205274BD9}"/>
+    <hyperlink ref="B1716" r:id="rId1489" display="https://leetcode.com/problems/maximum-number-of-words-you-can-type" xr:uid="{8E21FA9C-EBEA-4E91-AD8C-B9177EF763E8}"/>
     <hyperlink ref="B1696" r:id="rId1490" xr:uid="{A3071BE6-0034-43AE-BDF8-5799BAD6EB13}"/>
     <hyperlink ref="B1697" r:id="rId1491" display="https://leetcode.com/problems/merge-triplets-to-form-target-triplet" xr:uid="{EFBBCE90-7311-45FC-B707-92A6E1252460}"/>
-    <hyperlink ref="B1718" r:id="rId1492" xr:uid="{B409B537-7A7A-463A-A75E-53528F8E2853}"/>
-    <hyperlink ref="B1717" r:id="rId1493" xr:uid="{02C2B215-E3E3-4548-A2F1-DDB689E2C454}"/>
-    <hyperlink ref="B1716" r:id="rId1494" display="https://leetcode.com/problems/delete-duplicate-folders-in-system" xr:uid="{16B4D03D-ED3A-423A-8036-4E96E3C16067}"/>
-    <hyperlink ref="B1714" r:id="rId1495" xr:uid="{7C979346-7740-4A52-9F7D-050A4F57896C}"/>
-    <hyperlink ref="B1709" r:id="rId1496" display="https://leetcode.com/problems/painting-a-grid-with-three-different-colors" xr:uid="{B5ED7AD1-6A0E-45F7-B1AC-3F3817E32416}"/>
-    <hyperlink ref="B1708" r:id="rId1497" display="Minimum Cost to Reach Destination i" xr:uid="{3D85BE5F-F0CC-42FF-A640-8A8AE91D07EA}"/>
-    <hyperlink ref="B1702" r:id="rId1498" display="https://leetcode.com/problems/design-movie-rental-system" xr:uid="{19AF9215-7A21-4D3F-A616-43F376496623}"/>
+    <hyperlink ref="B1725" r:id="rId1492" xr:uid="{B409B537-7A7A-463A-A75E-53528F8E2853}"/>
+    <hyperlink ref="B1723" r:id="rId1493" xr:uid="{02C2B215-E3E3-4548-A2F1-DDB689E2C454}"/>
+    <hyperlink ref="B1721" r:id="rId1494" display="https://leetcode.com/problems/delete-duplicate-folders-in-system" xr:uid="{16B4D03D-ED3A-423A-8036-4E96E3C16067}"/>
+    <hyperlink ref="B1719" r:id="rId1495" xr:uid="{7C979346-7740-4A52-9F7D-050A4F57896C}"/>
+    <hyperlink ref="B1714" r:id="rId1496" display="https://leetcode.com/problems/painting-a-grid-with-three-different-colors" xr:uid="{B5ED7AD1-6A0E-45F7-B1AC-3F3817E32416}"/>
+    <hyperlink ref="B1712" r:id="rId1497" display="Minimum Cost to Reach Destination i" xr:uid="{3D85BE5F-F0CC-42FF-A640-8A8AE91D07EA}"/>
+    <hyperlink ref="B1705" r:id="rId1498" display="https://leetcode.com/problems/design-movie-rental-system" xr:uid="{19AF9215-7A21-4D3F-A616-43F376496623}"/>
+    <hyperlink ref="B1713" r:id="rId1499" display="https://leetcode.com/problems/concatenation-of-array" xr:uid="{4408C4DB-4EB9-4846-9A9D-74A69E6FC083}"/>
+    <hyperlink ref="B1702" r:id="rId1500" display="https://leetcode.com/problems/count-sub-islands" xr:uid="{618FF829-5060-41A7-93F8-CF7981307DFA}"/>
+    <hyperlink ref="B1701" r:id="rId1501" xr:uid="{3A86AED8-C09D-4BCF-A1D4-ADDD6E740309}"/>
+    <hyperlink ref="B1711" r:id="rId1502" display="https://leetcode.com/problems/count-square-sum-triples" xr:uid="{B8E45F4A-37F7-4057-AB54-687DAEB27C7E}"/>
+    <hyperlink ref="B1722" r:id="rId1503" display="https://leetcode.com/problems/three-divisors" xr:uid="{3D0A8A80-CBA1-408D-A123-C27B4A097F3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1499"/>
-  <drawing r:id="rId1500"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1504"/>
+  <drawing r:id="rId1505"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in SQL and easy problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E3DDAD-0DED-4A0F-8DB4-21380D1AAE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C537838-7937-4F4E-8210-D47C5BC6468E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Algorithm" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9358" uniqueCount="3426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9423" uniqueCount="3464">
   <si>
     <t>Difficulty</t>
   </si>
@@ -10315,6 +10315,120 @@
   </si>
   <si>
     <t>Count repeated characters</t>
+  </si>
+  <si>
+    <t>Leetcodify Similar Friends</t>
+  </si>
+  <si>
+    <t>Select common songs more than 3 and join with friendship</t>
+  </si>
+  <si>
+    <t>Users That Actively Request Confirmation Messages</t>
+  </si>
+  <si>
+    <t>Confirmation Rate</t>
+  </si>
+  <si>
+    <t>Confirmed count divided by total count</t>
+  </si>
+  <si>
+    <t>Self join with time1 &lt; time2 but time1 + 24h &gt;= time2.</t>
+  </si>
+  <si>
+    <t>Strong Friendship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self join with friend for common friend, exclude pair itself </t>
+  </si>
+  <si>
+    <t>All the Pairs With the Maximum Number of Common Followers</t>
+  </si>
+  <si>
+    <t>Self join with common friend and rank it.</t>
+  </si>
+  <si>
+    <t>Employees With Missing Information</t>
+  </si>
+  <si>
+    <t>Full outer join</t>
+  </si>
+  <si>
+    <t>First and Last Call On the Same Day</t>
+  </si>
+  <si>
+    <t>Sort asc and desc select first one on each day.</t>
+  </si>
+  <si>
+    <t>Employees Whose Manager Left the Company</t>
+  </si>
+  <si>
+    <t>Left join</t>
+  </si>
+  <si>
+    <t>Replace Employee ID With The Unique Identifier</t>
+  </si>
+  <si>
+    <t>Right Join</t>
+  </si>
+  <si>
+    <t>Total Sales Amount by Year</t>
+  </si>
+  <si>
+    <t>Calculate date range then join and cut</t>
+  </si>
+  <si>
+    <t>Capital Gain/Loss</t>
+  </si>
+  <si>
+    <t>Sort by row_number on by and sell, then join them.</t>
+  </si>
+  <si>
+    <t>Customers Who Bought Products A and B but Not C</t>
+  </si>
+  <si>
+    <t>Use operator IN</t>
+  </si>
+  <si>
+    <t>Leetcodify Friends Recommendations</t>
+  </si>
+  <si>
+    <t>Hopper Company Queries I</t>
+  </si>
+  <si>
+    <t>Calculate months and join with join date then join with acceptance</t>
+  </si>
+  <si>
+    <t>Hopper Company Queries II</t>
+  </si>
+  <si>
+    <t>Calculate months and join with join date then join with duration</t>
+  </si>
+  <si>
+    <t>Hopper Company Queries III</t>
+  </si>
+  <si>
+    <t>Count Salary Categories</t>
+  </si>
+  <si>
+    <t>Count salary range</t>
+  </si>
+  <si>
+    <t>Page Recommendations II</t>
+  </si>
+  <si>
+    <t>Friend Union join with likes</t>
+  </si>
+  <si>
+    <t>Top Travellers</t>
+  </si>
+  <si>
+    <t>Sum by rider</t>
+  </si>
+  <si>
+    <t>Find the Subtasks That Did Not Execute</t>
+  </si>
+  <si>
+    <t>Use values to get subtask id</t>
   </si>
 </sst>
 </file>
@@ -10359,7 +10473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10386,6 +10500,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -10844,7 +10959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1727"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1700" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A1700" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1725" sqref="A1725"/>
     </sheetView>
   </sheetViews>
@@ -52276,28 +52391,28 @@
       </c>
     </row>
     <row r="1726" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1726" s="92" t="s">
+      <c r="A1726" s="93" t="s">
         <v>1721</v>
       </c>
-      <c r="B1726" s="92"/>
-      <c r="C1726" s="92"/>
-      <c r="D1726" s="92"/>
-      <c r="E1726" s="92"/>
-      <c r="F1726" s="92"/>
-      <c r="G1726" s="92"/>
-      <c r="H1726" s="92"/>
+      <c r="B1726" s="93"/>
+      <c r="C1726" s="93"/>
+      <c r="D1726" s="93"/>
+      <c r="E1726" s="93"/>
+      <c r="F1726" s="93"/>
+      <c r="G1726" s="93"/>
+      <c r="H1726" s="93"/>
     </row>
     <row r="1727" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1727" s="93" t="s">
+      <c r="A1727" s="94" t="s">
         <v>2759</v>
       </c>
-      <c r="B1727" s="93"/>
-      <c r="C1727" s="93"/>
-      <c r="D1727" s="93"/>
-      <c r="E1727" s="93"/>
-      <c r="F1727" s="93"/>
-      <c r="G1727" s="93"/>
-      <c r="H1727" s="93"/>
+      <c r="B1727" s="94"/>
+      <c r="C1727" s="94"/>
+      <c r="D1727" s="94"/>
+      <c r="E1727" s="94"/>
+      <c r="F1727" s="94"/>
+      <c r="G1727" s="94"/>
+      <c r="H1727" s="94"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1727" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
@@ -53818,15 +53933,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01657D4-0457-4414-9EA3-8C4EB4AF3913}">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="49" customWidth="1"/>
+    <col min="2" max="2" width="52.265625" customWidth="1"/>
     <col min="3" max="4" width="9.19921875" style="26" customWidth="1"/>
     <col min="5" max="5" width="9.73046875" customWidth="1"/>
     <col min="6" max="6" width="54.46484375" customWidth="1"/>
@@ -53880,7 +53995,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>5</v>
@@ -54155,7 +54270,7 @@
         <v>4</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>12</v>
@@ -54175,7 +54290,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>9</v>
@@ -54195,7 +54310,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>12</v>
@@ -54283,7 +54398,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>9</v>
@@ -54558,7 +54673,7 @@
         <v>4</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>12</v>
@@ -54578,7 +54693,7 @@
         <v>4</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E43" s="26" t="s">
         <v>12</v>
@@ -54598,7 +54713,7 @@
         <v>3</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E44" s="26" t="s">
         <v>5</v>
@@ -54635,7 +54750,7 @@
         <v>3</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>1693</v>
+        <v>2923</v>
       </c>
       <c r="E46" s="26" t="s">
         <v>9</v>
@@ -54944,7 +55059,7 @@
         <v>3</v>
       </c>
       <c r="D64" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E64" s="26" t="s">
         <v>9</v>
@@ -54964,7 +55079,7 @@
         <v>4</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E65" s="26" t="s">
         <v>12</v>
@@ -55103,7 +55218,7 @@
         <v>3</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E73" s="26" t="s">
         <v>9</v>
@@ -55208,7 +55323,7 @@
         <v>3</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E79" s="26" t="s">
         <v>9</v>
@@ -55279,7 +55394,7 @@
         <v>5</v>
       </c>
       <c r="D83" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E83" s="26" t="s">
         <v>12</v>
@@ -55384,7 +55499,7 @@
         <v>4</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>1693</v>
+        <v>2934</v>
       </c>
       <c r="E89" s="26" t="s">
         <v>9</v>
@@ -55408,6 +55523,370 @@
       </c>
       <c r="F90" t="s">
         <v>2191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="92">
+        <v>1378</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>3442</v>
+      </c>
+      <c r="C92" s="92">
+        <v>1</v>
+      </c>
+      <c r="E92" s="92" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" s="92" t="s">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A93" s="92">
+        <v>1384</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>3444</v>
+      </c>
+      <c r="C93" s="92">
+        <v>4</v>
+      </c>
+      <c r="E93" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" s="92" t="s">
+        <v>3445</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A94" s="92">
+        <v>1393</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>3446</v>
+      </c>
+      <c r="C94" s="92">
+        <v>3</v>
+      </c>
+      <c r="D94" s="92" t="s">
+        <v>2934</v>
+      </c>
+      <c r="E94" s="92" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="92" t="s">
+        <v>3447</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A95" s="92">
+        <v>1398</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>3448</v>
+      </c>
+      <c r="C95" s="92">
+        <v>2</v>
+      </c>
+      <c r="D95" s="92" t="s">
+        <v>2934</v>
+      </c>
+      <c r="E95" s="92" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" s="92" t="s">
+        <v>3449</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A96" s="92">
+        <v>1407</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>3460</v>
+      </c>
+      <c r="C96" s="92">
+        <v>2</v>
+      </c>
+      <c r="E96" s="92" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96" s="92" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A97" s="92">
+        <v>1767</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>3462</v>
+      </c>
+      <c r="C97" s="92">
+        <v>4</v>
+      </c>
+      <c r="D97" s="92" t="s">
+        <v>2934</v>
+      </c>
+      <c r="E97" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" s="92" t="s">
+        <v>3463</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A99" s="92">
+        <v>1635</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>3451</v>
+      </c>
+      <c r="C99" s="92">
+        <v>5</v>
+      </c>
+      <c r="E99" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" s="92" t="s">
+        <v>3452</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A100" s="92">
+        <v>1645</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>3453</v>
+      </c>
+      <c r="C100" s="92">
+        <v>5</v>
+      </c>
+      <c r="E100" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" s="92" t="s">
+        <v>3454</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A101" s="92">
+        <v>1651</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>3455</v>
+      </c>
+      <c r="C101" s="92">
+        <v>5</v>
+      </c>
+      <c r="E101" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" s="92" t="s">
+        <v>3454</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A104" s="92">
+        <v>1892</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>3458</v>
+      </c>
+      <c r="C104" s="92">
+        <v>4</v>
+      </c>
+      <c r="E104" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104" s="92" t="s">
+        <v>3459</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A105" s="92">
+        <v>1907</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>3456</v>
+      </c>
+      <c r="C105" s="92">
+        <v>2</v>
+      </c>
+      <c r="E105" s="92" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" s="92" t="s">
+        <v>3457</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A106" s="92">
+        <v>1917</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>3450</v>
+      </c>
+      <c r="C106" s="92">
+        <v>4</v>
+      </c>
+      <c r="E106" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106" s="92" t="s">
+        <v>3427</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>1919</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>3426</v>
+      </c>
+      <c r="C107" s="26">
+        <v>4</v>
+      </c>
+      <c r="D107" s="26" t="s">
+        <v>2934</v>
+      </c>
+      <c r="E107" t="s">
+        <v>12</v>
+      </c>
+      <c r="F107" t="s">
+        <v>3427</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>1934</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>3429</v>
+      </c>
+      <c r="C108" s="26">
+        <v>2</v>
+      </c>
+      <c r="E108" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108" t="s">
+        <v>3430</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>1939</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>3428</v>
+      </c>
+      <c r="C109" s="26">
+        <v>2</v>
+      </c>
+      <c r="E109" t="s">
+        <v>5</v>
+      </c>
+      <c r="F109" t="s">
+        <v>3431</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>1949</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>3432</v>
+      </c>
+      <c r="C110" s="26">
+        <v>3</v>
+      </c>
+      <c r="D110" s="26" t="s">
+        <v>2934</v>
+      </c>
+      <c r="E110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" t="s">
+        <v>3433</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>1951</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>3434</v>
+      </c>
+      <c r="C111" s="26">
+        <v>3</v>
+      </c>
+      <c r="E111" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111" t="s">
+        <v>3435</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>1965</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>3436</v>
+      </c>
+      <c r="C112" s="26">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
+        <v>5</v>
+      </c>
+      <c r="F112" t="s">
+        <v>3437</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>1972</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>3438</v>
+      </c>
+      <c r="C113" s="26">
+        <v>4</v>
+      </c>
+      <c r="E113" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113" t="s">
+        <v>3439</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>1978</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>3440</v>
+      </c>
+      <c r="C114" s="26">
+        <v>2</v>
+      </c>
+      <c r="E114" t="s">
+        <v>9</v>
+      </c>
+      <c r="F114" t="s">
+        <v>3441</v>
       </c>
     </row>
   </sheetData>
@@ -55501,9 +55980,27 @@
     <hyperlink ref="B88" r:id="rId87" display="https://leetcode.com/problems/students-and-examinations" xr:uid="{2FF7198F-6469-4877-A49A-C76705A54BDB}"/>
     <hyperlink ref="B89" r:id="rId88" display="https://leetcode.com/problems/find-the-start-and-end-number-of-continuous-ranges" xr:uid="{93D84EE9-F4E0-4407-8E39-1C02175F5735}"/>
     <hyperlink ref="B90" r:id="rId89" display="https://leetcode.com/problems/weather-type-in-each-country" xr:uid="{E7B40668-DE2F-400B-9A62-2A66B2A30EF8}"/>
+    <hyperlink ref="B107" r:id="rId90" display="https://leetcode.com/problems/leetcodify-similar-friends" xr:uid="{31FC6E39-3A35-4FF6-8D5E-D880DD063AC4}"/>
+    <hyperlink ref="B108" r:id="rId91" display="https://leetcode.com/problems/confirmation-rate" xr:uid="{B57B6DFA-4A48-4708-AD19-2DCD85E441CC}"/>
+    <hyperlink ref="B109" r:id="rId92" xr:uid="{DAC9E0C9-5CB3-4ED6-91EF-0A2C851764FC}"/>
+    <hyperlink ref="B110" r:id="rId93" display="https://leetcode.com/problems/strong-friendship" xr:uid="{EFF9C5D4-F000-4FB3-8BB3-9F46BF776A2A}"/>
+    <hyperlink ref="B111" r:id="rId94" display="https://leetcode.com/problems/all-the-pairs-with-the-maximum-number-of-common-followers" xr:uid="{F7B4CE43-65EC-4468-8204-71D3A02EE015}"/>
+    <hyperlink ref="B112" r:id="rId95" display="https://leetcode.com/problems/employees-with-missing-information" xr:uid="{5477AE52-C753-4349-A154-EE4820F1F7DD}"/>
+    <hyperlink ref="B113" r:id="rId96" display="https://leetcode.com/problems/first-and-last-call-on-the-same-day" xr:uid="{B23F15FD-512C-4C2F-84C0-00849AB55923}"/>
+    <hyperlink ref="B114" r:id="rId97" xr:uid="{CD6AC747-121E-4A32-BE90-DDD55C170398}"/>
+    <hyperlink ref="B92" r:id="rId98" xr:uid="{8E793D3C-FBE6-49E6-87A9-DD428A609D40}"/>
+    <hyperlink ref="B93" r:id="rId99" display="https://leetcode.com/problems/total-sales-amount-by-year" xr:uid="{B59EE1B2-9413-4E48-96B1-D7DFD25D14EC}"/>
+    <hyperlink ref="B94" r:id="rId100" display="https://leetcode.com/problems/capital-gainloss" xr:uid="{7F22AD76-0A98-494C-8992-C0AAF0E043C0}"/>
+    <hyperlink ref="B95" r:id="rId101" display="https://leetcode.com/problems/customers-who-bought-products-a-and-b-but-not-c" xr:uid="{CF431385-0E27-46C1-B77B-D027B5927A1E}"/>
+    <hyperlink ref="B106" r:id="rId102" display="https://leetcode.com/problems/leetcodify-friends-recommendations" xr:uid="{B4798C0D-AA70-4BFE-9B96-80E02A492F2A}"/>
+    <hyperlink ref="B99" r:id="rId103" display="https://leetcode.com/problems/hopper-company-queries-i" xr:uid="{C1125A5B-1B89-401F-9E7F-78886D24DE33}"/>
+    <hyperlink ref="B100" r:id="rId104" display="https://leetcode.com/problems/hopper-company-queries-ii" xr:uid="{85FADCF8-4D22-420B-8FA3-CCD35E6692CA}"/>
+    <hyperlink ref="B104" r:id="rId105" display="https://leetcode.com/problems/page-recommendations-ii" xr:uid="{FB760DBC-1FAE-4F2C-B0D8-049AF3A16120}"/>
+    <hyperlink ref="B96" r:id="rId106" display="https://leetcode.com/problems/top-travellers" xr:uid="{0E265921-5208-498F-A406-6B4C2A7C080D}"/>
+    <hyperlink ref="B97" r:id="rId107" xr:uid="{6EF598F7-83DE-4CE7-BF66-DBF996C86CAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId90"/>
+  <pageSetup orientation="portrait" r:id="rId108"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in some hard problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C537838-7937-4F4E-8210-D47C5BC6468E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8FAF19-5D89-487E-8E43-54415C3AE481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Algorithm" sheetId="1" r:id="rId1"/>
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1727</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1799</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9423" uniqueCount="3464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9532" uniqueCount="3540">
   <si>
     <t>Difficulty</t>
   </si>
@@ -10429,6 +10429,234 @@
   </si>
   <si>
     <t>Use values to get subtask id</t>
+  </si>
+  <si>
+    <t>Remove All Occurrences of a Substring</t>
+  </si>
+  <si>
+    <t>Pop up target string</t>
+  </si>
+  <si>
+    <t>Maximum Alternating Subsequence Sum</t>
+  </si>
+  <si>
+    <t>Calculate current position as odd or even positions</t>
+  </si>
+  <si>
+    <t>Eliminate Maximum Number of Monsters</t>
+  </si>
+  <si>
+    <t>Count Good Numbers</t>
+  </si>
+  <si>
+    <t>Nearest Exit from Entrance in Maze</t>
+  </si>
+  <si>
+    <t>Sum Game</t>
+  </si>
+  <si>
+    <t>Unique Length-3 Palindromic Subsequences</t>
+  </si>
+  <si>
+    <t>Add Minimum Number of Rungs</t>
+  </si>
+  <si>
+    <t>Maximum Number of Points with Cost</t>
+  </si>
+  <si>
+    <t>The Number of the Smallest Unoccupied Chair</t>
+  </si>
+  <si>
+    <t>Describe the Painting</t>
+  </si>
+  <si>
+    <t>Largest Number After Mutating Substring</t>
+  </si>
+  <si>
+    <t>Maximum Compatibility Score Sum</t>
+  </si>
+  <si>
+    <t>Maximum Number of Weeks for Which You Can Work</t>
+  </si>
+  <si>
+    <t>Minimum Garden Perimeter to Collect Enough Apples</t>
+  </si>
+  <si>
+    <t>Check if Move is Legal</t>
+  </si>
+  <si>
+    <t>Minimum Total Space Wasted With K Resizing Operations</t>
+  </si>
+  <si>
+    <t>Check If String Is a Prefix of Array</t>
+  </si>
+  <si>
+    <t>Remove Stones to Minimize the Total</t>
+  </si>
+  <si>
+    <t>Minimum Number of Swaps to Make the String Balanced</t>
+  </si>
+  <si>
+    <t>Find the Longest Valid Obstacle Course at Each Position</t>
+  </si>
+  <si>
+    <t>Add words until reach the sentence size</t>
+  </si>
+  <si>
+    <t>Number of Strings That Appear as Substring</t>
+  </si>
+  <si>
+    <t>Array With Elements Not Equal to Average of Neighbors</t>
+  </si>
+  <si>
+    <t>Minimum Non-Zero Product of the Array Elements</t>
+  </si>
+  <si>
+    <t>Last Day Where You Can Still Cross</t>
+  </si>
+  <si>
+    <t>Find if Path Exists in Graph</t>
+  </si>
+  <si>
+    <t>Minimum Time to Type Word Using Special Typewriter</t>
+  </si>
+  <si>
+    <t>Maximum Matrix Sum</t>
+  </si>
+  <si>
+    <t>Number of Ways to Arrive at Destination</t>
+  </si>
+  <si>
+    <t>Number of Ways to Separate Numbers</t>
+  </si>
+  <si>
+    <t>Find Greatest Common Divisor of Array</t>
+  </si>
+  <si>
+    <t>Find Unique Binary String</t>
+  </si>
+  <si>
+    <t>Minimize the Difference Between Target and Chosen Elements</t>
+  </si>
+  <si>
+    <t>Find Array Given Subset Sums</t>
+  </si>
+  <si>
+    <t>Minimum Difference Between Highest and Lowest of K Scores</t>
+  </si>
+  <si>
+    <t>Find the Kth Largest Integer in the Array</t>
+  </si>
+  <si>
+    <t>Minimum Number of Work Sessions to Finish the Tasks</t>
+  </si>
+  <si>
+    <t>Number of Unique Good Subsequences</t>
+  </si>
+  <si>
+    <t>Find the Middle Index in Array</t>
+  </si>
+  <si>
+    <t>Find All Groups of Farmland</t>
+  </si>
+  <si>
+    <t>Operations on Tree</t>
+  </si>
+  <si>
+    <t>The Number of Good Subsets</t>
+  </si>
+  <si>
+    <t>Count Special Quadruplets</t>
+  </si>
+  <si>
+    <t>The Number of Weak Characters in the Game</t>
+  </si>
+  <si>
+    <t>GCD Sort of an Array</t>
+  </si>
+  <si>
+    <t>First Day Where You Have Been in All the Rooms</t>
+  </si>
+  <si>
+    <t>Reverse Prefix of Word</t>
+  </si>
+  <si>
+    <t>Number of Pairs of Interchangeable Rectangles</t>
+  </si>
+  <si>
+    <t>Maximum Product of the Length of Two Palindromic Subsequences</t>
+  </si>
+  <si>
+    <t>Smallest Missing Genetic Value in Each Subtree</t>
+  </si>
+  <si>
+    <t>Count Number of Pairs With Absolute Difference K</t>
+  </si>
+  <si>
+    <t>Find Original Array From Doubled Array</t>
+  </si>
+  <si>
+    <t>Maximum Earnings From Taxi</t>
+  </si>
+  <si>
+    <t>Minimum Number of Operations to Make Array Continuous</t>
+  </si>
+  <si>
+    <t>Final Value of Variable After Performing Operations</t>
+  </si>
+  <si>
+    <t>Sum of Beauty in the Array</t>
+  </si>
+  <si>
+    <t>Detect Squares</t>
+  </si>
+  <si>
+    <t>Longest Subsequence Repeated k Times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For subtree without node 1, the missing is 1, for others we track smallest seen node </t>
+  </si>
+  <si>
+    <t>Build up possible repeated target</t>
+  </si>
+  <si>
+    <t>26 ^ k (k&lt;7)</t>
+  </si>
+  <si>
+    <t>Maximum Difference Between Increasing Elements</t>
+  </si>
+  <si>
+    <t>Grid Game</t>
+  </si>
+  <si>
+    <t>Check if Word Can Be Placed In Crossword</t>
+  </si>
+  <si>
+    <t>The Score of Students Solving Math Expression</t>
+  </si>
+  <si>
+    <t>Convert 1D Array Into 2D Array</t>
+  </si>
+  <si>
+    <t>Number of Pairs of Strings With Concatenation Equal to Target</t>
+  </si>
+  <si>
+    <t>Maximize the Confusion of an Exam</t>
+  </si>
+  <si>
+    <t>Maximum Number of Ways to Partition an Array</t>
+  </si>
+  <si>
+    <t>Minimum Moves to Convert String</t>
+  </si>
+  <si>
+    <t>Find Missing Observations</t>
+  </si>
+  <si>
+    <t>Stone Game IX</t>
+  </si>
+  <si>
+    <t>Smallest K-Length Subsequence With Occurrences of a Letter</t>
   </si>
 </sst>
 </file>
@@ -10473,7 +10701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10571,6 +10799,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10957,10 +11190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1727"/>
+  <dimension ref="A1:J1799"/>
   <sheetViews>
-    <sheetView topLeftCell="A1700" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1725" sqref="A1725"/>
+    <sheetView tabSelected="1" topLeftCell="A1775" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1795" sqref="B1795"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -51826,599 +52059,1303 @@
         <v>2999</v>
       </c>
     </row>
-    <row r="1705" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1705" s="90">
+    <row r="1705" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1705" s="93">
+        <v>1910</v>
+      </c>
+      <c r="B1705" s="1" t="s">
+        <v>3464</v>
+      </c>
+      <c r="C1705" s="93">
+        <v>2</v>
+      </c>
+      <c r="D1705" s="93" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1705" s="93" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1705" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1705" s="93" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1705" s="93" t="s">
+        <v>3465</v>
+      </c>
+      <c r="I1705" s="93" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1706" s="93">
+        <v>1911</v>
+      </c>
+      <c r="B1706" s="1" t="s">
+        <v>3466</v>
+      </c>
+      <c r="C1706" s="93">
+        <v>3</v>
+      </c>
+      <c r="D1706" s="93" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1706" s="93" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1706" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1706" s="93" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1706" s="93" t="s">
+        <v>3467</v>
+      </c>
+      <c r="I1706" s="93" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1707" s="93">
         <v>1912</v>
       </c>
-      <c r="B1705" s="1" t="s">
+      <c r="B1707" s="1" t="s">
         <v>3410</v>
       </c>
-      <c r="C1705" s="90">
+      <c r="C1707" s="90">
         <v>4</v>
       </c>
-      <c r="D1705" s="90" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1705" s="90" t="s">
+      <c r="D1707" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1707" s="90" t="s">
         <v>2923</v>
       </c>
-      <c r="F1705" s="90" t="s">
+      <c r="F1707" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G1705" s="90" t="s">
+      <c r="G1707" s="90" t="s">
         <v>457</v>
       </c>
-      <c r="H1705" s="90" t="s">
+      <c r="H1707" s="90" t="s">
         <v>3411</v>
       </c>
-      <c r="I1705" s="90" t="s">
+      <c r="I1707" s="90" t="s">
         <v>3028</v>
-      </c>
-    </row>
-    <row r="1706" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1706" s="81">
-        <v>1913</v>
-      </c>
-      <c r="B1706" s="1" t="s">
-        <v>3342</v>
-      </c>
-      <c r="C1706" s="81">
-        <v>2</v>
-      </c>
-      <c r="D1706" s="81" t="s">
-        <v>1767</v>
-      </c>
-      <c r="F1706" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1706" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1706" s="81" t="s">
-        <v>3343</v>
-      </c>
-      <c r="I1706" s="81" t="s">
-        <v>2999</v>
-      </c>
-    </row>
-    <row r="1707" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1707" s="81">
-        <v>1914</v>
-      </c>
-      <c r="B1707" s="1" t="s">
-        <v>3345</v>
-      </c>
-      <c r="C1707" s="81">
-        <v>3</v>
-      </c>
-      <c r="D1707" s="81" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1707" s="81" t="s">
-        <v>2934</v>
-      </c>
-      <c r="F1707" s="81" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1707" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1707" s="81" t="s">
-        <v>3347</v>
-      </c>
-      <c r="I1707" s="81" t="s">
-        <v>2999</v>
       </c>
     </row>
     <row r="1708" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1708" s="81">
-        <v>1916</v>
+        <v>1913</v>
       </c>
       <c r="B1708" s="1" t="s">
-        <v>3346</v>
+        <v>3342</v>
       </c>
       <c r="C1708" s="81">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1708" s="81" t="s">
-        <v>1718</v>
+        <v>1767</v>
       </c>
       <c r="F1708" s="81" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G1708" s="81" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H1708" s="81" t="s">
-        <v>3348</v>
+        <v>3343</v>
       </c>
       <c r="I1708" s="81" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1709" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1709" s="88">
+    <row r="1709" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1709" s="81">
+        <v>1914</v>
+      </c>
+      <c r="B1709" s="1" t="s">
+        <v>3345</v>
+      </c>
+      <c r="C1709" s="81">
+        <v>3</v>
+      </c>
+      <c r="D1709" s="81" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1709" s="81" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1709" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1709" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1709" s="81" t="s">
+        <v>3347</v>
+      </c>
+      <c r="I1709" s="81" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:9" s="81" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1710" s="81">
+        <v>1916</v>
+      </c>
+      <c r="B1710" s="1" t="s">
+        <v>3346</v>
+      </c>
+      <c r="C1710" s="81">
+        <v>4</v>
+      </c>
+      <c r="D1710" s="81" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1710" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1710" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1710" s="81" t="s">
+        <v>3348</v>
+      </c>
+      <c r="I1710" s="81" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1711" s="88">
         <v>1920</v>
       </c>
-      <c r="B1709" s="1" t="s">
+      <c r="B1711" s="1" t="s">
         <v>3375</v>
       </c>
-      <c r="C1709" s="88">
+      <c r="C1711" s="88">
         <v>1</v>
       </c>
-      <c r="D1709" s="88" t="s">
+      <c r="D1711" s="88" t="s">
         <v>1767</v>
       </c>
-      <c r="F1709" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1709" s="88" t="s">
+      <c r="F1711" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1711" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="H1709" s="88" t="s">
+      <c r="H1711" s="88" t="s">
         <v>3376</v>
       </c>
-      <c r="I1709" s="88" t="s">
+      <c r="I1711" s="88" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1710" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1710" s="88">
+    <row r="1712" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1712" s="93">
+        <v>1921</v>
+      </c>
+      <c r="B1712" s="1" t="s">
+        <v>3468</v>
+      </c>
+      <c r="F1712" s="93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1713" s="93">
+        <v>1922</v>
+      </c>
+      <c r="B1713" s="1" t="s">
+        <v>3469</v>
+      </c>
+      <c r="F1713" s="93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1714" s="88">
         <v>1923</v>
       </c>
-      <c r="B1710" s="1" t="s">
+      <c r="B1714" s="1" t="s">
         <v>3377</v>
       </c>
-      <c r="C1710" s="88">
+      <c r="C1714" s="88">
         <v>6</v>
       </c>
-      <c r="D1710" s="88" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1710" s="88" t="s">
+      <c r="D1714" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1714" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="G1710" s="88" t="s">
+      <c r="G1714" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="H1710" s="88" t="s">
+      <c r="H1714" s="88" t="s">
         <v>3378</v>
       </c>
-      <c r="I1710" s="88" t="s">
+      <c r="I1714" s="88" t="s">
         <v>3381</v>
       </c>
     </row>
-    <row r="1711" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1711" s="91">
+    <row r="1715" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1715" s="91">
         <v>1925</v>
       </c>
-      <c r="B1711" s="1" t="s">
+      <c r="B1715" s="1" t="s">
         <v>3420</v>
       </c>
-      <c r="C1711" s="91">
+      <c r="C1715" s="91">
         <v>1</v>
       </c>
-      <c r="D1711" s="91" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1711" s="91" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1711" s="91" t="s">
+      <c r="D1715" s="91" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1715" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1715" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="H1711" s="91" t="s">
+      <c r="H1715" s="91" t="s">
         <v>3421</v>
       </c>
-      <c r="I1711" s="91" t="s">
+      <c r="I1715" s="91" t="s">
         <v>3184</v>
       </c>
     </row>
-    <row r="1712" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1712" s="90">
+    <row r="1716" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1716" s="93">
+        <v>1926</v>
+      </c>
+      <c r="B1716" s="1" t="s">
+        <v>3470</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1717" s="93">
+        <v>1927</v>
+      </c>
+      <c r="B1717" s="1" t="s">
+        <v>3471</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1718" s="90">
         <v>1928</v>
       </c>
-      <c r="B1712" s="1" t="s">
+      <c r="B1718" s="1" t="s">
         <v>3407</v>
       </c>
-      <c r="C1712" s="90">
+      <c r="C1718" s="90">
         <v>4</v>
       </c>
-      <c r="D1712" s="90" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1712" s="90" t="s">
+      <c r="D1718" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1718" s="90" t="s">
         <v>2923</v>
       </c>
-      <c r="F1712" s="90" t="s">
+      <c r="F1718" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G1712" s="90" t="s">
+      <c r="G1718" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="H1712" s="90" t="s">
+      <c r="H1718" s="90" t="s">
         <v>3408</v>
       </c>
-      <c r="I1712" s="90" t="s">
+      <c r="I1718" s="90" t="s">
         <v>3028</v>
       </c>
     </row>
-    <row r="1713" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1713" s="91">
+    <row r="1719" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1719" s="91">
         <v>1929</v>
       </c>
-      <c r="B1713" s="1" t="s">
+      <c r="B1719" s="1" t="s">
         <v>3412</v>
       </c>
-      <c r="C1713" s="91">
+      <c r="C1719" s="91">
         <v>1</v>
       </c>
-      <c r="D1713" s="91" t="s">
+      <c r="D1719" s="91" t="s">
         <v>1717</v>
       </c>
-      <c r="F1713" s="91" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1713" s="91" t="s">
+      <c r="F1719" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1719" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="H1713" s="91" t="s">
+      <c r="H1719" s="91" t="s">
         <v>3413</v>
       </c>
-      <c r="I1713" s="91" t="s">
+      <c r="I1719" s="91" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1714" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1714" s="90">
-        <v>1931</v>
-      </c>
-      <c r="B1714" s="1" t="s">
-        <v>3405</v>
-      </c>
-      <c r="C1714" s="90">
-        <v>4</v>
-      </c>
-      <c r="D1714" s="90" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1714" s="90" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1714" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1714" s="90" t="s">
-        <v>3406</v>
-      </c>
-      <c r="I1714" s="90" t="s">
-        <v>3409</v>
-      </c>
-    </row>
-    <row r="1715" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1715" s="88">
-        <v>1932</v>
-      </c>
-      <c r="B1715" s="1" t="s">
-        <v>3379</v>
-      </c>
-      <c r="C1715" s="88">
-        <v>4</v>
-      </c>
-      <c r="D1715" s="88" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1715" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1715" s="88" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1715" s="88" t="s">
-        <v>3380</v>
-      </c>
-      <c r="I1715" s="88" t="s">
-        <v>2999</v>
-      </c>
-    </row>
-    <row r="1716" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1716" s="89">
-        <v>1935</v>
-      </c>
-      <c r="B1716" s="1" t="s">
-        <v>3391</v>
-      </c>
-      <c r="C1716" s="89">
-        <v>2</v>
-      </c>
-      <c r="D1716" s="89" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1716" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1716" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1716" s="89" t="s">
-        <v>3392</v>
-      </c>
-      <c r="I1716" s="89" t="s">
-        <v>2999</v>
-      </c>
-    </row>
-    <row r="1717" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1717" s="88">
-        <v>1938</v>
-      </c>
-      <c r="B1717" s="1" t="s">
-        <v>3382</v>
-      </c>
-      <c r="C1717" s="88">
-        <v>6</v>
-      </c>
-      <c r="D1717" s="88" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1717" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1717" s="88" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1717" s="88" t="s">
-        <v>3383</v>
-      </c>
-      <c r="I1717" s="88" t="s">
-        <v>3178</v>
-      </c>
-    </row>
-    <row r="1718" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1718" s="89">
-        <v>1941</v>
-      </c>
-      <c r="B1718" s="1" t="s">
-        <v>3389</v>
-      </c>
-      <c r="C1718" s="89">
-        <v>1</v>
-      </c>
-      <c r="D1718" s="89" t="s">
-        <v>1717</v>
-      </c>
-      <c r="F1718" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1718" s="89" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1718" s="89" t="s">
-        <v>3390</v>
-      </c>
-      <c r="I1718" s="89" t="s">
-        <v>2999</v>
-      </c>
-    </row>
-    <row r="1719" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1719" s="90">
-        <v>1944</v>
-      </c>
-      <c r="B1719" s="1" t="s">
-        <v>3403</v>
-      </c>
-      <c r="C1719" s="90">
-        <v>4</v>
-      </c>
-      <c r="D1719" s="90" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1719" s="90" t="s">
-        <v>2923</v>
-      </c>
-      <c r="F1719" s="90" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1719" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1719" s="90" t="s">
-        <v>3404</v>
-      </c>
-      <c r="I1719" s="90" t="s">
-        <v>2999</v>
-      </c>
-    </row>
-    <row r="1720" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1720" s="89">
-        <v>1945</v>
+    <row r="1720" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1720" s="93">
+        <v>1930</v>
       </c>
       <c r="B1720" s="1" t="s">
-        <v>3387</v>
-      </c>
-      <c r="C1720" s="89">
-        <v>1</v>
-      </c>
-      <c r="D1720" s="89" t="s">
-        <v>1717</v>
-      </c>
-      <c r="F1720" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1720" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1720" s="89" t="s">
-        <v>3388</v>
-      </c>
-      <c r="I1720" s="89" t="s">
-        <v>2999</v>
+        <v>3472</v>
       </c>
     </row>
     <row r="1721" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1721" s="90">
-        <v>1948</v>
+        <v>1931</v>
       </c>
       <c r="B1721" s="1" t="s">
-        <v>3400</v>
+        <v>3405</v>
       </c>
       <c r="C1721" s="90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1721" s="90" t="s">
-        <v>2809</v>
+        <v>1720</v>
       </c>
       <c r="F1721" s="90" t="s">
         <v>12</v>
       </c>
       <c r="G1721" s="90" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1721" s="90" t="s">
+        <v>3406</v>
+      </c>
+      <c r="I1721" s="90" t="s">
+        <v>3409</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1722" s="88">
+        <v>1932</v>
+      </c>
+      <c r="B1722" s="1" t="s">
+        <v>3379</v>
+      </c>
+      <c r="C1722" s="88">
+        <v>4</v>
+      </c>
+      <c r="D1722" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1722" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1722" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1722" s="88" t="s">
+        <v>3380</v>
+      </c>
+      <c r="I1722" s="88" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1723" s="89">
+        <v>1935</v>
+      </c>
+      <c r="B1723" s="1" t="s">
+        <v>3391</v>
+      </c>
+      <c r="C1723" s="89">
+        <v>2</v>
+      </c>
+      <c r="D1723" s="89" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1723" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1723" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="H1721" s="90" t="s">
+      <c r="H1723" s="89" t="s">
+        <v>3392</v>
+      </c>
+      <c r="I1723" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1724" s="93">
+        <v>1936</v>
+      </c>
+      <c r="B1724" s="1" t="s">
+        <v>3473</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1725" s="93">
+        <v>1937</v>
+      </c>
+      <c r="B1725" s="1" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:9" s="88" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1726" s="88">
+        <v>1938</v>
+      </c>
+      <c r="B1726" s="1" t="s">
+        <v>3382</v>
+      </c>
+      <c r="C1726" s="88">
+        <v>6</v>
+      </c>
+      <c r="D1726" s="88" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1726" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1726" s="88" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1726" s="88" t="s">
+        <v>3383</v>
+      </c>
+      <c r="I1726" s="88" t="s">
+        <v>3178</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1727" s="89">
+        <v>1941</v>
+      </c>
+      <c r="B1727" s="1" t="s">
+        <v>3389</v>
+      </c>
+      <c r="C1727" s="89">
+        <v>1</v>
+      </c>
+      <c r="D1727" s="89" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1727" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1727" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1727" s="89" t="s">
+        <v>3390</v>
+      </c>
+      <c r="I1727" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1728" s="93">
+        <v>1942</v>
+      </c>
+      <c r="B1728" s="1" t="s">
+        <v>3475</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1729" s="93">
+        <v>1943</v>
+      </c>
+      <c r="B1729" s="1" t="s">
+        <v>3476</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1730" s="90">
+        <v>1944</v>
+      </c>
+      <c r="B1730" s="1" t="s">
+        <v>3403</v>
+      </c>
+      <c r="C1730" s="90">
+        <v>4</v>
+      </c>
+      <c r="D1730" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1730" s="90" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1730" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1730" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1730" s="90" t="s">
+        <v>3404</v>
+      </c>
+      <c r="I1730" s="90" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1731" s="89">
+        <v>1945</v>
+      </c>
+      <c r="B1731" s="1" t="s">
+        <v>3387</v>
+      </c>
+      <c r="C1731" s="89">
+        <v>1</v>
+      </c>
+      <c r="D1731" s="89" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1731" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1731" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1731" s="89" t="s">
+        <v>3388</v>
+      </c>
+      <c r="I1731" s="89" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1732" s="93">
+        <v>1946</v>
+      </c>
+      <c r="B1732" s="1" t="s">
+        <v>3477</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1733" s="93">
+        <v>1947</v>
+      </c>
+      <c r="B1733" s="1" t="s">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1734" s="90">
+        <v>1948</v>
+      </c>
+      <c r="B1734" s="1" t="s">
+        <v>3400</v>
+      </c>
+      <c r="C1734" s="90">
+        <v>5</v>
+      </c>
+      <c r="D1734" s="90" t="s">
+        <v>2809</v>
+      </c>
+      <c r="F1734" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1734" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1734" s="90" t="s">
         <v>3402</v>
       </c>
-      <c r="I1721" s="90" t="s">
+      <c r="I1734" s="90" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1722" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1722" s="91">
+    <row r="1735" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1735" s="91">
         <v>1952</v>
       </c>
-      <c r="B1722" s="1" t="s">
+      <c r="B1735" s="1" t="s">
         <v>3422</v>
       </c>
-      <c r="C1722" s="91">
+      <c r="C1735" s="91">
         <v>2</v>
       </c>
-      <c r="D1722" s="91" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F1722" s="91" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1722" s="91" t="s">
+      <c r="D1735" s="91" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1735" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1735" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="H1722" s="91" t="s">
+      <c r="H1735" s="91" t="s">
         <v>3423</v>
       </c>
-      <c r="I1722" s="91" t="s">
+      <c r="I1735" s="91" t="s">
         <v>3333</v>
       </c>
     </row>
-    <row r="1723" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1723" s="90">
+    <row r="1736" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1736" s="93">
+        <v>1953</v>
+      </c>
+      <c r="B1736" s="1" t="s">
+        <v>3479</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1737" s="93">
+        <v>1954</v>
+      </c>
+      <c r="B1737" s="1" t="s">
+        <v>3480</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1738" s="90">
         <v>1955</v>
       </c>
-      <c r="B1723" s="1" t="s">
+      <c r="B1738" s="1" t="s">
         <v>3399</v>
       </c>
-      <c r="C1723" s="90">
+      <c r="C1738" s="90">
         <v>4</v>
       </c>
-      <c r="D1723" s="90" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1723" s="90" t="s">
+      <c r="D1738" s="90" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1738" s="90" t="s">
         <v>2934</v>
       </c>
-      <c r="F1723" s="90" t="s">
+      <c r="F1738" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G1723" s="90" t="s">
+      <c r="G1738" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="H1723" s="90" t="s">
+      <c r="H1738" s="90" t="s">
         <v>3401</v>
       </c>
-      <c r="I1723" s="90" t="s">
+      <c r="I1738" s="90" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1724" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1724" s="91">
+    <row r="1739" spans="1:9" s="91" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1739" s="91">
         <v>1957</v>
       </c>
-      <c r="B1724" s="1" t="s">
+      <c r="B1739" s="1" t="s">
         <v>3424</v>
       </c>
-      <c r="C1724" s="91">
+      <c r="C1739" s="91">
         <v>2</v>
       </c>
-      <c r="D1724" s="91" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E1724" s="91" t="s">
+      <c r="D1739" s="91" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1739" s="91" t="s">
         <v>2934</v>
       </c>
-      <c r="F1724" s="91" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1724" s="91" t="s">
+      <c r="F1739" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1739" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="H1724" s="91" t="s">
+      <c r="H1739" s="91" t="s">
         <v>3425</v>
       </c>
-      <c r="I1724" s="91" t="s">
+      <c r="I1739" s="91" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1725" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1725" s="90">
+    <row r="1740" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1740" s="93">
+        <v>1958</v>
+      </c>
+      <c r="B1740" s="1" t="s">
+        <v>3481</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1741" s="93">
+        <v>1959</v>
+      </c>
+      <c r="B1741" s="1" t="s">
+        <v>3482</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:9" s="90" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1742" s="90">
         <v>1960</v>
       </c>
-      <c r="B1725" s="1" t="s">
+      <c r="B1742" s="1" t="s">
         <v>3397</v>
       </c>
-      <c r="C1725" s="90">
+      <c r="C1742" s="90">
         <v>6</v>
       </c>
-      <c r="D1725" s="90" t="s">
+      <c r="D1742" s="90" t="s">
         <v>2809</v>
       </c>
-      <c r="F1725" s="90" t="s">
+      <c r="F1742" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="G1725" s="90" t="s">
+      <c r="G1742" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="H1725" s="90" t="s">
+      <c r="H1742" s="90" t="s">
         <v>3398</v>
       </c>
-      <c r="I1725" s="90" t="s">
+      <c r="I1742" s="90" t="s">
         <v>2999</v>
       </c>
     </row>
-    <row r="1726" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1726" s="93" t="s">
+    <row r="1743" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1743" s="93">
+        <v>1961</v>
+      </c>
+      <c r="B1743" s="1" t="s">
+        <v>3483</v>
+      </c>
+      <c r="C1743" s="93">
+        <v>1</v>
+      </c>
+      <c r="D1743" s="93" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F1743" s="93" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1743" s="93" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1743" s="93" t="s">
+        <v>3487</v>
+      </c>
+      <c r="I1743" s="93" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1744" s="93">
+        <v>1962</v>
+      </c>
+      <c r="B1744" s="1" t="s">
+        <v>3484</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1745" s="93">
+        <v>1963</v>
+      </c>
+      <c r="B1745" s="1" t="s">
+        <v>3485</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1746" s="93">
+        <v>1964</v>
+      </c>
+      <c r="B1746" s="1" t="s">
+        <v>3486</v>
+      </c>
+      <c r="C1746" s="93">
+        <v>4</v>
+      </c>
+      <c r="D1746" s="93" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E1746" s="93" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1746" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1746" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1746" s="93" t="s">
+        <v>428</v>
+      </c>
+      <c r="I1746" s="93" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1747" s="93">
+        <v>1967</v>
+      </c>
+      <c r="B1747" s="1" t="s">
+        <v>3488</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1748" s="93">
+        <v>1968</v>
+      </c>
+      <c r="B1748" s="1" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1749" s="93">
+        <v>1969</v>
+      </c>
+      <c r="B1749" s="1" t="s">
+        <v>3490</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1750" s="93">
+        <v>1970</v>
+      </c>
+      <c r="B1750" s="1" t="s">
+        <v>3491</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1751" s="93">
+        <v>1971</v>
+      </c>
+      <c r="B1751" s="1" t="s">
+        <v>3492</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1752" s="93">
+        <v>1974</v>
+      </c>
+      <c r="B1752" s="1" t="s">
+        <v>3493</v>
+      </c>
+      <c r="C1752" s="93">
+        <v>2</v>
+      </c>
+      <c r="D1752" s="93" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E1752" s="93" t="s">
+        <v>2934</v>
+      </c>
+      <c r="F1752" s="93" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1752" s="93" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1753" s="93">
+        <v>1975</v>
+      </c>
+      <c r="B1753" s="1" t="s">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1754" s="93">
+        <v>1976</v>
+      </c>
+      <c r="B1754" s="1" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1755" s="93">
+        <v>1977</v>
+      </c>
+      <c r="B1755" s="1" t="s">
+        <v>3496</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1756" s="93">
+        <v>1979</v>
+      </c>
+      <c r="B1756" s="1" t="s">
+        <v>3497</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1757" s="93">
+        <v>1980</v>
+      </c>
+      <c r="B1757" s="1" t="s">
+        <v>3498</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1758" s="93">
+        <v>1981</v>
+      </c>
+      <c r="B1758" s="1" t="s">
+        <v>3499</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1759" s="93">
+        <v>1982</v>
+      </c>
+      <c r="B1759" s="1" t="s">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1760" s="93">
+        <v>1984</v>
+      </c>
+      <c r="B1760" s="1" t="s">
+        <v>3501</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1761" s="93">
+        <v>1985</v>
+      </c>
+      <c r="B1761" s="1" t="s">
+        <v>3502</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1762" s="93">
+        <v>1986</v>
+      </c>
+      <c r="B1762" s="1" t="s">
+        <v>3503</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1763" s="93">
+        <v>1987</v>
+      </c>
+      <c r="B1763" s="1" t="s">
+        <v>3504</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1764" s="93">
+        <v>1991</v>
+      </c>
+      <c r="B1764" s="1" t="s">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1765" s="93">
+        <v>1992</v>
+      </c>
+      <c r="B1765" s="1" t="s">
+        <v>3506</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1766" s="93">
+        <v>1993</v>
+      </c>
+      <c r="B1766" s="1" t="s">
+        <v>3507</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1767" s="93">
+        <v>1994</v>
+      </c>
+      <c r="B1767" s="1" t="s">
+        <v>3508</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1768" s="93">
+        <v>1995</v>
+      </c>
+      <c r="B1768" s="1" t="s">
+        <v>3509</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1769" s="93">
+        <v>1996</v>
+      </c>
+      <c r="B1769" s="1" t="s">
+        <v>3510</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1770" s="93">
+        <v>1997</v>
+      </c>
+      <c r="B1770" s="95" t="s">
+        <v>3512</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1771" s="93">
+        <v>1998</v>
+      </c>
+      <c r="B1771" s="1" t="s">
+        <v>3511</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1772" s="93">
+        <v>2000</v>
+      </c>
+      <c r="B1772" s="1" t="s">
+        <v>3513</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1773" s="93">
+        <v>2001</v>
+      </c>
+      <c r="B1773" s="1" t="s">
+        <v>3514</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1774" s="93">
+        <v>2002</v>
+      </c>
+      <c r="B1774" s="1" t="s">
+        <v>3515</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1775" s="93">
+        <v>2003</v>
+      </c>
+      <c r="B1775" s="1" t="s">
+        <v>3516</v>
+      </c>
+      <c r="C1775" s="93">
+        <v>4</v>
+      </c>
+      <c r="D1775" s="93" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1775" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1775" s="93" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1775" s="93" t="s">
+        <v>3525</v>
+      </c>
+      <c r="I1775" s="93" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1776" s="93">
+        <v>2006</v>
+      </c>
+      <c r="B1776" s="1" t="s">
+        <v>3517</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1777" s="93">
+        <v>2007</v>
+      </c>
+      <c r="B1777" s="1" t="s">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1778" s="93">
+        <v>2008</v>
+      </c>
+      <c r="B1778" s="1" t="s">
+        <v>3519</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1779" s="93">
+        <v>2009</v>
+      </c>
+      <c r="B1779" s="1" t="s">
+        <v>3520</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1780" s="93">
+        <v>2011</v>
+      </c>
+      <c r="B1780" s="1" t="s">
+        <v>3521</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1781" s="93">
+        <v>2012</v>
+      </c>
+      <c r="B1781" s="1" t="s">
+        <v>3522</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1782" s="93">
+        <v>2013</v>
+      </c>
+      <c r="B1782" s="1" t="s">
+        <v>3523</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1783" s="93">
+        <v>2014</v>
+      </c>
+      <c r="B1783" s="1" t="s">
+        <v>3524</v>
+      </c>
+      <c r="C1783" s="93">
+        <v>4</v>
+      </c>
+      <c r="D1783" s="93" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1783" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1783" s="93" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1783" s="93" t="s">
+        <v>3526</v>
+      </c>
+      <c r="I1783" s="93" t="s">
+        <v>3527</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1784" s="94">
+        <v>2016</v>
+      </c>
+      <c r="B1784" s="1" t="s">
+        <v>3528</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1785" s="94">
+        <v>2017</v>
+      </c>
+      <c r="B1785" s="1" t="s">
+        <v>3529</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1786" s="94">
+        <v>2018</v>
+      </c>
+      <c r="B1786" s="1" t="s">
+        <v>3530</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1787" s="94">
+        <v>2019</v>
+      </c>
+      <c r="B1787" s="95" t="s">
+        <v>3531</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1788" s="94">
+        <v>2022</v>
+      </c>
+      <c r="B1788" s="1" t="s">
+        <v>3532</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1789" s="94">
+        <v>2023</v>
+      </c>
+      <c r="B1789" s="95" t="s">
+        <v>3533</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1790" s="94">
+        <v>2024</v>
+      </c>
+      <c r="B1790" s="1" t="s">
+        <v>3534</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1791" s="94">
+        <v>2025</v>
+      </c>
+      <c r="B1791" s="95" t="s">
+        <v>3535</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1792" s="94">
+        <v>2027</v>
+      </c>
+      <c r="B1792" s="1" t="s">
+        <v>3536</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:8" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1793" s="94">
+        <v>2028</v>
+      </c>
+      <c r="B1793" s="1" t="s">
+        <v>3537</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:8" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1794" s="94">
+        <v>2029</v>
+      </c>
+      <c r="B1794" s="1" t="s">
+        <v>3538</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:8" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1795" s="94">
+        <v>2030</v>
+      </c>
+      <c r="B1795" s="95" t="s">
+        <v>3539</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:8" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1796" s="1"/>
+    </row>
+    <row r="1797" spans="1:8" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1797" s="1"/>
+    </row>
+    <row r="1798" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1798" s="96" t="s">
         <v>1721</v>
       </c>
-      <c r="B1726" s="93"/>
-      <c r="C1726" s="93"/>
-      <c r="D1726" s="93"/>
-      <c r="E1726" s="93"/>
-      <c r="F1726" s="93"/>
-      <c r="G1726" s="93"/>
-      <c r="H1726" s="93"/>
-    </row>
-    <row r="1727" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1727" s="94" t="s">
+      <c r="B1798" s="96"/>
+      <c r="C1798" s="96"/>
+      <c r="D1798" s="96"/>
+      <c r="E1798" s="96"/>
+      <c r="F1798" s="96"/>
+      <c r="G1798" s="96"/>
+      <c r="H1798" s="96"/>
+    </row>
+    <row r="1799" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1799" s="97" t="s">
         <v>2759</v>
       </c>
-      <c r="B1727" s="94"/>
-      <c r="C1727" s="94"/>
-      <c r="D1727" s="94"/>
-      <c r="E1727" s="94"/>
-      <c r="F1727" s="94"/>
-      <c r="G1727" s="94"/>
-      <c r="H1727" s="94"/>
+      <c r="B1799" s="97"/>
+      <c r="C1799" s="97"/>
+      <c r="D1799" s="97"/>
+      <c r="E1799" s="97"/>
+      <c r="F1799" s="97"/>
+      <c r="G1799" s="97"/>
+      <c r="H1799" s="97"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1727" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1799" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1726:H1726"/>
-    <mergeCell ref="A1727:H1727"/>
+    <mergeCell ref="A1798:H1798"/>
+    <mergeCell ref="A1799:H1799"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -53887,9 +54824,9 @@
     <hyperlink ref="B1700" r:id="rId1464" display="https://leetcode.com/problems/largest-odd-number-in-string" xr:uid="{C1F070FE-5338-44D3-AC2F-454F2F234B37}"/>
     <hyperlink ref="B1703" r:id="rId1465" display="https://leetcode.com/problems/minimum-absolute-difference-queries" xr:uid="{BC2F4066-1A7C-40E6-807A-59A6290C5130}"/>
     <hyperlink ref="B1704" r:id="rId1466" xr:uid="{701B89CB-0972-4CC9-B496-BFC2EA4D6053}"/>
-    <hyperlink ref="B1706" r:id="rId1467" xr:uid="{8495B600-B833-4B44-9931-395989DBBB7D}"/>
-    <hyperlink ref="B1707" r:id="rId1468" display="https://leetcode.com/problems/cyclically-rotating-a-grid" xr:uid="{3AFFE1F3-E05C-4E5B-AB9D-548519408295}"/>
-    <hyperlink ref="B1708" r:id="rId1469" display=" Count Ways to Build Rooms in an Ant Colony" xr:uid="{E356F1D9-1378-42C3-B1EC-4016F02C08FE}"/>
+    <hyperlink ref="B1708" r:id="rId1467" xr:uid="{8495B600-B833-4B44-9931-395989DBBB7D}"/>
+    <hyperlink ref="B1709" r:id="rId1468" display="https://leetcode.com/problems/cyclically-rotating-a-grid" xr:uid="{3AFFE1F3-E05C-4E5B-AB9D-548519408295}"/>
+    <hyperlink ref="B1710" r:id="rId1469" display=" Count Ways to Build Rooms in an Ant Colony" xr:uid="{E356F1D9-1378-42C3-B1EC-4016F02C08FE}"/>
     <hyperlink ref="B1671" r:id="rId1470" xr:uid="{68B63B60-AA23-4767-8102-9AA46D58D32F}"/>
     <hyperlink ref="B1672" r:id="rId1471" display="https://leetcode.com/problems/finding-pairs-with-a-certain-sum" xr:uid="{37561B08-BC65-437E-B174-B127301F6D30}"/>
     <hyperlink ref="B1675" r:id="rId1472" display="https://leetcode.com/problems/minimum-speed-to-arrive-on-time" xr:uid="{544CF080-940E-4B3B-8C0D-B8C5A249310B}"/>
@@ -53902,32 +54839,102 @@
     <hyperlink ref="B1686" r:id="rId1479" display="https://leetcode.com/problems/egg-drop-with-2-eggs-and-n-floors" xr:uid="{8F3F40B0-8D67-46A7-B467-4EEA5B9A8063}"/>
     <hyperlink ref="B1688" r:id="rId1480" display="https://leetcode.com/problems/reduction-operations-to-make-the-array-elements-equal" xr:uid="{93CBEB02-546F-4B36-807B-CAA599C9C2E1}"/>
     <hyperlink ref="B1695" r:id="rId1481" display="https://leetcode.com/problems/redistribute-characters-to-make-all-strings-equal" xr:uid="{514AD256-6C6F-423E-93EA-68F73246AB3C}"/>
-    <hyperlink ref="B1709" r:id="rId1482" display="https://leetcode.com/problems/build-array-from-permutation" xr:uid="{A7BA82A2-3CCD-45FF-8CCB-DCE423A9403F}"/>
-    <hyperlink ref="B1710" r:id="rId1483" display="https://leetcode.com/problems/longest-common-subpath" xr:uid="{62FFD7C8-6B95-49CF-877E-D2923644D1FD}"/>
-    <hyperlink ref="B1715" r:id="rId1484" display="https://leetcode.com/problems/merge-bsts-to-create-single-bst" xr:uid="{3C90ED05-B4E6-4A5B-8B92-92274CD6E3CB}"/>
-    <hyperlink ref="B1717" r:id="rId1485" display="https://leetcode.com/problems/maximum-genetic-difference-query" xr:uid="{1A25DDAD-A0E9-4DEA-9978-DBF0F9D4D3DF}"/>
+    <hyperlink ref="B1711" r:id="rId1482" display="https://leetcode.com/problems/build-array-from-permutation" xr:uid="{A7BA82A2-3CCD-45FF-8CCB-DCE423A9403F}"/>
+    <hyperlink ref="B1714" r:id="rId1483" display="https://leetcode.com/problems/longest-common-subpath" xr:uid="{62FFD7C8-6B95-49CF-877E-D2923644D1FD}"/>
+    <hyperlink ref="B1722" r:id="rId1484" display="https://leetcode.com/problems/merge-bsts-to-create-single-bst" xr:uid="{3C90ED05-B4E6-4A5B-8B92-92274CD6E3CB}"/>
+    <hyperlink ref="B1726" r:id="rId1485" display="https://leetcode.com/problems/maximum-genetic-difference-query" xr:uid="{1A25DDAD-A0E9-4DEA-9978-DBF0F9D4D3DF}"/>
     <hyperlink ref="B1692" r:id="rId1486" display="https://leetcode.com/problems/find-the-student-that-will-replace-the-chalk" xr:uid="{9D146C0C-5A16-4375-BDF0-B60367842FF7}"/>
-    <hyperlink ref="B1720" r:id="rId1487" display="https://leetcode.com/problems/sum-of-digits-of-string-after-convert" xr:uid="{6F22ECDB-6A6B-41D3-8CA9-6D76CAF5B4E8}"/>
-    <hyperlink ref="B1718" r:id="rId1488" xr:uid="{67E882AF-68DB-41AF-8071-513205274BD9}"/>
-    <hyperlink ref="B1716" r:id="rId1489" display="https://leetcode.com/problems/maximum-number-of-words-you-can-type" xr:uid="{8E21FA9C-EBEA-4E91-AD8C-B9177EF763E8}"/>
+    <hyperlink ref="B1731" r:id="rId1487" display="https://leetcode.com/problems/sum-of-digits-of-string-after-convert" xr:uid="{6F22ECDB-6A6B-41D3-8CA9-6D76CAF5B4E8}"/>
+    <hyperlink ref="B1727" r:id="rId1488" xr:uid="{67E882AF-68DB-41AF-8071-513205274BD9}"/>
+    <hyperlink ref="B1723" r:id="rId1489" display="https://leetcode.com/problems/maximum-number-of-words-you-can-type" xr:uid="{8E21FA9C-EBEA-4E91-AD8C-B9177EF763E8}"/>
     <hyperlink ref="B1696" r:id="rId1490" xr:uid="{A3071BE6-0034-43AE-BDF8-5799BAD6EB13}"/>
     <hyperlink ref="B1697" r:id="rId1491" display="https://leetcode.com/problems/merge-triplets-to-form-target-triplet" xr:uid="{EFBBCE90-7311-45FC-B707-92A6E1252460}"/>
-    <hyperlink ref="B1725" r:id="rId1492" xr:uid="{B409B537-7A7A-463A-A75E-53528F8E2853}"/>
-    <hyperlink ref="B1723" r:id="rId1493" xr:uid="{02C2B215-E3E3-4548-A2F1-DDB689E2C454}"/>
-    <hyperlink ref="B1721" r:id="rId1494" display="https://leetcode.com/problems/delete-duplicate-folders-in-system" xr:uid="{16B4D03D-ED3A-423A-8036-4E96E3C16067}"/>
-    <hyperlink ref="B1719" r:id="rId1495" xr:uid="{7C979346-7740-4A52-9F7D-050A4F57896C}"/>
-    <hyperlink ref="B1714" r:id="rId1496" display="https://leetcode.com/problems/painting-a-grid-with-three-different-colors" xr:uid="{B5ED7AD1-6A0E-45F7-B1AC-3F3817E32416}"/>
-    <hyperlink ref="B1712" r:id="rId1497" display="Minimum Cost to Reach Destination i" xr:uid="{3D85BE5F-F0CC-42FF-A640-8A8AE91D07EA}"/>
-    <hyperlink ref="B1705" r:id="rId1498" display="https://leetcode.com/problems/design-movie-rental-system" xr:uid="{19AF9215-7A21-4D3F-A616-43F376496623}"/>
-    <hyperlink ref="B1713" r:id="rId1499" display="https://leetcode.com/problems/concatenation-of-array" xr:uid="{4408C4DB-4EB9-4846-9A9D-74A69E6FC083}"/>
+    <hyperlink ref="B1742" r:id="rId1492" xr:uid="{B409B537-7A7A-463A-A75E-53528F8E2853}"/>
+    <hyperlink ref="B1738" r:id="rId1493" xr:uid="{02C2B215-E3E3-4548-A2F1-DDB689E2C454}"/>
+    <hyperlink ref="B1734" r:id="rId1494" display="https://leetcode.com/problems/delete-duplicate-folders-in-system" xr:uid="{16B4D03D-ED3A-423A-8036-4E96E3C16067}"/>
+    <hyperlink ref="B1730" r:id="rId1495" xr:uid="{7C979346-7740-4A52-9F7D-050A4F57896C}"/>
+    <hyperlink ref="B1721" r:id="rId1496" display="https://leetcode.com/problems/painting-a-grid-with-three-different-colors" xr:uid="{B5ED7AD1-6A0E-45F7-B1AC-3F3817E32416}"/>
+    <hyperlink ref="B1718" r:id="rId1497" display="Minimum Cost to Reach Destination i" xr:uid="{3D85BE5F-F0CC-42FF-A640-8A8AE91D07EA}"/>
+    <hyperlink ref="B1707" r:id="rId1498" display="https://leetcode.com/problems/design-movie-rental-system" xr:uid="{19AF9215-7A21-4D3F-A616-43F376496623}"/>
+    <hyperlink ref="B1719" r:id="rId1499" display="https://leetcode.com/problems/concatenation-of-array" xr:uid="{4408C4DB-4EB9-4846-9A9D-74A69E6FC083}"/>
     <hyperlink ref="B1702" r:id="rId1500" display="https://leetcode.com/problems/count-sub-islands" xr:uid="{618FF829-5060-41A7-93F8-CF7981307DFA}"/>
     <hyperlink ref="B1701" r:id="rId1501" xr:uid="{3A86AED8-C09D-4BCF-A1D4-ADDD6E740309}"/>
-    <hyperlink ref="B1711" r:id="rId1502" display="https://leetcode.com/problems/count-square-sum-triples" xr:uid="{B8E45F4A-37F7-4057-AB54-687DAEB27C7E}"/>
-    <hyperlink ref="B1722" r:id="rId1503" display="https://leetcode.com/problems/three-divisors" xr:uid="{3D0A8A80-CBA1-408D-A123-C27B4A097F3A}"/>
+    <hyperlink ref="B1715" r:id="rId1502" display="https://leetcode.com/problems/count-square-sum-triples" xr:uid="{B8E45F4A-37F7-4057-AB54-687DAEB27C7E}"/>
+    <hyperlink ref="B1735" r:id="rId1503" display="https://leetcode.com/problems/three-divisors" xr:uid="{3D0A8A80-CBA1-408D-A123-C27B4A097F3A}"/>
+    <hyperlink ref="B1705" r:id="rId1504" display="https://leetcode.com/problems/remove-all-occurrences-of-a-substring" xr:uid="{1FD774A7-EA6E-486E-B5B2-4DB1A2CAD603}"/>
+    <hyperlink ref="B1706" r:id="rId1505" display="https://leetcode.com/problems/maximum-alternating-subsequence-sum" xr:uid="{FD99D4AE-DB21-4402-8FA7-0B910189496A}"/>
+    <hyperlink ref="B1712" r:id="rId1506" display="https://leetcode.com/problems/eliminate-maximum-number-of-monsters" xr:uid="{2F2B9E94-63AD-422B-9A63-FD6F7EE7C629}"/>
+    <hyperlink ref="B1713" r:id="rId1507" display="https://leetcode.com/problems/count-good-numbers" xr:uid="{0D5DDF79-C46F-494C-9766-0E840A482CBC}"/>
+    <hyperlink ref="B1716" r:id="rId1508" display="https://leetcode.com/problems/nearest-exit-from-entrance-in-maze" xr:uid="{D6319B8E-5A12-491E-9CED-BE4A97644B7D}"/>
+    <hyperlink ref="B1717" r:id="rId1509" display="https://leetcode.com/problems/sum-game" xr:uid="{7257B159-3AAE-49C8-A194-28A7B0536879}"/>
+    <hyperlink ref="B1720" r:id="rId1510" display="https://leetcode.com/problems/unique-length-3-palindromic-subsequences" xr:uid="{3E328985-E0C1-4515-AD87-7AEBCA16FAC1}"/>
+    <hyperlink ref="B1724" r:id="rId1511" display="https://leetcode.com/problems/add-minimum-number-of-rungs" xr:uid="{5BA1D979-BF40-48B3-A017-A1F66313C277}"/>
+    <hyperlink ref="B1725" r:id="rId1512" display="https://leetcode.com/problems/maximum-number-of-points-with-cost" xr:uid="{046C6A21-E955-49B6-9C89-B84CCB55AE5A}"/>
+    <hyperlink ref="B1728" r:id="rId1513" xr:uid="{6CD14534-BD2F-4FB2-9ED6-FA0B3F435F34}"/>
+    <hyperlink ref="B1729" r:id="rId1514" display="https://leetcode.com/problems/describe-the-painting" xr:uid="{DA3A709A-251A-4B40-A861-28FC5064A859}"/>
+    <hyperlink ref="B1732" r:id="rId1515" display="https://leetcode.com/problems/largest-number-after-mutating-substring" xr:uid="{4886B7BF-B766-44D2-92F9-16172E855E7A}"/>
+    <hyperlink ref="B1733" r:id="rId1516" display="https://leetcode.com/problems/maximum-compatibility-score-sum" xr:uid="{6AA7EF38-CB22-4349-9BCA-68EEDB6BA60F}"/>
+    <hyperlink ref="B1736" r:id="rId1517" xr:uid="{780DD737-38FC-4E52-8E17-E1ED7D4828C2}"/>
+    <hyperlink ref="B1737" r:id="rId1518" xr:uid="{BD5305FA-C3E6-436C-A3A3-3B2AEC015409}"/>
+    <hyperlink ref="B1740" r:id="rId1519" display="https://leetcode.com/problems/check-if-move-is-legal" xr:uid="{037D07CA-C5E5-46F7-8A15-FF086FD68CEA}"/>
+    <hyperlink ref="B1741" r:id="rId1520" xr:uid="{4514D26A-1DEB-4898-B0C0-E35C803A917D}"/>
+    <hyperlink ref="B1743" r:id="rId1521" display="https://leetcode.com/problems/check-if-string-is-a-prefix-of-array" xr:uid="{ED238B07-DD69-47D7-9C99-70206F56431B}"/>
+    <hyperlink ref="B1744" r:id="rId1522" display="https://leetcode.com/problems/remove-stones-to-minimize-the-total" xr:uid="{A477D00D-45DD-4A17-8EC1-CAB601E47AFE}"/>
+    <hyperlink ref="B1745" r:id="rId1523" xr:uid="{7AED54AB-CAC5-468D-AEA4-30EF78C123D5}"/>
+    <hyperlink ref="B1746" r:id="rId1524" xr:uid="{C8B643C6-E285-4944-9FD0-0F3F95420C77}"/>
+    <hyperlink ref="B1747" r:id="rId1525" display="https://leetcode.com/problems/number-of-strings-that-appear-as-substrings-in-word" xr:uid="{9D135439-6404-469A-B0F3-B3CB3CC48006}"/>
+    <hyperlink ref="B1748" r:id="rId1526" xr:uid="{2D13F7E0-CA9F-41A5-9A27-D14C8E89D1D6}"/>
+    <hyperlink ref="B1749" r:id="rId1527" xr:uid="{6F03E324-C26B-45D0-A69E-667D05BCF4A6}"/>
+    <hyperlink ref="B1750" r:id="rId1528" display="https://leetcode.com/problems/last-day-where-you-can-still-cross" xr:uid="{6C0C733A-DFFC-47C4-8A74-549CE9EEC902}"/>
+    <hyperlink ref="B1751" r:id="rId1529" display="https://leetcode.com/problems/find-if-path-exists-in-graph" xr:uid="{280D74AA-F965-40BB-989B-D14BCDFED54C}"/>
+    <hyperlink ref="B1752" r:id="rId1530" xr:uid="{4E722A0F-0542-4D0F-944F-81A1882BDB67}"/>
+    <hyperlink ref="B1753" r:id="rId1531" display="https://leetcode.com/problems/maximum-matrix-sum" xr:uid="{85554A11-E7CC-4623-9832-CA974B90C2B5}"/>
+    <hyperlink ref="B1754" r:id="rId1532" display="https://leetcode.com/problems/number-of-ways-to-arrive-at-destination" xr:uid="{7C2B1C34-BFA8-4D6A-8BFD-2D13258003E9}"/>
+    <hyperlink ref="B1755" r:id="rId1533" display="https://leetcode.com/problems/number-of-ways-to-separate-numbers" xr:uid="{A1CD6E14-B30D-48A8-9C50-989B50718C66}"/>
+    <hyperlink ref="B1756" r:id="rId1534" display="https://leetcode.com/problems/find-greatest-common-divisor-of-array" xr:uid="{F13EAFBC-B285-401C-91EE-AC9A939A3669}"/>
+    <hyperlink ref="B1757" r:id="rId1535" display="https://leetcode.com/problems/find-unique-binary-string" xr:uid="{7ED88115-1A51-43E5-9996-61390F3D3742}"/>
+    <hyperlink ref="B1758" r:id="rId1536" xr:uid="{307A70C2-1A17-4713-8815-4B08BE79BC16}"/>
+    <hyperlink ref="B1759" r:id="rId1537" display="https://leetcode.com/problems/find-array-given-subset-sums" xr:uid="{24E810D6-01EB-4D57-B971-B9D6AD7C8465}"/>
+    <hyperlink ref="B1760" r:id="rId1538" xr:uid="{3AC2DE31-2D9A-47A8-BD4F-9E1BA94A6DBE}"/>
+    <hyperlink ref="B1761" r:id="rId1539" display="https://leetcode.com/problems/find-the-kth-largest-integer-in-the-array" xr:uid="{0E5050F7-33DD-4568-A9C5-F0BF63ABEF41}"/>
+    <hyperlink ref="B1762" r:id="rId1540" xr:uid="{74CBB63A-C6EA-4857-9FF1-DE3E60CAE238}"/>
+    <hyperlink ref="B1763" r:id="rId1541" display="https://leetcode.com/problems/number-of-unique-good-subsequences" xr:uid="{853BAECC-5442-42F3-89D7-4E811047F33B}"/>
+    <hyperlink ref="B1764" r:id="rId1542" display="https://leetcode.com/problems/find-the-middle-index-in-array" xr:uid="{D5BD54BC-4C9D-4080-92AB-7E0AD5447197}"/>
+    <hyperlink ref="B1765" r:id="rId1543" display="https://leetcode.com/problems/find-all-groups-of-farmland" xr:uid="{FA8829D0-40F2-4ECC-B6CF-DF0CB80F6744}"/>
+    <hyperlink ref="B1766" r:id="rId1544" display="https://leetcode.com/problems/operations-on-tree" xr:uid="{686B754D-FA97-4909-9B6F-604722737483}"/>
+    <hyperlink ref="B1767" r:id="rId1545" display="https://leetcode.com/problems/the-number-of-good-subsets" xr:uid="{CB7AE48D-6C96-4D56-9DD1-F6A59CF37370}"/>
+    <hyperlink ref="B1768" r:id="rId1546" display="https://leetcode.com/problems/count-special-quadruplets" xr:uid="{661C9BC6-DD29-4EEE-BDF8-A0046C960AAA}"/>
+    <hyperlink ref="B1769" r:id="rId1547" xr:uid="{4367FE0D-6B66-4E7B-B67D-D44932CCF53D}"/>
+    <hyperlink ref="B1771" r:id="rId1548" display="https://leetcode.com/problems/gcd-sort-of-an-array" xr:uid="{D51FF9FA-E1D0-4876-9671-0BECACA20C8E}"/>
+    <hyperlink ref="B1770" r:id="rId1549" xr:uid="{440A2BB5-BF04-43D0-B17E-3DB556DFF3D2}"/>
+    <hyperlink ref="B1772" r:id="rId1550" display="https://leetcode.com/problems/reverse-prefix-of-word" xr:uid="{CB9978C3-6422-40BB-8564-3202082A0B1A}"/>
+    <hyperlink ref="B1773" r:id="rId1551" xr:uid="{7923A955-AD8E-4813-A991-8D8A22CAA454}"/>
+    <hyperlink ref="B1774" r:id="rId1552" display="https://leetcode.com/problems/maximum-product-of-the-length-of-two-palindromic-subsequences" xr:uid="{8F9B0876-A47C-4346-BB3A-B28A932D0561}"/>
+    <hyperlink ref="B1775" r:id="rId1553" display="https://leetcode.com/problems/smallest-missing-genetic-value-in-each-subtree" xr:uid="{7B841850-C4EB-4B17-86ED-3C469EA47416}"/>
+    <hyperlink ref="B1776" r:id="rId1554" xr:uid="{8B9BFB7A-1876-405D-81AE-5D45D7B9CC99}"/>
+    <hyperlink ref="B1777" r:id="rId1555" display="https://leetcode.com/problems/find-original-array-from-doubled-array" xr:uid="{941F4524-2AB9-4B82-8506-2B0DDAE8E0C8}"/>
+    <hyperlink ref="B1778" r:id="rId1556" display="https://leetcode.com/problems/maximum-earnings-from-taxi" xr:uid="{2C7D8613-3F51-4CE1-89B7-0D2175417F32}"/>
+    <hyperlink ref="B1779" r:id="rId1557" display="https://leetcode.com/problems/minimum-number-of-operations-to-make-array-continuous" xr:uid="{7CA9A60C-BA8C-481E-B3A3-B022E1E11E93}"/>
+    <hyperlink ref="B1780" r:id="rId1558" display="https://leetcode.com/problems/final-value-of-variable-after-performing-operations" xr:uid="{878BB048-0ECD-4FAC-A96B-1A705EB95DEF}"/>
+    <hyperlink ref="B1781" r:id="rId1559" display="https://leetcode.com/problems/sum-of-beauty-in-the-array" xr:uid="{73619F0E-5E06-4E41-906A-4E0AE98A22B5}"/>
+    <hyperlink ref="B1782" r:id="rId1560" display="https://leetcode.com/problems/detect-squares" xr:uid="{973708F6-B02C-4F3B-9CD7-658CC285620D}"/>
+    <hyperlink ref="B1783" r:id="rId1561" display="https://leetcode.com/problems/longest-subsequence-repeated-k-times" xr:uid="{4C762D87-A9C5-4BD4-912E-7DF86A9410E2}"/>
+    <hyperlink ref="B1784" r:id="rId1562" xr:uid="{FCD62007-CC5B-42E2-9137-1D08C11A57E4}"/>
+    <hyperlink ref="B1785" r:id="rId1563" display="https://leetcode.com/problems/grid-game" xr:uid="{6BAF02C7-CF0B-4611-97F7-71B80B95A205}"/>
+    <hyperlink ref="B1786" r:id="rId1564" display="https://leetcode.com/problems/check-if-word-can-be-placed-in-crossword" xr:uid="{302A26FF-631E-42F2-9B60-01DDABC35248}"/>
+    <hyperlink ref="B1787" r:id="rId1565" display="https://leetcode.com/problems/the-score-of-students-solving-math-expression" xr:uid="{3D10BE58-1B14-440E-9A39-40F0A7CCC3A0}"/>
+    <hyperlink ref="B1788" r:id="rId1566" display="https://leetcode.com/problems/convert-1d-array-into-2d-array" xr:uid="{412ED7EE-16C1-4FBE-88AA-44300DC61B17}"/>
+    <hyperlink ref="B1789" r:id="rId1567" display="https://leetcode.com/problems/number-of-pairs-of-strings-with-concatenation-equal-to-target" xr:uid="{EDEDBE97-30D3-4D23-9530-0C8A3F620EE6}"/>
+    <hyperlink ref="B1790" r:id="rId1568" display="https://leetcode.com/problems/maximize-the-confusion-of-an-exam" xr:uid="{B38DEE78-20CA-494E-8F19-7DDF232265F7}"/>
+    <hyperlink ref="B1791" r:id="rId1569" display="https://leetcode.com/problems/maximum-number-of-ways-to-partition-an-array" xr:uid="{327D7573-701B-491A-A079-084FB4CF6A48}"/>
+    <hyperlink ref="B1792" r:id="rId1570" display="https://leetcode.com/problems/minimum-moves-to-convert-string" xr:uid="{560091BE-B96B-42CB-A09B-F78B509005A6}"/>
+    <hyperlink ref="B1793" r:id="rId1571" display="https://leetcode.com/problems/find-missing-observations" xr:uid="{9490467D-B31C-44AF-8D15-79AB6781FC3C}"/>
+    <hyperlink ref="B1794" r:id="rId1572" display="https://leetcode.com/problems/stone-game-ix" xr:uid="{C7AA6D81-752C-425D-81DA-FAF27F7ED6FA}"/>
+    <hyperlink ref="B1795" r:id="rId1573" display="https://leetcode.com/problems/smallest-k-length-subsequence-with-occurrences-of-a-letter" xr:uid="{A5C04344-98FD-4F50-9D84-0FBA98FAC48B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1504"/>
-  <drawing r:id="rId1505"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1574"/>
+  <drawing r:id="rId1575"/>
 </worksheet>
 </file>
 
@@ -53935,7 +54942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01657D4-0457-4414-9EA3-8C4EB4AF3913}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
check in 2004 and 2010 SQL problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8FAF19-5D89-487E-8E43-54415C3AE481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917A5B8E-FFBE-40F2-9797-88A7E6F60959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Algorithm" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9532" uniqueCount="3540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9538" uniqueCount="3543">
   <si>
     <t>Difficulty</t>
   </si>
@@ -10657,6 +10657,15 @@
   </si>
   <si>
     <t>Smallest K-Length Subsequence With Occurrences of a Letter</t>
+  </si>
+  <si>
+    <t>The Number of Seniors and Juniors to Join the Company</t>
+  </si>
+  <si>
+    <t>The Number of Seniors and Juniors to Join the Company II</t>
+  </si>
+  <si>
+    <t>Rank salary by experience and self join with sum</t>
   </si>
 </sst>
 </file>
@@ -11192,7 +11201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1799"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1775" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A1775" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1795" sqref="B1795"/>
     </sheetView>
   </sheetViews>
@@ -54940,10 +54949,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01657D4-0457-4414-9EA3-8C4EB4AF3913}">
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="F116" sqref="F116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -56894,6 +56903,40 @@
       </c>
       <c r="F114" t="s">
         <v>3441</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>2004</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>3540</v>
+      </c>
+      <c r="C115" s="26">
+        <v>4</v>
+      </c>
+      <c r="E115" t="s">
+        <v>12</v>
+      </c>
+      <c r="F115" t="s">
+        <v>3542</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>2010</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>3541</v>
+      </c>
+      <c r="C116" s="26">
+        <v>4</v>
+      </c>
+      <c r="E116" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116" t="s">
+        <v>3542</v>
       </c>
     </row>
   </sheetData>
@@ -57005,9 +57048,11 @@
     <hyperlink ref="B104" r:id="rId105" display="https://leetcode.com/problems/page-recommendations-ii" xr:uid="{FB760DBC-1FAE-4F2C-B0D8-049AF3A16120}"/>
     <hyperlink ref="B96" r:id="rId106" display="https://leetcode.com/problems/top-travellers" xr:uid="{0E265921-5208-498F-A406-6B4C2A7C080D}"/>
     <hyperlink ref="B97" r:id="rId107" xr:uid="{6EF598F7-83DE-4CE7-BF66-DBF996C86CAA}"/>
+    <hyperlink ref="B115" r:id="rId108" display="https://leetcode.com/problems/the-number-of-seniors-and-juniors-to-join-the-company" xr:uid="{1FD7A6B6-D127-40F1-AB82-13BEB016080C}"/>
+    <hyperlink ref="B116" r:id="rId109" display="https://leetcode.com/problems/the-number-of-seniors-and-juniors-to-join-the-company-ii" xr:uid="{E3EF10DB-DACD-4070-BA3A-D47998501C51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId108"/>
+  <pageSetup orientation="portrait" r:id="rId110"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in all hard problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABD7C69-5ADD-4B0B-93E1-CCD4119E6C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312AB7BC-6234-47F1-B674-DE1A3CD071F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1822</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1839</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9835" uniqueCount="3630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9913" uniqueCount="3660">
   <si>
     <t>Difficulty</t>
   </si>
@@ -10927,6 +10927,96 @@
   </si>
   <si>
     <t>if return in current room the 2 days to next room, otherwise calcluate difference with previous room</t>
+  </si>
+  <si>
+    <t>Count Vowel Substrings of a String</t>
+  </si>
+  <si>
+    <t>Vowels of All Substrings</t>
+  </si>
+  <si>
+    <t>Minimized Maximum of Products Distributed to Any Store</t>
+  </si>
+  <si>
+    <t>Maximum Path Quality of a Graph</t>
+  </si>
+  <si>
+    <t>DFS, tracking visited as score counting</t>
+  </si>
+  <si>
+    <t>Check Whether Two Strings are Almost Equivalent</t>
+  </si>
+  <si>
+    <t>Sum of k-Mirror Numbers</t>
+  </si>
+  <si>
+    <t>Generate numbers</t>
+  </si>
+  <si>
+    <t>Range Frequency Queries</t>
+  </si>
+  <si>
+    <t>Watering Plants</t>
+  </si>
+  <si>
+    <t>Two Furthest Houses With Different Colors</t>
+  </si>
+  <si>
+    <t>Process Restricted Friend Requests</t>
+  </si>
+  <si>
+    <t>Union Find, scan each request by enemy</t>
+  </si>
+  <si>
+    <t>Decode the Slanted Ciphertext</t>
+  </si>
+  <si>
+    <t>Reverse Nodes in Even Length Groups</t>
+  </si>
+  <si>
+    <t>Time Needed to Buy Tickets</t>
+  </si>
+  <si>
+    <t>Maximum Number of Tasks You Can Assign</t>
+  </si>
+  <si>
+    <t>Most Beautiful Item for Each Query</t>
+  </si>
+  <si>
+    <t>Walking Robot Simulation II</t>
+  </si>
+  <si>
+    <t>Use binary search to find maximum tasks can be assigned, assign from hardiest to easiest.</t>
+  </si>
+  <si>
+    <t>LOG(N) * N * LOG(N)</t>
+  </si>
+  <si>
+    <t>Determine stop position and travel position, stop position can not be too earlier and travel position can not be too late</t>
+  </si>
+  <si>
+    <t>32^N</t>
+  </si>
+  <si>
+    <t>Shortest Path, track each node with 2 distinct arriving time</t>
+  </si>
+  <si>
+    <t>Guess the answer and iterate array by two pointers.</t>
+  </si>
+  <si>
+    <t>(M + N) * LOG(N)</t>
+  </si>
+  <si>
+    <t>Push higher leading characters out</t>
+  </si>
+  <si>
+    <t>Prefix sum and track a particular value</t>
+  </si>
+  <si>
+    <t>Parse expersion with all answers, from center and spread.</t>
+  </si>
+  <si>
+    <t>From each number see how many in range and how many duplicate</t>
   </si>
 </sst>
 </file>
@@ -10971,7 +11061,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -11079,6 +11169,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -11466,10 +11557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1822"/>
+  <dimension ref="A1:J1839"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1805" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1780" sqref="A1780"/>
+    <sheetView tabSelected="1" topLeftCell="A1724" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1724" sqref="A1724"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -54153,6 +54244,27 @@
       <c r="B1780" s="1" t="s">
         <v>3515</v>
       </c>
+      <c r="C1780" s="93">
+        <v>4</v>
+      </c>
+      <c r="D1780" s="93" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E1780" s="93" t="s">
+        <v>2929</v>
+      </c>
+      <c r="F1780" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1780" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1780" s="93" t="s">
+        <v>3659</v>
+      </c>
+      <c r="I1780" s="93" t="s">
+        <v>3023</v>
+      </c>
     </row>
     <row r="1781" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1781" s="93">
@@ -54271,6 +54383,21 @@
       <c r="B1788" s="95" t="s">
         <v>3526</v>
       </c>
+      <c r="C1788" s="94">
+        <v>4</v>
+      </c>
+      <c r="D1788" s="94" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F1788" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1788" s="94" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1788" s="94" t="s">
+        <v>3658</v>
+      </c>
     </row>
     <row r="1789" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1789" s="94">
@@ -54321,6 +54448,27 @@
       <c r="B1792" s="95" t="s">
         <v>3530</v>
       </c>
+      <c r="C1792" s="94">
+        <v>4</v>
+      </c>
+      <c r="D1792" s="94" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E1792" s="94" t="s">
+        <v>2918</v>
+      </c>
+      <c r="F1792" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1792" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1792" s="94" t="s">
+        <v>3657</v>
+      </c>
+      <c r="I1792" s="94" t="s">
+        <v>2994</v>
+      </c>
     </row>
     <row r="1793" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1793" s="94">
@@ -54371,6 +54519,24 @@
       <c r="B1796" s="95" t="s">
         <v>3534</v>
       </c>
+      <c r="C1796" s="94">
+        <v>4</v>
+      </c>
+      <c r="D1796" s="94" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E1796" s="94" t="s">
+        <v>2929</v>
+      </c>
+      <c r="F1796" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1796" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1796" s="94" t="s">
+        <v>3656</v>
+      </c>
     </row>
     <row r="1797" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1797" s="97">
@@ -54492,6 +54658,24 @@
       <c r="B1804" s="1" t="s">
         <v>3555</v>
       </c>
+      <c r="C1804" s="97">
+        <v>5</v>
+      </c>
+      <c r="D1804" s="97" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F1804" s="97" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1804" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1804" s="97" t="s">
+        <v>3654</v>
+      </c>
+      <c r="I1804" s="97" t="s">
+        <v>3655</v>
+      </c>
     </row>
     <row r="1805" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1805" s="97">
@@ -54542,6 +54726,24 @@
       <c r="B1808" s="98" t="s">
         <v>3559</v>
       </c>
+      <c r="C1808" s="97">
+        <v>4</v>
+      </c>
+      <c r="D1808" s="97" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F1808" s="97" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1808" s="97" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1808" s="97" t="s">
+        <v>3653</v>
+      </c>
+      <c r="I1808" s="97" t="s">
+        <v>3023</v>
+      </c>
     </row>
     <row r="1809" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1809" s="97">
@@ -54592,6 +54794,27 @@
       <c r="B1812" s="1" t="s">
         <v>3563</v>
       </c>
+      <c r="C1812" s="97">
+        <v>4</v>
+      </c>
+      <c r="D1812" s="97" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E1812" s="97" t="s">
+        <v>2918</v>
+      </c>
+      <c r="F1812" s="97" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1812" s="97" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1812" s="97" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1812" s="97" t="s">
+        <v>2994</v>
+      </c>
     </row>
     <row r="1813" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1813" s="94">
@@ -54642,6 +54865,21 @@
       <c r="B1816" s="98" t="s">
         <v>3567</v>
       </c>
+      <c r="C1816" s="97">
+        <v>5</v>
+      </c>
+      <c r="F1816" s="97" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1816" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1816" s="97" t="s">
+        <v>3651</v>
+      </c>
+      <c r="I1816" s="97" t="s">
+        <v>3652</v>
+      </c>
     </row>
     <row r="1817" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1817" s="97">
@@ -54711,35 +54949,241 @@
         <v>3310</v>
       </c>
     </row>
-    <row r="1821" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1821" s="100" t="s">
+    <row r="1821" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1821" s="100">
+        <v>2062</v>
+      </c>
+      <c r="B1821" s="1" t="s">
+        <v>3630</v>
+      </c>
+      <c r="F1821" s="100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1822" s="100">
+        <v>2063</v>
+      </c>
+      <c r="B1822" s="1" t="s">
+        <v>3631</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1823" s="100">
+        <v>2064</v>
+      </c>
+      <c r="B1823" s="98" t="s">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1824" s="100">
+        <v>2065</v>
+      </c>
+      <c r="B1824" s="1" t="s">
+        <v>3633</v>
+      </c>
+      <c r="C1824" s="100">
+        <v>4</v>
+      </c>
+      <c r="D1824" s="100" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F1824" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1824" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1824" s="100" t="s">
+        <v>3634</v>
+      </c>
+      <c r="I1824" s="100" t="s">
+        <v>3628</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1825" s="100">
+        <v>2068</v>
+      </c>
+      <c r="B1825" s="1" t="s">
+        <v>3635</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1826" s="100">
+        <v>2069</v>
+      </c>
+      <c r="B1826" s="1" t="s">
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1827" s="100">
+        <v>2070</v>
+      </c>
+      <c r="B1827" s="1" t="s">
+        <v>3647</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1828" s="100">
+        <v>2071</v>
+      </c>
+      <c r="B1828" s="1" t="s">
+        <v>3646</v>
+      </c>
+      <c r="C1828" s="100">
+        <v>5</v>
+      </c>
+      <c r="D1828" s="100" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F1828" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1828" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1828" s="100" t="s">
+        <v>3649</v>
+      </c>
+      <c r="I1828" s="100" t="s">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1829" s="100">
+        <v>2073</v>
+      </c>
+      <c r="B1829" s="1" t="s">
+        <v>3645</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1830" s="100">
+        <v>2074</v>
+      </c>
+      <c r="B1830" s="1" t="s">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="1831" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1831" s="100">
+        <v>2075</v>
+      </c>
+      <c r="B1831" s="1" t="s">
+        <v>3643</v>
+      </c>
+    </row>
+    <row r="1832" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1832" s="100">
+        <v>2076</v>
+      </c>
+      <c r="B1832" s="1" t="s">
+        <v>3641</v>
+      </c>
+      <c r="C1832" s="100">
+        <v>4</v>
+      </c>
+      <c r="D1832" s="100" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E1832" s="100" t="s">
+        <v>2929</v>
+      </c>
+      <c r="F1832" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1832" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1832" s="100" t="s">
+        <v>3642</v>
+      </c>
+    </row>
+    <row r="1833" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1833" s="100">
+        <v>2078</v>
+      </c>
+      <c r="B1833" s="1" t="s">
+        <v>3640</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1834" s="100">
+        <v>2079</v>
+      </c>
+      <c r="B1834" s="1" t="s">
+        <v>3639</v>
+      </c>
+    </row>
+    <row r="1835" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1835" s="100">
+        <v>2080</v>
+      </c>
+      <c r="B1835" s="1" t="s">
+        <v>3638</v>
+      </c>
+    </row>
+    <row r="1836" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1836" s="100">
+        <v>2081</v>
+      </c>
+      <c r="B1836" s="1" t="s">
+        <v>3636</v>
+      </c>
+      <c r="C1836" s="100">
+        <v>4</v>
+      </c>
+      <c r="D1836" s="100" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F1836" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1836" s="100" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1836" s="100" t="s">
+        <v>3637</v>
+      </c>
+      <c r="I1836" s="100" t="s">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1837" s="98"/>
+    </row>
+    <row r="1838" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1838" s="101" t="s">
         <v>1717</v>
       </c>
-      <c r="B1821" s="100"/>
-      <c r="C1821" s="100"/>
-      <c r="D1821" s="100"/>
-      <c r="E1821" s="100"/>
-      <c r="F1821" s="100"/>
-      <c r="G1821" s="100"/>
-      <c r="H1821" s="100"/>
-    </row>
-    <row r="1822" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1822" s="101" t="s">
+      <c r="B1838" s="101"/>
+      <c r="C1838" s="101"/>
+      <c r="D1838" s="101"/>
+      <c r="E1838" s="101"/>
+      <c r="F1838" s="101"/>
+      <c r="G1838" s="101"/>
+      <c r="H1838" s="101"/>
+    </row>
+    <row r="1839" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1839" s="102" t="s">
         <v>2754</v>
       </c>
-      <c r="B1822" s="101"/>
-      <c r="C1822" s="101"/>
-      <c r="D1822" s="101"/>
-      <c r="E1822" s="101"/>
-      <c r="F1822" s="101"/>
-      <c r="G1822" s="101"/>
-      <c r="H1822" s="101"/>
+      <c r="B1839" s="102"/>
+      <c r="C1839" s="102"/>
+      <c r="D1839" s="102"/>
+      <c r="E1839" s="102"/>
+      <c r="F1839" s="102"/>
+      <c r="G1839" s="102"/>
+      <c r="H1839" s="102"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1822" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1839" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1821:H1821"/>
-    <mergeCell ref="A1822:H1822"/>
+    <mergeCell ref="A1838:H1838"/>
+    <mergeCell ref="A1839:H1839"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -56340,10 +56784,26 @@
     <hyperlink ref="B1820" r:id="rId1596" display="https://leetcode.com/problems/check-if-an-original-string-exists-given-two-encoded-strings" xr:uid="{0E2F5BE6-4251-43B0-902E-665D40B08A24}"/>
     <hyperlink ref="B605" r:id="rId1597" display="https://leetcode.com/problems/robot-return-to-origin" xr:uid="{F90BDC0D-FA70-41A1-A23C-878C1C1627B7}"/>
     <hyperlink ref="B1710" r:id="rId1598" display="https://leetcode.com/problems/number-of-wonderful-substrings" xr:uid="{9423D426-30DB-4078-B23A-2E94A3A02AA3}"/>
+    <hyperlink ref="B1821" r:id="rId1599" display="https://leetcode.com/problems/count-vowel-substrings-of-a-string" xr:uid="{7FCC5F29-7C62-4374-B0A9-2ABCC18104A5}"/>
+    <hyperlink ref="B1822" r:id="rId1600" display="https://leetcode.com/problems/vowels-of-all-substrings" xr:uid="{46C4B1C2-365D-40D1-B052-A17550370995}"/>
+    <hyperlink ref="B1823" r:id="rId1601" display="https://leetcode.com/problems/minimized-maximum-of-products-distributed-to-any-store" xr:uid="{10A9FF8C-86AD-4D91-B020-A08498C62B37}"/>
+    <hyperlink ref="B1824" r:id="rId1602" display="https://leetcode.com/problems/maximum-path-quality-of-a-graph" xr:uid="{0B2D1EBB-160D-4ED4-8B55-CE1BD0869125}"/>
+    <hyperlink ref="B1825" r:id="rId1603" xr:uid="{BB09D143-36DB-4DAD-8C50-2059028F1FE9}"/>
+    <hyperlink ref="B1836" r:id="rId1604" display="https://leetcode.com/problems/sum-of-k-mirror-numbers" xr:uid="{F0650F51-568A-4717-BC19-ABB1B6FFFDEC}"/>
+    <hyperlink ref="B1835" r:id="rId1605" display="https://leetcode.com/problems/range-frequency-queries" xr:uid="{1E229C2A-34B8-4A81-B0C6-5A3AD71CCF39}"/>
+    <hyperlink ref="B1834" r:id="rId1606" display="https://leetcode.com/problems/watering-plants" xr:uid="{A7EF29DE-DB3D-46A9-905D-C48EDDF5C996}"/>
+    <hyperlink ref="B1833" r:id="rId1607" display="https://leetcode.com/problems/two-furthest-houses-with-different-colors" xr:uid="{37BA5D04-9AF4-4ECA-A97D-39D90F766EF4}"/>
+    <hyperlink ref="B1832" r:id="rId1608" display="https://leetcode.com/problems/process-restricted-friend-requests" xr:uid="{C99C6F0C-8C7B-4E62-8AC6-A5A8F82F0410}"/>
+    <hyperlink ref="B1831" r:id="rId1609" display="https://leetcode.com/problems/decode-the-slanted-ciphertext" xr:uid="{2350D7FD-D03A-41C6-90F8-670D922F7173}"/>
+    <hyperlink ref="B1830" r:id="rId1610" display="https://leetcode.com/problems/reverse-nodes-in-even-length-groups" xr:uid="{D9BBD886-602B-46F9-97D3-B4CD877C9459}"/>
+    <hyperlink ref="B1829" r:id="rId1611" display="https://leetcode.com/problems/time-needed-to-buy-tickets" xr:uid="{B62F15D1-AFD5-4E07-A951-E2E37A83C871}"/>
+    <hyperlink ref="B1828" r:id="rId1612" display="https://leetcode.com/problems/maximum-number-of-tasks-you-can-assign" xr:uid="{953AE036-BD94-4947-9D3F-2342559633D4}"/>
+    <hyperlink ref="B1827" r:id="rId1613" display="https://leetcode.com/problems/most-beautiful-item-for-each-query" xr:uid="{285617BD-2F3A-412A-8F56-D5D10E9F2FA7}"/>
+    <hyperlink ref="B1826" r:id="rId1614" display="https://leetcode.com/problems/walking-robot-simulation-ii" xr:uid="{D2D1B95C-0388-40D9-8577-069CD220E305}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1599"/>
-  <drawing r:id="rId1600"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1615"/>
+  <drawing r:id="rId1616"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
complete all SQL problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4B9516-BF40-4168-9027-14BF7F1D3C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF83748-1109-4DAF-91E6-E1EAA50F5C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9960" uniqueCount="3664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9961" uniqueCount="3664">
   <si>
     <t>Difficulty</t>
   </si>
@@ -11571,8 +11571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1839"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1760" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1770" sqref="A1770"/>
+    <sheetView tabSelected="1" topLeftCell="A1735" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1307" sqref="E1307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -42347,9 +42347,11 @@
         <v>2</v>
       </c>
       <c r="D1307" s="38" t="s">
-        <v>1762</v>
-      </c>
-      <c r="E1307" s="61"/>
+        <v>1715</v>
+      </c>
+      <c r="E1307" s="61" t="s">
+        <v>2927</v>
+      </c>
       <c r="F1307" s="38" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
check 3 hard 1 medium and 1 easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB55782-9A4E-408A-B978-5C6987AEABCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE257F9-925A-4B08-9678-2026E8D08D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1886</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1890</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10409" uniqueCount="3779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10439" uniqueCount="3788">
   <si>
     <t>Difficulty</t>
   </si>
@@ -11374,6 +11374,33 @@
   </si>
   <si>
     <t>if K is odd, take one maximum even number otherwise take maximum two odd or even numbers</t>
+  </si>
+  <si>
+    <t>Sequentially Ordinal Rank Tracker</t>
+  </si>
+  <si>
+    <t>Keep two heap, added and queried, queried heap size is how many times query is done</t>
+  </si>
+  <si>
+    <t>Minimum Operations to Make the Array K-Increasing</t>
+  </si>
+  <si>
+    <t>LIS on each K skip array</t>
+  </si>
+  <si>
+    <t>Check how many invalid start brackets, (N + 1) / 2</t>
+  </si>
+  <si>
+    <t>Find First Palindromic String in the Array</t>
+  </si>
+  <si>
+    <t>Check palindromic string</t>
+  </si>
+  <si>
+    <t>Maximum Fruits Harvested After at Most K Steps</t>
+  </si>
+  <si>
+    <t>starting from left most position and keep on moving right, calculate optimal steps</t>
   </si>
 </sst>
 </file>
@@ -11418,7 +11445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -11526,6 +11553,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -11928,10 +11956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1886"/>
+  <dimension ref="A1:J1890"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1864" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1881" sqref="A1881"/>
+    <sheetView tabSelected="1" topLeftCell="A1872" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1885" sqref="A1885"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -54793,6 +54821,24 @@
       <c r="B1767" s="1" t="s">
         <v>3466</v>
       </c>
+      <c r="C1767" s="93">
+        <v>3</v>
+      </c>
+      <c r="D1767" s="93" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1767" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1767" s="93" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1767" s="93" t="s">
+        <v>3783</v>
+      </c>
+      <c r="I1767" s="93" t="s">
+        <v>2983</v>
+      </c>
     </row>
     <row r="1768" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1768" s="93">
@@ -57397,64 +57443,171 @@
         <v>3011</v>
       </c>
     </row>
-    <row r="1883" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1883" s="112">
+    <row r="1883" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1883" s="115">
+        <v>2102</v>
+      </c>
+      <c r="B1883" s="1" t="s">
+        <v>3779</v>
+      </c>
+      <c r="C1883" s="115">
+        <v>4</v>
+      </c>
+      <c r="D1883" s="115" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1883" s="115" t="s">
+        <v>2918</v>
+      </c>
+      <c r="F1883" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1883" s="115" t="s">
+        <v>455</v>
+      </c>
+      <c r="H1883" s="115" t="s">
+        <v>3780</v>
+      </c>
+      <c r="I1883" s="115" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1884" s="112">
         <v>2103</v>
       </c>
-      <c r="B1883" s="1" t="s">
+      <c r="B1884" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C1883" s="112">
+      <c r="C1884" s="112">
         <v>1</v>
       </c>
-      <c r="D1883" s="112" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1883" s="112" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1883" s="112" t="s">
+      <c r="D1884" s="112" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1884" s="112" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1884" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="H1883" s="112" t="s">
+      <c r="H1884" s="112" t="s">
         <v>3765</v>
       </c>
-      <c r="I1883" s="112" t="s">
+      <c r="I1884" s="112" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1884" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1884" s="98"/>
-    </row>
-    <row r="1885" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1885" s="115" t="s">
+    <row r="1885" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1885" s="115">
+        <v>2106</v>
+      </c>
+      <c r="B1885" s="98" t="s">
+        <v>3786</v>
+      </c>
+      <c r="C1885" s="115">
+        <v>4</v>
+      </c>
+      <c r="D1885" s="115" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1885" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1885" s="115" t="s">
+        <v>619</v>
+      </c>
+      <c r="H1885" s="115" t="s">
+        <v>3787</v>
+      </c>
+      <c r="I1885" s="115" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1886" s="115">
+        <v>2108</v>
+      </c>
+      <c r="B1886" s="1" t="s">
+        <v>3784</v>
+      </c>
+      <c r="C1886" s="115">
+        <v>1</v>
+      </c>
+      <c r="D1886" s="115" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1886" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1886" s="115" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1886" s="115" t="s">
+        <v>3785</v>
+      </c>
+      <c r="I1886" s="115" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1887" s="100">
+        <v>2111</v>
+      </c>
+      <c r="B1887" s="98" t="s">
+        <v>3781</v>
+      </c>
+      <c r="C1887" s="100">
+        <v>4</v>
+      </c>
+      <c r="D1887" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1887" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1887" s="100" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1887" s="100" t="s">
+        <v>3782</v>
+      </c>
+      <c r="I1887" s="100" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1888" s="98"/>
+    </row>
+    <row r="1889" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1889" s="116" t="s">
         <v>1714</v>
       </c>
-      <c r="B1885" s="115"/>
-      <c r="C1885" s="115"/>
-      <c r="D1885" s="115"/>
-      <c r="E1885" s="115"/>
-      <c r="F1885" s="115"/>
-      <c r="G1885" s="115"/>
-      <c r="H1885" s="115"/>
-    </row>
-    <row r="1886" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1886" s="116" t="s">
+      <c r="B1889" s="116"/>
+      <c r="C1889" s="116"/>
+      <c r="D1889" s="116"/>
+      <c r="E1889" s="116"/>
+      <c r="F1889" s="116"/>
+      <c r="G1889" s="116"/>
+      <c r="H1889" s="116"/>
+    </row>
+    <row r="1890" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1890" s="117" t="s">
         <v>2745</v>
       </c>
-      <c r="B1886" s="116"/>
-      <c r="C1886" s="116"/>
-      <c r="D1886" s="116"/>
-      <c r="E1886" s="116"/>
-      <c r="F1886" s="116"/>
-      <c r="G1886" s="116"/>
-      <c r="H1886" s="116"/>
+      <c r="B1890" s="117"/>
+      <c r="C1890" s="117"/>
+      <c r="D1890" s="117"/>
+      <c r="E1890" s="117"/>
+      <c r="F1890" s="117"/>
+      <c r="G1890" s="117"/>
+      <c r="H1890" s="117"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1886" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1890" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1885:H1885"/>
-    <mergeCell ref="A1886:H1886"/>
+    <mergeCell ref="A1889:H1889"/>
+    <mergeCell ref="A1890:H1890"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -59112,7 +59265,7 @@
     <hyperlink ref="B1798" r:id="rId1653" display="https://leetcode.com/problems/smallest-greater-multiple-made-of-two-digits" xr:uid="{8B3267DC-2D98-4C8C-B245-BBD0849BCC1A}"/>
     <hyperlink ref="B1879" r:id="rId1654" display="https://leetcode.com/problems/step-by-step-directions-from-a-binary-tree-node-to-another" xr:uid="{C5C7E5DC-8934-40E9-B69B-CF586656DD52}"/>
     <hyperlink ref="B1882" r:id="rId1655" display="https://leetcode.com/problems/find-subsequence-of-length-k-with-the-largest-sum" xr:uid="{3847A2FB-3BFE-44B9-BED6-56D6ECB82D82}"/>
-    <hyperlink ref="B1883" r:id="rId1656" display="https://leetcode.com/problems/rings-and-rods" xr:uid="{23A44248-878B-4CE4-AE7B-E9FEE1091067}"/>
+    <hyperlink ref="B1884" r:id="rId1656" display="https://leetcode.com/problems/rings-and-rods" xr:uid="{23A44248-878B-4CE4-AE7B-E9FEE1091067}"/>
     <hyperlink ref="B1705" r:id="rId1657" display="https://leetcode.com/problems/cutting-ribbons" xr:uid="{131BC84C-8E0F-4AF9-87AB-7B89E638ABD5}"/>
     <hyperlink ref="B1775" r:id="rId1658" display="https://leetcode.com/problems/count-nodes-equal-to-sum-of-descendants" xr:uid="{BFF8F8A7-A6A0-4A49-A8FC-453653B4257B}"/>
     <hyperlink ref="B1841" r:id="rId1659" display="https://leetcode.com/problems/minimum-cost-to-separate-sentence-into-rows" xr:uid="{2AC1A4DB-1946-4EA6-87C8-BFCBD335968E}"/>
@@ -59120,10 +59273,14 @@
     <hyperlink ref="B1414" r:id="rId1661" display="https://leetcode.com/problems/magnetic-force-between-two-balls" xr:uid="{7257B245-2713-4150-810D-6F2FA5EAEF89}"/>
     <hyperlink ref="B1728" r:id="rId1662" display="https://leetcode.com/problems/kth-smallest-subarray-sum" xr:uid="{9D83B952-41A0-405D-A753-C692921A798C}"/>
     <hyperlink ref="B1881" r:id="rId1663" display="https://leetcode.com/problems/subsequence-of-size-k-with-the-largest-even-sum" xr:uid="{0645F7F4-851F-4A5B-876D-2F23B7F1CB18}"/>
+    <hyperlink ref="B1883" r:id="rId1664" display="https://leetcode.com/problems/sequentially-ordinal-rank-tracker" xr:uid="{4AEEE917-FC1A-4441-8FCC-AAB33045CAAF}"/>
+    <hyperlink ref="B1887" r:id="rId1665" display="https://leetcode.com/problems/minimum-operations-to-make-the-array-k-increasing" xr:uid="{0A30673F-4EF8-4DD1-9D82-A9D62C3B11FC}"/>
+    <hyperlink ref="B1886" r:id="rId1666" display="https://leetcode.com/problems/find-first-palindromic-string-in-the-array" xr:uid="{5BDD994B-8936-496C-9380-FC41DA3F9A69}"/>
+    <hyperlink ref="B1885" r:id="rId1667" display="https://leetcode.com/problems/maximum-fruits-harvested-after-at-most-k-steps" xr:uid="{4833F7C7-BB0A-45D9-B2EE-0435CC7E66B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1664"/>
-  <drawing r:id="rId1665"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1668"/>
+  <drawing r:id="rId1669"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in 9 problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7637732D-FA0D-4C03-93EB-9DDB1153C119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094DF99F-0E91-4F16-8C0C-7B230C72CD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1891</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1899</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10457" uniqueCount="3792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10512" uniqueCount="3809">
   <si>
     <t>Difficulty</t>
   </si>
@@ -11413,6 +11413,57 @@
   </si>
   <si>
     <t>Track parents and children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate maximum before and minimum after </t>
+  </si>
+  <si>
+    <t>Calculate remaining sum and get average</t>
+  </si>
+  <si>
+    <t>use bit map to get all possible combinations</t>
+  </si>
+  <si>
+    <t>Binary search left and right candle position</t>
+  </si>
+  <si>
+    <t>Get index for minimum and maximum and calcualte both ends</t>
+  </si>
+  <si>
+    <t>Watering Plants II</t>
+  </si>
+  <si>
+    <t>Iterate from both sides</t>
+  </si>
+  <si>
+    <t>Number of Unique Flavors After Sharing K Candies</t>
+  </si>
+  <si>
+    <t>Minimum Coverage</t>
+  </si>
+  <si>
+    <t>Number of Smooth Descent Periods of a Stock</t>
+  </si>
+  <si>
+    <t>Adding Spaces to a String</t>
+  </si>
+  <si>
+    <t>Sum of Subarray Ranges</t>
+  </si>
+  <si>
+    <t>Detonate the Maximum Bombs</t>
+  </si>
+  <si>
+    <t>Find Good Days to Rob the Bank</t>
+  </si>
+  <si>
+    <t>Delete the Middle Node of a Linked List</t>
+  </si>
+  <si>
+    <t>Count vowels at the position and accumulate</t>
+  </si>
+  <si>
+    <t>count in hashtable then multiply</t>
   </si>
 </sst>
 </file>
@@ -11457,7 +11508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -11565,6 +11616,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -11969,10 +12021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1891"/>
+  <dimension ref="A1:J1899"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1783" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1793" sqref="A1793"/>
+    <sheetView tabSelected="1" topLeftCell="A1816" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1819" sqref="A1819"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -55988,6 +56040,24 @@
       <c r="B1810" s="1" t="s">
         <v>3503</v>
       </c>
+      <c r="C1810" s="93">
+        <v>2</v>
+      </c>
+      <c r="D1810" s="93" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1810" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1810" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1810" s="93" t="s">
+        <v>3792</v>
+      </c>
+      <c r="I1810" s="93" t="s">
+        <v>2983</v>
+      </c>
     </row>
     <row r="1811" spans="1:9" s="93" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1811" s="93">
@@ -56204,6 +56274,24 @@
       <c r="B1819" s="95" t="s">
         <v>3514</v>
       </c>
+      <c r="C1819" s="94">
+        <v>2</v>
+      </c>
+      <c r="D1819" s="94" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1819" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1819" s="94" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1819" s="94" t="s">
+        <v>3808</v>
+      </c>
+      <c r="I1819" s="94" t="s">
+        <v>3008</v>
+      </c>
     </row>
     <row r="1820" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1820" s="94">
@@ -56275,6 +56363,24 @@
       <c r="B1823" s="1" t="s">
         <v>3518</v>
       </c>
+      <c r="C1823" s="94">
+        <v>2</v>
+      </c>
+      <c r="D1823" s="94" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1823" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1823" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1823" s="94" t="s">
+        <v>3793</v>
+      </c>
+      <c r="I1823" s="94" t="s">
+        <v>2983</v>
+      </c>
     </row>
     <row r="1824" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1824" s="94">
@@ -56565,6 +56671,24 @@
       <c r="B1836" s="1" t="s">
         <v>3544</v>
       </c>
+      <c r="C1836" s="97">
+        <v>2</v>
+      </c>
+      <c r="D1836" s="97" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1836" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1836" s="97" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1836" s="97" t="s">
+        <v>3794</v>
+      </c>
+      <c r="I1836" s="97" t="s">
+        <v>3297</v>
+      </c>
     </row>
     <row r="1837" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1837" s="97">
@@ -56751,6 +56875,27 @@
       <c r="B1845" s="1" t="s">
         <v>3552</v>
       </c>
+      <c r="C1845" s="97">
+        <v>3</v>
+      </c>
+      <c r="D1845" s="97" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1845" s="97" t="s">
+        <v>2918</v>
+      </c>
+      <c r="F1845" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1845" s="97" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1845" s="97" t="s">
+        <v>3795</v>
+      </c>
+      <c r="I1845" s="97" t="s">
+        <v>3011</v>
+      </c>
     </row>
     <row r="1846" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1846" s="97">
@@ -56890,6 +57035,27 @@
       <c r="B1853" s="1" t="s">
         <v>3616</v>
       </c>
+      <c r="C1853" s="100">
+        <v>2</v>
+      </c>
+      <c r="D1853" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1853" s="100" t="s">
+        <v>2918</v>
+      </c>
+      <c r="F1853" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1853" s="100" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1853" s="100" t="s">
+        <v>3807</v>
+      </c>
+      <c r="I1853" s="100" t="s">
+        <v>2983</v>
+      </c>
     </row>
     <row r="1854" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1854" s="100">
@@ -57347,6 +57513,24 @@
       <c r="B1876" s="98" t="s">
         <v>3682</v>
       </c>
+      <c r="C1876" s="104">
+        <v>2</v>
+      </c>
+      <c r="D1876" s="104" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1876" s="104" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1876" s="104" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1876" s="104" t="s">
+        <v>3796</v>
+      </c>
+      <c r="I1876" s="104" t="s">
+        <v>2983</v>
+      </c>
     </row>
     <row r="1877" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1877" s="104">
@@ -57411,284 +57595,384 @@
         <v>3728</v>
       </c>
     </row>
-    <row r="1880" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1880" s="112">
+    <row r="1880" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1880" s="117">
+        <v>2095</v>
+      </c>
+      <c r="B1880" s="1" t="s">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1881" s="112">
         <v>2096</v>
       </c>
-      <c r="B1880" s="98" t="s">
+      <c r="B1881" s="98" t="s">
         <v>3760</v>
       </c>
-      <c r="C1880" s="112">
+      <c r="C1881" s="112">
         <v>3</v>
       </c>
-      <c r="D1880" s="112" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1880" s="112" t="s">
+      <c r="D1881" s="112" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1881" s="112" t="s">
         <v>2918</v>
       </c>
-      <c r="F1880" s="112" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1880" s="112" t="s">
+      <c r="F1881" s="112" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1881" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="H1880" s="112" t="s">
+      <c r="H1881" s="112" t="s">
         <v>3761</v>
       </c>
-      <c r="I1880" s="112" t="s">
+      <c r="I1881" s="112" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1881" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1881" s="109">
+    <row r="1882" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1882" s="109">
         <v>2097</v>
       </c>
-      <c r="B1881" s="1" t="s">
+      <c r="B1882" s="1" t="s">
         <v>3739</v>
       </c>
-      <c r="C1881" s="109">
+      <c r="C1882" s="109">
         <v>4</v>
       </c>
-      <c r="D1881" s="109" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1881" s="109" t="s">
+      <c r="D1882" s="109" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1882" s="109" t="s">
         <v>2918</v>
       </c>
-      <c r="F1881" s="109" t="s">
+      <c r="F1882" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="G1881" s="109" t="s">
+      <c r="G1882" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="H1881" s="109" t="s">
+      <c r="H1882" s="109" t="s">
         <v>3740</v>
       </c>
-      <c r="I1881" s="109" t="s">
+      <c r="I1882" s="109" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1882" spans="1:9" s="114" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1882" s="114">
+    <row r="1883" spans="1:9" s="114" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1883" s="114">
         <v>2098</v>
       </c>
-      <c r="B1882" s="1" t="s">
+      <c r="B1883" s="1" t="s">
         <v>3777</v>
       </c>
-      <c r="C1882" s="114">
+      <c r="C1883" s="114">
         <v>3</v>
       </c>
-      <c r="D1882" s="114" t="s">
+      <c r="D1883" s="114" t="s">
         <v>1706</v>
       </c>
-      <c r="F1882" s="114" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1882" s="114" t="s">
+      <c r="F1883" s="114" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1883" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="H1882" s="114" t="s">
+      <c r="H1883" s="114" t="s">
         <v>3778</v>
       </c>
-      <c r="I1882" s="114" t="s">
+      <c r="I1883" s="114" t="s">
         <v>3011</v>
       </c>
     </row>
-    <row r="1883" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1883" s="112">
+    <row r="1884" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1884" s="112">
         <v>2099</v>
       </c>
-      <c r="B1883" s="98" t="s">
+      <c r="B1884" s="98" t="s">
         <v>3762</v>
       </c>
-      <c r="C1883" s="112">
+      <c r="C1884" s="112">
         <v>3</v>
       </c>
-      <c r="D1883" s="112" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1883" s="112" t="s">
+      <c r="D1884" s="112" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1884" s="112" t="s">
         <v>2918</v>
       </c>
-      <c r="F1883" s="112" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1883" s="112" t="s">
+      <c r="F1884" s="112" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1884" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="H1883" s="112" t="s">
+      <c r="H1884" s="112" t="s">
         <v>3763</v>
       </c>
-      <c r="I1883" s="112" t="s">
+      <c r="I1884" s="112" t="s">
         <v>3011</v>
       </c>
     </row>
-    <row r="1884" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1884" s="115">
-        <v>2102</v>
-      </c>
-      <c r="B1884" s="1" t="s">
-        <v>3779</v>
-      </c>
-      <c r="C1884" s="115">
-        <v>4</v>
-      </c>
-      <c r="D1884" s="115" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1884" s="115" t="s">
-        <v>2918</v>
-      </c>
-      <c r="F1884" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1884" s="115" t="s">
-        <v>455</v>
-      </c>
-      <c r="H1884" s="115" t="s">
-        <v>3780</v>
-      </c>
-      <c r="I1884" s="115" t="s">
-        <v>3011</v>
-      </c>
-    </row>
-    <row r="1885" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1885" s="112">
-        <v>2103</v>
+    <row r="1885" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1885" s="117">
+        <v>2100</v>
       </c>
       <c r="B1885" s="1" t="s">
-        <v>3764</v>
-      </c>
-      <c r="C1885" s="112">
-        <v>1</v>
-      </c>
-      <c r="D1885" s="112" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1885" s="112" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1885" s="112" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1885" s="112" t="s">
-        <v>3765</v>
-      </c>
-      <c r="I1885" s="112" t="s">
-        <v>2983</v>
-      </c>
-    </row>
-    <row r="1886" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1886" s="115">
-        <v>2106</v>
-      </c>
-      <c r="B1886" s="98" t="s">
-        <v>3786</v>
-      </c>
-      <c r="C1886" s="115">
-        <v>4</v>
-      </c>
-      <c r="D1886" s="115" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1886" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1886" s="115" t="s">
-        <v>619</v>
-      </c>
-      <c r="H1886" s="115" t="s">
-        <v>3787</v>
-      </c>
-      <c r="I1886" s="115" t="s">
-        <v>3011</v>
+        <v>3805</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1886" s="117">
+        <v>2101</v>
+      </c>
+      <c r="B1886" s="1" t="s">
+        <v>3804</v>
       </c>
     </row>
     <row r="1887" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1887" s="115">
+        <v>2102</v>
+      </c>
+      <c r="B1887" s="1" t="s">
+        <v>3779</v>
+      </c>
+      <c r="C1887" s="115">
+        <v>4</v>
+      </c>
+      <c r="D1887" s="115" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1887" s="115" t="s">
+        <v>2918</v>
+      </c>
+      <c r="F1887" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1887" s="115" t="s">
+        <v>455</v>
+      </c>
+      <c r="H1887" s="115" t="s">
+        <v>3780</v>
+      </c>
+      <c r="I1887" s="115" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1888" s="112">
+        <v>2103</v>
+      </c>
+      <c r="B1888" s="1" t="s">
+        <v>3764</v>
+      </c>
+      <c r="C1888" s="112">
+        <v>1</v>
+      </c>
+      <c r="D1888" s="112" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1888" s="112" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1888" s="112" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1888" s="112" t="s">
+        <v>3765</v>
+      </c>
+      <c r="I1888" s="112" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1889" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1889" s="117">
+        <v>2104</v>
+      </c>
+      <c r="B1889" s="1" t="s">
+        <v>3803</v>
+      </c>
+    </row>
+    <row r="1890" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1890" s="117">
+        <v>2105</v>
+      </c>
+      <c r="B1890" s="1" t="s">
+        <v>3797</v>
+      </c>
+      <c r="C1890" s="117">
+        <v>2</v>
+      </c>
+      <c r="D1890" s="117" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1890" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1890" s="117" t="s">
+        <v>619</v>
+      </c>
+      <c r="H1890" s="117" t="s">
+        <v>3798</v>
+      </c>
+      <c r="I1890" s="117" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1891" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1891" s="115">
+        <v>2106</v>
+      </c>
+      <c r="B1891" s="98" t="s">
+        <v>3786</v>
+      </c>
+      <c r="C1891" s="115">
+        <v>4</v>
+      </c>
+      <c r="D1891" s="115" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1891" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1891" s="115" t="s">
+        <v>619</v>
+      </c>
+      <c r="H1891" s="115" t="s">
+        <v>3787</v>
+      </c>
+      <c r="I1891" s="115" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1892" s="117">
+        <v>2107</v>
+      </c>
+      <c r="B1892" s="1" t="s">
+        <v>3799</v>
+      </c>
+      <c r="C1892" s="117">
+        <v>2</v>
+      </c>
+      <c r="D1892" s="117" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1892" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1892" s="117" t="s">
+        <v>619</v>
+      </c>
+      <c r="H1892" s="117" t="s">
+        <v>3800</v>
+      </c>
+      <c r="I1892" s="117" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1893" s="115">
         <v>2108</v>
       </c>
-      <c r="B1887" s="1" t="s">
+      <c r="B1893" s="1" t="s">
         <v>3784</v>
       </c>
-      <c r="C1887" s="115">
+      <c r="C1893" s="115">
         <v>1</v>
       </c>
-      <c r="D1887" s="115" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1887" s="115" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1887" s="115" t="s">
+      <c r="D1893" s="115" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1893" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1893" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="H1887" s="115" t="s">
+      <c r="H1893" s="115" t="s">
         <v>3785</v>
       </c>
-      <c r="I1887" s="115" t="s">
+      <c r="I1893" s="115" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1888" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1888" s="100">
+    <row r="1894" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1894" s="117">
+        <v>2109</v>
+      </c>
+      <c r="B1894" s="1" t="s">
+        <v>3802</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1895" s="117">
+        <v>2110</v>
+      </c>
+      <c r="B1895" s="98" t="s">
+        <v>3801</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1896" s="100">
         <v>2111</v>
       </c>
-      <c r="B1888" s="98" t="s">
+      <c r="B1896" s="98" t="s">
         <v>3781</v>
       </c>
-      <c r="C1888" s="100">
+      <c r="C1896" s="100">
         <v>4</v>
       </c>
-      <c r="D1888" s="100" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1888" s="100" t="s">
+      <c r="D1896" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1896" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="G1888" s="100" t="s">
+      <c r="G1896" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="H1888" s="100" t="s">
+      <c r="H1896" s="100" t="s">
         <v>3782</v>
       </c>
-      <c r="I1888" s="100" t="s">
+      <c r="I1896" s="100" t="s">
         <v>3011</v>
       </c>
     </row>
-    <row r="1889" spans="1:8" s="115" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1889" s="98"/>
-    </row>
-    <row r="1890" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1890" s="117" t="s">
+    <row r="1897" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1897" s="98"/>
+    </row>
+    <row r="1898" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1898" s="118" t="s">
         <v>1714</v>
       </c>
-      <c r="B1890" s="117"/>
-      <c r="C1890" s="117"/>
-      <c r="D1890" s="117"/>
-      <c r="E1890" s="117"/>
-      <c r="F1890" s="117"/>
-      <c r="G1890" s="117"/>
-      <c r="H1890" s="117"/>
-    </row>
-    <row r="1891" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1891" s="118" t="s">
+      <c r="B1898" s="118"/>
+      <c r="C1898" s="118"/>
+      <c r="D1898" s="118"/>
+      <c r="E1898" s="118"/>
+      <c r="F1898" s="118"/>
+      <c r="G1898" s="118"/>
+      <c r="H1898" s="118"/>
+    </row>
+    <row r="1899" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1899" s="119" t="s">
         <v>2745</v>
       </c>
-      <c r="B1891" s="118"/>
-      <c r="C1891" s="118"/>
-      <c r="D1891" s="118"/>
-      <c r="E1891" s="118"/>
-      <c r="F1891" s="118"/>
-      <c r="G1891" s="118"/>
-      <c r="H1891" s="118"/>
+      <c r="B1899" s="119"/>
+      <c r="C1899" s="119"/>
+      <c r="D1899" s="119"/>
+      <c r="E1899" s="119"/>
+      <c r="F1899" s="119"/>
+      <c r="G1899" s="119"/>
+      <c r="H1899" s="119"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1891" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1899" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1890:H1890"/>
-    <mergeCell ref="A1891:H1891"/>
+    <mergeCell ref="A1898:H1898"/>
+    <mergeCell ref="A1899:H1899"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -59337,32 +59621,40 @@
     <hyperlink ref="B1631" r:id="rId1644" display="https://leetcode.com/problems/implement-trie-ii-prefix-tree" xr:uid="{0FA20FE6-CB70-47B0-AE0C-73C2608CE4DE}"/>
     <hyperlink ref="B1851" r:id="rId1645" display="https://leetcode.com/problems/number-of-spaces-cleaning-robot-cleaned" xr:uid="{1843E481-A377-4508-844C-1566B0EB6A81}"/>
     <hyperlink ref="B1676" r:id="rId1646" display="https://leetcode.com/problems/longest-word-with-all-prefixes" xr:uid="{0630A561-7DF9-4C20-99BC-717B5D8F07BC}"/>
-    <hyperlink ref="B1881" r:id="rId1647" display="https://leetcode.com/problems/valid-arrangement-of-pairs" xr:uid="{E627A316-ECC0-45DA-A6B4-61105C3B4B1A}"/>
+    <hyperlink ref="B1882" r:id="rId1647" display="https://leetcode.com/problems/valid-arrangement-of-pairs" xr:uid="{E627A316-ECC0-45DA-A6B4-61105C3B4B1A}"/>
     <hyperlink ref="B1490" r:id="rId1648" display="https://leetcode.com/problems/number-of-ways-to-form-a-target-string-given-a-dictionary" xr:uid="{FF624C95-49DF-4169-B628-19629A6F243A}"/>
     <hyperlink ref="B1685" r:id="rId1649" display="https://leetcode.com/problems/product-of-two-run-length-encoded-arrays" xr:uid="{6A748179-BE2C-43B5-937C-0971F2E9B84E}"/>
     <hyperlink ref="B1700" r:id="rId1650" display="https://leetcode.com/problems/count-pairs-in-two-arrays" xr:uid="{161319D6-6334-4E03-AC0B-73EEDE5AFBF7}"/>
     <hyperlink ref="B1747" r:id="rId1651" display="https://leetcode.com/problems/longest-common-subsequence-between-sorted-arrays" xr:uid="{AE4203E3-43C5-40FC-8B78-1EF6EFA8B799}"/>
     <hyperlink ref="B1785" r:id="rId1652" display="https://leetcode.com/problems/widest-pair-of-indices-with-equal-range-sum" xr:uid="{620D8C9E-B0DA-477A-AA3C-2F635E95F462}"/>
     <hyperlink ref="B1799" r:id="rId1653" display="https://leetcode.com/problems/smallest-greater-multiple-made-of-two-digits" xr:uid="{8B3267DC-2D98-4C8C-B245-BBD0849BCC1A}"/>
-    <hyperlink ref="B1880" r:id="rId1654" display="https://leetcode.com/problems/step-by-step-directions-from-a-binary-tree-node-to-another" xr:uid="{C5C7E5DC-8934-40E9-B69B-CF586656DD52}"/>
-    <hyperlink ref="B1883" r:id="rId1655" display="https://leetcode.com/problems/find-subsequence-of-length-k-with-the-largest-sum" xr:uid="{3847A2FB-3BFE-44B9-BED6-56D6ECB82D82}"/>
-    <hyperlink ref="B1885" r:id="rId1656" display="https://leetcode.com/problems/rings-and-rods" xr:uid="{23A44248-878B-4CE4-AE7B-E9FEE1091067}"/>
+    <hyperlink ref="B1881" r:id="rId1654" display="https://leetcode.com/problems/step-by-step-directions-from-a-binary-tree-node-to-another" xr:uid="{C5C7E5DC-8934-40E9-B69B-CF586656DD52}"/>
+    <hyperlink ref="B1884" r:id="rId1655" display="https://leetcode.com/problems/find-subsequence-of-length-k-with-the-largest-sum" xr:uid="{3847A2FB-3BFE-44B9-BED6-56D6ECB82D82}"/>
+    <hyperlink ref="B1888" r:id="rId1656" display="https://leetcode.com/problems/rings-and-rods" xr:uid="{23A44248-878B-4CE4-AE7B-E9FEE1091067}"/>
     <hyperlink ref="B1705" r:id="rId1657" display="https://leetcode.com/problems/cutting-ribbons" xr:uid="{131BC84C-8E0F-4AF9-87AB-7B89E638ABD5}"/>
     <hyperlink ref="B1776" r:id="rId1658" display="https://leetcode.com/problems/count-nodes-equal-to-sum-of-descendants" xr:uid="{BFF8F8A7-A6A0-4A49-A8FC-453653B4257B}"/>
     <hyperlink ref="B1842" r:id="rId1659" display="https://leetcode.com/problems/minimum-cost-to-separate-sentence-into-rows" xr:uid="{2AC1A4DB-1946-4EA6-87C8-BFCBD335968E}"/>
     <hyperlink ref="B1353" r:id="rId1660" display="https://leetcode.com/problems/minimum-number-of-days-to-make-m-bouquets" xr:uid="{A226ED4B-9ECC-43EF-8EE3-94598D2C0FDF}"/>
     <hyperlink ref="B1414" r:id="rId1661" display="https://leetcode.com/problems/magnetic-force-between-two-balls" xr:uid="{7257B245-2713-4150-810D-6F2FA5EAEF89}"/>
     <hyperlink ref="B1728" r:id="rId1662" display="https://leetcode.com/problems/kth-smallest-subarray-sum" xr:uid="{9D83B952-41A0-405D-A753-C692921A798C}"/>
-    <hyperlink ref="B1882" r:id="rId1663" display="https://leetcode.com/problems/subsequence-of-size-k-with-the-largest-even-sum" xr:uid="{0645F7F4-851F-4A5B-876D-2F23B7F1CB18}"/>
-    <hyperlink ref="B1884" r:id="rId1664" display="https://leetcode.com/problems/sequentially-ordinal-rank-tracker" xr:uid="{4AEEE917-FC1A-4441-8FCC-AAB33045CAAF}"/>
-    <hyperlink ref="B1888" r:id="rId1665" display="https://leetcode.com/problems/minimum-operations-to-make-the-array-k-increasing" xr:uid="{0A30673F-4EF8-4DD1-9D82-A9D62C3B11FC}"/>
-    <hyperlink ref="B1887" r:id="rId1666" display="https://leetcode.com/problems/find-first-palindromic-string-in-the-array" xr:uid="{5BDD994B-8936-496C-9380-FC41DA3F9A69}"/>
-    <hyperlink ref="B1886" r:id="rId1667" display="https://leetcode.com/problems/maximum-fruits-harvested-after-at-most-k-steps" xr:uid="{4833F7C7-BB0A-45D9-B2EE-0435CC7E66B4}"/>
+    <hyperlink ref="B1883" r:id="rId1663" display="https://leetcode.com/problems/subsequence-of-size-k-with-the-largest-even-sum" xr:uid="{0645F7F4-851F-4A5B-876D-2F23B7F1CB18}"/>
+    <hyperlink ref="B1887" r:id="rId1664" display="https://leetcode.com/problems/sequentially-ordinal-rank-tracker" xr:uid="{4AEEE917-FC1A-4441-8FCC-AAB33045CAAF}"/>
+    <hyperlink ref="B1896" r:id="rId1665" display="https://leetcode.com/problems/minimum-operations-to-make-the-array-k-increasing" xr:uid="{0A30673F-4EF8-4DD1-9D82-A9D62C3B11FC}"/>
+    <hyperlink ref="B1893" r:id="rId1666" display="https://leetcode.com/problems/find-first-palindromic-string-in-the-array" xr:uid="{5BDD994B-8936-496C-9380-FC41DA3F9A69}"/>
+    <hyperlink ref="B1891" r:id="rId1667" display="https://leetcode.com/problems/maximum-fruits-harvested-after-at-most-k-steps" xr:uid="{4833F7C7-BB0A-45D9-B2EE-0435CC7E66B4}"/>
     <hyperlink ref="B1756" r:id="rId1668" display="https://leetcode.com/problems/maximum-of-minimum-values-in-all-subarrays" xr:uid="{6C5E9DC6-3B50-49DC-BA32-49B36A65631E}"/>
+    <hyperlink ref="B1890" r:id="rId1669" display="https://leetcode.com/problems/watering-plants-ii" xr:uid="{79ECD953-36CF-458D-946D-FCA45C267265}"/>
+    <hyperlink ref="B1892" r:id="rId1670" display="https://leetcode.com/problems/number-of-unique-flavors-after-sharing-k-candies" xr:uid="{8A15FC64-50EC-426A-8219-51F8F3F422B1}"/>
+    <hyperlink ref="B1895" r:id="rId1671" display="https://leetcode.com/problems/number-of-smooth-descent-periods-of-a-stock" xr:uid="{AB604653-CB6D-4FE8-949B-F9118F1FF4A9}"/>
+    <hyperlink ref="B1894" r:id="rId1672" display="https://leetcode.com/problems/adding-spaces-to-a-string" xr:uid="{88559B2E-A9F0-42CE-9D42-9875A4CCB6B6}"/>
+    <hyperlink ref="B1889" r:id="rId1673" display="https://leetcode.com/problems/sum-of-subarray-ranges" xr:uid="{14DB1AC6-E7C9-4533-B452-AB20E94B322C}"/>
+    <hyperlink ref="B1886" r:id="rId1674" display="https://leetcode.com/problems/detonate-the-maximum-bombs" xr:uid="{3354A4B4-953A-42B6-8A0E-05F8BB5CEF2A}"/>
+    <hyperlink ref="B1885" r:id="rId1675" display="https://leetcode.com/problems/find-good-days-to-rob-the-bank" xr:uid="{0F986755-A1C6-4B47-80BE-5140A48911DA}"/>
+    <hyperlink ref="B1880" r:id="rId1676" display="https://leetcode.com/problems/delete-the-middle-node-of-a-linked-list" xr:uid="{33F47B67-91EB-4460-B400-78D6212E468E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1669"/>
-  <drawing r:id="rId1670"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1677"/>
+  <drawing r:id="rId1678"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add two new problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75477E90-5D3E-4D8C-8E57-175DA10F30E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EE16B0-ED21-4E84-B28A-0BB46831FD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1899</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1900</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10520" uniqueCount="3809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10531" uniqueCount="3813">
   <si>
     <t>Difficulty</t>
   </si>
@@ -11464,6 +11464,18 @@
   </si>
   <si>
     <t>count in hashtable then multiply</t>
+  </si>
+  <si>
+    <t>Elements in Array After Removing and Replacing Elements</t>
+  </si>
+  <si>
+    <t>Calculate repeated circle</t>
+  </si>
+  <si>
+    <t>Brute force</t>
+  </si>
+  <si>
+    <t>10^N</t>
   </si>
 </sst>
 </file>
@@ -11508,7 +11520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -11616,6 +11628,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -12021,10 +12034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1899"/>
+  <dimension ref="A1:J1900"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A1830" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1840" sqref="A1840"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -56771,6 +56784,24 @@
       <c r="B1839" s="1" t="s">
         <v>3547</v>
       </c>
+      <c r="C1839" s="97">
+        <v>3</v>
+      </c>
+      <c r="D1839" s="97" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F1839" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1839" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1839" s="97" t="s">
+        <v>3811</v>
+      </c>
+      <c r="I1839" s="97" t="s">
+        <v>3812</v>
+      </c>
     </row>
     <row r="1840" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1840" s="97">
@@ -57963,24 +57994,38 @@
         <v>3011</v>
       </c>
     </row>
-    <row r="1897" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1897" s="98"/>
-    </row>
-    <row r="1898" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1898" s="118" t="s">
-        <v>1714</v>
-      </c>
-      <c r="B1898" s="118"/>
-      <c r="C1898" s="118"/>
-      <c r="D1898" s="118"/>
-      <c r="E1898" s="118"/>
-      <c r="F1898" s="118"/>
-      <c r="G1898" s="118"/>
-      <c r="H1898" s="118"/>
+    <row r="1897" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1897" s="118">
+        <v>2113</v>
+      </c>
+      <c r="B1897" s="1" t="s">
+        <v>3809</v>
+      </c>
+      <c r="C1897" s="118">
+        <v>2</v>
+      </c>
+      <c r="D1897" s="118" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1897" s="118" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1897" s="118" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1897" s="118" t="s">
+        <v>3810</v>
+      </c>
+      <c r="I1897" s="118" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1898" s="98"/>
     </row>
     <row r="1899" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1899" s="119" t="s">
-        <v>2745</v>
+        <v>1714</v>
       </c>
       <c r="B1899" s="119"/>
       <c r="C1899" s="119"/>
@@ -57990,11 +58035,23 @@
       <c r="G1899" s="119"/>
       <c r="H1899" s="119"/>
     </row>
+    <row r="1900" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1900" s="120" t="s">
+        <v>2745</v>
+      </c>
+      <c r="B1900" s="120"/>
+      <c r="C1900" s="120"/>
+      <c r="D1900" s="120"/>
+      <c r="E1900" s="120"/>
+      <c r="F1900" s="120"/>
+      <c r="G1900" s="120"/>
+      <c r="H1900" s="120"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J1899" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1900" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1898:H1898"/>
     <mergeCell ref="A1899:H1899"/>
+    <mergeCell ref="A1900:H1900"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -59673,10 +59730,11 @@
     <hyperlink ref="B1886" r:id="rId1674" display="https://leetcode.com/problems/detonate-the-maximum-bombs" xr:uid="{3354A4B4-953A-42B6-8A0E-05F8BB5CEF2A}"/>
     <hyperlink ref="B1885" r:id="rId1675" display="https://leetcode.com/problems/find-good-days-to-rob-the-bank" xr:uid="{0F986755-A1C6-4B47-80BE-5140A48911DA}"/>
     <hyperlink ref="B1880" r:id="rId1676" display="https://leetcode.com/problems/delete-the-middle-node-of-a-linked-list" xr:uid="{33F47B67-91EB-4460-B400-78D6212E468E}"/>
+    <hyperlink ref="B1897" r:id="rId1677" display="https://leetcode.com/problems/elements-in-array-after-removing-and-replacing-elements" xr:uid="{C65FB836-5A2E-4D03-94EF-C3385C2A46E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1677"/>
-  <drawing r:id="rId1678"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1678"/>
+  <drawing r:id="rId1679"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in 7 problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B512528A-6F67-4E56-851E-1FFE290BDF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC9BEB0-9231-4E14-9749-7B557A6B982F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1901</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1903</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10560" uniqueCount="3819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10599" uniqueCount="3827">
   <si>
     <t>Difficulty</t>
   </si>
@@ -11494,6 +11494,30 @@
   </si>
   <si>
     <t>Sort in 1D array and scan from both side</t>
+  </si>
+  <si>
+    <t>Sort Linked List Already Sorted Using Absolute Values</t>
+  </si>
+  <si>
+    <t>Split negative and postive linked list and the merge</t>
+  </si>
+  <si>
+    <t>Iterate group by group and check size (only last group matters), reverse even size</t>
+  </si>
+  <si>
+    <t>Use fast and slow pointer.</t>
+  </si>
+  <si>
+    <t>Number of Equal Count Substrings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slide window is size of unique * count </t>
+  </si>
+  <si>
+    <t>Sort by price and maximum beauty on price</t>
+  </si>
+  <si>
+    <t>Count by every starting characters</t>
   </si>
 </sst>
 </file>
@@ -11538,7 +11562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -11646,6 +11670,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -12053,10 +12078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1901"/>
+  <dimension ref="A1:J1903"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1925" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1925" sqref="A1925"/>
+    <sheetView tabSelected="1" topLeftCell="A1855" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1872" sqref="A1872"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -56838,38 +56863,38 @@
         <v>3011</v>
       </c>
     </row>
-    <row r="1839" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1839" s="97">
-        <v>2047</v>
-      </c>
-      <c r="B1839" s="1" t="s">
-        <v>3546</v>
-      </c>
-      <c r="C1839" s="97">
-        <v>3</v>
-      </c>
-      <c r="D1839" s="97" t="s">
-        <v>1706</v>
-      </c>
-      <c r="F1839" s="97" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1839" s="97" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1839" s="97" t="s">
-        <v>3560</v>
-      </c>
-      <c r="I1839" s="97" t="s">
+    <row r="1839" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1839" s="120">
+        <v>2046</v>
+      </c>
+      <c r="B1839" s="98" t="s">
+        <v>3819</v>
+      </c>
+      <c r="C1839" s="120">
+        <v>2</v>
+      </c>
+      <c r="D1839" s="120" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1839" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1839" s="120" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1839" s="120" t="s">
+        <v>3820</v>
+      </c>
+      <c r="I1839" s="120" t="s">
         <v>2983</v>
       </c>
     </row>
     <row r="1840" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1840" s="97">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="B1840" s="1" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="C1840" s="97">
         <v>3</v>
@@ -56878,145 +56903,142 @@
         <v>1706</v>
       </c>
       <c r="F1840" s="97" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1840" s="97" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="H1840" s="97" t="s">
-        <v>3811</v>
+        <v>3560</v>
       </c>
       <c r="I1840" s="97" t="s">
-        <v>3812</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="1841" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1841" s="97">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B1841" s="1" t="s">
-        <v>3548</v>
+        <v>3547</v>
+      </c>
+      <c r="C1841" s="97">
+        <v>3</v>
+      </c>
+      <c r="D1841" s="97" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F1841" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1841" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1841" s="97" t="s">
+        <v>3811</v>
+      </c>
+      <c r="I1841" s="97" t="s">
+        <v>3812</v>
       </c>
     </row>
     <row r="1842" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1842" s="97">
+        <v>2049</v>
+      </c>
+      <c r="B1842" s="1" t="s">
+        <v>3548</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1843" s="97">
         <v>2050</v>
       </c>
-      <c r="B1842" s="1" t="s">
+      <c r="B1843" s="1" t="s">
         <v>3549</v>
       </c>
-      <c r="C1842" s="97">
+      <c r="C1843" s="97">
         <v>4</v>
       </c>
-      <c r="D1842" s="97" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1842" s="97" t="s">
+      <c r="D1843" s="97" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1843" s="97" t="s">
         <v>2907</v>
       </c>
-      <c r="F1842" s="97" t="s">
+      <c r="F1843" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="G1842" s="97" t="s">
+      <c r="G1843" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="H1842" s="97" t="s">
+      <c r="H1843" s="97" t="s">
         <v>265</v>
       </c>
-      <c r="I1842" s="97" t="s">
+      <c r="I1843" s="97" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1843" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1843" s="113">
+    <row r="1844" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1844" s="113">
         <v>2052</v>
       </c>
-      <c r="B1843" s="98" t="s">
+      <c r="B1844" s="98" t="s">
         <v>3774</v>
       </c>
-      <c r="C1843" s="113">
+      <c r="C1844" s="113">
         <v>4</v>
       </c>
-      <c r="D1843" s="113" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1843" s="113" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1843" s="113" t="s">
+      <c r="D1844" s="113" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1844" s="113" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1844" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="H1843" s="113" t="s">
+      <c r="H1844" s="113" t="s">
         <v>3775</v>
       </c>
-      <c r="I1843" s="113" t="s">
+      <c r="I1844" s="113" t="s">
         <v>3005</v>
       </c>
     </row>
-    <row r="1844" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1844" s="94">
+    <row r="1845" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1845" s="94">
         <v>2053</v>
       </c>
-      <c r="B1844" s="1" t="s">
+      <c r="B1845" s="1" t="s">
         <v>3550</v>
       </c>
-      <c r="C1844" s="94">
+      <c r="C1845" s="94">
         <v>2</v>
       </c>
-      <c r="D1844" s="94" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1844" s="94" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1844" s="94" t="s">
+      <c r="D1845" s="94" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1845" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1845" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="H1844" s="94" t="s">
+      <c r="H1845" s="94" t="s">
         <v>3559</v>
       </c>
-      <c r="I1844" s="94" t="s">
+      <c r="I1845" s="94" t="s">
         <v>2983</v>
-      </c>
-    </row>
-    <row r="1845" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1845" s="97">
-        <v>2054</v>
-      </c>
-      <c r="B1845" s="1" t="s">
-        <v>3551</v>
-      </c>
-      <c r="C1845" s="97">
-        <v>2</v>
-      </c>
-      <c r="D1845" s="97" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1845" s="97" t="s">
-        <v>2918</v>
-      </c>
-      <c r="F1845" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1845" s="97" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1845" s="97" t="s">
-        <v>3747</v>
-      </c>
-      <c r="I1845" s="97" t="s">
-        <v>3011</v>
       </c>
     </row>
     <row r="1846" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1846" s="97">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="B1846" s="1" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="C1846" s="97">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1846" s="97" t="s">
         <v>1713</v>
@@ -57028,10 +57050,10 @@
         <v>9</v>
       </c>
       <c r="G1846" s="97" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H1846" s="97" t="s">
-        <v>3795</v>
+        <v>3747</v>
       </c>
       <c r="I1846" s="97" t="s">
         <v>3011</v>
@@ -57039,306 +57061,348 @@
     </row>
     <row r="1847" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1847" s="97">
-        <v>2056</v>
-      </c>
-      <c r="B1847" s="98" t="s">
-        <v>3553</v>
+        <v>2055</v>
+      </c>
+      <c r="B1847" s="1" t="s">
+        <v>3552</v>
       </c>
       <c r="C1847" s="97">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1847" s="97" t="s">
-        <v>2794</v>
+        <v>1713</v>
+      </c>
+      <c r="E1847" s="97" t="s">
+        <v>2918</v>
       </c>
       <c r="F1847" s="97" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1847" s="97" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="H1847" s="97" t="s">
-        <v>3636</v>
+        <v>3795</v>
       </c>
       <c r="I1847" s="97" t="s">
-        <v>3637</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="1848" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1848" s="97">
-        <v>2057</v>
-      </c>
-      <c r="B1848" s="1" t="s">
-        <v>3554</v>
+        <v>2056</v>
+      </c>
+      <c r="B1848" s="98" t="s">
+        <v>3553</v>
       </c>
       <c r="C1848" s="97">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D1848" s="97" t="s">
-        <v>1710</v>
+        <v>2794</v>
       </c>
       <c r="F1848" s="97" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1848" s="97" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H1848" s="97" t="s">
-        <v>3558</v>
+        <v>3636</v>
       </c>
       <c r="I1848" s="97" t="s">
-        <v>2983</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="1849" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1849" s="97">
-        <v>2058</v>
-      </c>
-      <c r="B1849" s="98" t="s">
-        <v>3555</v>
+        <v>2057</v>
+      </c>
+      <c r="B1849" s="1" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C1849" s="97">
+        <v>1</v>
+      </c>
+      <c r="D1849" s="97" t="s">
+        <v>1710</v>
+      </c>
+      <c r="F1849" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1849" s="97" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1849" s="97" t="s">
+        <v>3558</v>
+      </c>
+      <c r="I1849" s="97" t="s">
+        <v>2983</v>
       </c>
     </row>
     <row r="1850" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1850" s="97">
+        <v>2058</v>
+      </c>
+      <c r="B1850" s="98" t="s">
+        <v>3555</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1851" s="97">
         <v>2059</v>
       </c>
-      <c r="B1850" s="98" t="s">
+      <c r="B1851" s="98" t="s">
         <v>3556</v>
       </c>
     </row>
-    <row r="1851" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1851" s="94">
+    <row r="1852" spans="1:9" s="94" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1852" s="94">
         <v>2060</v>
       </c>
-      <c r="B1851" s="98" t="s">
+      <c r="B1852" s="98" t="s">
         <v>3557</v>
       </c>
-      <c r="C1851" s="94">
-        <v>5</v>
-      </c>
-      <c r="D1851" s="94" t="s">
+      <c r="C1852" s="94">
+        <v>5</v>
+      </c>
+      <c r="D1852" s="94" t="s">
         <v>1711</v>
       </c>
-      <c r="F1851" s="94" t="s">
+      <c r="F1852" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="G1851" s="94" t="s">
+      <c r="G1852" s="94" t="s">
         <v>121</v>
       </c>
-      <c r="H1851" s="94" t="s">
+      <c r="H1852" s="94" t="s">
         <v>3590</v>
       </c>
-      <c r="I1851" s="94" t="s">
+      <c r="I1852" s="94" t="s">
         <v>3297</v>
       </c>
     </row>
-    <row r="1852" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1852" s="109">
+    <row r="1853" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1853" s="109">
         <v>2061</v>
       </c>
-      <c r="B1852" s="1" t="s">
+      <c r="B1853" s="1" t="s">
         <v>3735</v>
       </c>
-      <c r="C1852" s="109">
+      <c r="C1853" s="109">
         <v>2</v>
       </c>
-      <c r="D1852" s="109" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1852" s="109" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1852" s="109" t="s">
+      <c r="D1853" s="109" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1853" s="109" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1853" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="H1852" s="109" t="s">
+      <c r="H1853" s="109" t="s">
         <v>3736</v>
       </c>
-      <c r="I1852" s="109" t="s">
+      <c r="I1853" s="109" t="s">
         <v>3027</v>
-      </c>
-    </row>
-    <row r="1853" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1853" s="100">
-        <v>2062</v>
-      </c>
-      <c r="B1853" s="1" t="s">
-        <v>3615</v>
-      </c>
-      <c r="F1853" s="100" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="1854" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1854" s="100">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="B1854" s="1" t="s">
-        <v>3616</v>
-      </c>
-      <c r="C1854" s="100">
-        <v>2</v>
-      </c>
-      <c r="D1854" s="100" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1854" s="100" t="s">
-        <v>2918</v>
+        <v>3615</v>
       </c>
       <c r="F1854" s="100" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1854" s="100" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1854" s="100" t="s">
-        <v>3807</v>
-      </c>
-      <c r="I1854" s="100" t="s">
-        <v>2983</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1855" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1855" s="100">
-        <v>2064</v>
-      </c>
-      <c r="B1855" s="98" t="s">
-        <v>3617</v>
+        <v>2063</v>
+      </c>
+      <c r="B1855" s="1" t="s">
+        <v>3616</v>
+      </c>
+      <c r="C1855" s="100">
+        <v>2</v>
+      </c>
+      <c r="D1855" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1855" s="100" t="s">
+        <v>2918</v>
+      </c>
+      <c r="F1855" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1855" s="100" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1855" s="100" t="s">
+        <v>3807</v>
+      </c>
+      <c r="I1855" s="100" t="s">
+        <v>2983</v>
       </c>
     </row>
     <row r="1856" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1856" s="100">
-        <v>2065</v>
-      </c>
-      <c r="B1856" s="1" t="s">
-        <v>3618</v>
-      </c>
-      <c r="C1856" s="100">
-        <v>4</v>
-      </c>
-      <c r="D1856" s="100" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1856" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1856" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1856" s="100" t="s">
-        <v>3619</v>
-      </c>
-      <c r="I1856" s="100" t="s">
-        <v>3613</v>
+        <v>2064</v>
+      </c>
+      <c r="B1856" s="98" t="s">
+        <v>3617</v>
       </c>
     </row>
     <row r="1857" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1857" s="100">
-        <v>2068</v>
+        <v>2065</v>
       </c>
       <c r="B1857" s="1" t="s">
-        <v>3620</v>
+        <v>3618</v>
       </c>
       <c r="C1857" s="100">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1857" s="100" t="s">
         <v>1713</v>
       </c>
       <c r="F1857" s="100" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1857" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1857" s="100" t="s">
+        <v>3619</v>
+      </c>
+      <c r="I1857" s="100" t="s">
+        <v>3613</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1858" s="120">
+        <v>2067</v>
+      </c>
+      <c r="B1858" s="1" t="s">
+        <v>3823</v>
+      </c>
+      <c r="C1858" s="120">
+        <v>4</v>
+      </c>
+      <c r="D1858" s="120" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1858" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1858" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="H1857" s="100" t="s">
-        <v>3692</v>
-      </c>
-      <c r="I1857" s="100" t="s">
-        <v>2983</v>
-      </c>
-    </row>
-    <row r="1858" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1858" s="100">
-        <v>2069</v>
-      </c>
-      <c r="B1858" s="1" t="s">
-        <v>3633</v>
+      <c r="H1858" s="120" t="s">
+        <v>3824</v>
+      </c>
+      <c r="I1858" s="120" t="s">
+        <v>3244</v>
       </c>
     </row>
     <row r="1859" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1859" s="100">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="B1859" s="1" t="s">
-        <v>3632</v>
+        <v>3620</v>
+      </c>
+      <c r="C1859" s="100">
+        <v>1</v>
+      </c>
+      <c r="D1859" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1859" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1859" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1859" s="100" t="s">
+        <v>3692</v>
+      </c>
+      <c r="I1859" s="100" t="s">
+        <v>2983</v>
       </c>
     </row>
     <row r="1860" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1860" s="100">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="B1860" s="1" t="s">
-        <v>3631</v>
-      </c>
-      <c r="C1860" s="100">
-        <v>5</v>
-      </c>
-      <c r="D1860" s="100" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1860" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1860" s="100" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1860" s="100" t="s">
-        <v>3634</v>
-      </c>
-      <c r="I1860" s="100" t="s">
-        <v>3635</v>
+        <v>3633</v>
       </c>
     </row>
     <row r="1861" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1861" s="100">
-        <v>2073</v>
+        <v>2070</v>
       </c>
       <c r="B1861" s="1" t="s">
-        <v>3630</v>
+        <v>3632</v>
       </c>
       <c r="C1861" s="100">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1861" s="100" t="s">
         <v>1713</v>
       </c>
+      <c r="E1861" s="100" t="s">
+        <v>2918</v>
+      </c>
       <c r="F1861" s="100" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1861" s="100" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H1861" s="100" t="s">
-        <v>3723</v>
+        <v>3825</v>
       </c>
       <c r="I1861" s="100" t="s">
-        <v>2983</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="1862" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1862" s="100">
-        <v>2074</v>
+        <v>2071</v>
       </c>
       <c r="B1862" s="1" t="s">
-        <v>3629</v>
+        <v>3631</v>
+      </c>
+      <c r="C1862" s="100">
+        <v>5</v>
+      </c>
+      <c r="D1862" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1862" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1862" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1862" s="100" t="s">
+        <v>3634</v>
+      </c>
+      <c r="I1862" s="100" t="s">
+        <v>3635</v>
       </c>
     </row>
     <row r="1863" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1863" s="100">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="B1863" s="1" t="s">
-        <v>3628</v>
+        <v>3630</v>
       </c>
       <c r="C1863" s="100">
         <v>2</v>
@@ -57346,28 +57410,25 @@
       <c r="D1863" s="100" t="s">
         <v>1713</v>
       </c>
-      <c r="E1863" s="100" t="s">
-        <v>2918</v>
-      </c>
       <c r="F1863" s="100" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1863" s="100" t="s">
         <v>21</v>
       </c>
       <c r="H1863" s="100" t="s">
-        <v>3703</v>
+        <v>3723</v>
       </c>
       <c r="I1863" s="100" t="s">
-        <v>3027</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="1864" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1864" s="100">
-        <v>2076</v>
+        <v>2074</v>
       </c>
       <c r="B1864" s="1" t="s">
-        <v>3626</v>
+        <v>3629</v>
       </c>
       <c r="C1864" s="100">
         <v>4</v>
@@ -57375,174 +57436,195 @@
       <c r="D1864" s="100" t="s">
         <v>1713</v>
       </c>
-      <c r="E1864" s="100" t="s">
+      <c r="F1864" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1864" s="100" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1864" s="100" t="s">
+        <v>3821</v>
+      </c>
+      <c r="I1864" s="100" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1865" s="100">
+        <v>2075</v>
+      </c>
+      <c r="B1865" s="1" t="s">
+        <v>3628</v>
+      </c>
+      <c r="C1865" s="100">
+        <v>2</v>
+      </c>
+      <c r="D1865" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1865" s="100" t="s">
         <v>2918</v>
       </c>
-      <c r="F1864" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1864" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1864" s="100" t="s">
-        <v>3627</v>
-      </c>
-    </row>
-    <row r="1865" spans="1:9" s="107" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1865" s="107">
-        <v>2077</v>
-      </c>
-      <c r="B1865" s="1" t="s">
-        <v>3724</v>
-      </c>
-      <c r="C1865" s="107">
-        <v>3</v>
-      </c>
-      <c r="D1865" s="107" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1865" s="107" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1865" s="107" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1865" s="107" t="s">
-        <v>3725</v>
-      </c>
-      <c r="I1865" s="107" t="s">
-        <v>3224</v>
+      <c r="F1865" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1865" s="100" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1865" s="100" t="s">
+        <v>3703</v>
+      </c>
+      <c r="I1865" s="100" t="s">
+        <v>3027</v>
       </c>
     </row>
     <row r="1866" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1866" s="100">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="B1866" s="1" t="s">
-        <v>3625</v>
-      </c>
-    </row>
-    <row r="1867" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1867" s="100">
-        <v>2079</v>
+        <v>3626</v>
+      </c>
+      <c r="C1866" s="100">
+        <v>4</v>
+      </c>
+      <c r="D1866" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1866" s="100" t="s">
+        <v>2918</v>
+      </c>
+      <c r="F1866" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1866" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1866" s="100" t="s">
+        <v>3627</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:9" s="107" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1867" s="107">
+        <v>2077</v>
       </c>
       <c r="B1867" s="1" t="s">
-        <v>3624</v>
-      </c>
-      <c r="C1867" s="100">
-        <v>2</v>
-      </c>
-      <c r="D1867" s="100" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1867" s="100" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1867" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1867" s="100" t="s">
-        <v>3685</v>
-      </c>
-      <c r="I1867" s="100" t="s">
-        <v>2983</v>
+        <v>3724</v>
+      </c>
+      <c r="C1867" s="107">
+        <v>3</v>
+      </c>
+      <c r="D1867" s="107" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1867" s="107" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1867" s="107" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1867" s="107" t="s">
+        <v>3725</v>
+      </c>
+      <c r="I1867" s="107" t="s">
+        <v>3224</v>
       </c>
     </row>
     <row r="1868" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1868" s="100">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="B1868" s="1" t="s">
-        <v>3623</v>
-      </c>
-      <c r="C1868" s="100">
-        <v>2</v>
-      </c>
-      <c r="D1868" s="100" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1868" s="100" t="s">
-        <v>2918</v>
-      </c>
-      <c r="F1868" s="100" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1868" s="100" t="s">
-        <v>455</v>
-      </c>
-      <c r="H1868" s="100" t="s">
-        <v>3790</v>
-      </c>
-      <c r="I1868" s="100" t="s">
-        <v>3011</v>
+        <v>3625</v>
       </c>
     </row>
     <row r="1869" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1869" s="100">
+        <v>2079</v>
+      </c>
+      <c r="B1869" s="1" t="s">
+        <v>3624</v>
+      </c>
+      <c r="C1869" s="100">
+        <v>2</v>
+      </c>
+      <c r="D1869" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1869" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1869" s="100" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1869" s="100" t="s">
+        <v>3685</v>
+      </c>
+      <c r="I1869" s="100" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1870" s="100">
+        <v>2080</v>
+      </c>
+      <c r="B1870" s="1" t="s">
+        <v>3623</v>
+      </c>
+      <c r="C1870" s="100">
+        <v>2</v>
+      </c>
+      <c r="D1870" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1870" s="100" t="s">
+        <v>2918</v>
+      </c>
+      <c r="F1870" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1870" s="100" t="s">
+        <v>455</v>
+      </c>
+      <c r="H1870" s="100" t="s">
+        <v>3790</v>
+      </c>
+      <c r="I1870" s="100" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1871" s="100">
         <v>2081</v>
       </c>
-      <c r="B1869" s="1" t="s">
+      <c r="B1871" s="1" t="s">
         <v>3621</v>
       </c>
-      <c r="C1869" s="100">
+      <c r="C1871" s="100">
         <v>4</v>
       </c>
-      <c r="D1869" s="100" t="s">
+      <c r="D1871" s="100" t="s">
         <v>1711</v>
       </c>
-      <c r="F1869" s="100" t="s">
+      <c r="F1871" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="G1869" s="100" t="s">
+      <c r="G1871" s="100" t="s">
         <v>121</v>
       </c>
-      <c r="H1869" s="100" t="s">
+      <c r="H1871" s="100" t="s">
         <v>3622</v>
       </c>
-      <c r="I1869" s="100" t="s">
+      <c r="I1871" s="100" t="s">
         <v>3009</v>
-      </c>
-    </row>
-    <row r="1870" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1870" s="104">
-        <v>2083</v>
-      </c>
-      <c r="B1870" s="1" t="s">
-        <v>3671</v>
-      </c>
-    </row>
-    <row r="1871" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1871" s="104">
-        <v>2085</v>
-      </c>
-      <c r="B1871" s="1" t="s">
-        <v>3672</v>
-      </c>
-      <c r="C1871" s="104">
-        <v>2</v>
-      </c>
-      <c r="D1871" s="104" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1871" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1871" s="104" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1871" s="104" t="s">
-        <v>3673</v>
-      </c>
-      <c r="I1871" s="104" t="s">
-        <v>2983</v>
       </c>
     </row>
     <row r="1872" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1872" s="104">
-        <v>2086</v>
+        <v>2083</v>
       </c>
       <c r="B1872" s="1" t="s">
-        <v>3674</v>
+        <v>3671</v>
       </c>
       <c r="C1872" s="104">
         <v>2</v>
@@ -57550,14 +57632,17 @@
       <c r="D1872" s="104" t="s">
         <v>1713</v>
       </c>
+      <c r="E1872" s="104" t="s">
+        <v>2918</v>
+      </c>
       <c r="F1872" s="104" t="s">
         <v>9</v>
       </c>
       <c r="G1872" s="104" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H1872" s="104" t="s">
-        <v>3726</v>
+        <v>3826</v>
       </c>
       <c r="I1872" s="104" t="s">
         <v>2983</v>
@@ -57565,455 +57650,473 @@
     </row>
     <row r="1873" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1873" s="104">
-        <v>2087</v>
+        <v>2085</v>
       </c>
       <c r="B1873" s="1" t="s">
-        <v>3675</v>
+        <v>3672</v>
+      </c>
+      <c r="C1873" s="104">
+        <v>2</v>
+      </c>
+      <c r="D1873" s="104" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1873" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1873" s="104" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1873" s="104" t="s">
+        <v>3673</v>
+      </c>
+      <c r="I1873" s="104" t="s">
+        <v>2983</v>
       </c>
     </row>
     <row r="1874" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1874" s="104">
-        <v>2088</v>
+        <v>2086</v>
       </c>
       <c r="B1874" s="1" t="s">
-        <v>3676</v>
+        <v>3674</v>
       </c>
       <c r="C1874" s="104">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1874" s="104" t="s">
         <v>1713</v>
       </c>
       <c r="F1874" s="104" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1874" s="104" t="s">
         <v>21</v>
       </c>
       <c r="H1874" s="104" t="s">
-        <v>3677</v>
+        <v>3726</v>
       </c>
       <c r="I1874" s="104" t="s">
-        <v>3027</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="1875" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1875" s="104">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="B1875" s="1" t="s">
-        <v>3678</v>
-      </c>
-      <c r="C1875" s="104">
-        <v>1</v>
-      </c>
-      <c r="D1875" s="104" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1875" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1875" s="104" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1875" s="104" t="s">
-        <v>3679</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="1876" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1876" s="104">
-        <v>2090</v>
+        <v>2088</v>
       </c>
       <c r="B1876" s="1" t="s">
-        <v>3680</v>
+        <v>3676</v>
       </c>
       <c r="C1876" s="104">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1876" s="104" t="s">
         <v>1713</v>
       </c>
       <c r="F1876" s="104" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G1876" s="104" t="s">
         <v>21</v>
       </c>
       <c r="H1876" s="104" t="s">
-        <v>3681</v>
+        <v>3677</v>
       </c>
       <c r="I1876" s="104" t="s">
-        <v>2983</v>
+        <v>3027</v>
       </c>
     </row>
     <row r="1877" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1877" s="104">
-        <v>2091</v>
-      </c>
-      <c r="B1877" s="98" t="s">
-        <v>3682</v>
+        <v>2089</v>
+      </c>
+      <c r="B1877" s="1" t="s">
+        <v>3678</v>
       </c>
       <c r="C1877" s="104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1877" s="104" t="s">
         <v>1713</v>
       </c>
       <c r="F1877" s="104" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1877" s="104" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H1877" s="104" t="s">
-        <v>3796</v>
-      </c>
-      <c r="I1877" s="104" t="s">
-        <v>2983</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="1878" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1878" s="104">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="B1878" s="1" t="s">
-        <v>3683</v>
+        <v>3680</v>
       </c>
       <c r="C1878" s="104">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1878" s="104" t="s">
         <v>1713</v>
       </c>
-      <c r="E1878" s="104" t="s">
-        <v>2906</v>
-      </c>
       <c r="F1878" s="104" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1878" s="104" t="s">
-        <v>187</v>
+        <v>21</v>
       </c>
       <c r="H1878" s="104" t="s">
-        <v>3704</v>
+        <v>3681</v>
       </c>
       <c r="I1878" s="104" t="s">
-        <v>3011</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="1879" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1879" s="104">
+        <v>2091</v>
+      </c>
+      <c r="B1879" s="98" t="s">
+        <v>3682</v>
+      </c>
+      <c r="C1879" s="104">
+        <v>2</v>
+      </c>
+      <c r="D1879" s="104" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1879" s="104" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1879" s="104" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1879" s="104" t="s">
+        <v>3796</v>
+      </c>
+      <c r="I1879" s="104" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1880" s="104">
+        <v>2092</v>
+      </c>
+      <c r="B1880" s="1" t="s">
+        <v>3683</v>
+      </c>
+      <c r="C1880" s="104">
+        <v>4</v>
+      </c>
+      <c r="D1880" s="104" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1880" s="104" t="s">
+        <v>2906</v>
+      </c>
+      <c r="F1880" s="104" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1880" s="104" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1880" s="104" t="s">
+        <v>3704</v>
+      </c>
+      <c r="I1880" s="104" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1881" s="104">
         <v>2093</v>
       </c>
-      <c r="B1879" s="1" t="s">
+      <c r="B1881" s="1" t="s">
         <v>3684</v>
       </c>
     </row>
-    <row r="1880" spans="1:9" s="107" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1880" s="107">
+    <row r="1882" spans="1:9" s="107" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1882" s="107">
         <v>2094</v>
       </c>
-      <c r="B1880" s="1" t="s">
+      <c r="B1882" s="1" t="s">
         <v>3727</v>
       </c>
-      <c r="C1880" s="107">
+      <c r="C1882" s="107">
         <v>2</v>
       </c>
-      <c r="D1880" s="107" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1880" s="107" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1880" s="107" t="s">
+      <c r="D1882" s="107" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1882" s="107" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1882" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="H1880" s="107" t="s">
+      <c r="H1882" s="107" t="s">
         <v>3725</v>
       </c>
-      <c r="I1880" s="107" t="s">
+      <c r="I1882" s="107" t="s">
         <v>3728</v>
       </c>
     </row>
-    <row r="1881" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1881" s="117">
+    <row r="1883" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1883" s="117">
         <v>2095</v>
       </c>
-      <c r="B1881" s="1" t="s">
+      <c r="B1883" s="1" t="s">
         <v>3806</v>
       </c>
-    </row>
-    <row r="1882" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1882" s="112">
+      <c r="C1883" s="117">
+        <v>2</v>
+      </c>
+      <c r="D1883" s="117" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1883" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1883" s="117" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1883" s="117" t="s">
+        <v>3822</v>
+      </c>
+      <c r="I1883" s="117" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1884" s="112">
         <v>2096</v>
       </c>
-      <c r="B1882" s="98" t="s">
+      <c r="B1884" s="98" t="s">
         <v>3760</v>
       </c>
-      <c r="C1882" s="112">
+      <c r="C1884" s="112">
         <v>3</v>
       </c>
-      <c r="D1882" s="112" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1882" s="112" t="s">
+      <c r="D1884" s="112" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1884" s="112" t="s">
         <v>2918</v>
       </c>
-      <c r="F1882" s="112" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1882" s="112" t="s">
+      <c r="F1884" s="112" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1884" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="H1882" s="112" t="s">
+      <c r="H1884" s="112" t="s">
         <v>3761</v>
       </c>
-      <c r="I1882" s="112" t="s">
+      <c r="I1884" s="112" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1883" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1883" s="109">
+    <row r="1885" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1885" s="109">
         <v>2097</v>
       </c>
-      <c r="B1883" s="1" t="s">
+      <c r="B1885" s="1" t="s">
         <v>3739</v>
       </c>
-      <c r="C1883" s="109">
+      <c r="C1885" s="109">
         <v>4</v>
       </c>
-      <c r="D1883" s="109" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1883" s="109" t="s">
+      <c r="D1885" s="109" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1885" s="109" t="s">
         <v>2918</v>
       </c>
-      <c r="F1883" s="109" t="s">
+      <c r="F1885" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="G1883" s="109" t="s">
+      <c r="G1885" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="H1883" s="109" t="s">
+      <c r="H1885" s="109" t="s">
         <v>3740</v>
       </c>
-      <c r="I1883" s="109" t="s">
+      <c r="I1885" s="109" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1884" spans="1:9" s="114" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1884" s="114">
+    <row r="1886" spans="1:9" s="114" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1886" s="114">
         <v>2098</v>
       </c>
-      <c r="B1884" s="1" t="s">
+      <c r="B1886" s="1" t="s">
         <v>3777</v>
       </c>
-      <c r="C1884" s="114">
+      <c r="C1886" s="114">
         <v>3</v>
       </c>
-      <c r="D1884" s="114" t="s">
+      <c r="D1886" s="114" t="s">
         <v>1706</v>
       </c>
-      <c r="F1884" s="114" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1884" s="114" t="s">
+      <c r="F1886" s="114" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1886" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="H1884" s="114" t="s">
+      <c r="H1886" s="114" t="s">
         <v>3778</v>
       </c>
-      <c r="I1884" s="114" t="s">
+      <c r="I1886" s="114" t="s">
         <v>3011</v>
       </c>
     </row>
-    <row r="1885" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1885" s="112">
+    <row r="1887" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1887" s="112">
         <v>2099</v>
       </c>
-      <c r="B1885" s="98" t="s">
+      <c r="B1887" s="98" t="s">
         <v>3762</v>
       </c>
-      <c r="C1885" s="112">
+      <c r="C1887" s="112">
         <v>3</v>
       </c>
-      <c r="D1885" s="112" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1885" s="112" t="s">
+      <c r="D1887" s="112" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1887" s="112" t="s">
         <v>2918</v>
       </c>
-      <c r="F1885" s="112" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1885" s="112" t="s">
+      <c r="F1887" s="112" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1887" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="H1885" s="112" t="s">
+      <c r="H1887" s="112" t="s">
         <v>3763</v>
       </c>
-      <c r="I1885" s="112" t="s">
+      <c r="I1887" s="112" t="s">
         <v>3011</v>
       </c>
     </row>
-    <row r="1886" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1886" s="117">
+    <row r="1888" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1888" s="117">
         <v>2100</v>
       </c>
-      <c r="B1886" s="1" t="s">
+      <c r="B1888" s="1" t="s">
         <v>3805</v>
       </c>
-      <c r="C1886" s="117">
+      <c r="C1888" s="117">
         <v>2</v>
       </c>
-      <c r="D1886" s="117" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1886" s="117" t="s">
+      <c r="D1888" s="117" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1888" s="117" t="s">
         <v>2918</v>
       </c>
-      <c r="F1886" s="117" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1886" s="117" t="s">
+      <c r="F1888" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1888" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="H1886" s="117" t="s">
+      <c r="H1888" s="117" t="s">
         <v>3816</v>
       </c>
-      <c r="I1886" s="117" t="s">
+      <c r="I1888" s="117" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1887" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1887" s="117">
+    <row r="1889" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1889" s="117">
         <v>2101</v>
       </c>
-      <c r="B1887" s="1" t="s">
+      <c r="B1889" s="1" t="s">
         <v>3804</v>
       </c>
     </row>
-    <row r="1888" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1888" s="115">
+    <row r="1890" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1890" s="115">
         <v>2102</v>
       </c>
-      <c r="B1888" s="1" t="s">
+      <c r="B1890" s="1" t="s">
         <v>3779</v>
       </c>
-      <c r="C1888" s="115">
+      <c r="C1890" s="115">
         <v>4</v>
       </c>
-      <c r="D1888" s="115" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E1888" s="115" t="s">
+      <c r="D1890" s="115" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1890" s="115" t="s">
         <v>2918</v>
       </c>
-      <c r="F1888" s="115" t="s">
+      <c r="F1890" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="G1888" s="115" t="s">
+      <c r="G1890" s="115" t="s">
         <v>455</v>
       </c>
-      <c r="H1888" s="115" t="s">
+      <c r="H1890" s="115" t="s">
         <v>3780</v>
       </c>
-      <c r="I1888" s="115" t="s">
+      <c r="I1890" s="115" t="s">
         <v>3011</v>
       </c>
     </row>
-    <row r="1889" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1889" s="112">
+    <row r="1891" spans="1:9" s="112" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1891" s="112">
         <v>2103</v>
       </c>
-      <c r="B1889" s="1" t="s">
+      <c r="B1891" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C1889" s="112">
+      <c r="C1891" s="112">
         <v>1</v>
       </c>
-      <c r="D1889" s="112" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1889" s="112" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1889" s="112" t="s">
+      <c r="D1891" s="112" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1891" s="112" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1891" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="H1889" s="112" t="s">
+      <c r="H1891" s="112" t="s">
         <v>3765</v>
       </c>
-      <c r="I1889" s="112" t="s">
+      <c r="I1891" s="112" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1890" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1890" s="117">
+    <row r="1892" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1892" s="117">
         <v>2104</v>
       </c>
-      <c r="B1890" s="1" t="s">
+      <c r="B1892" s="1" t="s">
         <v>3803</v>
-      </c>
-    </row>
-    <row r="1891" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1891" s="117">
-        <v>2105</v>
-      </c>
-      <c r="B1891" s="1" t="s">
-        <v>3797</v>
-      </c>
-      <c r="C1891" s="117">
-        <v>2</v>
-      </c>
-      <c r="D1891" s="117" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1891" s="117" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1891" s="117" t="s">
-        <v>619</v>
-      </c>
-      <c r="H1891" s="117" t="s">
-        <v>3798</v>
-      </c>
-      <c r="I1891" s="117" t="s">
-        <v>2983</v>
-      </c>
-    </row>
-    <row r="1892" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1892" s="115">
-        <v>2106</v>
-      </c>
-      <c r="B1892" s="98" t="s">
-        <v>3786</v>
-      </c>
-      <c r="C1892" s="115">
-        <v>4</v>
-      </c>
-      <c r="D1892" s="115" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1892" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1892" s="115" t="s">
-        <v>619</v>
-      </c>
-      <c r="H1892" s="115" t="s">
-        <v>3787</v>
-      </c>
-      <c r="I1892" s="115" t="s">
-        <v>3011</v>
       </c>
     </row>
     <row r="1893" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1893" s="117">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="B1893" s="1" t="s">
-        <v>3799</v>
+        <v>3797</v>
       </c>
       <c r="C1893" s="117">
         <v>2</v>
@@ -58028,7 +58131,7 @@
         <v>619</v>
       </c>
       <c r="H1893" s="117" t="s">
-        <v>3800</v>
+        <v>3798</v>
       </c>
       <c r="I1893" s="117" t="s">
         <v>2983</v>
@@ -58036,148 +58139,218 @@
     </row>
     <row r="1894" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1894" s="115">
-        <v>2108</v>
-      </c>
-      <c r="B1894" s="1" t="s">
-        <v>3784</v>
+        <v>2106</v>
+      </c>
+      <c r="B1894" s="98" t="s">
+        <v>3786</v>
       </c>
       <c r="C1894" s="115">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1894" s="115" t="s">
         <v>1713</v>
       </c>
       <c r="F1894" s="115" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1894" s="115" t="s">
-        <v>36</v>
+        <v>619</v>
       </c>
       <c r="H1894" s="115" t="s">
-        <v>3785</v>
+        <v>3787</v>
       </c>
       <c r="I1894" s="115" t="s">
-        <v>2983</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="1895" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1895" s="117">
+        <v>2107</v>
+      </c>
+      <c r="B1895" s="1" t="s">
+        <v>3799</v>
+      </c>
+      <c r="C1895" s="117">
+        <v>2</v>
+      </c>
+      <c r="D1895" s="117" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1895" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1895" s="117" t="s">
+        <v>619</v>
+      </c>
+      <c r="H1895" s="117" t="s">
+        <v>3800</v>
+      </c>
+      <c r="I1895" s="117" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1896" s="115">
+        <v>2108</v>
+      </c>
+      <c r="B1896" s="1" t="s">
+        <v>3784</v>
+      </c>
+      <c r="C1896" s="115">
+        <v>1</v>
+      </c>
+      <c r="D1896" s="115" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1896" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1896" s="115" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1896" s="115" t="s">
+        <v>3785</v>
+      </c>
+      <c r="I1896" s="115" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1897" s="117">
         <v>2109</v>
       </c>
-      <c r="B1895" s="1" t="s">
+      <c r="B1897" s="1" t="s">
         <v>3802</v>
       </c>
-    </row>
-    <row r="1896" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1896" s="117">
+      <c r="C1897" s="117">
+        <v>2</v>
+      </c>
+      <c r="D1897" s="117" t="s">
+        <v>1710</v>
+      </c>
+      <c r="F1897" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1897" s="117" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1897" s="117" t="s">
+        <v>2359</v>
+      </c>
+      <c r="I1897" s="117" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1898" s="117">
         <v>2110</v>
       </c>
-      <c r="B1896" s="98" t="s">
+      <c r="B1898" s="98" t="s">
         <v>3801</v>
       </c>
-      <c r="C1896" s="117">
+      <c r="C1898" s="117">
         <v>2</v>
       </c>
-      <c r="D1896" s="117" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1896" s="117" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1896" s="117" t="s">
+      <c r="D1898" s="117" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1898" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1898" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="H1896" s="117" t="s">
+      <c r="H1898" s="117" t="s">
         <v>3817</v>
       </c>
-      <c r="I1896" s="117" t="s">
+      <c r="I1898" s="117" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1897" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1897" s="100">
+    <row r="1899" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1899" s="100">
         <v>2111</v>
       </c>
-      <c r="B1897" s="98" t="s">
+      <c r="B1899" s="98" t="s">
         <v>3781</v>
       </c>
-      <c r="C1897" s="100">
+      <c r="C1899" s="100">
         <v>4</v>
       </c>
-      <c r="D1897" s="100" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1897" s="100" t="s">
+      <c r="D1899" s="100" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1899" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="G1897" s="100" t="s">
+      <c r="G1899" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="H1897" s="100" t="s">
+      <c r="H1899" s="100" t="s">
         <v>3782</v>
       </c>
-      <c r="I1897" s="100" t="s">
+      <c r="I1899" s="100" t="s">
         <v>3011</v>
       </c>
     </row>
-    <row r="1898" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1898" s="118">
+    <row r="1900" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1900" s="118">
         <v>2113</v>
       </c>
-      <c r="B1898" s="1" t="s">
+      <c r="B1900" s="1" t="s">
         <v>3809</v>
       </c>
-      <c r="C1898" s="118">
+      <c r="C1900" s="118">
         <v>2</v>
       </c>
-      <c r="D1898" s="118" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F1898" s="118" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1898" s="118" t="s">
+      <c r="D1900" s="118" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F1900" s="118" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1900" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="H1898" s="118" t="s">
+      <c r="H1900" s="118" t="s">
         <v>3810</v>
       </c>
-      <c r="I1898" s="118" t="s">
+      <c r="I1900" s="118" t="s">
         <v>2983</v>
       </c>
     </row>
-    <row r="1899" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1899" s="98"/>
-    </row>
-    <row r="1900" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1900" s="120" t="s">
+    <row r="1901" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1901" s="98"/>
+    </row>
+    <row r="1902" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1902" s="121" t="s">
         <v>1714</v>
       </c>
-      <c r="B1900" s="120"/>
-      <c r="C1900" s="120"/>
-      <c r="D1900" s="120"/>
-      <c r="E1900" s="120"/>
-      <c r="F1900" s="120"/>
-      <c r="G1900" s="120"/>
-      <c r="H1900" s="120"/>
-    </row>
-    <row r="1901" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1901" s="121" t="s">
+      <c r="B1902" s="121"/>
+      <c r="C1902" s="121"/>
+      <c r="D1902" s="121"/>
+      <c r="E1902" s="121"/>
+      <c r="F1902" s="121"/>
+      <c r="G1902" s="121"/>
+      <c r="H1902" s="121"/>
+    </row>
+    <row r="1903" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1903" s="122" t="s">
         <v>2745</v>
       </c>
-      <c r="B1901" s="121"/>
-      <c r="C1901" s="121"/>
-      <c r="D1901" s="121"/>
-      <c r="E1901" s="121"/>
-      <c r="F1901" s="121"/>
-      <c r="G1901" s="121"/>
-      <c r="H1901" s="121"/>
+      <c r="B1903" s="122"/>
+      <c r="C1903" s="122"/>
+      <c r="D1903" s="122"/>
+      <c r="E1903" s="122"/>
+      <c r="F1903" s="122"/>
+      <c r="G1903" s="122"/>
+      <c r="H1903" s="122"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1901" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1903" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1900:H1900"/>
-    <mergeCell ref="A1901:H1901"/>
+    <mergeCell ref="A1902:H1902"/>
+    <mergeCell ref="A1903:H1903"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -59761,36 +59934,36 @@
     <hyperlink ref="B1836" r:id="rId1579" display="https://leetcode.com/problems/simple-bank-system" xr:uid="{2D5E5F4E-907C-4728-A902-7D10B6514920}"/>
     <hyperlink ref="B1837" r:id="rId1580" xr:uid="{D5EDB803-F602-4ABD-9E68-1113D2A2A40A}"/>
     <hyperlink ref="B1838" r:id="rId1581" display="https://leetcode.com/problems/second-minimum-time-to-reach-destination" xr:uid="{6ACF2F93-7EDE-4F1E-AA71-8112DE7ABF63}"/>
-    <hyperlink ref="B1839" r:id="rId1582" display="https://leetcode.com/problems/number-of-valid-words-in-a-sentence" xr:uid="{BCE84EEA-54FF-4E5A-9955-C02227468918}"/>
-    <hyperlink ref="B1840" r:id="rId1583" display="https://leetcode.com/problems/next-greater-numerically-balanced-number" xr:uid="{9FD27FA2-0676-4160-BC27-2E0F89E752A4}"/>
-    <hyperlink ref="B1841" r:id="rId1584" display="https://leetcode.com/problems/count-nodes-with-the-highest-score" xr:uid="{F7F71D15-EF63-42B1-BD71-1EB9E5AFAAEC}"/>
-    <hyperlink ref="B1842" r:id="rId1585" display="https://leetcode.com/problems/parallel-courses-iii" xr:uid="{10B385A3-FDEE-4123-AC9C-4F7EF85C3982}"/>
-    <hyperlink ref="B1844" r:id="rId1586" display="https://leetcode.com/problems/kth-distinct-string-in-an-array" xr:uid="{C8004808-B8BB-4E39-B2BC-980704DF7D4E}"/>
-    <hyperlink ref="B1845" r:id="rId1587" display="https://leetcode.com/problems/two-best-non-overlapping-events" xr:uid="{F29009B4-E1BD-443F-8480-1775C9682530}"/>
-    <hyperlink ref="B1846" r:id="rId1588" display="https://leetcode.com/problems/plates-between-candles" xr:uid="{A118D0C8-0288-4E36-8D25-A4774630A76B}"/>
-    <hyperlink ref="B1847" r:id="rId1589" display="https://leetcode.com/problems/number-of-valid-move-combinations-on-chessboard" xr:uid="{AEC5E678-B4A1-445C-B8F4-DE74236CAC53}"/>
-    <hyperlink ref="B1848" r:id="rId1590" display="https://leetcode.com/problems/smallest-index-with-equal-value" xr:uid="{E7A8904C-9D51-49EC-A910-9EE0B60892CD}"/>
-    <hyperlink ref="B1849" r:id="rId1591" display="https://leetcode.com/problems/find-the-minimum-and-maximum-number-of-nodes-between-critical-points" xr:uid="{0AC3439C-F776-4E62-B906-4FEDA4902BCA}"/>
-    <hyperlink ref="B1850" r:id="rId1592" display="https://leetcode.com/problems/minimum-operations-to-convert-number" xr:uid="{E72F9ECF-969F-4732-A4BD-D6C619ECE110}"/>
-    <hyperlink ref="B1851" r:id="rId1593" display="https://leetcode.com/problems/check-if-an-original-string-exists-given-two-encoded-strings" xr:uid="{0E2F5BE6-4251-43B0-902E-665D40B08A24}"/>
+    <hyperlink ref="B1840" r:id="rId1582" display="https://leetcode.com/problems/number-of-valid-words-in-a-sentence" xr:uid="{BCE84EEA-54FF-4E5A-9955-C02227468918}"/>
+    <hyperlink ref="B1841" r:id="rId1583" display="https://leetcode.com/problems/next-greater-numerically-balanced-number" xr:uid="{9FD27FA2-0676-4160-BC27-2E0F89E752A4}"/>
+    <hyperlink ref="B1842" r:id="rId1584" display="https://leetcode.com/problems/count-nodes-with-the-highest-score" xr:uid="{F7F71D15-EF63-42B1-BD71-1EB9E5AFAAEC}"/>
+    <hyperlink ref="B1843" r:id="rId1585" display="https://leetcode.com/problems/parallel-courses-iii" xr:uid="{10B385A3-FDEE-4123-AC9C-4F7EF85C3982}"/>
+    <hyperlink ref="B1845" r:id="rId1586" display="https://leetcode.com/problems/kth-distinct-string-in-an-array" xr:uid="{C8004808-B8BB-4E39-B2BC-980704DF7D4E}"/>
+    <hyperlink ref="B1846" r:id="rId1587" display="https://leetcode.com/problems/two-best-non-overlapping-events" xr:uid="{F29009B4-E1BD-443F-8480-1775C9682530}"/>
+    <hyperlink ref="B1847" r:id="rId1588" display="https://leetcode.com/problems/plates-between-candles" xr:uid="{A118D0C8-0288-4E36-8D25-A4774630A76B}"/>
+    <hyperlink ref="B1848" r:id="rId1589" display="https://leetcode.com/problems/number-of-valid-move-combinations-on-chessboard" xr:uid="{AEC5E678-B4A1-445C-B8F4-DE74236CAC53}"/>
+    <hyperlink ref="B1849" r:id="rId1590" display="https://leetcode.com/problems/smallest-index-with-equal-value" xr:uid="{E7A8904C-9D51-49EC-A910-9EE0B60892CD}"/>
+    <hyperlink ref="B1850" r:id="rId1591" display="https://leetcode.com/problems/find-the-minimum-and-maximum-number-of-nodes-between-critical-points" xr:uid="{0AC3439C-F776-4E62-B906-4FEDA4902BCA}"/>
+    <hyperlink ref="B1851" r:id="rId1592" display="https://leetcode.com/problems/minimum-operations-to-convert-number" xr:uid="{E72F9ECF-969F-4732-A4BD-D6C619ECE110}"/>
+    <hyperlink ref="B1852" r:id="rId1593" display="https://leetcode.com/problems/check-if-an-original-string-exists-given-two-encoded-strings" xr:uid="{0E2F5BE6-4251-43B0-902E-665D40B08A24}"/>
     <hyperlink ref="B605" r:id="rId1594" display="https://leetcode.com/problems/robot-return-to-origin" xr:uid="{F90BDC0D-FA70-41A1-A23C-878C1C1627B7}"/>
     <hyperlink ref="B1726" r:id="rId1595" display="https://leetcode.com/problems/number-of-wonderful-substrings" xr:uid="{9423D426-30DB-4078-B23A-2E94A3A02AA3}"/>
-    <hyperlink ref="B1853" r:id="rId1596" display="https://leetcode.com/problems/count-vowel-substrings-of-a-string" xr:uid="{7FCC5F29-7C62-4374-B0A9-2ABCC18104A5}"/>
-    <hyperlink ref="B1854" r:id="rId1597" display="https://leetcode.com/problems/vowels-of-all-substrings" xr:uid="{46C4B1C2-365D-40D1-B052-A17550370995}"/>
-    <hyperlink ref="B1855" r:id="rId1598" display="https://leetcode.com/problems/minimized-maximum-of-products-distributed-to-any-store" xr:uid="{10A9FF8C-86AD-4D91-B020-A08498C62B37}"/>
-    <hyperlink ref="B1856" r:id="rId1599" display="https://leetcode.com/problems/maximum-path-quality-of-a-graph" xr:uid="{0B2D1EBB-160D-4ED4-8B55-CE1BD0869125}"/>
-    <hyperlink ref="B1857" r:id="rId1600" xr:uid="{BB09D143-36DB-4DAD-8C50-2059028F1FE9}"/>
-    <hyperlink ref="B1869" r:id="rId1601" display="https://leetcode.com/problems/sum-of-k-mirror-numbers" xr:uid="{F0650F51-568A-4717-BC19-ABB1B6FFFDEC}"/>
-    <hyperlink ref="B1868" r:id="rId1602" display="https://leetcode.com/problems/range-frequency-queries" xr:uid="{1E229C2A-34B8-4A81-B0C6-5A3AD71CCF39}"/>
-    <hyperlink ref="B1867" r:id="rId1603" display="https://leetcode.com/problems/watering-plants" xr:uid="{A7EF29DE-DB3D-46A9-905D-C48EDDF5C996}"/>
-    <hyperlink ref="B1866" r:id="rId1604" display="https://leetcode.com/problems/two-furthest-houses-with-different-colors" xr:uid="{37BA5D04-9AF4-4ECA-A97D-39D90F766EF4}"/>
-    <hyperlink ref="B1864" r:id="rId1605" display="https://leetcode.com/problems/process-restricted-friend-requests" xr:uid="{C99C6F0C-8C7B-4E62-8AC6-A5A8F82F0410}"/>
-    <hyperlink ref="B1863" r:id="rId1606" display="https://leetcode.com/problems/decode-the-slanted-ciphertext" xr:uid="{2350D7FD-D03A-41C6-90F8-670D922F7173}"/>
-    <hyperlink ref="B1862" r:id="rId1607" display="https://leetcode.com/problems/reverse-nodes-in-even-length-groups" xr:uid="{D9BBD886-602B-46F9-97D3-B4CD877C9459}"/>
-    <hyperlink ref="B1861" r:id="rId1608" display="https://leetcode.com/problems/time-needed-to-buy-tickets" xr:uid="{B62F15D1-AFD5-4E07-A951-E2E37A83C871}"/>
-    <hyperlink ref="B1860" r:id="rId1609" display="https://leetcode.com/problems/maximum-number-of-tasks-you-can-assign" xr:uid="{953AE036-BD94-4947-9D3F-2342559633D4}"/>
-    <hyperlink ref="B1859" r:id="rId1610" display="https://leetcode.com/problems/most-beautiful-item-for-each-query" xr:uid="{285617BD-2F3A-412A-8F56-D5D10E9F2FA7}"/>
-    <hyperlink ref="B1858" r:id="rId1611" display="https://leetcode.com/problems/walking-robot-simulation-ii" xr:uid="{D2D1B95C-0388-40D9-8577-069CD220E305}"/>
+    <hyperlink ref="B1854" r:id="rId1596" display="https://leetcode.com/problems/count-vowel-substrings-of-a-string" xr:uid="{7FCC5F29-7C62-4374-B0A9-2ABCC18104A5}"/>
+    <hyperlink ref="B1855" r:id="rId1597" display="https://leetcode.com/problems/vowels-of-all-substrings" xr:uid="{46C4B1C2-365D-40D1-B052-A17550370995}"/>
+    <hyperlink ref="B1856" r:id="rId1598" display="https://leetcode.com/problems/minimized-maximum-of-products-distributed-to-any-store" xr:uid="{10A9FF8C-86AD-4D91-B020-A08498C62B37}"/>
+    <hyperlink ref="B1857" r:id="rId1599" display="https://leetcode.com/problems/maximum-path-quality-of-a-graph" xr:uid="{0B2D1EBB-160D-4ED4-8B55-CE1BD0869125}"/>
+    <hyperlink ref="B1859" r:id="rId1600" xr:uid="{BB09D143-36DB-4DAD-8C50-2059028F1FE9}"/>
+    <hyperlink ref="B1871" r:id="rId1601" display="https://leetcode.com/problems/sum-of-k-mirror-numbers" xr:uid="{F0650F51-568A-4717-BC19-ABB1B6FFFDEC}"/>
+    <hyperlink ref="B1870" r:id="rId1602" display="https://leetcode.com/problems/range-frequency-queries" xr:uid="{1E229C2A-34B8-4A81-B0C6-5A3AD71CCF39}"/>
+    <hyperlink ref="B1869" r:id="rId1603" display="https://leetcode.com/problems/watering-plants" xr:uid="{A7EF29DE-DB3D-46A9-905D-C48EDDF5C996}"/>
+    <hyperlink ref="B1868" r:id="rId1604" display="https://leetcode.com/problems/two-furthest-houses-with-different-colors" xr:uid="{37BA5D04-9AF4-4ECA-A97D-39D90F766EF4}"/>
+    <hyperlink ref="B1866" r:id="rId1605" display="https://leetcode.com/problems/process-restricted-friend-requests" xr:uid="{C99C6F0C-8C7B-4E62-8AC6-A5A8F82F0410}"/>
+    <hyperlink ref="B1865" r:id="rId1606" display="https://leetcode.com/problems/decode-the-slanted-ciphertext" xr:uid="{2350D7FD-D03A-41C6-90F8-670D922F7173}"/>
+    <hyperlink ref="B1864" r:id="rId1607" display="https://leetcode.com/problems/reverse-nodes-in-even-length-groups" xr:uid="{D9BBD886-602B-46F9-97D3-B4CD877C9459}"/>
+    <hyperlink ref="B1863" r:id="rId1608" display="https://leetcode.com/problems/time-needed-to-buy-tickets" xr:uid="{B62F15D1-AFD5-4E07-A951-E2E37A83C871}"/>
+    <hyperlink ref="B1862" r:id="rId1609" display="https://leetcode.com/problems/maximum-number-of-tasks-you-can-assign" xr:uid="{953AE036-BD94-4947-9D3F-2342559633D4}"/>
+    <hyperlink ref="B1861" r:id="rId1610" display="https://leetcode.com/problems/most-beautiful-item-for-each-query" xr:uid="{285617BD-2F3A-412A-8F56-D5D10E9F2FA7}"/>
+    <hyperlink ref="B1860" r:id="rId1611" display="https://leetcode.com/problems/walking-robot-simulation-ii" xr:uid="{D2D1B95C-0388-40D9-8577-069CD220E305}"/>
     <hyperlink ref="B1719" r:id="rId1612" display="https://leetcode.com/problems/game-of-nim" xr:uid="{F7C1BC10-B697-4EAB-BF17-994FAC810FD6}"/>
     <hyperlink ref="B1804" r:id="rId1613" display="https://leetcode.com/problems/subtree-removal-game-with-fibonacci-tree" xr:uid="{17B02D5B-1FCE-4E9C-8C56-6E4E46955393}"/>
     <hyperlink ref="B1733" r:id="rId1614" display="https://leetcode.com/problems/erect-the-fence-ii" xr:uid="{163A8356-4805-4487-9659-BAA81F2755CA}"/>
@@ -59798,16 +59971,16 @@
     <hyperlink ref="B1617" r:id="rId1616" display="https://leetcode.com/problems/maximize-the-beauty-of-the-garden" xr:uid="{4C08B654-05A0-43E7-823B-C1078A0C20EE}"/>
     <hyperlink ref="B1663" r:id="rId1617" display="https://leetcode.com/problems/next-palindrome-using-same-digits" xr:uid="{F261E6B6-D5B7-4AC3-A1A5-61C002B301AB}"/>
     <hyperlink ref="B1761" r:id="rId1618" display="https://leetcode.com/problems/minimum-time-for-k-virus-variants-to-spread" xr:uid="{C3148FB5-10D8-401C-A298-918872231696}"/>
-    <hyperlink ref="B1870" r:id="rId1619" display="https://leetcode.com/problems/substrings-that-begin-and-end-with-the-same-letter" xr:uid="{1A96836C-C517-44D4-BE69-C35A3422D314}"/>
-    <hyperlink ref="B1871" r:id="rId1620" display="https://leetcode.com/problems/count-common-words-with-one-occurrence" xr:uid="{630A6D17-E28C-4098-AB77-C747F784C276}"/>
-    <hyperlink ref="B1872" r:id="rId1621" display="https://leetcode.com/problems/minimum-number-of-buckets-required-to-collect-rainwater-from-houses" xr:uid="{EF3FA606-DDC8-4678-8304-ED307B2DEFA5}"/>
-    <hyperlink ref="B1873" r:id="rId1622" display="https://leetcode.com/problems/minimum-cost-homecoming-of-a-robot-in-a-grid" xr:uid="{EB28E187-BA64-4B07-A8AF-517C1E5B347D}"/>
-    <hyperlink ref="B1874" r:id="rId1623" display="https://leetcode.com/problems/count-fertile-pyramids-in-a-land" xr:uid="{A0AE5EA8-B452-4A97-AB6E-EE8BB9FC7139}"/>
-    <hyperlink ref="B1875" r:id="rId1624" display="https://leetcode.com/problems/find-target-indices-after-sorting-array" xr:uid="{2FACAB89-3C3B-4D3D-AE5D-A25342EA2DFE}"/>
-    <hyperlink ref="B1876" r:id="rId1625" display="https://leetcode.com/problems/k-radius-subarray-averages" xr:uid="{B1B5727F-2B0E-466D-88BC-9117D19D2707}"/>
-    <hyperlink ref="B1877" r:id="rId1626" display="https://leetcode.com/problems/removing-minimum-and-maximum-from-array" xr:uid="{2EF3E8B8-45ED-464B-BC2C-DDF6408612CE}"/>
-    <hyperlink ref="B1878" r:id="rId1627" display="https://leetcode.com/problems/find-all-people-with-secret" xr:uid="{68D82AB9-0DC2-4905-B285-710D207BC1F4}"/>
-    <hyperlink ref="B1879" r:id="rId1628" display="https://leetcode.com/problems/minimum-cost-to-reach-city-with-discounts" xr:uid="{F946E785-616E-4505-8314-3D44773E90A0}"/>
+    <hyperlink ref="B1872" r:id="rId1619" display="https://leetcode.com/problems/substrings-that-begin-and-end-with-the-same-letter" xr:uid="{1A96836C-C517-44D4-BE69-C35A3422D314}"/>
+    <hyperlink ref="B1873" r:id="rId1620" display="https://leetcode.com/problems/count-common-words-with-one-occurrence" xr:uid="{630A6D17-E28C-4098-AB77-C747F784C276}"/>
+    <hyperlink ref="B1874" r:id="rId1621" display="https://leetcode.com/problems/minimum-number-of-buckets-required-to-collect-rainwater-from-houses" xr:uid="{EF3FA606-DDC8-4678-8304-ED307B2DEFA5}"/>
+    <hyperlink ref="B1875" r:id="rId1622" display="https://leetcode.com/problems/minimum-cost-homecoming-of-a-robot-in-a-grid" xr:uid="{EB28E187-BA64-4B07-A8AF-517C1E5B347D}"/>
+    <hyperlink ref="B1876" r:id="rId1623" display="https://leetcode.com/problems/count-fertile-pyramids-in-a-land" xr:uid="{A0AE5EA8-B452-4A97-AB6E-EE8BB9FC7139}"/>
+    <hyperlink ref="B1877" r:id="rId1624" display="https://leetcode.com/problems/find-target-indices-after-sorting-array" xr:uid="{2FACAB89-3C3B-4D3D-AE5D-A25342EA2DFE}"/>
+    <hyperlink ref="B1878" r:id="rId1625" display="https://leetcode.com/problems/k-radius-subarray-averages" xr:uid="{B1B5727F-2B0E-466D-88BC-9117D19D2707}"/>
+    <hyperlink ref="B1879" r:id="rId1626" display="https://leetcode.com/problems/removing-minimum-and-maximum-from-array" xr:uid="{2EF3E8B8-45ED-464B-BC2C-DDF6408612CE}"/>
+    <hyperlink ref="B1880" r:id="rId1627" display="https://leetcode.com/problems/find-all-people-with-secret" xr:uid="{68D82AB9-0DC2-4905-B285-710D207BC1F4}"/>
+    <hyperlink ref="B1881" r:id="rId1628" display="https://leetcode.com/problems/minimum-cost-to-reach-city-with-discounts" xr:uid="{F946E785-616E-4505-8314-3D44773E90A0}"/>
     <hyperlink ref="B1690" r:id="rId1629" display="https://leetcode.com/problems/minimize-product-sum-of-two-arrays" xr:uid="{DB973D4E-5CC5-44D0-B497-F5D58E80E896}"/>
     <hyperlink ref="B1604" r:id="rId1630" display="https://leetcode.com/problems/sort-features-by-popularity" xr:uid="{0A19E2C6-068B-4B27-AA59-A0D28BDABF3B}"/>
     <hyperlink ref="B1742" r:id="rId1631" display="https://leetcode.com/problems/check-if-string-is-decomposable-into-value-equal-substrings" xr:uid="{BFF77354-A49F-4852-988D-F79B7794C549}"/>
@@ -59820,48 +59993,50 @@
     <hyperlink ref="B1791" r:id="rId1638" display="https://leetcode.com/problems/find-the-middle-index-in-array" xr:uid="{D5BD54BC-4C9D-4080-92AB-7E0AD5447197}"/>
     <hyperlink ref="B1790" r:id="rId1639" display="https://leetcode.com/problems/maximum-number-of-people-that-can-be-caught-in-tag" xr:uid="{3BF1B1EF-9567-40FA-BA27-DF380FD64512}"/>
     <hyperlink ref="B1817" r:id="rId1640" display="https://leetcode.com/problems/brightest-position-on-street" xr:uid="{69ADC44D-E8E3-492F-9021-9CFB8D96A649}"/>
-    <hyperlink ref="B1865" r:id="rId1641" display="https://leetcode.com/problems/paths-in-maze-that-lead-to-same-room" xr:uid="{2D8290E2-711B-4E9E-94BE-6E1693EE8078}"/>
-    <hyperlink ref="B1880" r:id="rId1642" display="https://leetcode.com/problems/finding-3-digit-even-numbers" xr:uid="{8AF3467E-9095-4911-85B4-C5C65A0F89DC}"/>
+    <hyperlink ref="B1867" r:id="rId1641" display="https://leetcode.com/problems/paths-in-maze-that-lead-to-same-room" xr:uid="{2D8290E2-711B-4E9E-94BE-6E1693EE8078}"/>
+    <hyperlink ref="B1882" r:id="rId1642" display="https://leetcode.com/problems/finding-3-digit-even-numbers" xr:uid="{8AF3467E-9095-4911-85B4-C5C65A0F89DC}"/>
     <hyperlink ref="B1622" r:id="rId1643" display="https://leetcode.com/problems/count-pairs-of-equal-substrings-with-minimum-difference" xr:uid="{C299AFD5-375F-453E-93F2-586F77C93D99}"/>
     <hyperlink ref="B1631" r:id="rId1644" display="https://leetcode.com/problems/implement-trie-ii-prefix-tree" xr:uid="{0FA20FE6-CB70-47B0-AE0C-73C2608CE4DE}"/>
-    <hyperlink ref="B1852" r:id="rId1645" display="https://leetcode.com/problems/number-of-spaces-cleaning-robot-cleaned" xr:uid="{1843E481-A377-4508-844C-1566B0EB6A81}"/>
+    <hyperlink ref="B1853" r:id="rId1645" display="https://leetcode.com/problems/number-of-spaces-cleaning-robot-cleaned" xr:uid="{1843E481-A377-4508-844C-1566B0EB6A81}"/>
     <hyperlink ref="B1676" r:id="rId1646" display="https://leetcode.com/problems/longest-word-with-all-prefixes" xr:uid="{0630A561-7DF9-4C20-99BC-717B5D8F07BC}"/>
-    <hyperlink ref="B1883" r:id="rId1647" display="https://leetcode.com/problems/valid-arrangement-of-pairs" xr:uid="{E627A316-ECC0-45DA-A6B4-61105C3B4B1A}"/>
+    <hyperlink ref="B1885" r:id="rId1647" display="https://leetcode.com/problems/valid-arrangement-of-pairs" xr:uid="{E627A316-ECC0-45DA-A6B4-61105C3B4B1A}"/>
     <hyperlink ref="B1490" r:id="rId1648" display="https://leetcode.com/problems/number-of-ways-to-form-a-target-string-given-a-dictionary" xr:uid="{FF624C95-49DF-4169-B628-19629A6F243A}"/>
     <hyperlink ref="B1685" r:id="rId1649" display="https://leetcode.com/problems/product-of-two-run-length-encoded-arrays" xr:uid="{6A748179-BE2C-43B5-937C-0971F2E9B84E}"/>
     <hyperlink ref="B1700" r:id="rId1650" display="https://leetcode.com/problems/count-pairs-in-two-arrays" xr:uid="{161319D6-6334-4E03-AC0B-73EEDE5AFBF7}"/>
     <hyperlink ref="B1747" r:id="rId1651" display="https://leetcode.com/problems/longest-common-subsequence-between-sorted-arrays" xr:uid="{AE4203E3-43C5-40FC-8B78-1EF6EFA8B799}"/>
     <hyperlink ref="B1785" r:id="rId1652" display="https://leetcode.com/problems/widest-pair-of-indices-with-equal-range-sum" xr:uid="{620D8C9E-B0DA-477A-AA3C-2F635E95F462}"/>
     <hyperlink ref="B1799" r:id="rId1653" display="https://leetcode.com/problems/smallest-greater-multiple-made-of-two-digits" xr:uid="{8B3267DC-2D98-4C8C-B245-BBD0849BCC1A}"/>
-    <hyperlink ref="B1882" r:id="rId1654" display="https://leetcode.com/problems/step-by-step-directions-from-a-binary-tree-node-to-another" xr:uid="{C5C7E5DC-8934-40E9-B69B-CF586656DD52}"/>
-    <hyperlink ref="B1885" r:id="rId1655" display="https://leetcode.com/problems/find-subsequence-of-length-k-with-the-largest-sum" xr:uid="{3847A2FB-3BFE-44B9-BED6-56D6ECB82D82}"/>
-    <hyperlink ref="B1889" r:id="rId1656" display="https://leetcode.com/problems/rings-and-rods" xr:uid="{23A44248-878B-4CE4-AE7B-E9FEE1091067}"/>
+    <hyperlink ref="B1884" r:id="rId1654" display="https://leetcode.com/problems/step-by-step-directions-from-a-binary-tree-node-to-another" xr:uid="{C5C7E5DC-8934-40E9-B69B-CF586656DD52}"/>
+    <hyperlink ref="B1887" r:id="rId1655" display="https://leetcode.com/problems/find-subsequence-of-length-k-with-the-largest-sum" xr:uid="{3847A2FB-3BFE-44B9-BED6-56D6ECB82D82}"/>
+    <hyperlink ref="B1891" r:id="rId1656" display="https://leetcode.com/problems/rings-and-rods" xr:uid="{23A44248-878B-4CE4-AE7B-E9FEE1091067}"/>
     <hyperlink ref="B1705" r:id="rId1657" display="https://leetcode.com/problems/cutting-ribbons" xr:uid="{131BC84C-8E0F-4AF9-87AB-7B89E638ABD5}"/>
     <hyperlink ref="B1776" r:id="rId1658" display="https://leetcode.com/problems/count-nodes-equal-to-sum-of-descendants" xr:uid="{BFF8F8A7-A6A0-4A49-A8FC-453653B4257B}"/>
-    <hyperlink ref="B1843" r:id="rId1659" display="https://leetcode.com/problems/minimum-cost-to-separate-sentence-into-rows" xr:uid="{2AC1A4DB-1946-4EA6-87C8-BFCBD335968E}"/>
+    <hyperlink ref="B1844" r:id="rId1659" display="https://leetcode.com/problems/minimum-cost-to-separate-sentence-into-rows" xr:uid="{2AC1A4DB-1946-4EA6-87C8-BFCBD335968E}"/>
     <hyperlink ref="B1353" r:id="rId1660" display="https://leetcode.com/problems/minimum-number-of-days-to-make-m-bouquets" xr:uid="{A226ED4B-9ECC-43EF-8EE3-94598D2C0FDF}"/>
     <hyperlink ref="B1414" r:id="rId1661" display="https://leetcode.com/problems/magnetic-force-between-two-balls" xr:uid="{7257B245-2713-4150-810D-6F2FA5EAEF89}"/>
     <hyperlink ref="B1728" r:id="rId1662" display="https://leetcode.com/problems/kth-smallest-subarray-sum" xr:uid="{9D83B952-41A0-405D-A753-C692921A798C}"/>
-    <hyperlink ref="B1884" r:id="rId1663" display="https://leetcode.com/problems/subsequence-of-size-k-with-the-largest-even-sum" xr:uid="{0645F7F4-851F-4A5B-876D-2F23B7F1CB18}"/>
-    <hyperlink ref="B1888" r:id="rId1664" display="https://leetcode.com/problems/sequentially-ordinal-rank-tracker" xr:uid="{4AEEE917-FC1A-4441-8FCC-AAB33045CAAF}"/>
-    <hyperlink ref="B1897" r:id="rId1665" display="https://leetcode.com/problems/minimum-operations-to-make-the-array-k-increasing" xr:uid="{0A30673F-4EF8-4DD1-9D82-A9D62C3B11FC}"/>
-    <hyperlink ref="B1894" r:id="rId1666" display="https://leetcode.com/problems/find-first-palindromic-string-in-the-array" xr:uid="{5BDD994B-8936-496C-9380-FC41DA3F9A69}"/>
-    <hyperlink ref="B1892" r:id="rId1667" display="https://leetcode.com/problems/maximum-fruits-harvested-after-at-most-k-steps" xr:uid="{4833F7C7-BB0A-45D9-B2EE-0435CC7E66B4}"/>
+    <hyperlink ref="B1886" r:id="rId1663" display="https://leetcode.com/problems/subsequence-of-size-k-with-the-largest-even-sum" xr:uid="{0645F7F4-851F-4A5B-876D-2F23B7F1CB18}"/>
+    <hyperlink ref="B1890" r:id="rId1664" display="https://leetcode.com/problems/sequentially-ordinal-rank-tracker" xr:uid="{4AEEE917-FC1A-4441-8FCC-AAB33045CAAF}"/>
+    <hyperlink ref="B1899" r:id="rId1665" display="https://leetcode.com/problems/minimum-operations-to-make-the-array-k-increasing" xr:uid="{0A30673F-4EF8-4DD1-9D82-A9D62C3B11FC}"/>
+    <hyperlink ref="B1896" r:id="rId1666" display="https://leetcode.com/problems/find-first-palindromic-string-in-the-array" xr:uid="{5BDD994B-8936-496C-9380-FC41DA3F9A69}"/>
+    <hyperlink ref="B1894" r:id="rId1667" display="https://leetcode.com/problems/maximum-fruits-harvested-after-at-most-k-steps" xr:uid="{4833F7C7-BB0A-45D9-B2EE-0435CC7E66B4}"/>
     <hyperlink ref="B1756" r:id="rId1668" display="https://leetcode.com/problems/maximum-of-minimum-values-in-all-subarrays" xr:uid="{6C5E9DC6-3B50-49DC-BA32-49B36A65631E}"/>
-    <hyperlink ref="B1891" r:id="rId1669" display="https://leetcode.com/problems/watering-plants-ii" xr:uid="{79ECD953-36CF-458D-946D-FCA45C267265}"/>
-    <hyperlink ref="B1893" r:id="rId1670" display="https://leetcode.com/problems/number-of-unique-flavors-after-sharing-k-candies" xr:uid="{8A15FC64-50EC-426A-8219-51F8F3F422B1}"/>
-    <hyperlink ref="B1896" r:id="rId1671" display="https://leetcode.com/problems/number-of-smooth-descent-periods-of-a-stock" xr:uid="{AB604653-CB6D-4FE8-949B-F9118F1FF4A9}"/>
-    <hyperlink ref="B1895" r:id="rId1672" display="https://leetcode.com/problems/adding-spaces-to-a-string" xr:uid="{88559B2E-A9F0-42CE-9D42-9875A4CCB6B6}"/>
-    <hyperlink ref="B1890" r:id="rId1673" display="https://leetcode.com/problems/sum-of-subarray-ranges" xr:uid="{14DB1AC6-E7C9-4533-B452-AB20E94B322C}"/>
-    <hyperlink ref="B1887" r:id="rId1674" display="https://leetcode.com/problems/detonate-the-maximum-bombs" xr:uid="{3354A4B4-953A-42B6-8A0E-05F8BB5CEF2A}"/>
-    <hyperlink ref="B1886" r:id="rId1675" display="https://leetcode.com/problems/find-good-days-to-rob-the-bank" xr:uid="{0F986755-A1C6-4B47-80BE-5140A48911DA}"/>
-    <hyperlink ref="B1881" r:id="rId1676" display="https://leetcode.com/problems/delete-the-middle-node-of-a-linked-list" xr:uid="{33F47B67-91EB-4460-B400-78D6212E468E}"/>
-    <hyperlink ref="B1898" r:id="rId1677" display="https://leetcode.com/problems/elements-in-array-after-removing-and-replacing-elements" xr:uid="{C65FB836-5A2E-4D03-94EF-C3385C2A46E2}"/>
+    <hyperlink ref="B1893" r:id="rId1669" display="https://leetcode.com/problems/watering-plants-ii" xr:uid="{79ECD953-36CF-458D-946D-FCA45C267265}"/>
+    <hyperlink ref="B1895" r:id="rId1670" display="https://leetcode.com/problems/number-of-unique-flavors-after-sharing-k-candies" xr:uid="{8A15FC64-50EC-426A-8219-51F8F3F422B1}"/>
+    <hyperlink ref="B1898" r:id="rId1671" display="https://leetcode.com/problems/number-of-smooth-descent-periods-of-a-stock" xr:uid="{AB604653-CB6D-4FE8-949B-F9118F1FF4A9}"/>
+    <hyperlink ref="B1897" r:id="rId1672" display="https://leetcode.com/problems/adding-spaces-to-a-string" xr:uid="{88559B2E-A9F0-42CE-9D42-9875A4CCB6B6}"/>
+    <hyperlink ref="B1892" r:id="rId1673" display="https://leetcode.com/problems/sum-of-subarray-ranges" xr:uid="{14DB1AC6-E7C9-4533-B452-AB20E94B322C}"/>
+    <hyperlink ref="B1889" r:id="rId1674" display="https://leetcode.com/problems/detonate-the-maximum-bombs" xr:uid="{3354A4B4-953A-42B6-8A0E-05F8BB5CEF2A}"/>
+    <hyperlink ref="B1888" r:id="rId1675" display="https://leetcode.com/problems/find-good-days-to-rob-the-bank" xr:uid="{0F986755-A1C6-4B47-80BE-5140A48911DA}"/>
+    <hyperlink ref="B1883" r:id="rId1676" display="https://leetcode.com/problems/delete-the-middle-node-of-a-linked-list" xr:uid="{33F47B67-91EB-4460-B400-78D6212E468E}"/>
+    <hyperlink ref="B1900" r:id="rId1677" display="https://leetcode.com/problems/elements-in-array-after-removing-and-replacing-elements" xr:uid="{C65FB836-5A2E-4D03-94EF-C3385C2A46E2}"/>
     <hyperlink ref="B1826" r:id="rId1678" display="https://leetcode.com/problems/count-subarrays-with-more-ones-than-zeros" xr:uid="{93F608F2-80AF-4898-8678-DD82BE752DF5}"/>
+    <hyperlink ref="B1839" r:id="rId1679" display="https://leetcode.com/problems/sort-linked-list-already-sorted-using-absolute-values" xr:uid="{64E70F0D-BEEE-4A0A-8111-8E54C2021B79}"/>
+    <hyperlink ref="B1858" r:id="rId1680" display="https://leetcode.com/problems/number-of-equal-count-substrings" xr:uid="{7AD31592-94A2-46AE-9592-F904EEAB0046}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1679"/>
-  <drawing r:id="rId1680"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1681"/>
+  <drawing r:id="rId1682"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in 2022 Jan first half
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93707E8F-3B30-4AB8-B658-9B9D80E1D757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF781B69-0134-49E2-83DA-2791768F09A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1910</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$1960</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10733" uniqueCount="3852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10853" uniqueCount="3890">
   <si>
     <t>Difficulty</t>
   </si>
@@ -11593,6 +11593,120 @@
   </si>
   <si>
     <t xml:space="preserve">Prefix hashset </t>
+  </si>
+  <si>
+    <t>Minimum Operations to Remove Adjacent Ones in Matrix</t>
+  </si>
+  <si>
+    <t>Max Bipartite Matching</t>
+  </si>
+  <si>
+    <t>N^3</t>
+  </si>
+  <si>
+    <t>Check if All A's Appears Before All B's</t>
+  </si>
+  <si>
+    <t>Number of Laser Beams in a Bank</t>
+  </si>
+  <si>
+    <t>Calculate devices current and previous</t>
+  </si>
+  <si>
+    <t>Destroying Asteroids</t>
+  </si>
+  <si>
+    <t>Sort asteriod, take from small to large</t>
+  </si>
+  <si>
+    <t>Maximum Employees to Be Invited to a Meeting</t>
+  </si>
+  <si>
+    <t>Extend from cross favroite and loop</t>
+  </si>
+  <si>
+    <t>Remove All Ones With Row and Column Flips</t>
+  </si>
+  <si>
+    <t>flip first row and first column</t>
+  </si>
+  <si>
+    <t>Capitalize the Title</t>
+  </si>
+  <si>
+    <t>Split string to word then captilization</t>
+  </si>
+  <si>
+    <t>Maximum Twin Sum of a Linked List</t>
+  </si>
+  <si>
+    <t>Find the middle and reverse second half</t>
+  </si>
+  <si>
+    <t>Longest Palindrome by Concatenating Two </t>
+  </si>
+  <si>
+    <t>Store reversed word and match, add self reversed word as center</t>
+  </si>
+  <si>
+    <t>Stamping the Grid</t>
+  </si>
+  <si>
+    <t>2D array sub sum as zero as stamp position, each free cell must be covered by a stamp position</t>
+  </si>
+  <si>
+    <t>Check if Every Row and Column Contains All Numbers</t>
+  </si>
+  <si>
+    <t>Store numbers in hash set in row and column</t>
+  </si>
+  <si>
+    <t>2134. Minimum Swaps to Group All 1's Together II</t>
+  </si>
+  <si>
+    <t>Two pointer slides window, extended as twice of size</t>
+  </si>
+  <si>
+    <t>Count Words Obtained After Adding a Letter</t>
+  </si>
+  <si>
+    <t>Sort characters in source and target and assemble it with one character less</t>
+  </si>
+  <si>
+    <t>Earliest Possible Day of Full Bloom</t>
+  </si>
+  <si>
+    <t>Start to plant the one with longest growing time</t>
+  </si>
+  <si>
+    <t>Pour Water Between Buckets to Make Water Levels Equal</t>
+  </si>
+  <si>
+    <t>Calculate more water against less water with loss rate</t>
+  </si>
+  <si>
+    <t>Divide a String Into Groups of Size k</t>
+  </si>
+  <si>
+    <t>Divide string by round up k</t>
+  </si>
+  <si>
+    <t>Minimum Moves to Reach Target Score</t>
+  </si>
+  <si>
+    <t>Calculate from target to source</t>
+  </si>
+  <si>
+    <t>Solving Questions With Brainpower</t>
+  </si>
+  <si>
+    <t>Maximum Running Time of N Computers</t>
+  </si>
+  <si>
+    <t>Look forward and calculate accumulated points</t>
+  </si>
+  <si>
+    <t>Search by running time, for batteries with more time, we will waste some.</t>
   </si>
 </sst>
 </file>
@@ -11637,7 +11751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -11745,6 +11859,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -12155,10 +12270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1910"/>
+  <dimension ref="A1:J1960"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D950" sqref="D950"/>
+    <sheetView tabSelected="1" topLeftCell="A1909" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1927" sqref="A1927"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -58895,35 +59010,640 @@
         <v>2996</v>
       </c>
     </row>
-    <row r="1909" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1909" s="123" t="s">
+    <row r="1909" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1909" s="123">
+        <v>2123</v>
+      </c>
+      <c r="B1909" s="98" t="s">
+        <v>3852</v>
+      </c>
+      <c r="C1909" s="123">
+        <v>4</v>
+      </c>
+      <c r="D1909" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F1909" s="123" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1909" s="123" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1909" s="123" t="s">
+        <v>3853</v>
+      </c>
+      <c r="I1909" s="123" t="s">
+        <v>3854</v>
+      </c>
+    </row>
+    <row r="1910" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1910" s="123">
+        <v>2124</v>
+      </c>
+      <c r="B1910" s="1" t="s">
+        <v>3855</v>
+      </c>
+      <c r="C1910" s="123">
+        <v>1</v>
+      </c>
+      <c r="D1910" s="123" t="s">
+        <v>1697</v>
+      </c>
+      <c r="F1910" s="123" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1910" s="123" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1910" s="123" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1910" s="123" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="1911" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1911" s="123">
+        <v>2125</v>
+      </c>
+      <c r="B1911" s="1" t="s">
+        <v>3856</v>
+      </c>
+      <c r="C1911" s="123">
+        <v>2</v>
+      </c>
+      <c r="D1911" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F1911" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1911" s="123" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1911" s="123" t="s">
+        <v>3857</v>
+      </c>
+      <c r="I1911" s="123" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="1912" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1912" s="123">
+        <v>2126</v>
+      </c>
+      <c r="B1912" s="1" t="s">
+        <v>3858</v>
+      </c>
+      <c r="C1912" s="123">
+        <v>2</v>
+      </c>
+      <c r="D1912" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E1912" s="123" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F1912" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1912" s="123" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1912" s="123" t="s">
+        <v>3859</v>
+      </c>
+      <c r="I1912" s="123" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="1913" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1913" s="123">
+        <v>2127</v>
+      </c>
+      <c r="B1913" s="98" t="s">
+        <v>3860</v>
+      </c>
+      <c r="C1913" s="123">
+        <v>5</v>
+      </c>
+      <c r="D1913" s="123" t="s">
+        <v>2779</v>
+      </c>
+      <c r="F1913" s="123" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1913" s="123" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1913" s="123" t="s">
+        <v>3861</v>
+      </c>
+      <c r="I1913" s="123" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="1914" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1914" s="123">
+        <v>2128</v>
+      </c>
+      <c r="B1914" s="1" t="s">
+        <v>3862</v>
+      </c>
+      <c r="C1914" s="123">
+        <v>2</v>
+      </c>
+      <c r="D1914" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F1914" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1914" s="123" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1914" s="123" t="s">
+        <v>3863</v>
+      </c>
+      <c r="I1914" s="123" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="1915" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1915" s="123">
+        <v>2129</v>
+      </c>
+      <c r="B1915" s="1" t="s">
+        <v>3864</v>
+      </c>
+      <c r="C1915" s="123">
+        <v>2</v>
+      </c>
+      <c r="D1915" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E1915" s="123" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F1915" s="123" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1915" s="123" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1915" s="123" t="s">
+        <v>3865</v>
+      </c>
+      <c r="I1915" s="123" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="1916" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1916" s="123">
+        <v>2130</v>
+      </c>
+      <c r="B1916" s="1" t="s">
+        <v>3866</v>
+      </c>
+      <c r="C1916" s="123">
+        <v>3</v>
+      </c>
+      <c r="D1916" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F1916" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1916" s="123" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1916" s="123" t="s">
+        <v>3867</v>
+      </c>
+      <c r="I1916" s="123" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="1917" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1917" s="123">
+        <v>2131</v>
+      </c>
+      <c r="B1917" s="1" t="s">
+        <v>3868</v>
+      </c>
+      <c r="C1917" s="123">
+        <v>2</v>
+      </c>
+      <c r="D1917" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F1917" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1917" s="123" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1917" s="123" t="s">
+        <v>3869</v>
+      </c>
+      <c r="I1917" s="123" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="1918" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1918" s="123">
+        <v>2132</v>
+      </c>
+      <c r="B1918" s="1" t="s">
+        <v>3870</v>
+      </c>
+      <c r="C1918" s="123">
+        <v>4</v>
+      </c>
+      <c r="D1918" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E1918" s="123" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F1918" s="123" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1918" s="123" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1918" s="123" t="s">
+        <v>3871</v>
+      </c>
+      <c r="I1918" s="123" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="1919" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1919" s="123">
+        <v>2133</v>
+      </c>
+      <c r="B1919" s="98" t="s">
+        <v>3872</v>
+      </c>
+      <c r="C1919" s="123">
+        <v>2</v>
+      </c>
+      <c r="D1919" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F1919" s="123" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1919" s="123" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1919" s="123" t="s">
+        <v>3873</v>
+      </c>
+      <c r="I1919" s="123" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="1920" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1920" s="123">
+        <v>2134</v>
+      </c>
+      <c r="B1920" s="98" t="s">
+        <v>3874</v>
+      </c>
+      <c r="C1920" s="123">
+        <v>3</v>
+      </c>
+      <c r="D1920" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F1920" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1920" s="123" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1920" s="123" t="s">
+        <v>3875</v>
+      </c>
+      <c r="I1920" s="123" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="1921" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1921" s="123">
+        <v>2135</v>
+      </c>
+      <c r="B1921" s="98" t="s">
+        <v>3876</v>
+      </c>
+      <c r="C1921" s="123">
+        <v>3</v>
+      </c>
+      <c r="D1921" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E1921" s="123" t="s">
+        <v>2892</v>
+      </c>
+      <c r="F1921" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1921" s="123" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1921" s="123" t="s">
+        <v>3877</v>
+      </c>
+      <c r="I1921" s="123" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1922" s="123">
+        <v>2136</v>
+      </c>
+      <c r="B1922" s="1" t="s">
+        <v>3878</v>
+      </c>
+      <c r="C1922" s="123">
+        <v>4</v>
+      </c>
+      <c r="D1922" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F1922" s="123" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1922" s="123" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1922" s="123" t="s">
+        <v>3879</v>
+      </c>
+      <c r="I1922" s="123" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="1923" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1923" s="123">
+        <v>2137</v>
+      </c>
+      <c r="B1923" s="1" t="s">
+        <v>3880</v>
+      </c>
+      <c r="C1923" s="123">
+        <v>4</v>
+      </c>
+      <c r="D1923" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E1923" s="123" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F1923" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1923" s="123" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1923" s="123" t="s">
+        <v>3881</v>
+      </c>
+      <c r="I1923" s="123" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="1924" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1924" s="123">
+        <v>2138</v>
+      </c>
+      <c r="B1924" s="1" t="s">
+        <v>3882</v>
+      </c>
+      <c r="C1924" s="123">
+        <v>1</v>
+      </c>
+      <c r="D1924" s="123" t="s">
+        <v>1697</v>
+      </c>
+      <c r="F1924" s="123" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1924" s="123" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1924" s="123" t="s">
+        <v>3883</v>
+      </c>
+      <c r="I1924" s="123" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1925" s="123">
+        <v>2139</v>
+      </c>
+      <c r="B1925" s="1" t="s">
+        <v>3884</v>
+      </c>
+      <c r="C1925" s="123">
+        <v>2</v>
+      </c>
+      <c r="D1925" s="123" t="s">
+        <v>1698</v>
+      </c>
+      <c r="F1925" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1925" s="123" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1925" s="123" t="s">
+        <v>3885</v>
+      </c>
+      <c r="I1925" s="123" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="1926" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1926" s="123">
+        <v>2140</v>
+      </c>
+      <c r="B1926" s="1" t="s">
+        <v>3886</v>
+      </c>
+      <c r="C1926" s="123">
+        <v>3</v>
+      </c>
+      <c r="D1926" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E1926" s="123" t="s">
+        <v>2892</v>
+      </c>
+      <c r="F1926" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1926" s="123" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1926" s="123" t="s">
+        <v>3888</v>
+      </c>
+      <c r="I1926" s="123" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="1927" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1927" s="123">
+        <v>2141</v>
+      </c>
+      <c r="B1927" s="1" t="s">
+        <v>3887</v>
+      </c>
+      <c r="C1927" s="123">
+        <v>4</v>
+      </c>
+      <c r="D1927" s="123" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F1927" s="123" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1927" s="123" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1927" s="123" t="s">
+        <v>3889</v>
+      </c>
+      <c r="I1927" s="123" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="1928" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1928" s="1"/>
+    </row>
+    <row r="1929" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1929" s="1"/>
+    </row>
+    <row r="1930" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1930" s="1"/>
+    </row>
+    <row r="1931" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1931" s="1"/>
+    </row>
+    <row r="1932" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1932" s="1"/>
+    </row>
+    <row r="1933" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1933" s="1"/>
+    </row>
+    <row r="1934" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1934" s="1"/>
+    </row>
+    <row r="1935" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1935" s="1"/>
+    </row>
+    <row r="1936" spans="1:9" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1936" s="1"/>
+    </row>
+    <row r="1937" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1937" s="1"/>
+    </row>
+    <row r="1938" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1938" s="1"/>
+    </row>
+    <row r="1939" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1939" s="1"/>
+    </row>
+    <row r="1940" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1940" s="1"/>
+    </row>
+    <row r="1941" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1941" s="1"/>
+    </row>
+    <row r="1942" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1942" s="1"/>
+    </row>
+    <row r="1943" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1943" s="1"/>
+    </row>
+    <row r="1944" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1944" s="1"/>
+    </row>
+    <row r="1945" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1945" s="1"/>
+    </row>
+    <row r="1946" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1946" s="1"/>
+    </row>
+    <row r="1947" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1947" s="1"/>
+    </row>
+    <row r="1948" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1948" s="1"/>
+    </row>
+    <row r="1949" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1949" s="1"/>
+    </row>
+    <row r="1950" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1950" s="1"/>
+    </row>
+    <row r="1951" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1951" s="1"/>
+    </row>
+    <row r="1952" spans="2:2" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1952" s="1"/>
+    </row>
+    <row r="1953" spans="1:8" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1953" s="1"/>
+    </row>
+    <row r="1954" spans="1:8" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1954" s="1"/>
+    </row>
+    <row r="1955" spans="1:8" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1955" s="1"/>
+    </row>
+    <row r="1956" spans="1:8" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1956" s="1"/>
+    </row>
+    <row r="1957" spans="1:8" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1957" s="1"/>
+    </row>
+    <row r="1958" spans="1:8" s="123" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1958" s="1"/>
+    </row>
+    <row r="1959" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1959" s="124" t="s">
         <v>1701</v>
       </c>
-      <c r="B1909" s="123"/>
-      <c r="C1909" s="123"/>
-      <c r="D1909" s="123"/>
-      <c r="E1909" s="123"/>
-      <c r="F1909" s="123"/>
-      <c r="G1909" s="123"/>
-      <c r="H1909" s="123"/>
-    </row>
-    <row r="1910" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1910" s="124" t="s">
+      <c r="B1959" s="124"/>
+      <c r="C1959" s="124"/>
+      <c r="D1959" s="124"/>
+      <c r="E1959" s="124"/>
+      <c r="F1959" s="124"/>
+      <c r="G1959" s="124"/>
+      <c r="H1959" s="124"/>
+    </row>
+    <row r="1960" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1960" s="125" t="s">
         <v>2730</v>
       </c>
-      <c r="B1910" s="124"/>
-      <c r="C1910" s="124"/>
-      <c r="D1910" s="124"/>
-      <c r="E1910" s="124"/>
-      <c r="F1910" s="124"/>
-      <c r="G1910" s="124"/>
-      <c r="H1910" s="124"/>
+      <c r="B1960" s="125"/>
+      <c r="C1960" s="125"/>
+      <c r="D1960" s="125"/>
+      <c r="E1960" s="125"/>
+      <c r="F1960" s="125"/>
+      <c r="G1960" s="125"/>
+      <c r="H1960" s="125"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1910" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J1960" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A1909:H1909"/>
-    <mergeCell ref="A1910:H1910"/>
+    <mergeCell ref="A1959:H1959"/>
+    <mergeCell ref="A1960:H1960"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -60616,10 +61336,29 @@
     <hyperlink ref="B1908" r:id="rId1688" display="https://leetcode.com/problems/recover-the-original-array" xr:uid="{303F328C-7B7B-4BD7-9A91-8792773D19BA}"/>
     <hyperlink ref="B1418" r:id="rId1689" display="https://leetcode.com/problems/minimum-number-of-vertices-to-reach-all-nodes" xr:uid="{561B729C-79E8-45A4-80AB-7C6CC13D44FC}"/>
     <hyperlink ref="B1364" r:id="rId1690" display="https://leetcode.com/problems/parallel-courses-ii" xr:uid="{9BC004B7-26A5-42F5-BB2E-3238C95DFE97}"/>
+    <hyperlink ref="B1909" r:id="rId1691" display="https://leetcode.com/problems/minimum-operations-to-remove-adjacent-ones-in-matrix" xr:uid="{C083BD97-028C-43F8-860C-7B6BC37F7369}"/>
+    <hyperlink ref="B1910" r:id="rId1692" display="https://leetcode.com/problems/check-if-all-as-appears-before-all-bs" xr:uid="{65793955-95B2-47D7-B65B-37BBACD5E3C3}"/>
+    <hyperlink ref="B1911" r:id="rId1693" display="https://leetcode.com/problems/number-of-laser-beams-in-a-bank" xr:uid="{D2F40FF1-43F2-499F-8452-AD641215BFE5}"/>
+    <hyperlink ref="B1912" r:id="rId1694" display="https://leetcode.com/problems/destroying-asteroids" xr:uid="{A7F585DF-2C71-40CD-8F18-1FA0BFD16CAC}"/>
+    <hyperlink ref="B1913" r:id="rId1695" display="https://leetcode.com/problems/maximum-employees-to-be-invited-to-a-meeting" xr:uid="{9F73F08B-934F-4659-931C-9ED00C2E207C}"/>
+    <hyperlink ref="B1914" r:id="rId1696" display="https://leetcode.com/problems/remove-all-ones-with-row-and-column-flips" xr:uid="{8241506F-9D85-4E9B-902E-90FDC7E1958E}"/>
+    <hyperlink ref="B1915" r:id="rId1697" display="https://leetcode.com/problems/capitalize-the-title" xr:uid="{D09E46A9-3DB7-41A4-9460-E4A2741B7D2F}"/>
+    <hyperlink ref="B1916" r:id="rId1698" display="https://leetcode.com/problems/maximum-twin-sum-of-a-linked-list" xr:uid="{72F6EE39-0AF3-4DE1-BD22-598C647F139D}"/>
+    <hyperlink ref="B1917" r:id="rId1699" display="https://leetcode.com/problems/longest-palindrome-by-concatenating-two-letter-words" xr:uid="{A54FD5F3-25AD-4BC4-8C51-3A8EA12A786D}"/>
+    <hyperlink ref="B1918" r:id="rId1700" display="https://leetcode.com/problems/stamping-the-grid" xr:uid="{966A836D-C417-41A3-ADBE-EDA52E134C51}"/>
+    <hyperlink ref="B1919" r:id="rId1701" display="https://leetcode.com/problems/check-if-every-row-and-column-contains-all-numbers" xr:uid="{A88A8C58-7789-4165-93ED-20D90B2AE733}"/>
+    <hyperlink ref="B1920" r:id="rId1702" display="https://leetcode.com/problems/minimum-swaps-to-group-all-1s-together-ii" xr:uid="{88C05BEF-A1FB-422F-B6A0-020DEFC92955}"/>
+    <hyperlink ref="B1921" r:id="rId1703" display="https://leetcode.com/problems/count-words-obtained-after-adding-a-letter" xr:uid="{976FFA72-1E5A-4F33-8784-0785B623D921}"/>
+    <hyperlink ref="B1922" r:id="rId1704" display="https://leetcode.com/problems/earliest-possible-day-of-full-bloom" xr:uid="{C54191BF-2B34-4BC1-94B1-20EEB4A28E17}"/>
+    <hyperlink ref="B1923" r:id="rId1705" display="https://leetcode.com/problems/pour-water-between-buckets-to-make-water-levels-equal" xr:uid="{6BD4DEDD-3F01-4C0F-AB0C-EB505E4B4CC2}"/>
+    <hyperlink ref="B1924" r:id="rId1706" display="https://leetcode.com/problems/divide-a-string-into-groups-of-size-k" xr:uid="{9D21FD17-1E4A-4ED2-9D34-B7FF5DDA43DF}"/>
+    <hyperlink ref="B1925" r:id="rId1707" display="https://leetcode.com/problems/minimum-moves-to-reach-target-score" xr:uid="{36D724D8-D9C3-4060-9C99-A7969C0ABE14}"/>
+    <hyperlink ref="B1926" r:id="rId1708" display="https://leetcode.com/problems/solving-questions-with-brainpower" xr:uid="{39766A05-57F8-4C7B-88B3-C312FEC7FF0F}"/>
+    <hyperlink ref="B1927" r:id="rId1709" display="https://leetcode.com/problems/maximum-running-time-of-n-computers" xr:uid="{19DD5411-F22B-4D14-9D86-AAED3B112E48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1691"/>
-  <drawing r:id="rId1692"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1710"/>
+  <drawing r:id="rId1711"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
check in new chapter
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF781B69-0134-49E2-83DA-2791768F09A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF414DB7-F2F6-4914-B304-885CBF9F7BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12272,8 +12272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1909" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1927" sqref="A1927"/>
+    <sheetView tabSelected="1" topLeftCell="A1288" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1298" sqref="B1298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -34379,7 +34379,7 @@
         <v>1700</v>
       </c>
       <c r="F942" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G942" t="s">
         <v>151</v>
@@ -46509,7 +46509,7 @@
         <v>3</v>
       </c>
       <c r="D1439" s="57" t="s">
-        <v>1752</v>
+        <v>1700</v>
       </c>
       <c r="E1439" s="61"/>
       <c r="F1439" s="57" t="s">

</xml_diff>

<commit_message>
check in some past contest
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38D89C0-98FE-4FF1-97DB-F1BE27AC5AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79C077F0-D599-40EA-869C-32225A8F7C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,10 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$2095</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$2144</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11901" uniqueCount="4238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11992" uniqueCount="4292">
   <si>
     <t>Difficulty</t>
   </si>
@@ -12751,6 +12752,168 @@
   </si>
   <si>
     <t>Keep maximum and mimum subarray with difference between nums1 and nums2</t>
+  </si>
+  <si>
+    <t>Find Minimum Time to Finish All Jobs II</t>
+  </si>
+  <si>
+    <t>Decode the Message</t>
+  </si>
+  <si>
+    <t>Spiral Matrix IV</t>
+  </si>
+  <si>
+    <t>Number of People Aware of a Secret</t>
+  </si>
+  <si>
+    <t>Number of Increasing Paths in a Grid</t>
+  </si>
+  <si>
+    <t>Valid Palindrome IV</t>
+  </si>
+  <si>
+    <t>Evaluate Boolean Binary Tree</t>
+  </si>
+  <si>
+    <t>The Latest Time to Catch a Bus</t>
+  </si>
+  <si>
+    <t>Minimum Sum of Squared Difference</t>
+  </si>
+  <si>
+    <t>Subarray With Elements Greater Than Varying Threshold</t>
+  </si>
+  <si>
+    <t>Minimum Amount of Time to Fill Cups</t>
+  </si>
+  <si>
+    <t>Smallest Number in Infinite Set</t>
+  </si>
+  <si>
+    <t>Move Pieces to Obtain a String</t>
+  </si>
+  <si>
+    <t>Count the Number of Ideal Arrays</t>
+  </si>
+  <si>
+    <t>Minimum Adjacent Swaps to Make a Valid Array</t>
+  </si>
+  <si>
+    <t>Maximum Number of Pairs in Array</t>
+  </si>
+  <si>
+    <t>Max Sum of a Pair With Equal Sum of Digits</t>
+  </si>
+  <si>
+    <t>Query Kth Smallest Trimmed Number</t>
+  </si>
+  <si>
+    <t>Minimum Deletions to Make Array Divisible</t>
+  </si>
+  <si>
+    <t>Finding the Number of Visible Mountains</t>
+  </si>
+  <si>
+    <t>Best Poker Hand</t>
+  </si>
+  <si>
+    <t>Number of Zero-Filled Subarrays</t>
+  </si>
+  <si>
+    <t>Design a Number Container System</t>
+  </si>
+  <si>
+    <t>Shortest Impossible Sequence of Rolls</t>
+  </si>
+  <si>
+    <t>First Letter to Appear Twice</t>
+  </si>
+  <si>
+    <t>Equal Row and Column Pairs</t>
+  </si>
+  <si>
+    <t>Design a Food Rating System</t>
+  </si>
+  <si>
+    <t>Number of Excellent Pairs</t>
+  </si>
+  <si>
+    <t>Maximum Number of Books You Can Take</t>
+  </si>
+  <si>
+    <t>Make Array Zero by Subtracting Equal Amounts</t>
+  </si>
+  <si>
+    <t>Maximum Number of Groups Entering a Competition</t>
+  </si>
+  <si>
+    <t>Find Closest Node to Given Two Nodes</t>
+  </si>
+  <si>
+    <t>Longest Cycle in a Graph</t>
+  </si>
+  <si>
+    <t>Minimum Costs Using the Train Line</t>
+  </si>
+  <si>
+    <t>Merge Similar Items</t>
+  </si>
+  <si>
+    <t>Count Number of Bad Pairs</t>
+  </si>
+  <si>
+    <t>Task Scheduler II</t>
+  </si>
+  <si>
+    <t>Minimum Replacements to Sort the Array</t>
+  </si>
+  <si>
+    <t>Number of Arithmetic Triplets</t>
+  </si>
+  <si>
+    <t>Reachable Nodes With Restrictions</t>
+  </si>
+  <si>
+    <t>Check if There is a Valid Partition For The Array</t>
+  </si>
+  <si>
+    <t>Longest Ideal Subsequence</t>
+  </si>
+  <si>
+    <t>Minimize Maximum Value in a Grid</t>
+  </si>
+  <si>
+    <t>Largest Local Values in a Matrix</t>
+  </si>
+  <si>
+    <t>Node With Highest Edge Score</t>
+  </si>
+  <si>
+    <t>Construct Smallest Number From DI String</t>
+  </si>
+  <si>
+    <t>Count Special Integers</t>
+  </si>
+  <si>
+    <t>Sort job and worker</t>
+  </si>
+  <si>
+    <t>Search first occurrence of character</t>
+  </si>
+  <si>
+    <t>Rotate and search for empty cell</t>
+  </si>
+  <si>
+    <t>Use two pointer to track know the secret and forget secret</t>
+  </si>
+  <si>
+    <t>Shortest path to track with minimum number</t>
+  </si>
+  <si>
+    <t>Search from begin and end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capture any empty time slot on passenger arrvie time -1 or bus arrive </t>
   </si>
 </sst>
 </file>
@@ -13197,10 +13360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2095"/>
+  <dimension ref="A1:J2144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2073" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2092" sqref="D2092"/>
+    <sheetView tabSelected="1" topLeftCell="A2082" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2101" sqref="C2101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -64518,37 +64681,575 @@
       </c>
     </row>
     <row r="2093" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2093" s="6"/>
+      <c r="A2093">
+        <v>2323</v>
+      </c>
+      <c r="B2093" s="1" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C2093">
+        <v>2</v>
+      </c>
+      <c r="D2093" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2093" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2093" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2093" t="s">
+        <v>4285</v>
+      </c>
+      <c r="I2093" t="s">
+        <v>2996</v>
+      </c>
     </row>
     <row r="2094" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2094" s="7" t="s">
+      <c r="A2094">
+        <v>2325</v>
+      </c>
+      <c r="B2094" s="1" t="s">
+        <v>4239</v>
+      </c>
+      <c r="C2094">
+        <v>1</v>
+      </c>
+      <c r="D2094" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2094" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2094" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2094" t="s">
+        <v>4286</v>
+      </c>
+      <c r="I2094" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2095" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2095">
+        <v>2326</v>
+      </c>
+      <c r="B2095" s="1" t="s">
+        <v>4240</v>
+      </c>
+      <c r="C2095">
+        <v>2</v>
+      </c>
+      <c r="D2095" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2095" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2095" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2095" t="s">
+        <v>4287</v>
+      </c>
+      <c r="I2095" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="2096" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2096">
+        <v>2327</v>
+      </c>
+      <c r="B2096" s="1" t="s">
+        <v>4241</v>
+      </c>
+      <c r="C2096">
+        <v>3</v>
+      </c>
+      <c r="D2096" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2096" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2096" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2096" t="s">
+        <v>618</v>
+      </c>
+      <c r="H2096" t="s">
+        <v>4288</v>
+      </c>
+      <c r="I2096" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2097" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2097">
+        <v>2328</v>
+      </c>
+      <c r="B2097" s="1" t="s">
+        <v>4242</v>
+      </c>
+      <c r="C2097">
+        <v>4</v>
+      </c>
+      <c r="D2097" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2097" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2097" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2097" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2097" t="s">
+        <v>4289</v>
+      </c>
+      <c r="I2097" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="2098" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2098">
+        <v>2330</v>
+      </c>
+      <c r="B2098" s="1" t="s">
+        <v>4243</v>
+      </c>
+      <c r="C2098">
+        <v>2</v>
+      </c>
+      <c r="D2098" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2098" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2098" t="s">
+        <v>618</v>
+      </c>
+      <c r="H2098" t="s">
+        <v>4290</v>
+      </c>
+      <c r="I2098" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2099" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2099">
+        <v>2331</v>
+      </c>
+      <c r="B2099" s="1" t="s">
+        <v>4244</v>
+      </c>
+      <c r="C2099">
+        <v>2</v>
+      </c>
+      <c r="D2099" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2099" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2099" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2099" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2099" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I2099" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2100" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2100">
+        <v>2332</v>
+      </c>
+      <c r="B2100" s="1" t="s">
+        <v>4245</v>
+      </c>
+      <c r="C2100">
+        <v>4</v>
+      </c>
+      <c r="D2100" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2100" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2100" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2100" t="s">
+        <v>4291</v>
+      </c>
+      <c r="I2100" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="2101" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2101">
+        <v>2333</v>
+      </c>
+      <c r="B2101" s="1" t="s">
+        <v>4246</v>
+      </c>
+    </row>
+    <row r="2102" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2102">
+        <v>2334</v>
+      </c>
+      <c r="B2102" s="6" t="s">
+        <v>4247</v>
+      </c>
+    </row>
+    <row r="2103" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2103">
+        <v>2335</v>
+      </c>
+      <c r="B2103" s="1" t="s">
+        <v>4248</v>
+      </c>
+    </row>
+    <row r="2104" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2104">
+        <v>2336</v>
+      </c>
+      <c r="B2104" s="1" t="s">
+        <v>4249</v>
+      </c>
+    </row>
+    <row r="2105" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2105">
+        <v>2337</v>
+      </c>
+      <c r="B2105" s="1" t="s">
+        <v>4250</v>
+      </c>
+    </row>
+    <row r="2106" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2106">
+        <v>2338</v>
+      </c>
+      <c r="B2106" s="1" t="s">
+        <v>4251</v>
+      </c>
+    </row>
+    <row r="2107" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2107">
+        <v>2340</v>
+      </c>
+      <c r="B2107" s="1" t="s">
+        <v>4252</v>
+      </c>
+    </row>
+    <row r="2108" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2108">
+        <v>2341</v>
+      </c>
+      <c r="B2108" s="1" t="s">
+        <v>4253</v>
+      </c>
+    </row>
+    <row r="2109" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2109">
+        <v>2342</v>
+      </c>
+      <c r="B2109" s="6" t="s">
+        <v>4254</v>
+      </c>
+    </row>
+    <row r="2110" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2110">
+        <v>2343</v>
+      </c>
+      <c r="B2110" s="1" t="s">
+        <v>4255</v>
+      </c>
+    </row>
+    <row r="2111" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2111">
+        <v>2344</v>
+      </c>
+      <c r="B2111" s="6" t="s">
+        <v>4256</v>
+      </c>
+    </row>
+    <row r="2112" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2112">
+        <v>2345</v>
+      </c>
+      <c r="B2112" s="6" t="s">
+        <v>4257</v>
+      </c>
+    </row>
+    <row r="2113" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2113">
+        <v>2347</v>
+      </c>
+      <c r="B2113" s="1" t="s">
+        <v>4258</v>
+      </c>
+    </row>
+    <row r="2114" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2114">
+        <v>2348</v>
+      </c>
+      <c r="B2114" s="1" t="s">
+        <v>4259</v>
+      </c>
+    </row>
+    <row r="2115" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2115">
+        <v>2349</v>
+      </c>
+      <c r="B2115" s="1" t="s">
+        <v>4260</v>
+      </c>
+    </row>
+    <row r="2116" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2116">
+        <v>2350</v>
+      </c>
+      <c r="B2116" s="1" t="s">
+        <v>4261</v>
+      </c>
+    </row>
+    <row r="2117" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2117">
+        <v>2351</v>
+      </c>
+      <c r="B2117" s="1" t="s">
+        <v>4262</v>
+      </c>
+    </row>
+    <row r="2118" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2118">
+        <v>2352</v>
+      </c>
+      <c r="B2118" s="1" t="s">
+        <v>4263</v>
+      </c>
+    </row>
+    <row r="2119" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2119">
+        <v>2353</v>
+      </c>
+      <c r="B2119" s="1" t="s">
+        <v>4264</v>
+      </c>
+    </row>
+    <row r="2120" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2120">
+        <v>2354</v>
+      </c>
+      <c r="B2120" s="1" t="s">
+        <v>4265</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2121">
+        <v>2355</v>
+      </c>
+      <c r="B2121" s="6" t="s">
+        <v>4266</v>
+      </c>
+    </row>
+    <row r="2122" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2122">
+        <v>2357</v>
+      </c>
+      <c r="B2122" s="6" t="s">
+        <v>4267</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2123">
+        <v>2358</v>
+      </c>
+      <c r="B2123" s="6" t="s">
+        <v>4268</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2124">
+        <v>2359</v>
+      </c>
+      <c r="B2124" s="6" t="s">
+        <v>4269</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2125">
+        <v>2360</v>
+      </c>
+      <c r="B2125" s="1" t="s">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2126">
+        <v>2361</v>
+      </c>
+      <c r="B2126" s="6" t="s">
+        <v>4271</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2127">
+        <v>2363</v>
+      </c>
+      <c r="B2127" s="1" t="s">
+        <v>4272</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2128">
+        <v>2364</v>
+      </c>
+      <c r="B2128" s="6" t="s">
+        <v>4273</v>
+      </c>
+    </row>
+    <row r="2129" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2129">
+        <v>2365</v>
+      </c>
+      <c r="B2129" s="1" t="s">
+        <v>4274</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2130">
+        <v>2366</v>
+      </c>
+      <c r="B2130" s="1" t="s">
+        <v>4275</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2131">
+        <v>2367</v>
+      </c>
+      <c r="B2131" s="1" t="s">
+        <v>4276</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2132">
+        <v>2368</v>
+      </c>
+      <c r="B2132" s="1" t="s">
+        <v>4277</v>
+      </c>
+    </row>
+    <row r="2133" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2133">
+        <v>2369</v>
+      </c>
+      <c r="B2133" s="6" t="s">
+        <v>4278</v>
+      </c>
+    </row>
+    <row r="2134" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2134">
+        <v>2370</v>
+      </c>
+      <c r="B2134" s="1" t="s">
+        <v>4279</v>
+      </c>
+    </row>
+    <row r="2135" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2135">
+        <v>2371</v>
+      </c>
+      <c r="B2135" s="1" t="s">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="2136" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2136">
+        <v>2373</v>
+      </c>
+      <c r="B2136" s="1" t="s">
+        <v>4281</v>
+      </c>
+    </row>
+    <row r="2137" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2137">
+        <v>2374</v>
+      </c>
+      <c r="B2137" s="1" t="s">
+        <v>4282</v>
+      </c>
+    </row>
+    <row r="2138" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2138">
+        <v>2375</v>
+      </c>
+      <c r="B2138" s="6" t="s">
+        <v>4283</v>
+      </c>
+    </row>
+    <row r="2139" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2139">
+        <v>2376</v>
+      </c>
+      <c r="B2139" s="1" t="s">
+        <v>4284</v>
+      </c>
+    </row>
+    <row r="2140" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B2140" s="6"/>
+    </row>
+    <row r="2141" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B2141" s="1"/>
+    </row>
+    <row r="2142" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B2142" s="6"/>
+    </row>
+    <row r="2143" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2143" s="7" t="s">
         <v>1701</v>
       </c>
-      <c r="B2094" s="7"/>
-      <c r="C2094" s="7"/>
-      <c r="D2094" s="7"/>
-      <c r="E2094" s="7"/>
-      <c r="F2094" s="7"/>
-      <c r="G2094" s="7"/>
-      <c r="H2094" s="7"/>
-    </row>
-    <row r="2095" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2095" s="8" t="s">
+      <c r="B2143" s="7"/>
+      <c r="C2143" s="7"/>
+      <c r="D2143" s="7"/>
+      <c r="E2143" s="7"/>
+      <c r="F2143" s="7"/>
+      <c r="G2143" s="7"/>
+      <c r="H2143" s="7"/>
+    </row>
+    <row r="2144" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2144" s="8" t="s">
         <v>2730</v>
       </c>
-      <c r="B2095" s="8"/>
-      <c r="C2095" s="8"/>
-      <c r="D2095" s="8"/>
-      <c r="E2095" s="8"/>
-      <c r="F2095" s="8"/>
-      <c r="G2095" s="8"/>
-      <c r="H2095" s="8"/>
+      <c r="B2144" s="8"/>
+      <c r="C2144" s="8"/>
+      <c r="D2144" s="8"/>
+      <c r="E2144" s="8"/>
+      <c r="F2144" s="8"/>
+      <c r="G2144" s="8"/>
+      <c r="H2144" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J2095" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J2144" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A2094:H2094"/>
-    <mergeCell ref="A2095:H2095"/>
+    <mergeCell ref="A2143:H2143"/>
+    <mergeCell ref="A2144:H2144"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -66425,10 +67126,57 @@
     <hyperlink ref="B2090" r:id="rId1872" display="https://leetcode.com/problems/count-number-of-ways-to-place-houses" xr:uid="{3A4BF8FC-775A-42F3-97B5-5CDB4570E9F3}"/>
     <hyperlink ref="B2091" r:id="rId1873" display="https://leetcode.com/problems/maximum-score-of-spliced-array" xr:uid="{ED32201D-2186-4AAD-AD4C-685997EEA4E9}"/>
     <hyperlink ref="B2092" r:id="rId1874" display="https://leetcode.com/problems/minimum-score-after-removals-on-a-tree" xr:uid="{63FFD92B-669D-47BD-B35E-98CA1DFB6229}"/>
+    <hyperlink ref="B2093" r:id="rId1875" display="https://leetcode.com/problems/find-minimum-time-to-finish-all-jobs-ii" xr:uid="{6B97A986-5983-4885-92BA-DA5DD588CF3B}"/>
+    <hyperlink ref="B2094" r:id="rId1876" display="https://leetcode.com/problems/decode-the-message" xr:uid="{5CE3173F-AA1F-4423-8A99-ED0D13BB917E}"/>
+    <hyperlink ref="B2095" r:id="rId1877" display="https://leetcode.com/problems/spiral-matrix-iv" xr:uid="{05A11281-0579-4C01-A44E-48A4B693F816}"/>
+    <hyperlink ref="B2096" r:id="rId1878" display="https://leetcode.com/problems/number-of-people-aware-of-a-secret" xr:uid="{5D7AE4B1-99D4-46DE-8DDF-11903D07EF62}"/>
+    <hyperlink ref="B2097" r:id="rId1879" display="https://leetcode.com/problems/number-of-increasing-paths-in-a-grid" xr:uid="{26455AEB-7B79-4134-9119-FDF0CCF94703}"/>
+    <hyperlink ref="B2098" r:id="rId1880" display="https://leetcode.com/problems/valid-palindrome-iv" xr:uid="{A674D015-C147-4BB0-9452-FF507DF7897B}"/>
+    <hyperlink ref="B2099" r:id="rId1881" display="https://leetcode.com/problems/evaluate-boolean-binary-tree" xr:uid="{987255C1-9882-468E-B6E1-EB7DE2DA1120}"/>
+    <hyperlink ref="B2100" r:id="rId1882" display="https://leetcode.com/problems/the-latest-time-to-catch-a-bus" xr:uid="{38C1CEB2-5C21-4854-B6D9-3062A4C0FD51}"/>
+    <hyperlink ref="B2101" r:id="rId1883" display="https://leetcode.com/problems/minimum-sum-of-squared-difference" xr:uid="{3B981F27-98DE-43C7-9F58-D9EC3911E1D8}"/>
+    <hyperlink ref="B2102" r:id="rId1884" display="https://leetcode.com/problems/subarray-with-elements-greater-than-varying-threshold" xr:uid="{808AC964-B6A0-4D87-B09B-E457FA8A8CF0}"/>
+    <hyperlink ref="B2103" r:id="rId1885" display="https://leetcode.com/problems/minimum-amount-of-time-to-fill-cups" xr:uid="{2D8E5234-5297-43CE-BA25-008C014EBBC7}"/>
+    <hyperlink ref="B2104" r:id="rId1886" display="https://leetcode.com/problems/smallest-number-in-infinite-set" xr:uid="{3BA4EA5F-114D-4FF1-B577-0A8345D7BA04}"/>
+    <hyperlink ref="B2105" r:id="rId1887" display="https://leetcode.com/problems/move-pieces-to-obtain-a-string" xr:uid="{AB585ED7-9027-4381-9E3A-A5B5353A1430}"/>
+    <hyperlink ref="B2106" r:id="rId1888" display="https://leetcode.com/problems/count-the-number-of-ideal-arrays" xr:uid="{5146C719-BAE2-4E88-A363-6C43AEA944CE}"/>
+    <hyperlink ref="B2107" r:id="rId1889" display="https://leetcode.com/problems/minimum-adjacent-swaps-to-make-a-valid-array" xr:uid="{FAAB5284-292D-4D9A-A4AC-7EC3BB43B320}"/>
+    <hyperlink ref="B2108" r:id="rId1890" display="https://leetcode.com/problems/maximum-number-of-pairs-in-array" xr:uid="{1266E8CD-C740-46C2-82BC-462C99454183}"/>
+    <hyperlink ref="B2109" r:id="rId1891" display="https://leetcode.com/problems/max-sum-of-a-pair-with-equal-sum-of-digits" xr:uid="{89ADEAB8-EDE8-4A02-A471-B6B9478C8F74}"/>
+    <hyperlink ref="B2110" r:id="rId1892" display="https://leetcode.com/problems/query-kth-smallest-trimmed-number" xr:uid="{E11360C1-1DF6-4A15-9128-2001A61DBAD4}"/>
+    <hyperlink ref="B2111" r:id="rId1893" display="https://leetcode.com/problems/minimum-deletions-to-make-array-divisible" xr:uid="{6BD11646-A99B-4253-B219-7302995BCEEC}"/>
+    <hyperlink ref="B2112" r:id="rId1894" display="https://leetcode.com/problems/finding-the-number-of-visible-mountains" xr:uid="{5034667D-BBF0-4AD3-8FC5-C6F495AE8A6A}"/>
+    <hyperlink ref="B2113" r:id="rId1895" display="https://leetcode.com/problems/best-poker-hand" xr:uid="{501B5AE9-C86A-44C9-A630-9CEDF670F18D}"/>
+    <hyperlink ref="B2114" r:id="rId1896" display="https://leetcode.com/problems/number-of-zero-filled-subarrays" xr:uid="{26D53BBB-1FB7-488F-8F3C-9CFC25E96914}"/>
+    <hyperlink ref="B2115" r:id="rId1897" display="https://leetcode.com/problems/design-a-number-container-system" xr:uid="{2264F5FB-6330-4FFB-BFDF-2E9F2CE4FC61}"/>
+    <hyperlink ref="B2116" r:id="rId1898" display="https://leetcode.com/problems/shortest-impossible-sequence-of-rolls" xr:uid="{68BDE87F-57AD-4F31-8668-16D327586175}"/>
+    <hyperlink ref="B2117" r:id="rId1899" display="https://leetcode.com/problems/first-letter-to-appear-twice" xr:uid="{FD5C6416-652C-40A0-8C30-6E598C8E7B73}"/>
+    <hyperlink ref="B2118" r:id="rId1900" display="https://leetcode.com/problems/equal-row-and-column-pairs" xr:uid="{9FB0EAC3-805C-440A-80CE-ABCD6728DED0}"/>
+    <hyperlink ref="B2119" r:id="rId1901" display="https://leetcode.com/problems/design-a-food-rating-system" xr:uid="{52C8242B-9358-491D-AD3F-D66CB4284446}"/>
+    <hyperlink ref="B2120" r:id="rId1902" display="https://leetcode.com/problems/number-of-excellent-pairs" xr:uid="{A89E940C-B52F-4977-8B67-2C96B733AA50}"/>
+    <hyperlink ref="B2121" r:id="rId1903" display="https://leetcode.com/problems/maximum-number-of-books-you-can-take" xr:uid="{0013984D-6AB0-4E6A-8C6E-B0F43D8438DA}"/>
+    <hyperlink ref="B2122" r:id="rId1904" display="https://leetcode.com/problems/make-array-zero-by-subtracting-equal-amounts" xr:uid="{C0FD1B08-FE35-47EF-9CA4-D90482205731}"/>
+    <hyperlink ref="B2123" r:id="rId1905" display="https://leetcode.com/problems/maximum-number-of-groups-entering-a-competition" xr:uid="{5EC33322-2D51-4764-8598-EA08855EA04E}"/>
+    <hyperlink ref="B2124" r:id="rId1906" display="https://leetcode.com/problems/find-closest-node-to-given-two-nodes" xr:uid="{319A030F-E050-4D7F-A77C-D5CBABAE557D}"/>
+    <hyperlink ref="B2125" r:id="rId1907" display="https://leetcode.com/problems/longest-cycle-in-a-graph" xr:uid="{821559B8-AC92-4D20-BF86-A9E13AC3CD96}"/>
+    <hyperlink ref="B2126" r:id="rId1908" display="https://leetcode.com/problems/minimum-costs-using-the-train-line" xr:uid="{67021357-2275-4D22-9E22-7541EC77F4D9}"/>
+    <hyperlink ref="B2127" r:id="rId1909" display="https://leetcode.com/problems/merge-similar-items" xr:uid="{CB0E0459-F9E4-4A94-B45A-74A8AB8AF71B}"/>
+    <hyperlink ref="B2128" r:id="rId1910" display="https://leetcode.com/problems/count-number-of-bad-pairs" xr:uid="{0E287FB0-75E0-441B-92C5-B374F6AA6AD9}"/>
+    <hyperlink ref="B2129" r:id="rId1911" display="https://leetcode.com/problems/task-scheduler-ii" xr:uid="{64737896-E1AD-4928-8E3F-46CCC3AD7267}"/>
+    <hyperlink ref="B2130" r:id="rId1912" display="https://leetcode.com/problems/minimum-replacements-to-sort-the-array" xr:uid="{1C5DD237-2367-404B-B51C-4B5FB292D805}"/>
+    <hyperlink ref="B2131" r:id="rId1913" display="https://leetcode.com/problems/number-of-arithmetic-triplets" xr:uid="{3945E842-6A3C-4A00-961B-3CC8189FF742}"/>
+    <hyperlink ref="B2132" r:id="rId1914" display="https://leetcode.com/problems/reachable-nodes-with-restrictions" xr:uid="{EFA85FE3-CB7E-4D36-8B60-F88AD7A4D125}"/>
+    <hyperlink ref="B2133" r:id="rId1915" display="https://leetcode.com/problems/check-if-there-is-a-valid-partition-for-the-array" xr:uid="{BE74FAF8-D5C2-4D02-B356-FD5705954B53}"/>
+    <hyperlink ref="B2134" r:id="rId1916" display="https://leetcode.com/problems/longest-ideal-subsequence" xr:uid="{D32B6C66-65C4-49AD-AF05-80C237AFA55B}"/>
+    <hyperlink ref="B2135" r:id="rId1917" display="https://leetcode.com/problems/minimize-maximum-value-in-a-grid" xr:uid="{E2743C74-6A46-4740-B487-202A321BDBE9}"/>
+    <hyperlink ref="B2136" r:id="rId1918" display="https://leetcode.com/problems/largest-local-values-in-a-matrix" xr:uid="{66163439-FBCD-4169-9D95-F547B38FA445}"/>
+    <hyperlink ref="B2137" r:id="rId1919" display="https://leetcode.com/problems/node-with-highest-edge-score" xr:uid="{814DAADD-024A-4E73-9291-C83DB0CD071D}"/>
+    <hyperlink ref="B2138" r:id="rId1920" display="https://leetcode.com/problems/construct-smallest-number-from-di-string" xr:uid="{57DFF274-FBD8-45F1-9D4F-239B0C604A56}"/>
+    <hyperlink ref="B2139" r:id="rId1921" display="https://leetcode.com/problems/count-special-integers" xr:uid="{CE018E0E-0D3E-482C-AD39-0EDC0A156A5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1875"/>
-  <drawing r:id="rId1876"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1922"/>
+  <drawing r:id="rId1923"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add notes for recent weekly contest
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E086576-AA8E-423A-BABC-2A99CC87DEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9733B528-1230-4141-A0C2-BF359DF7AB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$2464</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Algorithm'!$A$1:$J$2482</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14215" uniqueCount="4973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14397" uniqueCount="5029">
   <si>
     <t>Difficulty</t>
   </si>
@@ -14956,6 +14956,174 @@
   </si>
   <si>
     <t>Sort by queries and request, count by hashtable</t>
+  </si>
+  <si>
+    <t>Count Paths That Can Form a Palindrome in a Tree</t>
+  </si>
+  <si>
+    <t>Track path for parity in bits</t>
+  </si>
+  <si>
+    <t>Maximum Number of Groups With Increasing Length</t>
+  </si>
+  <si>
+    <t>Accumulate sums as 1+….+K</t>
+  </si>
+  <si>
+    <t>Largest Element in an Array after Merge Operations</t>
+  </si>
+  <si>
+    <t>Calculate from back to front</t>
+  </si>
+  <si>
+    <t>Split Strings by Separator</t>
+  </si>
+  <si>
+    <t>Word split</t>
+  </si>
+  <si>
+    <t>Ways to Express an Integer as Sum of Powers</t>
+  </si>
+  <si>
+    <t>0, 1 knapsack, track remaining n and searched power numbers</t>
+  </si>
+  <si>
+    <t>Visit Array Positions to Maximize Score</t>
+  </si>
+  <si>
+    <t>Track previous odd or even</t>
+  </si>
+  <si>
+    <t>Sort Vowels in a String</t>
+  </si>
+  <si>
+    <t>Sort vowels and put it back</t>
+  </si>
+  <si>
+    <t>Check if Array is Good</t>
+  </si>
+  <si>
+    <t>Loop array from 1 to N</t>
+  </si>
+  <si>
+    <t>Number of Unique Categories</t>
+  </si>
+  <si>
+    <t>Check against each group</t>
+  </si>
+  <si>
+    <t>Length of the Longest Valid Substring</t>
+  </si>
+  <si>
+    <t>Check reverse word in length of 10, get new left position (incremental)</t>
+  </si>
+  <si>
+    <t>Minimum Index of a Valid Split</t>
+  </si>
+  <si>
+    <t>Get majority item then search in array</t>
+  </si>
+  <si>
+    <t>Maximum Beauty of an Array After Applying Operation</t>
+  </si>
+  <si>
+    <t>Sum of Squares of Special Elements</t>
+  </si>
+  <si>
+    <t>Calculate each item</t>
+  </si>
+  <si>
+    <t>Count Houses in a Circular Street II</t>
+  </si>
+  <si>
+    <t>remember previous open window</t>
+  </si>
+  <si>
+    <t>Longest Even Odd Subarray With Threshold</t>
+  </si>
+  <si>
+    <t>Start with even, the alternative, reset on violation</t>
+  </si>
+  <si>
+    <t>Prime Pairs With Target Sum</t>
+  </si>
+  <si>
+    <t>Find all prime numbers first</t>
+  </si>
+  <si>
+    <t>Height of Special Binary Tree</t>
+  </si>
+  <si>
+    <t>Check leaf by comparing with its children</t>
+  </si>
+  <si>
+    <t>Apply Operations to Make All Array Elements Equal to Zero</t>
+  </si>
+  <si>
+    <t>Check range with difference between maximum and minmum as 2 K</t>
+  </si>
+  <si>
+    <t>Keep track deductable accumulated</t>
+  </si>
+  <si>
+    <t>Longest Non-decreasing Subarray From Two Arrays</t>
+  </si>
+  <si>
+    <t>Track on maximum length based on large and small number</t>
+  </si>
+  <si>
+    <t>Continuous Subarrays</t>
+  </si>
+  <si>
+    <t>Keep track the range with difference between maximum and minimum within 2</t>
+  </si>
+  <si>
+    <t>Sum of Imbalance Numbers of All Subarrays</t>
+  </si>
+  <si>
+    <t>Keep data in sorted map, and compare neighbors in two sides</t>
+  </si>
+  <si>
+    <t>is Array a Preorder of Some ‌Binary Tree</t>
+  </si>
+  <si>
+    <t>Push the visited node in stack and pop it up to match next parent</t>
+  </si>
+  <si>
+    <t>Longest Alternating Subarray</t>
+  </si>
+  <si>
+    <t>Start with +1 and then alternative, reset on violation</t>
+  </si>
+  <si>
+    <t>Relocate Marbles</t>
+  </si>
+  <si>
+    <t>Transition numbers in hash set</t>
+  </si>
+  <si>
+    <t>Maximum Number of Jumps to Reach the Last Index</t>
+  </si>
+  <si>
+    <t>Check from back to front</t>
+  </si>
+  <si>
+    <t>Find the Maximum Achievable Number</t>
+  </si>
+  <si>
+    <t>The gap between two number should be less than 2 K</t>
+  </si>
+  <si>
+    <t>Partition String Into Minimum Beautiful Substrings</t>
+  </si>
+  <si>
+    <t>Search from back to front seach all parkable position</t>
+  </si>
+  <si>
+    <t>Number of Black Blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track on left top corner </t>
   </si>
 </sst>
 </file>
@@ -15402,10 +15570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2464"/>
+  <dimension ref="A1:J2482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2438" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2448" sqref="H2448"/>
+    <sheetView tabSelected="1" topLeftCell="A2451" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2463" sqref="A2463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -76512,61 +76680,804 @@
       </c>
     </row>
     <row r="2453" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2453" s="6"/>
+      <c r="A2453">
+        <v>2753</v>
+      </c>
+      <c r="B2453" s="1" t="s">
+        <v>4998</v>
+      </c>
+      <c r="C2453">
+        <v>4</v>
+      </c>
+      <c r="D2453" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2453" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2453" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2453" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2453" t="s">
+        <v>4999</v>
+      </c>
+      <c r="I2453" t="s">
+        <v>2990</v>
+      </c>
     </row>
     <row r="2454" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2454" s="6"/>
+      <c r="A2454">
+        <v>2760</v>
+      </c>
+      <c r="B2454" s="6" t="s">
+        <v>5000</v>
+      </c>
+      <c r="C2454">
+        <v>2</v>
+      </c>
+      <c r="D2454" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2454" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2454" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2454" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2454" t="s">
+        <v>5001</v>
+      </c>
+      <c r="I2454" t="s">
+        <v>2968</v>
+      </c>
     </row>
     <row r="2455" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2455" s="6"/>
+      <c r="A2455">
+        <v>2761</v>
+      </c>
+      <c r="B2455" s="1" t="s">
+        <v>5002</v>
+      </c>
+      <c r="C2455">
+        <v>3</v>
+      </c>
+      <c r="D2455" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2455" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2455" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2455" t="s">
+        <v>5003</v>
+      </c>
+      <c r="I2455" t="s">
+        <v>2996</v>
+      </c>
     </row>
     <row r="2456" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2456" s="6"/>
+      <c r="A2456">
+        <v>2762</v>
+      </c>
+      <c r="B2456" s="1" t="s">
+        <v>5011</v>
+      </c>
+      <c r="C2456">
+        <v>3</v>
+      </c>
+      <c r="D2456" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2456" t="s">
+        <v>2892</v>
+      </c>
+      <c r="F2456" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2456" t="s">
+        <v>618</v>
+      </c>
+      <c r="H2456" t="s">
+        <v>5012</v>
+      </c>
+      <c r="I2456" t="s">
+        <v>2968</v>
+      </c>
     </row>
     <row r="2457" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2457" s="6"/>
+      <c r="A2457">
+        <v>2763</v>
+      </c>
+      <c r="B2457" s="6" t="s">
+        <v>5013</v>
+      </c>
+      <c r="C2457">
+        <v>4</v>
+      </c>
+      <c r="D2457" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2457" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2457" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2457" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2457" t="s">
+        <v>5014</v>
+      </c>
+      <c r="I2457" t="s">
+        <v>2996</v>
+      </c>
     </row>
     <row r="2458" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2458" s="6"/>
+      <c r="A2458">
+        <v>2764</v>
+      </c>
+      <c r="B2458" s="6" t="s">
+        <v>5015</v>
+      </c>
+      <c r="C2458">
+        <v>3</v>
+      </c>
+      <c r="D2458" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2458" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2458" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2458" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2458" t="s">
+        <v>5016</v>
+      </c>
+      <c r="I2458" t="s">
+        <v>2968</v>
+      </c>
     </row>
     <row r="2459" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2459" s="6"/>
+      <c r="A2459">
+        <v>2765</v>
+      </c>
+      <c r="B2459" s="1" t="s">
+        <v>5017</v>
+      </c>
+      <c r="C2459">
+        <v>2</v>
+      </c>
+      <c r="D2459" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2459" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2459" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2459" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2459" t="s">
+        <v>5018</v>
+      </c>
+      <c r="I2459" t="s">
+        <v>2968</v>
+      </c>
     </row>
     <row r="2460" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2460" s="6"/>
+      <c r="A2460">
+        <v>2766</v>
+      </c>
+      <c r="B2460" s="1" t="s">
+        <v>5019</v>
+      </c>
+      <c r="C2460">
+        <v>2</v>
+      </c>
+      <c r="D2460" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2460" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2460" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2460" t="s">
+        <v>5020</v>
+      </c>
+      <c r="I2460" t="s">
+        <v>2968</v>
+      </c>
     </row>
     <row r="2461" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2461" s="6"/>
+      <c r="A2461">
+        <v>2767</v>
+      </c>
+      <c r="B2461" s="6" t="s">
+        <v>5025</v>
+      </c>
+      <c r="C2461">
+        <v>3</v>
+      </c>
+      <c r="D2461" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2461" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2461" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2461" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2461" t="s">
+        <v>5026</v>
+      </c>
+      <c r="I2461" t="s">
+        <v>3152</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2462">
+        <v>2768</v>
+      </c>
+      <c r="B2462" s="1" t="s">
+        <v>5027</v>
+      </c>
+      <c r="C2462">
+        <v>4</v>
+      </c>
+      <c r="D2462" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2462" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2462" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2462" t="s">
+        <v>5028</v>
+      </c>
+      <c r="I2462" t="s">
+        <v>2968</v>
+      </c>
     </row>
     <row r="2463" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2463" s="7" t="s">
+      <c r="A2463">
+        <v>2769</v>
+      </c>
+      <c r="B2463" s="6" t="s">
+        <v>5023</v>
+      </c>
+      <c r="C2463">
+        <v>1</v>
+      </c>
+      <c r="D2463" t="s">
+        <v>1698</v>
+      </c>
+      <c r="F2463" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2463" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2463" t="s">
+        <v>5024</v>
+      </c>
+      <c r="I2463" t="s">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2464">
+        <v>2770</v>
+      </c>
+      <c r="B2464" s="6" t="s">
+        <v>5021</v>
+      </c>
+      <c r="C2464">
+        <v>4</v>
+      </c>
+      <c r="D2464" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2464" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2464" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2464" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2464" t="s">
+        <v>5022</v>
+      </c>
+      <c r="I2464" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2465">
+        <v>2771</v>
+      </c>
+      <c r="B2465" s="6" t="s">
+        <v>5009</v>
+      </c>
+      <c r="C2465">
+        <v>3</v>
+      </c>
+      <c r="D2465" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2465" t="s">
+        <v>2892</v>
+      </c>
+      <c r="F2465" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2465" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2465" t="s">
+        <v>5010</v>
+      </c>
+      <c r="I2465" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2466">
+        <v>2772</v>
+      </c>
+      <c r="B2466" s="6" t="s">
+        <v>5006</v>
+      </c>
+      <c r="C2466">
+        <v>4</v>
+      </c>
+      <c r="D2466" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2466" t="s">
+        <v>2892</v>
+      </c>
+      <c r="F2466" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2466" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2466" t="s">
+        <v>5008</v>
+      </c>
+      <c r="I2466" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2467">
+        <v>2773</v>
+      </c>
+      <c r="B2467" s="1" t="s">
+        <v>5004</v>
+      </c>
+      <c r="C2467">
+        <v>2</v>
+      </c>
+      <c r="D2467" t="s">
+        <v>1693</v>
+      </c>
+      <c r="F2467" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2467" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2467" t="s">
+        <v>5005</v>
+      </c>
+      <c r="I2467" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2468" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2468">
+        <v>2778</v>
+      </c>
+      <c r="B2468" s="1" t="s">
+        <v>4996</v>
+      </c>
+      <c r="C2468">
+        <v>1</v>
+      </c>
+      <c r="D2468" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2468" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2468" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2468" t="s">
+        <v>4997</v>
+      </c>
+      <c r="I2468" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2469" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2469">
+        <v>2779</v>
+      </c>
+      <c r="B2469" s="6" t="s">
+        <v>4995</v>
+      </c>
+      <c r="C2469">
+        <v>3</v>
+      </c>
+      <c r="D2469" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2469" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2469" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2469" t="s">
+        <v>618</v>
+      </c>
+      <c r="H2469" t="s">
+        <v>5007</v>
+      </c>
+      <c r="I2469" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2470">
+        <v>2780</v>
+      </c>
+      <c r="B2470" s="1" t="s">
+        <v>4993</v>
+      </c>
+      <c r="C2470">
+        <v>2</v>
+      </c>
+      <c r="D2470" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2470" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2470" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2470" t="s">
+        <v>4994</v>
+      </c>
+      <c r="I2470" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2471">
+        <v>2781</v>
+      </c>
+      <c r="B2471" s="1" t="s">
+        <v>4991</v>
+      </c>
+      <c r="C2471">
+        <v>4</v>
+      </c>
+      <c r="D2471" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2471" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2471" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2471" t="s">
+        <v>4992</v>
+      </c>
+      <c r="I2471" t="s">
+        <v>4205</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2472">
+        <v>2782</v>
+      </c>
+      <c r="B2472" s="1" t="s">
+        <v>4989</v>
+      </c>
+      <c r="C2472">
+        <v>2</v>
+      </c>
+      <c r="D2472" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2472" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2472" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2472" t="s">
+        <v>4990</v>
+      </c>
+      <c r="I2472" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="2473" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2473">
+        <v>2784</v>
+      </c>
+      <c r="B2473" s="1" t="s">
+        <v>4987</v>
+      </c>
+      <c r="C2473">
+        <v>1</v>
+      </c>
+      <c r="D2473" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2473" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2473" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2473" t="s">
+        <v>4988</v>
+      </c>
+      <c r="I2473" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2474">
+        <v>2785</v>
+      </c>
+      <c r="B2474" s="1" t="s">
+        <v>4985</v>
+      </c>
+      <c r="C2474">
+        <v>2</v>
+      </c>
+      <c r="D2474" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2474" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2474" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2474" t="s">
+        <v>4986</v>
+      </c>
+      <c r="I2474" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2475">
+        <v>2786</v>
+      </c>
+      <c r="B2475" s="6" t="s">
+        <v>4983</v>
+      </c>
+      <c r="C2475">
+        <v>3</v>
+      </c>
+      <c r="D2475" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2475" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2475" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2475" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2475" t="s">
+        <v>4984</v>
+      </c>
+      <c r="I2475" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2476">
+        <v>2787</v>
+      </c>
+      <c r="B2476" s="6" t="s">
+        <v>4981</v>
+      </c>
+      <c r="C2476">
+        <v>3</v>
+      </c>
+      <c r="D2476" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2476" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F2476" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2476" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2476" t="s">
+        <v>4982</v>
+      </c>
+      <c r="I2476" t="s">
+        <v>2969</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2477">
+        <v>2788</v>
+      </c>
+      <c r="B2477" s="1" t="s">
+        <v>4979</v>
+      </c>
+      <c r="C2477">
+        <v>2</v>
+      </c>
+      <c r="D2477" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2477" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2477" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2477" t="s">
+        <v>4980</v>
+      </c>
+      <c r="I2477" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2478">
+        <v>2789</v>
+      </c>
+      <c r="B2478" s="6" t="s">
+        <v>4977</v>
+      </c>
+      <c r="C2478">
+        <v>2</v>
+      </c>
+      <c r="D2478" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F2478" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2478" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2478" t="s">
+        <v>4978</v>
+      </c>
+      <c r="I2478" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2479">
+        <v>2790</v>
+      </c>
+      <c r="B2479" s="6" t="s">
+        <v>4975</v>
+      </c>
+      <c r="C2479">
+        <v>4</v>
+      </c>
+      <c r="D2479" t="s">
+        <v>1698</v>
+      </c>
+      <c r="F2479" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2479" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2479" t="s">
+        <v>4976</v>
+      </c>
+      <c r="I2479" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2480">
+        <v>2791</v>
+      </c>
+      <c r="B2480" s="6" t="s">
+        <v>4973</v>
+      </c>
+      <c r="C2480">
+        <v>4</v>
+      </c>
+      <c r="D2480" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E2480" t="s">
+        <v>2892</v>
+      </c>
+      <c r="F2480" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2480" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2480" t="s">
+        <v>4974</v>
+      </c>
+      <c r="I2480" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2481" s="7" t="s">
         <v>1701</v>
       </c>
-      <c r="B2463" s="7"/>
-      <c r="C2463" s="7"/>
-      <c r="D2463" s="7"/>
-      <c r="E2463" s="7"/>
-      <c r="F2463" s="7"/>
-      <c r="G2463" s="7"/>
-      <c r="H2463" s="7"/>
-    </row>
-    <row r="2464" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2464" s="8" t="s">
+      <c r="B2481" s="7"/>
+      <c r="C2481" s="7"/>
+      <c r="D2481" s="7"/>
+      <c r="E2481" s="7"/>
+      <c r="F2481" s="7"/>
+      <c r="G2481" s="7"/>
+      <c r="H2481" s="7"/>
+    </row>
+    <row r="2482" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2482" s="8" t="s">
         <v>2730</v>
       </c>
-      <c r="B2464" s="8"/>
-      <c r="C2464" s="8"/>
-      <c r="D2464" s="8"/>
-      <c r="E2464" s="8"/>
-      <c r="F2464" s="8"/>
-      <c r="G2464" s="8"/>
-      <c r="H2464" s="8"/>
+      <c r="B2482" s="8"/>
+      <c r="C2482" s="8"/>
+      <c r="D2482" s="8"/>
+      <c r="E2482" s="8"/>
+      <c r="F2482" s="8"/>
+      <c r="G2482" s="8"/>
+      <c r="H2482" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J2464" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
+  <autoFilter ref="A1:J2482" xr:uid="{CB07CE66-8F15-46FF-A90A-43FDB2DB428F}"/>
   <mergeCells count="2">
-    <mergeCell ref="A2463:H2463"/>
-    <mergeCell ref="A2464:H2464"/>
+    <mergeCell ref="A2481:H2481"/>
+    <mergeCell ref="A2482:H2482"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://leetcode.com/problems/zigzag-conversion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -78802,10 +79713,38 @@
     <hyperlink ref="B2450" r:id="rId2231" display="https://leetcode.com/problems/minimum-operations-to-make-the-integer-zero/" xr:uid="{3A3E3123-7C79-4E34-B5F7-65879B638918}"/>
     <hyperlink ref="B2451" r:id="rId2232" display="https://leetcode.com/problems/ways-to-split-array-into-good-subarrays/" xr:uid="{63245DB8-89CE-4FE7-A87A-8E65B312EE64}"/>
     <hyperlink ref="B2452" r:id="rId2233" display="https://leetcode.com/problems/robot-collisions/" xr:uid="{23CBBC70-E980-4461-A34A-864896FA16BB}"/>
+    <hyperlink ref="B2453" r:id="rId2234" display="https://leetcode.com/problems/count-houses-in-a-circular-street-ii/" xr:uid="{21CF947F-14EB-4B5A-B121-EA5513FED6AA}"/>
+    <hyperlink ref="B2454" r:id="rId2235" display="https://leetcode.com/problems/longest-even-odd-subarray-with-threshold/" xr:uid="{BFCEEFBC-289B-430D-BE0A-2991C5655ACF}"/>
+    <hyperlink ref="B2455" r:id="rId2236" display="https://leetcode.com/problems/prime-pairs-with-target-sum/" xr:uid="{9024C319-2B1F-4B1F-83F3-8EDD42F2B770}"/>
+    <hyperlink ref="B2456" r:id="rId2237" display="https://leetcode.com/problems/continuous-subarrays/" xr:uid="{D1620AFA-16E1-42D8-A540-53FEA977CB29}"/>
+    <hyperlink ref="B2457" r:id="rId2238" display="https://leetcode.com/problems/sum-of-imbalance-numbers-of-all-subarrays/" xr:uid="{70892454-F872-440D-A812-E01483240184}"/>
+    <hyperlink ref="B2458" r:id="rId2239" display="https://leetcode.com/problems/is-array-a-preorder-of-some-binary-tree/" xr:uid="{32C4467D-5527-476A-BAF1-9230DF7ABA1D}"/>
+    <hyperlink ref="B2459" r:id="rId2240" display="https://leetcode.com/problems/longest-alternating-subarray/" xr:uid="{8715DCC1-DA7C-4F21-8E92-EE5EFB4CD7A4}"/>
+    <hyperlink ref="B2460" r:id="rId2241" display="https://leetcode.com/problems/relocate-marbles/" xr:uid="{417C321B-FAD0-4632-9912-ED7441CDA402}"/>
+    <hyperlink ref="B2461" r:id="rId2242" display="https://leetcode.com/problems/partition-string-into-minimum-beautiful-substrings/" xr:uid="{D29C4D0A-7269-41E0-A7F1-683A222CBB1B}"/>
+    <hyperlink ref="B2462" r:id="rId2243" display="https://leetcode.com/problems/number-of-black-blocks/" xr:uid="{B3CDBDD6-89DD-4E25-89FE-F799652E4AD3}"/>
+    <hyperlink ref="B2463" r:id="rId2244" display="https://leetcode.com/problems/find-the-maximum-achievable-number/" xr:uid="{4320C2CE-0512-44D7-BCF7-851D1F6EC624}"/>
+    <hyperlink ref="B2464" r:id="rId2245" display="https://leetcode.com/problems/maximum-number-of-jumps-to-reach-the-last-index/" xr:uid="{CACD1EE0-B699-4A0E-A6B0-D62BBAD4A369}"/>
+    <hyperlink ref="B2465" r:id="rId2246" display="https://leetcode.com/problems/longest-non-decreasing-subarray-from-two-arrays/" xr:uid="{83FCAFD7-60C2-4A62-A958-B855180E65F7}"/>
+    <hyperlink ref="B2466" r:id="rId2247" display="https://leetcode.com/problems/apply-operations-to-make-all-array-elements-equal-to-zero/" xr:uid="{44485EFD-73A9-4752-B37F-9D1232AC936E}"/>
+    <hyperlink ref="B2467" r:id="rId2248" display="https://leetcode.com/problems/height-of-special-binary-tree/" xr:uid="{8CA0108D-FC9B-4949-B00C-0D1C0E13A8B7}"/>
+    <hyperlink ref="B2468" r:id="rId2249" display="https://leetcode.com/problems/sum-of-squares-of-special-elements/" xr:uid="{C775FCE7-A095-4010-9D85-F02DEAF609AE}"/>
+    <hyperlink ref="B2469" r:id="rId2250" display="https://leetcode.com/problems/maximum-beauty-of-an-array-after-applying-operation/" xr:uid="{DB251C19-350C-4324-89A7-9849DF6678C2}"/>
+    <hyperlink ref="B2470" r:id="rId2251" display="https://leetcode.com/problems/minimum-index-of-a-valid-split/" xr:uid="{A83A8D9E-EC4B-4F64-B244-E77B7CED2A70}"/>
+    <hyperlink ref="B2471" r:id="rId2252" display="https://leetcode.com/problems/length-of-the-longest-valid-substring/" xr:uid="{846235E7-0FE7-4716-8AA2-DEEA70E4DAF2}"/>
+    <hyperlink ref="B2472" r:id="rId2253" display="https://leetcode.com/problems/number-of-unique-categories/" xr:uid="{072D1212-86FF-47B5-92EE-A21F53C2BA27}"/>
+    <hyperlink ref="B2473" r:id="rId2254" display="https://leetcode.com/problems/check-if-array-is-good/" xr:uid="{28BE78EA-96BC-4550-B998-B98EF2308CA0}"/>
+    <hyperlink ref="B2474" r:id="rId2255" display="https://leetcode.com/problems/sort-vowels-in-a-string/" xr:uid="{A911AD42-528D-4A9A-A091-72CC64F1450C}"/>
+    <hyperlink ref="B2475" r:id="rId2256" display="https://leetcode.com/problems/visit-array-positions-to-maximize-score/" xr:uid="{9D704516-8CD5-4D4A-85F1-24BC68E21571}"/>
+    <hyperlink ref="B2476" r:id="rId2257" display="https://leetcode.com/problems/ways-to-express-an-integer-as-sum-of-powers/" xr:uid="{69D0F58C-F6C7-4D1D-8F20-AA1898B6FADC}"/>
+    <hyperlink ref="B2477" r:id="rId2258" display="https://leetcode.com/problems/split-strings-by-separator/" xr:uid="{5AE27A1C-8AB0-4B41-BF2B-482E6B267B0C}"/>
+    <hyperlink ref="B2478" r:id="rId2259" display="https://leetcode.com/problems/largest-element-in-an-array-after-merge-operations/" xr:uid="{41EA6F20-EFF2-45BF-93B1-7E8517DD0D98}"/>
+    <hyperlink ref="B2479" r:id="rId2260" display="https://leetcode.com/problems/maximum-number-of-groups-with-increasing-length/" xr:uid="{76AC9861-9CC0-458C-949B-20C2D00231B5}"/>
+    <hyperlink ref="B2480" r:id="rId2261" display="https://leetcode.com/problems/count-paths-that-can-form-a-palindrome-in-a-tree/" xr:uid="{0FE1C52E-A24D-46AC-9E47-9651DF04154C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2234"/>
-  <drawing r:id="rId2235"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2262"/>
+  <drawing r:id="rId2263"/>
 </worksheet>
 </file>
 

</xml_diff>